<commit_message>
Updating name from Budget to Budgetary per official schema
</commit_message>
<xml_diff>
--- a/usaspending_api/data/USAspendingGlossary.xlsx
+++ b/usaspending_api/data/USAspendingGlossary.xlsx
@@ -997,13 +997,13 @@
 [Read more about Award Type](http://fedspendingtransparency.github.io/whitepapers/types/)</t>
   </si>
   <si>
-    <t>Budget Resources</t>
-  </si>
-  <si>
     <t>Budgetary resources mean amounts available to incur obligations in a given year. Budgetary resources consist of new budget authority (from appropriations, borrowing authority, contract authority, or offsetting collections) and unobligated balances of budget authority provided in previous years.</t>
   </si>
   <si>
     <t>Budget Resources Available Amount Total</t>
+  </si>
+  <si>
+    <t>Budgetary Resources</t>
   </si>
 </sst>
 </file>
@@ -1470,8 +1470,8 @@
   <dimension ref="A1:Y1018"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2154,13 +2154,13 @@
     </row>
     <row r="20" spans="1:25" s="24" customFormat="1" ht="78" x14ac:dyDescent="0.15">
       <c r="A20" s="14" t="s">
+        <v>287</v>
+      </c>
+      <c r="B20" s="14" t="s">
         <v>285</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="C20" s="14" t="s">
         <v>286</v>
-      </c>
-      <c r="C20" s="14" t="s">
-        <v>287</v>
       </c>
       <c r="E20" s="16"/>
       <c r="F20" s="23"/>

</xml_diff>

<commit_message>
Change "though the digits are letters, not numbers" to "though the digits may be both letters and numbers"
</commit_message>
<xml_diff>
--- a/usaspending_api/data/USAspendingGlossary.xlsx
+++ b/usaspending_api/data/USAspendingGlossary.xlsx
@@ -455,9 +455,6 @@
   </si>
   <si>
     <t>FAIN</t>
-  </si>
-  <si>
-    <t>An identification code assigned to a specific financial assistance award by an agency for tracking purposes. The FAIN is tied to that award (and all future modifications to that award) throughout the award's life. Within an agency, FAINs are unique; a new award must be issued a new FAIN. FAIN stands for Federal Award Identification Number, though the digits are letters, not numbers.</t>
   </si>
   <si>
     <t>The Federal Award Identification Number (FAIN) is the unique ID within the Federal agency for each financial assistance award.</t>
@@ -1005,6 +1002,9 @@
   <si>
     <t>Budgetary Resources</t>
   </si>
+  <si>
+    <t>An identification code assigned to a specific financial assistance award by an agency for tracking purposes. The FAIN is tied to that award (and all future modifications to that award) throughout the award's life. Within an agency, FAINs are unique; a new award must be issued a new FAIN. FAIN stands for Federal Award Identification Number, though the digits may be both letters and numbers.</t>
+  </si>
 </sst>
 </file>
 
@@ -1019,58 +1019,69 @@
     <font>
       <sz val="12"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color theme="11"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1470,8 +1481,8 @@
   <dimension ref="A1:Y1018"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1777,7 +1788,7 @@
         <v>31</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G9" s="10"/>
       <c r="H9" s="10"/>
@@ -1886,7 +1897,7 @@
         <v>43</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G12" s="10"/>
       <c r="H12" s="10"/>
@@ -2154,13 +2165,13 @@
     </row>
     <row r="20" spans="1:25" s="24" customFormat="1" ht="78" x14ac:dyDescent="0.15">
       <c r="A20" s="14" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B20" s="14" t="s">
+        <v>284</v>
+      </c>
+      <c r="C20" s="14" t="s">
         <v>285</v>
-      </c>
-      <c r="C20" s="14" t="s">
-        <v>286</v>
       </c>
       <c r="E20" s="16"/>
       <c r="F20" s="23"/>
@@ -2652,13 +2663,13 @@
         <v>125</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>126</v>
+        <v>287</v>
       </c>
       <c r="C34" s="8" t="s">
         <v>125</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E34" s="10"/>
       <c r="F34" s="11"/>
@@ -2684,18 +2695,18 @@
     </row>
     <row r="35" spans="1:25" ht="39" x14ac:dyDescent="0.15">
       <c r="A35" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="B35" s="7" t="s">
         <v>128</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>129</v>
       </c>
       <c r="C35" s="6"/>
       <c r="D35" s="9"/>
       <c r="E35" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="F35" s="20" t="s">
         <v>130</v>
-      </c>
-      <c r="F35" s="20" t="s">
-        <v>131</v>
       </c>
       <c r="G35" s="10"/>
       <c r="H35" s="10"/>
@@ -2719,17 +2730,17 @@
     </row>
     <row r="36" spans="1:25" ht="52" x14ac:dyDescent="0.15">
       <c r="A36" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="B36" s="8" t="s">
         <v>132</v>
-      </c>
-      <c r="B36" s="8" t="s">
-        <v>133</v>
       </c>
       <c r="C36" s="14"/>
       <c r="E36" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="F36" s="11" t="s">
         <v>134</v>
-      </c>
-      <c r="F36" s="11" t="s">
-        <v>135</v>
       </c>
       <c r="G36" s="10"/>
       <c r="H36" s="10"/>
@@ -2753,10 +2764,10 @@
     </row>
     <row r="37" spans="1:25" ht="78" x14ac:dyDescent="0.15">
       <c r="A37" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="B37" s="8" t="s">
         <v>136</v>
-      </c>
-      <c r="B37" s="8" t="s">
-        <v>137</v>
       </c>
       <c r="C37" s="6"/>
       <c r="D37" s="9"/>
@@ -2784,10 +2795,10 @@
     </row>
     <row r="38" spans="1:25" ht="156" x14ac:dyDescent="0.15">
       <c r="A38" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="B38" s="8" t="s">
         <v>138</v>
-      </c>
-      <c r="B38" s="8" t="s">
-        <v>139</v>
       </c>
       <c r="C38" s="6"/>
       <c r="D38" s="9"/>
@@ -2815,16 +2826,16 @@
     </row>
     <row r="39" spans="1:25" ht="65" x14ac:dyDescent="0.15">
       <c r="A39" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="B39" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="B39" s="8" t="s">
+      <c r="C39" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="C39" s="8" t="s">
+      <c r="D39" s="8" t="s">
         <v>142</v>
-      </c>
-      <c r="D39" s="8" t="s">
-        <v>143</v>
       </c>
       <c r="E39" s="10"/>
       <c r="F39" s="11"/>
@@ -2850,18 +2861,18 @@
     </row>
     <row r="40" spans="1:25" ht="169" x14ac:dyDescent="0.15">
       <c r="A40" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="B40" s="12" t="s">
         <v>144</v>
-      </c>
-      <c r="B40" s="12" t="s">
-        <v>145</v>
       </c>
       <c r="C40" s="14"/>
       <c r="D40" s="22"/>
       <c r="E40" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="F40" s="11" t="s">
         <v>146</v>
-      </c>
-      <c r="F40" s="11" t="s">
-        <v>147</v>
       </c>
       <c r="G40" s="10"/>
       <c r="H40" s="10"/>
@@ -2885,10 +2896,10 @@
     </row>
     <row r="41" spans="1:25" ht="117" x14ac:dyDescent="0.15">
       <c r="A41" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="B41" s="8" t="s">
         <v>148</v>
-      </c>
-      <c r="B41" s="8" t="s">
-        <v>149</v>
       </c>
       <c r="C41" s="6"/>
       <c r="D41" s="23"/>
@@ -2896,7 +2907,7 @@
         <v>107</v>
       </c>
       <c r="F41" s="11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G41" s="10"/>
       <c r="H41" s="10"/>
@@ -2920,17 +2931,17 @@
     </row>
     <row r="42" spans="1:25" ht="117" x14ac:dyDescent="0.15">
       <c r="A42" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="B42" s="7" t="s">
         <v>151</v>
-      </c>
-      <c r="B42" s="7" t="s">
-        <v>152</v>
       </c>
       <c r="C42" s="6"/>
       <c r="E42" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="F42" s="11" t="s">
         <v>153</v>
-      </c>
-      <c r="F42" s="11" t="s">
-        <v>154</v>
       </c>
       <c r="G42" s="10"/>
       <c r="H42" s="10"/>
@@ -2954,10 +2965,10 @@
     </row>
     <row r="43" spans="1:25" ht="143" x14ac:dyDescent="0.15">
       <c r="A43" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="B43" s="14" t="s">
         <v>155</v>
-      </c>
-      <c r="B43" s="14" t="s">
-        <v>156</v>
       </c>
       <c r="C43" s="6"/>
       <c r="D43" s="9"/>
@@ -2985,16 +2996,16 @@
     </row>
     <row r="44" spans="1:25" ht="59" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="B44" s="29" t="s">
         <v>157</v>
       </c>
-      <c r="B44" s="29" t="s">
+      <c r="C44" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="C44" s="8" t="s">
+      <c r="D44" s="8" t="s">
         <v>159</v>
-      </c>
-      <c r="D44" s="8" t="s">
-        <v>160</v>
       </c>
       <c r="E44" s="10"/>
       <c r="F44" s="11"/>
@@ -3020,16 +3031,16 @@
     </row>
     <row r="45" spans="1:25" ht="156" x14ac:dyDescent="0.15">
       <c r="A45" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="B45" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="B45" s="7" t="s">
+      <c r="C45" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="D45" s="19" t="s">
         <v>162</v>
-      </c>
-      <c r="C45" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="D45" s="19" t="s">
-        <v>163</v>
       </c>
       <c r="E45" s="22"/>
       <c r="F45" s="11"/>
@@ -3055,16 +3066,16 @@
     </row>
     <row r="46" spans="1:25" ht="39" x14ac:dyDescent="0.15">
       <c r="A46" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="B46" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="B46" s="7" t="s">
+      <c r="C46" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="C46" s="8" t="s">
+      <c r="D46" s="19" t="s">
         <v>166</v>
-      </c>
-      <c r="D46" s="19" t="s">
-        <v>167</v>
       </c>
       <c r="E46" s="22"/>
       <c r="F46" s="22"/>
@@ -3090,17 +3101,17 @@
     </row>
     <row r="47" spans="1:25" ht="52" x14ac:dyDescent="0.15">
       <c r="A47" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="B47" s="8" t="s">
         <v>168</v>
-      </c>
-      <c r="B47" s="8" t="s">
-        <v>169</v>
       </c>
       <c r="C47" s="6"/>
       <c r="E47" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="F47" s="22" t="s">
         <v>170</v>
-      </c>
-      <c r="F47" s="22" t="s">
-        <v>171</v>
       </c>
       <c r="G47" s="10"/>
       <c r="H47" s="10"/>
@@ -3124,22 +3135,22 @@
     </row>
     <row r="48" spans="1:25" ht="65" x14ac:dyDescent="0.15">
       <c r="A48" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="B48" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="B48" s="8" t="s">
+      <c r="C48" s="19" t="s">
         <v>173</v>
       </c>
-      <c r="C48" s="19" t="s">
+      <c r="D48" s="19" t="s">
         <v>174</v>
       </c>
-      <c r="D48" s="19" t="s">
+      <c r="E48" s="16" t="s">
         <v>175</v>
       </c>
-      <c r="E48" s="16" t="s">
+      <c r="F48" s="11" t="s">
         <v>176</v>
-      </c>
-      <c r="F48" s="11" t="s">
-        <v>177</v>
       </c>
       <c r="G48" s="10"/>
       <c r="H48" s="10"/>
@@ -3163,22 +3174,22 @@
     </row>
     <row r="49" spans="1:25" ht="104" x14ac:dyDescent="0.15">
       <c r="A49" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="B49" s="8" t="s">
         <v>178</v>
       </c>
-      <c r="B49" s="8" t="s">
+      <c r="C49" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="D49" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="C49" s="8" t="s">
-        <v>178</v>
-      </c>
-      <c r="D49" s="8" t="s">
+      <c r="E49" s="15" t="s">
         <v>180</v>
       </c>
-      <c r="E49" s="15" t="s">
+      <c r="F49" s="11" t="s">
         <v>181</v>
-      </c>
-      <c r="F49" s="11" t="s">
-        <v>182</v>
       </c>
       <c r="G49" s="10"/>
       <c r="H49" s="10"/>
@@ -3202,22 +3213,22 @@
     </row>
     <row r="50" spans="1:25" ht="91" x14ac:dyDescent="0.15">
       <c r="A50" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="B50" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="B50" s="7" t="s">
+      <c r="C50" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="D50" s="8" t="s">
         <v>184</v>
-      </c>
-      <c r="C50" s="8" t="s">
-        <v>183</v>
-      </c>
-      <c r="D50" s="8" t="s">
-        <v>185</v>
       </c>
       <c r="E50" s="15" t="s">
         <v>73</v>
       </c>
       <c r="F50" s="11" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G50" s="10"/>
       <c r="H50" s="10"/>
@@ -3241,16 +3252,16 @@
     </row>
     <row r="51" spans="1:25" ht="104" x14ac:dyDescent="0.15">
       <c r="A51" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="B51" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="B51" s="7" t="s">
+      <c r="C51" s="8" t="s">
         <v>188</v>
       </c>
-      <c r="C51" s="8" t="s">
+      <c r="D51" s="8" t="s">
         <v>189</v>
-      </c>
-      <c r="D51" s="8" t="s">
-        <v>190</v>
       </c>
       <c r="E51" s="10"/>
       <c r="F51" s="11"/>
@@ -3276,10 +3287,10 @@
     </row>
     <row r="52" spans="1:25" ht="91" x14ac:dyDescent="0.15">
       <c r="A52" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="B52" s="8" t="s">
         <v>191</v>
-      </c>
-      <c r="B52" s="8" t="s">
-        <v>192</v>
       </c>
       <c r="C52" s="25"/>
       <c r="D52" s="26"/>
@@ -3307,16 +3318,16 @@
     </row>
     <row r="53" spans="1:25" ht="65" x14ac:dyDescent="0.15">
       <c r="A53" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="B53" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="B53" s="7" t="s">
+      <c r="C53" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="D53" s="8" t="s">
         <v>194</v>
-      </c>
-      <c r="C53" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="D53" s="8" t="s">
-        <v>195</v>
       </c>
       <c r="E53" s="10"/>
       <c r="F53" s="11"/>
@@ -3342,17 +3353,17 @@
     </row>
     <row r="54" spans="1:25" ht="277.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="B54" s="8" t="s">
         <v>196</v>
-      </c>
-      <c r="B54" s="8" t="s">
-        <v>197</v>
       </c>
       <c r="C54" s="6"/>
       <c r="E54" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="F54" s="14" t="s">
         <v>198</v>
-      </c>
-      <c r="F54" s="14" t="s">
-        <v>199</v>
       </c>
       <c r="G54" s="10"/>
       <c r="H54" s="10"/>
@@ -3376,16 +3387,16 @@
     </row>
     <row r="55" spans="1:25" ht="169" x14ac:dyDescent="0.15">
       <c r="A55" s="14" t="s">
+        <v>199</v>
+      </c>
+      <c r="B55" s="14" t="s">
         <v>200</v>
       </c>
-      <c r="B55" s="14" t="s">
+      <c r="C55" s="8" t="s">
         <v>201</v>
       </c>
-      <c r="C55" s="8" t="s">
+      <c r="D55" s="8" t="s">
         <v>202</v>
-      </c>
-      <c r="D55" s="8" t="s">
-        <v>203</v>
       </c>
       <c r="E55" s="10"/>
       <c r="F55" s="11"/>
@@ -3411,16 +3422,16 @@
     </row>
     <row r="56" spans="1:25" ht="52" x14ac:dyDescent="0.15">
       <c r="A56" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="B56" s="14" t="s">
         <v>204</v>
       </c>
-      <c r="B56" s="14" t="s">
+      <c r="C56" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="D56" s="8" t="s">
         <v>205</v>
-      </c>
-      <c r="C56" s="8" t="s">
-        <v>204</v>
-      </c>
-      <c r="D56" s="8" t="s">
-        <v>206</v>
       </c>
       <c r="E56" s="10"/>
       <c r="F56" s="11"/>
@@ -3446,10 +3457,10 @@
     </row>
     <row r="57" spans="1:25" ht="65" x14ac:dyDescent="0.15">
       <c r="A57" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="B57" s="8" t="s">
         <v>207</v>
-      </c>
-      <c r="B57" s="8" t="s">
-        <v>208</v>
       </c>
       <c r="C57" s="6"/>
       <c r="D57" s="9"/>
@@ -3477,16 +3488,16 @@
     </row>
     <row r="58" spans="1:25" ht="65" x14ac:dyDescent="0.15">
       <c r="A58" s="14" t="s">
+        <v>208</v>
+      </c>
+      <c r="B58" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="B58" s="8" t="s">
+      <c r="C58" s="8" t="s">
         <v>210</v>
       </c>
-      <c r="C58" s="8" t="s">
+      <c r="D58" s="8" t="s">
         <v>211</v>
-      </c>
-      <c r="D58" s="8" t="s">
-        <v>212</v>
       </c>
       <c r="E58" s="10"/>
       <c r="F58" s="11"/>
@@ -3512,16 +3523,16 @@
     </row>
     <row r="59" spans="1:25" ht="91" x14ac:dyDescent="0.15">
       <c r="A59" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="B59" s="14" t="s">
         <v>213</v>
       </c>
-      <c r="B59" s="14" t="s">
+      <c r="C59" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="C59" s="8" t="s">
+      <c r="D59" s="8" t="s">
         <v>215</v>
-      </c>
-      <c r="D59" s="8" t="s">
-        <v>216</v>
       </c>
       <c r="E59" s="10"/>
       <c r="F59" s="11"/>
@@ -3547,16 +3558,16 @@
     </row>
     <row r="60" spans="1:25" ht="117" x14ac:dyDescent="0.15">
       <c r="A60" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="B60" s="8" t="s">
         <v>217</v>
       </c>
-      <c r="B60" s="8" t="s">
+      <c r="C60" s="8" t="s">
         <v>218</v>
       </c>
-      <c r="C60" s="8" t="s">
+      <c r="D60" s="8" t="s">
         <v>219</v>
-      </c>
-      <c r="D60" s="8" t="s">
-        <v>220</v>
       </c>
       <c r="E60" s="10"/>
       <c r="F60" s="11"/>
@@ -3582,22 +3593,22 @@
     </row>
     <row r="61" spans="1:25" ht="104" x14ac:dyDescent="0.15">
       <c r="A61" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="B61" s="8" t="s">
         <v>221</v>
       </c>
-      <c r="B61" s="8" t="s">
+      <c r="C61" s="8" t="s">
         <v>222</v>
       </c>
-      <c r="C61" s="8" t="s">
+      <c r="D61" s="8" t="s">
         <v>223</v>
       </c>
-      <c r="D61" s="8" t="s">
+      <c r="E61" s="16" t="s">
         <v>224</v>
       </c>
-      <c r="E61" s="16" t="s">
+      <c r="F61" s="11" t="s">
         <v>225</v>
-      </c>
-      <c r="F61" s="11" t="s">
-        <v>226</v>
       </c>
       <c r="G61" s="10"/>
       <c r="H61" s="10"/>
@@ -3621,10 +3632,10 @@
     </row>
     <row r="62" spans="1:25" ht="39" x14ac:dyDescent="0.15">
       <c r="A62" s="14" t="s">
+        <v>226</v>
+      </c>
+      <c r="B62" s="7" t="s">
         <v>227</v>
-      </c>
-      <c r="B62" s="7" t="s">
-        <v>228</v>
       </c>
       <c r="C62" s="6"/>
       <c r="D62" s="9"/>
@@ -3652,22 +3663,22 @@
     </row>
     <row r="63" spans="1:25" ht="234" x14ac:dyDescent="0.15">
       <c r="A63" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="B63" s="7" t="s">
         <v>229</v>
       </c>
-      <c r="B63" s="7" t="s">
+      <c r="C63" s="8" t="s">
         <v>230</v>
       </c>
-      <c r="C63" s="8" t="s">
+      <c r="D63" s="8" t="s">
         <v>231</v>
       </c>
-      <c r="D63" s="8" t="s">
+      <c r="E63" s="15" t="s">
         <v>232</v>
       </c>
-      <c r="E63" s="15" t="s">
+      <c r="F63" s="11" t="s">
         <v>233</v>
-      </c>
-      <c r="F63" s="11" t="s">
-        <v>234</v>
       </c>
       <c r="G63" s="10"/>
       <c r="H63" s="10"/>
@@ -3691,16 +3702,16 @@
     </row>
     <row r="64" spans="1:25" ht="52" x14ac:dyDescent="0.15">
       <c r="A64" s="14" t="s">
+        <v>234</v>
+      </c>
+      <c r="B64" s="14" t="s">
         <v>235</v>
       </c>
-      <c r="B64" s="14" t="s">
+      <c r="C64" s="14" t="s">
         <v>236</v>
       </c>
-      <c r="C64" s="14" t="s">
+      <c r="D64" s="14" t="s">
         <v>237</v>
-      </c>
-      <c r="D64" s="14" t="s">
-        <v>238</v>
       </c>
       <c r="E64" s="10"/>
       <c r="F64" s="11"/>
@@ -3726,16 +3737,16 @@
     </row>
     <row r="65" spans="1:25" ht="104" x14ac:dyDescent="0.15">
       <c r="A65" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="B65" s="7" t="s">
         <v>239</v>
       </c>
-      <c r="B65" s="7" t="s">
+      <c r="C65" s="8" t="s">
         <v>240</v>
       </c>
-      <c r="C65" s="8" t="s">
+      <c r="D65" s="8" t="s">
         <v>241</v>
-      </c>
-      <c r="D65" s="8" t="s">
-        <v>242</v>
       </c>
       <c r="E65" s="10"/>
       <c r="F65" s="11"/>
@@ -3761,22 +3772,22 @@
     </row>
     <row r="66" spans="1:25" ht="65" x14ac:dyDescent="0.15">
       <c r="A66" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="B66" s="7" t="s">
         <v>243</v>
       </c>
-      <c r="B66" s="7" t="s">
+      <c r="C66" s="8" t="s">
         <v>244</v>
       </c>
-      <c r="C66" s="8" t="s">
+      <c r="D66" s="19" t="s">
         <v>245</v>
       </c>
-      <c r="D66" s="19" t="s">
+      <c r="E66" s="16" t="s">
         <v>246</v>
       </c>
-      <c r="E66" s="16" t="s">
+      <c r="F66" s="8" t="s">
         <v>247</v>
-      </c>
-      <c r="F66" s="8" t="s">
-        <v>248</v>
       </c>
       <c r="G66" s="10"/>
       <c r="H66" s="10"/>
@@ -3800,17 +3811,17 @@
     </row>
     <row r="67" spans="1:25" ht="52" x14ac:dyDescent="0.15">
       <c r="A67" s="8" t="s">
+        <v>248</v>
+      </c>
+      <c r="B67" s="27" t="s">
         <v>249</v>
-      </c>
-      <c r="B67" s="27" t="s">
-        <v>250</v>
       </c>
       <c r="C67" s="6"/>
       <c r="E67" s="15" t="s">
+        <v>250</v>
+      </c>
+      <c r="F67" s="8" t="s">
         <v>251</v>
-      </c>
-      <c r="F67" s="8" t="s">
-        <v>252</v>
       </c>
       <c r="G67" s="10"/>
       <c r="H67" s="10"/>
@@ -3834,10 +3845,10 @@
     </row>
     <row r="68" spans="1:25" ht="52" x14ac:dyDescent="0.15">
       <c r="A68" s="14" t="s">
+        <v>252</v>
+      </c>
+      <c r="B68" s="14" t="s">
         <v>253</v>
-      </c>
-      <c r="B68" s="14" t="s">
-        <v>254</v>
       </c>
       <c r="C68" s="6"/>
       <c r="D68" s="9"/>
@@ -3865,16 +3876,16 @@
     </row>
     <row r="69" spans="1:25" ht="52" x14ac:dyDescent="0.15">
       <c r="A69" s="14" t="s">
+        <v>254</v>
+      </c>
+      <c r="B69" s="14" t="s">
         <v>255</v>
       </c>
-      <c r="B69" s="14" t="s">
+      <c r="C69" s="8" t="s">
         <v>256</v>
       </c>
-      <c r="C69" s="8" t="s">
+      <c r="D69" s="8" t="s">
         <v>257</v>
-      </c>
-      <c r="D69" s="8" t="s">
-        <v>258</v>
       </c>
       <c r="E69" s="10"/>
       <c r="F69" s="11"/>
@@ -3900,10 +3911,10 @@
     </row>
     <row r="70" spans="1:25" ht="39" x14ac:dyDescent="0.15">
       <c r="A70" s="14" t="s">
+        <v>258</v>
+      </c>
+      <c r="B70" s="14" t="s">
         <v>259</v>
-      </c>
-      <c r="B70" s="14" t="s">
-        <v>260</v>
       </c>
       <c r="C70" s="6"/>
       <c r="D70" s="9"/>
@@ -3931,10 +3942,10 @@
     </row>
     <row r="71" spans="1:25" ht="78" x14ac:dyDescent="0.15">
       <c r="A71" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="B71" s="14" t="s">
         <v>261</v>
-      </c>
-      <c r="B71" s="14" t="s">
-        <v>262</v>
       </c>
       <c r="C71" s="6"/>
       <c r="D71" s="9"/>
@@ -3962,16 +3973,16 @@
     </row>
     <row r="72" spans="1:25" ht="182" x14ac:dyDescent="0.15">
       <c r="A72" s="8" t="s">
+        <v>262</v>
+      </c>
+      <c r="B72" s="7" t="s">
         <v>263</v>
       </c>
-      <c r="B72" s="7" t="s">
+      <c r="C72" s="8" t="s">
         <v>264</v>
       </c>
-      <c r="C72" s="8" t="s">
+      <c r="D72" s="8" t="s">
         <v>265</v>
-      </c>
-      <c r="D72" s="8" t="s">
-        <v>266</v>
       </c>
       <c r="E72" s="10"/>
       <c r="F72" s="11"/>
@@ -3997,10 +4008,10 @@
     </row>
     <row r="73" spans="1:25" ht="78" x14ac:dyDescent="0.15">
       <c r="A73" s="14" t="s">
+        <v>266</v>
+      </c>
+      <c r="B73" s="8" t="s">
         <v>267</v>
-      </c>
-      <c r="B73" s="8" t="s">
-        <v>268</v>
       </c>
       <c r="C73" s="6"/>
       <c r="D73" s="9"/>
@@ -4008,7 +4019,7 @@
         <v>107</v>
       </c>
       <c r="F73" s="11" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G73" s="10"/>
       <c r="H73" s="10"/>
@@ -4032,10 +4043,10 @@
     </row>
     <row r="74" spans="1:25" ht="42" x14ac:dyDescent="0.15">
       <c r="A74" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="B74" s="28" t="s">
         <v>270</v>
-      </c>
-      <c r="B74" s="28" t="s">
-        <v>271</v>
       </c>
       <c r="C74" s="6"/>
       <c r="D74" s="9"/>
@@ -4063,14 +4074,14 @@
     </row>
     <row r="75" spans="1:25" ht="286" x14ac:dyDescent="0.15">
       <c r="A75" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="B75" s="12" t="s">
         <v>272</v>
-      </c>
-      <c r="B75" s="12" t="s">
-        <v>273</v>
       </c>
       <c r="C75" s="6"/>
       <c r="D75" s="19" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E75" s="10"/>
       <c r="F75" s="11"/>
@@ -4096,16 +4107,16 @@
     </row>
     <row r="76" spans="1:25" ht="91" x14ac:dyDescent="0.15">
       <c r="A76" s="8" t="s">
+        <v>274</v>
+      </c>
+      <c r="B76" s="7" t="s">
         <v>275</v>
       </c>
-      <c r="B76" s="7" t="s">
+      <c r="C76" s="8" t="s">
+        <v>274</v>
+      </c>
+      <c r="D76" s="8" t="s">
         <v>276</v>
-      </c>
-      <c r="C76" s="8" t="s">
-        <v>275</v>
-      </c>
-      <c r="D76" s="8" t="s">
-        <v>277</v>
       </c>
       <c r="E76" s="17"/>
       <c r="F76" s="11"/>
@@ -4131,22 +4142,22 @@
     </row>
     <row r="77" spans="1:25" ht="52" x14ac:dyDescent="0.15">
       <c r="A77" s="14" t="s">
+        <v>277</v>
+      </c>
+      <c r="B77" s="14" t="s">
         <v>278</v>
       </c>
-      <c r="B77" s="14" t="s">
+      <c r="C77" s="8" t="s">
+        <v>277</v>
+      </c>
+      <c r="D77" s="8" t="s">
         <v>279</v>
       </c>
-      <c r="C77" s="8" t="s">
-        <v>278</v>
-      </c>
-      <c r="D77" s="8" t="s">
+      <c r="E77" s="16" t="s">
         <v>280</v>
       </c>
-      <c r="E77" s="16" t="s">
+      <c r="F77" s="11" t="s">
         <v>281</v>
-      </c>
-      <c r="F77" s="11" t="s">
-        <v>282</v>
       </c>
       <c r="G77" s="10"/>
       <c r="H77" s="10"/>

</xml_diff>

<commit_message>
Updating glossary content to populate empty, required fields. Fixed unit tests
</commit_message>
<xml_diff>
--- a/usaspending_api/data/USAspendingGlossary.xlsx
+++ b/usaspending_api/data/USAspendingGlossary.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10116"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rmazia01\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gitapabla/Documents/Projects/Bureau of Fiscal Service/Website/Admin/Glossary/030218_PM/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-75" yWindow="5385" windowWidth="20565" windowHeight="2235" tabRatio="500"/>
+    <workbookView xWindow="-20" yWindow="460" windowWidth="25620" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="405">
   <si>
     <t>Term</t>
   </si>
@@ -1905,22 +1905,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y1017"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B103" sqref="B103"/>
+    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D119" sqref="D119"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="27" style="1" customWidth="1"/>
     <col min="2" max="2" width="43" style="1" customWidth="1"/>
-    <col min="3" max="3" width="27.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="44.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="44.33203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="29" style="1" customWidth="1"/>
-    <col min="6" max="6" width="24.7109375" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="14.42578125" style="2"/>
+    <col min="6" max="6" width="24.6640625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="14.5" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" ht="26" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1959,7 +1959,7 @@
       <c r="X1" s="5"/>
       <c r="Y1" s="5"/>
     </row>
-    <row r="2" spans="1:25" s="6" customFormat="1" ht="127.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:25" s="6" customFormat="1" ht="130" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
         <v>240</v>
       </c>
@@ -1977,9 +1977,13 @@
       </c>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:25" s="6" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
+    <row r="3" spans="1:25" s="6" customFormat="1" ht="39" x14ac:dyDescent="0.15">
+      <c r="A3" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>272</v>
+      </c>
       <c r="C3" s="3" t="s">
         <v>271</v>
       </c>
@@ -1989,7 +1993,7 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:25" s="6" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:25" s="6" customFormat="1" ht="104" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
         <v>273</v>
       </c>
@@ -2005,19 +2009,23 @@
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:25" s="6" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:25" s="6" customFormat="1" ht="65" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>311</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
+      <c r="C5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>311</v>
+      </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" spans="1:25" s="6" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:25" s="6" customFormat="1" ht="39" x14ac:dyDescent="0.15">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -2033,7 +2041,7 @@
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="1:25" s="6" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:25" s="6" customFormat="1" ht="52" x14ac:dyDescent="0.15">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
@@ -2049,19 +2057,23 @@
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="1:25" s="6" customFormat="1" ht="178.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:25" s="6" customFormat="1" ht="169" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
+      <c r="C8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="1:25" s="6" customFormat="1" ht="191.25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:25" s="6" customFormat="1" ht="169" x14ac:dyDescent="0.15">
       <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
@@ -2079,7 +2091,7 @@
       </c>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="1:25" s="6" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:25" s="6" customFormat="1" ht="78" x14ac:dyDescent="0.15">
       <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
@@ -2095,19 +2107,23 @@
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
     </row>
-    <row r="11" spans="1:25" s="6" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:25" s="6" customFormat="1" ht="78" x14ac:dyDescent="0.15">
       <c r="A11" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>370</v>
       </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>370</v>
+      </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
     </row>
-    <row r="12" spans="1:25" s="6" customFormat="1" ht="153" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:25" s="6" customFormat="1" ht="143" x14ac:dyDescent="0.15">
       <c r="A12" s="3" t="s">
         <v>23</v>
       </c>
@@ -2127,7 +2143,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="13" spans="1:25" s="6" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:25" s="6" customFormat="1" ht="52" x14ac:dyDescent="0.15">
       <c r="A13" s="3" t="s">
         <v>26</v>
       </c>
@@ -2143,7 +2159,7 @@
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
     </row>
-    <row r="14" spans="1:25" s="6" customFormat="1" ht="140.25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:25" s="6" customFormat="1" ht="130" x14ac:dyDescent="0.15">
       <c r="A14" s="3" t="s">
         <v>30</v>
       </c>
@@ -2163,7 +2179,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="15" spans="1:25" s="6" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:25" s="6" customFormat="1" ht="65" x14ac:dyDescent="0.15">
       <c r="A15" s="3" t="s">
         <v>34</v>
       </c>
@@ -2179,7 +2195,7 @@
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
     </row>
-    <row r="16" spans="1:25" s="6" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:25" s="6" customFormat="1" ht="39" x14ac:dyDescent="0.15">
       <c r="A16" s="3" t="s">
         <v>353</v>
       </c>
@@ -2195,7 +2211,7 @@
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
     </row>
-    <row r="17" spans="1:6" s="6" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" s="6" customFormat="1" ht="52" x14ac:dyDescent="0.15">
       <c r="A17" s="3" t="s">
         <v>347</v>
       </c>
@@ -2211,7 +2227,7 @@
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="1:6" s="6" customFormat="1" ht="127.5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" s="6" customFormat="1" ht="130" x14ac:dyDescent="0.15">
       <c r="A18" s="3" t="s">
         <v>36</v>
       </c>
@@ -2229,15 +2245,19 @@
       </c>
       <c r="F18" s="3"/>
     </row>
-    <row r="19" spans="1:6" s="6" customFormat="1" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" s="6" customFormat="1" ht="70.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="3" t="s">
         <v>40</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
+      <c r="C19" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="E19" s="8" t="s">
         <v>42</v>
       </c>
@@ -2245,7 +2265,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:6" s="6" customFormat="1" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" s="6" customFormat="1" ht="70.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="3" t="s">
         <v>44</v>
       </c>
@@ -2261,15 +2281,19 @@
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="1:6" s="6" customFormat="1" ht="344.25" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" s="6" customFormat="1" ht="325" x14ac:dyDescent="0.15">
       <c r="A21" s="3" t="s">
         <v>47</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
+      <c r="C21" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>48</v>
+      </c>
       <c r="E21" s="8" t="s">
         <v>49</v>
       </c>
@@ -2277,21 +2301,23 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:6" s="6" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" s="6" customFormat="1" ht="117" x14ac:dyDescent="0.15">
       <c r="A22" s="3" t="s">
         <v>243</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="C22" s="3"/>
+      <c r="C22" s="3" t="s">
+        <v>243</v>
+      </c>
       <c r="D22" s="3" t="s">
         <v>396</v>
       </c>
       <c r="E22" s="8"/>
       <c r="F22" s="3"/>
     </row>
-    <row r="23" spans="1:6" s="6" customFormat="1" ht="191.25" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" s="6" customFormat="1" ht="182" x14ac:dyDescent="0.15">
       <c r="A23" s="3" t="s">
         <v>51</v>
       </c>
@@ -2307,12 +2333,16 @@
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
     </row>
-    <row r="24" spans="1:6" s="6" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" s="6" customFormat="1" ht="91" x14ac:dyDescent="0.15">
       <c r="A24" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
+      <c r="B24" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="D24" s="3" t="s">
         <v>259</v>
       </c>
@@ -2321,47 +2351,59 @@
       </c>
       <c r="F24" s="3"/>
     </row>
-    <row r="25" spans="1:6" s="6" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" s="6" customFormat="1" ht="104" x14ac:dyDescent="0.15">
       <c r="A25" s="3" t="s">
         <v>54</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>385</v>
       </c>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
+      <c r="C25" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>385</v>
+      </c>
       <c r="E25" s="8" t="s">
         <v>315</v>
       </c>
       <c r="F25" s="3"/>
     </row>
-    <row r="26" spans="1:6" s="6" customFormat="1" ht="153" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" s="6" customFormat="1" ht="156" x14ac:dyDescent="0.15">
       <c r="A26" s="3" t="s">
         <v>386</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>387</v>
       </c>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
+      <c r="C26" s="3" t="s">
+        <v>386</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>387</v>
+      </c>
       <c r="E26" s="8" t="s">
         <v>315</v>
       </c>
       <c r="F26" s="3"/>
     </row>
-    <row r="27" spans="1:6" s="6" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" s="6" customFormat="1" ht="91" x14ac:dyDescent="0.15">
       <c r="A27" s="3" t="s">
         <v>233</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
+      <c r="C27" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>232</v>
+      </c>
       <c r="E27" s="8"/>
       <c r="F27" s="3"/>
     </row>
-    <row r="28" spans="1:6" s="6" customFormat="1" ht="140.25" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" s="6" customFormat="1" ht="130" x14ac:dyDescent="0.15">
       <c r="A28" s="3" t="s">
         <v>59</v>
       </c>
@@ -2381,7 +2423,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:6" s="6" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" s="6" customFormat="1" ht="52" x14ac:dyDescent="0.15">
       <c r="A29" s="3" t="s">
         <v>55</v>
       </c>
@@ -2397,21 +2439,23 @@
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
     </row>
-    <row r="30" spans="1:6" s="6" customFormat="1" ht="204" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" s="6" customFormat="1" ht="195" x14ac:dyDescent="0.15">
       <c r="A30" s="3" t="s">
         <v>241</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="C30" s="3"/>
+      <c r="C30" s="3" t="s">
+        <v>241</v>
+      </c>
       <c r="D30" s="3" t="s">
         <v>397</v>
       </c>
       <c r="E30" s="8"/>
       <c r="F30" s="3"/>
     </row>
-    <row r="31" spans="1:6" s="6" customFormat="1" ht="242.25" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" s="6" customFormat="1" ht="247" x14ac:dyDescent="0.15">
       <c r="A31" s="3" t="s">
         <v>63</v>
       </c>
@@ -2431,19 +2475,23 @@
         <v>68</v>
       </c>
     </row>
-    <row r="32" spans="1:6" s="6" customFormat="1" ht="127.5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" s="6" customFormat="1" ht="130" x14ac:dyDescent="0.15">
       <c r="A32" s="3" t="s">
         <v>69</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
+      <c r="C32" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>70</v>
+      </c>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
     </row>
-    <row r="33" spans="1:6" s="6" customFormat="1" ht="382.5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" s="6" customFormat="1" ht="377" x14ac:dyDescent="0.15">
       <c r="A33" s="3" t="s">
         <v>238</v>
       </c>
@@ -2461,15 +2509,19 @@
       </c>
       <c r="F33" s="3"/>
     </row>
-    <row r="34" spans="1:6" s="6" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" s="6" customFormat="1" ht="104" x14ac:dyDescent="0.15">
       <c r="A34" s="3" t="s">
         <v>71</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
+      <c r="C34" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>72</v>
+      </c>
       <c r="E34" s="8" t="s">
         <v>73</v>
       </c>
@@ -2477,7 +2529,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="35" spans="1:6" s="6" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" s="6" customFormat="1" ht="52" x14ac:dyDescent="0.15">
       <c r="A35" s="3" t="s">
         <v>75</v>
       </c>
@@ -2493,7 +2545,7 @@
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
     </row>
-    <row r="36" spans="1:6" s="6" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" s="6" customFormat="1" ht="104" x14ac:dyDescent="0.15">
       <c r="A36" s="3" t="s">
         <v>78</v>
       </c>
@@ -2513,15 +2565,19 @@
         <v>83</v>
       </c>
     </row>
-    <row r="37" spans="1:6" s="6" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" s="6" customFormat="1" ht="78" x14ac:dyDescent="0.15">
       <c r="A37" s="3" t="s">
         <v>84</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
+      <c r="C37" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>85</v>
+      </c>
       <c r="E37" s="8" t="s">
         <v>86</v>
       </c>
@@ -2529,7 +2585,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="38" spans="1:6" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A38" s="3" t="s">
         <v>328</v>
       </c>
@@ -2545,19 +2601,23 @@
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
     </row>
-    <row r="39" spans="1:6" s="6" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" s="6" customFormat="1" ht="39" x14ac:dyDescent="0.15">
       <c r="A39" s="3" t="s">
         <v>250</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>251</v>
       </c>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
+      <c r="C39" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>251</v>
+      </c>
       <c r="E39" s="8"/>
       <c r="F39" s="3"/>
     </row>
-    <row r="40" spans="1:6" s="6" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" s="6" customFormat="1" ht="104" x14ac:dyDescent="0.15">
       <c r="A40" s="3" t="s">
         <v>252</v>
       </c>
@@ -2573,7 +2633,7 @@
       <c r="E40" s="8"/>
       <c r="F40" s="3"/>
     </row>
-    <row r="41" spans="1:6" s="6" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" s="6" customFormat="1" ht="91" x14ac:dyDescent="0.15">
       <c r="A41" s="3" t="s">
         <v>254</v>
       </c>
@@ -2589,7 +2649,7 @@
       <c r="E41" s="8"/>
       <c r="F41" s="3"/>
     </row>
-    <row r="42" spans="1:6" s="6" customFormat="1" ht="127.5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" s="6" customFormat="1" ht="130" x14ac:dyDescent="0.15">
       <c r="A42" s="3" t="s">
         <v>88</v>
       </c>
@@ -2609,7 +2669,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="43" spans="1:6" s="6" customFormat="1" ht="153" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" s="6" customFormat="1" ht="143" x14ac:dyDescent="0.15">
       <c r="A43" s="3" t="s">
         <v>93</v>
       </c>
@@ -2629,7 +2689,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="44" spans="1:6" s="6" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" s="6" customFormat="1" ht="65" x14ac:dyDescent="0.15">
       <c r="A44" s="3" t="s">
         <v>97</v>
       </c>
@@ -2645,7 +2705,7 @@
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
     </row>
-    <row r="45" spans="1:6" s="6" customFormat="1" ht="191.25" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" s="6" customFormat="1" ht="195" x14ac:dyDescent="0.15">
       <c r="A45" s="3" t="s">
         <v>100</v>
       </c>
@@ -2663,7 +2723,7 @@
       </c>
       <c r="F45" s="3"/>
     </row>
-    <row r="46" spans="1:6" s="6" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" s="6" customFormat="1" ht="91" x14ac:dyDescent="0.15">
       <c r="A46" s="3" t="s">
         <v>316</v>
       </c>
@@ -2679,7 +2739,7 @@
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
     </row>
-    <row r="47" spans="1:6" s="6" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" s="6" customFormat="1" ht="104" x14ac:dyDescent="0.15">
       <c r="A47" s="3" t="s">
         <v>103</v>
       </c>
@@ -2695,7 +2755,7 @@
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
     </row>
-    <row r="48" spans="1:6" s="6" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" s="6" customFormat="1" ht="65" x14ac:dyDescent="0.15">
       <c r="A48" s="3" t="s">
         <v>105</v>
       </c>
@@ -2711,9 +2771,13 @@
         <v>108</v>
       </c>
     </row>
-    <row r="49" spans="1:6" s="6" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A49" s="3"/>
-      <c r="B49" s="3"/>
+    <row r="49" spans="1:6" s="6" customFormat="1" ht="39" x14ac:dyDescent="0.15">
+      <c r="A49" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>297</v>
+      </c>
       <c r="C49" s="3" t="s">
         <v>295</v>
       </c>
@@ -2723,27 +2787,35 @@
       <c r="E49" s="3"/>
       <c r="F49" s="3"/>
     </row>
-    <row r="50" spans="1:6" s="6" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" s="6" customFormat="1" ht="91" x14ac:dyDescent="0.15">
       <c r="A50" s="3" t="s">
         <v>113</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
+      <c r="C50" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>114</v>
+      </c>
       <c r="E50" s="3"/>
       <c r="F50" s="3"/>
     </row>
-    <row r="51" spans="1:6" s="6" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" s="6" customFormat="1" ht="65" x14ac:dyDescent="0.15">
       <c r="A51" s="3" t="s">
         <v>109</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
+      <c r="C51" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>110</v>
+      </c>
       <c r="E51" s="8" t="s">
         <v>111</v>
       </c>
@@ -2751,19 +2823,23 @@
         <v>112</v>
       </c>
     </row>
-    <row r="52" spans="1:6" s="6" customFormat="1" ht="153" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" s="6" customFormat="1" ht="156" x14ac:dyDescent="0.15">
       <c r="A52" s="3" t="s">
         <v>115</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="C52" s="3"/>
-      <c r="D52" s="3"/>
+      <c r="C52" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>116</v>
+      </c>
       <c r="E52" s="3"/>
       <c r="F52" s="3"/>
     </row>
-    <row r="53" spans="1:6" s="6" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" s="6" customFormat="1" ht="65" x14ac:dyDescent="0.15">
       <c r="A53" s="3" t="s">
         <v>245</v>
       </c>
@@ -2779,7 +2855,7 @@
       <c r="E53" s="3"/>
       <c r="F53" s="3"/>
     </row>
-    <row r="54" spans="1:6" s="6" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" s="6" customFormat="1" ht="78" x14ac:dyDescent="0.15">
       <c r="A54" s="3" t="s">
         <v>117</v>
       </c>
@@ -2795,7 +2871,7 @@
       <c r="E54" s="3"/>
       <c r="F54" s="3"/>
     </row>
-    <row r="55" spans="1:6" s="6" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" s="6" customFormat="1" ht="104" x14ac:dyDescent="0.15">
       <c r="A55" s="3" t="s">
         <v>366</v>
       </c>
@@ -2811,7 +2887,7 @@
       <c r="E55" s="3"/>
       <c r="F55" s="3"/>
     </row>
-    <row r="56" spans="1:6" s="6" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" s="6" customFormat="1" ht="39" x14ac:dyDescent="0.15">
       <c r="A56" s="3" t="s">
         <v>352</v>
       </c>
@@ -2827,7 +2903,7 @@
       <c r="E56" s="3"/>
       <c r="F56" s="3"/>
     </row>
-    <row r="57" spans="1:6" s="6" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" s="6" customFormat="1" ht="65" x14ac:dyDescent="0.15">
       <c r="A57" s="3" t="s">
         <v>391</v>
       </c>
@@ -2843,15 +2919,19 @@
       <c r="E57" s="3"/>
       <c r="F57" s="3"/>
     </row>
-    <row r="58" spans="1:6" s="6" customFormat="1" ht="165.75" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" s="6" customFormat="1" ht="169" x14ac:dyDescent="0.15">
       <c r="A58" s="3" t="s">
         <v>388</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="C58" s="3"/>
-      <c r="D58" s="3"/>
+      <c r="C58" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>119</v>
+      </c>
       <c r="E58" s="8" t="s">
         <v>120</v>
       </c>
@@ -2859,7 +2939,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="59" spans="1:6" s="6" customFormat="1" ht="191.25" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6" s="6" customFormat="1" ht="182" x14ac:dyDescent="0.15">
       <c r="A59" s="3" t="s">
         <v>236</v>
       </c>
@@ -2875,7 +2955,7 @@
       <c r="E59" s="8"/>
       <c r="F59" s="3"/>
     </row>
-    <row r="60" spans="1:6" s="6" customFormat="1" ht="140.25" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" s="6" customFormat="1" ht="143" x14ac:dyDescent="0.15">
       <c r="A60" s="3" t="s">
         <v>237</v>
       </c>
@@ -2893,9 +2973,13 @@
       </c>
       <c r="F60" s="3"/>
     </row>
-    <row r="61" spans="1:6" s="6" customFormat="1" ht="216.75" x14ac:dyDescent="0.2">
-      <c r="A61" s="3"/>
-      <c r="B61" s="3"/>
+    <row r="61" spans="1:6" s="6" customFormat="1" ht="221" x14ac:dyDescent="0.15">
+      <c r="A61" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>305</v>
+      </c>
       <c r="C61" s="3" t="s">
         <v>300</v>
       </c>
@@ -2905,9 +2989,13 @@
       <c r="E61" s="3"/>
       <c r="F61" s="3"/>
     </row>
-    <row r="62" spans="1:6" s="6" customFormat="1" ht="140.25" x14ac:dyDescent="0.2">
-      <c r="A62" s="3"/>
-      <c r="B62" s="3"/>
+    <row r="62" spans="1:6" s="6" customFormat="1" ht="130" x14ac:dyDescent="0.15">
+      <c r="A62" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>306</v>
+      </c>
       <c r="C62" s="3" t="s">
         <v>301</v>
       </c>
@@ -2917,15 +3005,19 @@
       <c r="E62" s="3"/>
       <c r="F62" s="3"/>
     </row>
-    <row r="63" spans="1:6" s="6" customFormat="1" ht="127.5" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6" s="6" customFormat="1" ht="130" x14ac:dyDescent="0.15">
       <c r="A63" s="3" t="s">
         <v>122</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="C63" s="3"/>
-      <c r="D63" s="3"/>
+      <c r="C63" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>123</v>
+      </c>
       <c r="E63" s="8" t="s">
         <v>86</v>
       </c>
@@ -2933,15 +3025,19 @@
         <v>124</v>
       </c>
     </row>
-    <row r="64" spans="1:6" s="6" customFormat="1" ht="140.25" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:6" s="6" customFormat="1" ht="130" x14ac:dyDescent="0.15">
       <c r="A64" s="3" t="s">
         <v>125</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="C64" s="3"/>
-      <c r="D64" s="3"/>
+      <c r="C64" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>126</v>
+      </c>
       <c r="E64" s="8" t="s">
         <v>127</v>
       </c>
@@ -2949,21 +3045,29 @@
         <v>128</v>
       </c>
     </row>
-    <row r="65" spans="1:6" s="6" customFormat="1" ht="153" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6" s="6" customFormat="1" ht="156" x14ac:dyDescent="0.15">
       <c r="A65" s="3" t="s">
         <v>129</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="C65" s="3"/>
-      <c r="D65" s="3"/>
+      <c r="C65" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>130</v>
+      </c>
       <c r="E65" s="3"/>
       <c r="F65" s="3"/>
     </row>
-    <row r="66" spans="1:6" s="6" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A66" s="3"/>
-      <c r="B66" s="3"/>
+    <row r="66" spans="1:6" s="6" customFormat="1" ht="65" x14ac:dyDescent="0.15">
+      <c r="A66" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>360</v>
+      </c>
       <c r="C66" s="3" t="s">
         <v>359</v>
       </c>
@@ -2973,19 +3077,23 @@
       <c r="E66" s="3"/>
       <c r="F66" s="3"/>
     </row>
-    <row r="67" spans="1:6" s="6" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6" s="6" customFormat="1" ht="91" x14ac:dyDescent="0.15">
       <c r="A67" s="3" t="s">
         <v>256</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>404</v>
       </c>
-      <c r="C67" s="3"/>
-      <c r="D67" s="3"/>
+      <c r="C67" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>404</v>
+      </c>
       <c r="E67" s="3"/>
       <c r="F67" s="3"/>
     </row>
-    <row r="68" spans="1:6" s="6" customFormat="1" ht="178.5" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6" s="6" customFormat="1" ht="169" x14ac:dyDescent="0.15">
       <c r="A68" s="3" t="s">
         <v>132</v>
       </c>
@@ -3001,7 +3109,7 @@
       <c r="E68" s="3"/>
       <c r="F68" s="3"/>
     </row>
-    <row r="69" spans="1:6" s="6" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6" s="6" customFormat="1" ht="39" x14ac:dyDescent="0.15">
       <c r="A69" s="3" t="s">
         <v>136</v>
       </c>
@@ -3017,7 +3125,7 @@
       <c r="E69" s="3"/>
       <c r="F69" s="3"/>
     </row>
-    <row r="70" spans="1:6" s="6" customFormat="1" ht="277.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6" s="6" customFormat="1" ht="277.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A70" s="3" t="s">
         <v>329</v>
       </c>
@@ -3033,15 +3141,19 @@
       <c r="E70" s="3"/>
       <c r="F70" s="3"/>
     </row>
-    <row r="71" spans="1:6" s="6" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6" s="6" customFormat="1" ht="52" x14ac:dyDescent="0.15">
       <c r="A71" s="3" t="s">
         <v>138</v>
       </c>
       <c r="B71" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="C71" s="3"/>
-      <c r="D71" s="3"/>
+      <c r="C71" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>139</v>
+      </c>
       <c r="E71" s="8" t="s">
         <v>140</v>
       </c>
@@ -3049,19 +3161,23 @@
         <v>141</v>
       </c>
     </row>
-    <row r="72" spans="1:6" s="6" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6" s="6" customFormat="1" ht="78" x14ac:dyDescent="0.15">
       <c r="A72" s="3" t="s">
         <v>257</v>
       </c>
       <c r="B72" s="3" t="s">
         <v>390</v>
       </c>
-      <c r="C72" s="3"/>
-      <c r="D72" s="3"/>
+      <c r="C72" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>390</v>
+      </c>
       <c r="E72" s="8"/>
       <c r="F72" s="3"/>
     </row>
-    <row r="73" spans="1:6" s="6" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:6" s="6" customFormat="1" ht="117" x14ac:dyDescent="0.15">
       <c r="A73" s="3" t="s">
         <v>147</v>
       </c>
@@ -3081,9 +3197,13 @@
         <v>150</v>
       </c>
     </row>
-    <row r="74" spans="1:6" s="6" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A74" s="3"/>
-      <c r="B74" s="3"/>
+    <row r="74" spans="1:6" s="6" customFormat="1" ht="65" x14ac:dyDescent="0.15">
+      <c r="A74" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>298</v>
+      </c>
       <c r="C74" s="3" t="s">
         <v>296</v>
       </c>
@@ -3093,7 +3213,7 @@
       <c r="E74" s="3"/>
       <c r="F74" s="3"/>
     </row>
-    <row r="75" spans="1:6" s="6" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:6" s="6" customFormat="1" ht="78" x14ac:dyDescent="0.15">
       <c r="A75" s="3" t="s">
         <v>151</v>
       </c>
@@ -3113,7 +3233,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="76" spans="1:6" s="6" customFormat="1" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:6" s="6" customFormat="1" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A76" s="3" t="s">
         <v>155</v>
       </c>
@@ -3129,7 +3249,7 @@
       <c r="E76" s="3"/>
       <c r="F76" s="3"/>
     </row>
-    <row r="77" spans="1:6" s="6" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:6" s="6" customFormat="1" ht="104" x14ac:dyDescent="0.15">
       <c r="A77" s="3" t="s">
         <v>157</v>
       </c>
@@ -3145,7 +3265,7 @@
       <c r="E77" s="3"/>
       <c r="F77" s="3"/>
     </row>
-    <row r="78" spans="1:6" s="6" customFormat="1" ht="140.25" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:6" s="6" customFormat="1" ht="143" x14ac:dyDescent="0.15">
       <c r="A78" s="3" t="s">
         <v>372</v>
       </c>
@@ -3163,15 +3283,19 @@
       </c>
       <c r="F78" s="3"/>
     </row>
-    <row r="79" spans="1:6" s="6" customFormat="1" ht="267.75" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:6" s="6" customFormat="1" ht="260" x14ac:dyDescent="0.15">
       <c r="A79" s="3" t="s">
         <v>159</v>
       </c>
       <c r="B79" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="C79" s="3"/>
-      <c r="D79" s="3"/>
+      <c r="C79" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="D79" s="3" t="s">
+        <v>160</v>
+      </c>
       <c r="E79" s="8" t="s">
         <v>161</v>
       </c>
@@ -3179,9 +3303,13 @@
         <v>162</v>
       </c>
     </row>
-    <row r="80" spans="1:6" s="6" customFormat="1" ht="140.25" x14ac:dyDescent="0.2">
-      <c r="A80" s="3"/>
-      <c r="B80" s="3"/>
+    <row r="80" spans="1:6" s="6" customFormat="1" ht="130" x14ac:dyDescent="0.15">
+      <c r="A80" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>286</v>
+      </c>
       <c r="C80" s="3" t="s">
         <v>277</v>
       </c>
@@ -3191,7 +3319,7 @@
       <c r="E80" s="3"/>
       <c r="F80" s="3"/>
     </row>
-    <row r="81" spans="1:6" s="6" customFormat="1" ht="153" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:6" s="6" customFormat="1" ht="156" x14ac:dyDescent="0.15">
       <c r="A81" s="3" t="s">
         <v>163</v>
       </c>
@@ -3207,9 +3335,13 @@
       <c r="E81" s="3"/>
       <c r="F81" s="3"/>
     </row>
-    <row r="82" spans="1:6" s="6" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A82" s="3"/>
-      <c r="B82" s="3"/>
+    <row r="82" spans="1:6" s="6" customFormat="1" ht="52" x14ac:dyDescent="0.15">
+      <c r="A82" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>287</v>
+      </c>
       <c r="C82" s="3" t="s">
         <v>278</v>
       </c>
@@ -3219,7 +3351,7 @@
       <c r="E82" s="3"/>
       <c r="F82" s="3"/>
     </row>
-    <row r="83" spans="1:6" s="6" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:6" s="6" customFormat="1" ht="91" x14ac:dyDescent="0.15">
       <c r="A83" s="3" t="s">
         <v>368</v>
       </c>
@@ -3239,7 +3371,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="84" spans="1:6" s="6" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:6" s="6" customFormat="1" ht="91" x14ac:dyDescent="0.15">
       <c r="A84" s="3" t="s">
         <v>361</v>
       </c>
@@ -3255,9 +3387,13 @@
       <c r="E84" s="3"/>
       <c r="F84" s="3"/>
     </row>
-    <row r="85" spans="1:6" s="6" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
-      <c r="A85" s="3"/>
-      <c r="B85" s="3"/>
+    <row r="85" spans="1:6" s="6" customFormat="1" ht="117" x14ac:dyDescent="0.15">
+      <c r="A85" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>289</v>
+      </c>
       <c r="C85" s="3" t="s">
         <v>280</v>
       </c>
@@ -3267,7 +3403,7 @@
       <c r="E85" s="3"/>
       <c r="F85" s="3"/>
     </row>
-    <row r="86" spans="1:6" s="6" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:6" s="6" customFormat="1" ht="39" x14ac:dyDescent="0.15">
       <c r="A86" s="3" t="s">
         <v>281</v>
       </c>
@@ -3283,7 +3419,7 @@
       <c r="E86" s="3"/>
       <c r="F86" s="3"/>
     </row>
-    <row r="87" spans="1:6" s="6" customFormat="1" ht="331.5" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:6" s="6" customFormat="1" ht="338" x14ac:dyDescent="0.15">
       <c r="A87" s="3" t="s">
         <v>239</v>
       </c>
@@ -3301,7 +3437,7 @@
       </c>
       <c r="F87" s="3"/>
     </row>
-    <row r="88" spans="1:6" s="6" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:6" s="6" customFormat="1" ht="91" x14ac:dyDescent="0.15">
       <c r="A88" s="3" t="s">
         <v>312</v>
       </c>
@@ -3317,7 +3453,7 @@
       <c r="E88" s="3"/>
       <c r="F88" s="3"/>
     </row>
-    <row r="89" spans="1:6" s="6" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:6" s="6" customFormat="1" ht="52" x14ac:dyDescent="0.15">
       <c r="A89" s="3" t="s">
         <v>165</v>
       </c>
@@ -3333,7 +3469,7 @@
       <c r="E89" s="3"/>
       <c r="F89" s="3"/>
     </row>
-    <row r="90" spans="1:6" s="6" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:6" s="6" customFormat="1" ht="65" x14ac:dyDescent="0.15">
       <c r="A90" s="3" t="s">
         <v>282</v>
       </c>
@@ -3349,7 +3485,7 @@
       <c r="E90" s="3"/>
       <c r="F90" s="3"/>
     </row>
-    <row r="91" spans="1:6" s="6" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:6" s="6" customFormat="1" ht="52" x14ac:dyDescent="0.15">
       <c r="A91" s="3" t="s">
         <v>394</v>
       </c>
@@ -3365,19 +3501,23 @@
       <c r="E91" s="3"/>
       <c r="F91" s="3"/>
     </row>
-    <row r="92" spans="1:6" s="6" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:6" s="6" customFormat="1" ht="78" x14ac:dyDescent="0.15">
       <c r="A92" s="3" t="s">
         <v>167</v>
       </c>
       <c r="B92" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="C92" s="3"/>
-      <c r="D92" s="3"/>
+      <c r="C92" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="D92" s="3" t="s">
+        <v>168</v>
+      </c>
       <c r="E92" s="3"/>
       <c r="F92" s="3"/>
     </row>
-    <row r="93" spans="1:6" s="6" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:6" s="6" customFormat="1" ht="78" x14ac:dyDescent="0.15">
       <c r="A93" s="3" t="s">
         <v>169</v>
       </c>
@@ -3393,7 +3533,7 @@
       <c r="E93" s="3"/>
       <c r="F93" s="3"/>
     </row>
-    <row r="94" spans="1:6" s="6" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:6" s="6" customFormat="1" ht="117" x14ac:dyDescent="0.15">
       <c r="A94" s="3" t="s">
         <v>364</v>
       </c>
@@ -3413,7 +3553,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="95" spans="1:6" s="6" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:6" s="6" customFormat="1" ht="65" x14ac:dyDescent="0.15">
       <c r="A95" s="3" t="s">
         <v>171</v>
       </c>
@@ -3429,7 +3569,7 @@
       <c r="E95" s="3"/>
       <c r="F95" s="3"/>
     </row>
-    <row r="96" spans="1:6" s="6" customFormat="1" ht="140.25" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:6" s="6" customFormat="1" ht="130" x14ac:dyDescent="0.15">
       <c r="A96" s="3" t="s">
         <v>174</v>
       </c>
@@ -3445,7 +3585,7 @@
       <c r="E96" s="3"/>
       <c r="F96" s="3"/>
     </row>
-    <row r="97" spans="1:6" s="6" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:6" s="6" customFormat="1" ht="52" x14ac:dyDescent="0.15">
       <c r="A97" s="3" t="s">
         <v>246</v>
       </c>
@@ -3461,7 +3601,7 @@
       <c r="E97" s="3"/>
       <c r="F97" s="3"/>
     </row>
-    <row r="98" spans="1:6" s="6" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:6" s="6" customFormat="1" ht="104" x14ac:dyDescent="0.15">
       <c r="A98" s="3" t="s">
         <v>341</v>
       </c>
@@ -3477,19 +3617,23 @@
       <c r="E98" s="3"/>
       <c r="F98" s="3"/>
     </row>
-    <row r="99" spans="1:6" s="6" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:6" s="6" customFormat="1" ht="39" x14ac:dyDescent="0.15">
       <c r="A99" s="3" t="s">
         <v>183</v>
       </c>
       <c r="B99" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="C99" s="3"/>
-      <c r="D99" s="3"/>
+      <c r="C99" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="D99" s="3" t="s">
+        <v>184</v>
+      </c>
       <c r="E99" s="3"/>
       <c r="F99" s="3"/>
     </row>
-    <row r="100" spans="1:6" s="6" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:6" s="6" customFormat="1" ht="39" x14ac:dyDescent="0.15">
       <c r="A100" s="3" t="s">
         <v>357</v>
       </c>
@@ -3505,7 +3649,7 @@
       <c r="E100" s="3"/>
       <c r="F100" s="3"/>
     </row>
-    <row r="101" spans="1:6" s="6" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:6" s="6" customFormat="1" ht="104" x14ac:dyDescent="0.15">
       <c r="A101" s="3" t="s">
         <v>190</v>
       </c>
@@ -3521,7 +3665,7 @@
       <c r="E101" s="3"/>
       <c r="F101" s="3"/>
     </row>
-    <row r="102" spans="1:6" s="6" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:6" s="6" customFormat="1" ht="117" x14ac:dyDescent="0.15">
       <c r="A102" s="3" t="s">
         <v>193</v>
       </c>
@@ -3537,7 +3681,7 @@
       <c r="E102" s="3"/>
       <c r="F102" s="3"/>
     </row>
-    <row r="103" spans="1:6" s="6" customFormat="1" ht="242.25" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:6" s="6" customFormat="1" ht="234" x14ac:dyDescent="0.15">
       <c r="A103" s="3" t="s">
         <v>185</v>
       </c>
@@ -3557,9 +3701,13 @@
         <v>189</v>
       </c>
     </row>
-    <row r="104" spans="1:6" s="6" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A104" s="3"/>
-      <c r="B104" s="3"/>
+    <row r="104" spans="1:6" s="6" customFormat="1" ht="26" x14ac:dyDescent="0.15">
+      <c r="A104" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>294</v>
+      </c>
       <c r="C104" s="3" t="s">
         <v>293</v>
       </c>
@@ -3569,7 +3717,7 @@
       <c r="E104" s="3"/>
       <c r="F104" s="3"/>
     </row>
-    <row r="105" spans="1:6" s="6" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:6" s="6" customFormat="1" ht="65" x14ac:dyDescent="0.15">
       <c r="A105" s="3" t="s">
         <v>365</v>
       </c>
@@ -3589,7 +3737,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="106" spans="1:6" s="6" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:6" s="6" customFormat="1" ht="78" x14ac:dyDescent="0.15">
       <c r="A106" s="3" t="s">
         <v>197</v>
       </c>
@@ -3609,15 +3757,19 @@
         <v>202</v>
       </c>
     </row>
-    <row r="107" spans="1:6" s="6" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:6" s="6" customFormat="1" ht="65" x14ac:dyDescent="0.15">
       <c r="A107" s="3" t="s">
         <v>203</v>
       </c>
       <c r="B107" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="C107" s="3"/>
-      <c r="D107" s="3"/>
+      <c r="C107" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="D107" s="3" t="s">
+        <v>204</v>
+      </c>
       <c r="E107" s="8" t="s">
         <v>205</v>
       </c>
@@ -3625,31 +3777,39 @@
         <v>206</v>
       </c>
     </row>
-    <row r="108" spans="1:6" s="6" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:6" s="6" customFormat="1" ht="65" x14ac:dyDescent="0.15">
       <c r="A108" s="3" t="s">
         <v>207</v>
       </c>
       <c r="B108" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="C108" s="3"/>
-      <c r="D108" s="3"/>
+      <c r="C108" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="D108" s="3" t="s">
+        <v>208</v>
+      </c>
       <c r="E108" s="3"/>
       <c r="F108" s="3"/>
     </row>
-    <row r="109" spans="1:6" s="6" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:6" s="6" customFormat="1" ht="39" x14ac:dyDescent="0.15">
       <c r="A109" s="3" t="s">
         <v>235</v>
       </c>
       <c r="B109" s="3" t="s">
         <v>321</v>
       </c>
-      <c r="C109" s="3"/>
-      <c r="D109" s="3"/>
+      <c r="C109" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="D109" s="3" t="s">
+        <v>321</v>
+      </c>
       <c r="E109" s="3"/>
       <c r="F109" s="3"/>
     </row>
-    <row r="110" spans="1:6" s="6" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:6" s="6" customFormat="1" ht="52" x14ac:dyDescent="0.15">
       <c r="A110" s="3" t="s">
         <v>209</v>
       </c>
@@ -3665,19 +3825,23 @@
       <c r="E110" s="3"/>
       <c r="F110" s="3"/>
     </row>
-    <row r="111" spans="1:6" s="6" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:6" s="6" customFormat="1" ht="78" x14ac:dyDescent="0.15">
       <c r="A111" s="3" t="s">
         <v>212</v>
       </c>
       <c r="B111" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="C111" s="3"/>
-      <c r="D111" s="3"/>
+      <c r="C111" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="D111" s="3" t="s">
+        <v>213</v>
+      </c>
       <c r="E111" s="3"/>
       <c r="F111" s="3"/>
     </row>
-    <row r="112" spans="1:6" s="6" customFormat="1" ht="204" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:6" s="6" customFormat="1" ht="208" x14ac:dyDescent="0.15">
       <c r="A112" s="3" t="s">
         <v>214</v>
       </c>
@@ -3693,15 +3857,19 @@
       <c r="E112" s="3"/>
       <c r="F112" s="3"/>
     </row>
-    <row r="113" spans="1:6" s="6" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:6" s="6" customFormat="1" ht="78" x14ac:dyDescent="0.15">
       <c r="A113" s="3" t="s">
         <v>218</v>
       </c>
       <c r="B113" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="C113" s="3"/>
-      <c r="D113" s="3"/>
+      <c r="C113" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="D113" s="3" t="s">
+        <v>219</v>
+      </c>
       <c r="E113" s="8" t="s">
         <v>86</v>
       </c>
@@ -3709,19 +3877,23 @@
         <v>220</v>
       </c>
     </row>
-    <row r="114" spans="1:6" s="6" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:6" s="6" customFormat="1" ht="39" x14ac:dyDescent="0.15">
       <c r="A114" s="3" t="s">
         <v>221</v>
       </c>
       <c r="B114" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="C114" s="3"/>
-      <c r="D114" s="3"/>
+      <c r="C114" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="D114" s="3" t="s">
+        <v>222</v>
+      </c>
       <c r="E114" s="3"/>
       <c r="F114" s="3"/>
     </row>
-    <row r="115" spans="1:6" s="6" customFormat="1" ht="306" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:6" s="6" customFormat="1" ht="312" x14ac:dyDescent="0.15">
       <c r="A115" s="3" t="s">
         <v>223</v>
       </c>
@@ -3737,9 +3909,13 @@
       <c r="E115" s="3"/>
       <c r="F115" s="3"/>
     </row>
-    <row r="116" spans="1:6" s="6" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A116" s="3"/>
-      <c r="B116" s="3"/>
+    <row r="116" spans="1:6" s="6" customFormat="1" ht="39" x14ac:dyDescent="0.15">
+      <c r="A116" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="B116" s="3" t="s">
+        <v>309</v>
+      </c>
       <c r="C116" s="3" t="s">
         <v>302</v>
       </c>
@@ -3749,7 +3925,7 @@
       <c r="E116" s="3"/>
       <c r="F116" s="3"/>
     </row>
-    <row r="117" spans="1:6" s="6" customFormat="1" ht="127.5" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:6" s="6" customFormat="1" ht="130" x14ac:dyDescent="0.15">
       <c r="A117" s="3" t="s">
         <v>225</v>
       </c>
@@ -3765,27 +3941,35 @@
       <c r="E117" s="3"/>
       <c r="F117" s="3"/>
     </row>
-    <row r="118" spans="1:6" s="6" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:6" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A118" s="3" t="s">
         <v>248</v>
       </c>
       <c r="B118" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="C118" s="3"/>
-      <c r="D118" s="3"/>
+      <c r="C118" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="D118" s="3" t="s">
+        <v>249</v>
+      </c>
       <c r="E118" s="3"/>
       <c r="F118" s="3"/>
     </row>
-    <row r="119" spans="1:6" s="6" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:6" s="6" customFormat="1" ht="52" x14ac:dyDescent="0.15">
       <c r="A119" s="3" t="s">
         <v>227</v>
       </c>
       <c r="B119" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="C119" s="3"/>
-      <c r="D119" s="3"/>
+      <c r="C119" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="D119" s="3" t="s">
+        <v>228</v>
+      </c>
       <c r="E119" s="8" t="s">
         <v>229</v>
       </c>
@@ -3793,7 +3977,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="120" spans="1:6" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:6" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A120" s="3"/>
       <c r="B120" s="3"/>
       <c r="C120" s="3"/>
@@ -3801,903 +3985,903 @@
       <c r="E120" s="3"/>
       <c r="F120" s="3"/>
     </row>
-    <row r="121" spans="1:6" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="122" spans="1:6" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="123" spans="1:6" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="124" spans="1:6" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="125" spans="1:6" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="126" spans="1:6" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="127" spans="1:6" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="128" spans="1:6" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="129" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="130" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="131" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="132" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="133" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="134" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="135" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="136" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="137" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="138" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="139" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="140" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="141" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="142" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="143" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="144" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="145" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="146" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="147" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="148" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="149" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="150" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="151" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="152" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="153" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="154" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="155" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="156" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="157" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="158" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="159" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="160" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="161" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="162" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="163" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="164" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="165" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="166" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="167" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="168" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="169" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="170" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="171" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="172" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="173" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="174" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="175" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="176" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="177" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="178" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="179" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="180" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="181" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="182" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="183" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="184" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="185" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="186" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="187" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="188" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="189" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="190" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="191" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="192" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="193" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="194" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="195" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="196" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="197" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="198" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="199" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="200" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="201" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="202" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="203" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="204" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="205" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="206" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="207" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="208" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="209" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="210" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="211" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="212" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="213" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="214" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="215" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="216" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="217" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="218" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="219" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="220" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="221" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="222" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="223" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="224" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="225" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="226" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="227" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="228" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="229" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="230" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="231" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="232" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="233" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="234" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="235" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="236" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="237" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="238" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="239" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="240" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="241" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="242" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="243" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="244" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="245" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="246" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="247" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="248" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="249" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="250" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="251" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="252" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="253" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="254" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="255" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="256" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="257" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="258" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="259" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="260" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="261" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="262" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="263" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="264" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="265" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="266" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="267" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="268" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="269" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="270" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="271" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="272" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="273" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="274" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="275" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="276" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="277" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="278" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="279" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="280" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="281" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="282" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="283" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="284" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="285" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="286" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="287" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="288" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="289" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="290" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="291" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="292" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="293" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="294" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="295" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="296" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="297" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="298" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="299" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="300" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="301" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="302" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="303" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="304" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="305" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="306" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="307" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="308" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="309" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="310" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="311" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="312" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="313" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="314" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="315" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="316" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="317" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="318" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="319" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="320" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="321" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="322" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="323" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="324" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="325" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="326" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="327" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="328" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="329" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="330" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="331" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="332" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="333" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="334" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="335" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="336" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="337" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="338" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="339" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="340" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="341" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="342" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="343" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="344" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="345" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="346" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="347" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="348" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="349" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="350" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="351" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="352" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="353" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="354" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="355" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="356" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="357" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="358" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="359" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="360" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="361" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="362" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="363" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="364" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="365" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="366" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="367" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="368" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="369" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="370" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="371" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="372" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="373" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="374" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="375" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="376" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="377" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="378" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="379" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="380" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="381" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="382" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="383" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="384" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="385" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="386" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="387" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="388" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="389" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="390" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="391" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="392" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="393" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="394" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="395" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="396" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="397" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="398" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="399" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="400" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="401" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="402" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="403" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="404" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="405" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="406" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="407" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="408" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="409" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="410" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="411" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="412" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="413" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="414" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="415" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="416" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="417" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="418" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="419" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="420" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="421" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="422" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="423" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="424" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="425" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="426" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="427" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="428" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="429" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="430" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="431" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="432" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="433" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="434" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="435" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="436" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="437" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="438" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="439" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="440" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="441" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="442" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="443" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="444" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="445" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="446" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="447" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="448" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="449" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="450" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="451" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="452" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="453" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="454" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="455" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="456" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="457" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="458" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="459" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="460" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="461" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="462" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="463" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="464" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="465" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="466" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="467" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="468" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="469" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="470" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="471" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="472" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="473" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="474" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="475" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="476" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="477" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="478" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="479" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="480" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="481" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="482" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="483" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="484" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="485" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="486" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="487" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="488" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="489" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="490" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="491" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="492" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="493" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="494" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="495" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="496" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="497" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="498" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="499" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="500" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="501" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="502" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="503" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="504" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="505" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="506" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="507" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="508" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="509" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="510" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="511" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="512" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="513" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="514" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="515" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="516" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="517" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="518" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="519" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="520" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="521" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="522" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="523" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="524" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="525" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="526" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="527" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="528" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="529" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="530" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="531" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="532" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="533" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="534" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="535" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="536" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="537" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="538" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="539" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="540" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="541" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="542" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="543" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="544" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="545" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="546" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="547" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="548" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="549" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="550" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="551" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="552" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="553" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="554" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="555" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="556" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="557" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="558" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="559" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="560" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="561" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="562" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="563" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="564" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="565" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="566" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="567" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="568" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="569" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="570" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="571" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="572" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="573" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="574" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="575" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="576" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="577" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="578" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="579" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="580" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="581" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="582" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="583" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="584" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="585" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="586" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="587" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="588" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="589" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="590" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="591" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="592" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="593" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="594" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="595" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="596" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="597" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="598" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="599" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="600" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="601" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="602" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="603" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="604" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="605" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="606" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="607" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="608" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="609" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="610" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="611" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="612" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="613" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="614" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="615" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="616" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="617" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="618" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="619" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="620" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="621" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="622" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="623" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="624" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="625" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="626" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="627" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="628" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="629" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="630" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="631" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="632" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="633" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="634" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="635" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="636" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="637" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="638" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="639" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="640" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="641" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="642" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="643" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="644" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="645" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="646" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="647" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="648" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="649" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="650" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="651" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="652" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="653" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="654" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="655" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="656" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="657" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="658" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="659" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="660" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="661" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="662" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="663" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="664" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="665" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="666" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="667" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="668" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="669" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="670" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="671" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="672" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="673" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="674" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="675" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="676" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="677" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="678" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="679" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="680" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="681" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="682" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="683" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="684" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="685" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="686" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="687" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="688" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="689" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="690" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="691" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="692" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="693" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="694" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="695" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="696" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="697" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="698" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="699" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="700" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="701" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="702" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="703" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="704" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="705" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="706" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="707" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="708" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="709" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="710" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="711" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="712" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="713" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="714" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="715" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="716" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="717" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="718" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="719" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="720" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="721" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="722" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="723" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="724" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="725" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="726" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="727" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="728" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="729" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="730" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="731" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="732" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="733" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="734" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="735" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="736" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="737" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="738" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="739" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="740" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="741" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="742" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="743" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="744" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="745" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="746" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="747" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="748" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="749" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="750" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="751" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="752" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="753" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="754" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="755" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="756" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="757" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="758" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="759" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="760" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="761" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="762" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="763" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="764" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="765" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="766" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="767" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="768" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="769" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="770" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="771" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="772" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="773" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="774" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="775" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="776" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="777" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="778" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="779" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="780" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="781" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="782" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="783" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="784" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="785" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="786" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="787" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="788" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="789" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="790" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="791" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="792" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="793" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="794" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="795" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="796" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="797" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="798" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="799" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="800" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="801" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="802" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="803" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="804" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="805" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="806" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="807" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="808" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="809" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="810" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="811" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="812" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="813" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="814" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="815" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="816" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="817" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="818" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="819" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="820" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="821" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="822" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="823" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="824" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="825" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="826" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="827" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="828" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="829" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="830" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="831" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="832" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="833" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="834" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="835" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="836" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="837" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="838" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="839" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="840" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="841" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="842" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="843" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="844" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="845" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="846" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="847" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="848" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="849" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="850" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="851" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="852" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="853" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="854" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="855" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="856" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="857" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="858" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="859" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="860" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="861" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="862" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="863" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="864" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="865" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="866" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="867" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="868" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="869" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="870" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="871" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="872" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="873" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="874" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="875" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="876" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="877" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="878" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="879" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="880" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="881" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="882" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="883" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="884" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="885" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="886" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="887" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="888" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="889" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="890" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="891" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="892" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="893" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="894" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="895" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="896" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="897" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="898" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="899" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="900" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="901" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="902" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="903" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="904" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="905" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="906" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="907" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="908" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="909" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="910" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="911" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="912" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="913" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="914" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="915" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="916" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="917" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="918" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="919" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="920" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="921" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="922" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="923" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="924" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="925" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="926" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="927" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="928" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="929" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="930" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="931" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="932" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="933" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="934" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="935" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="936" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="937" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="938" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="939" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="940" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="941" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="942" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="943" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="944" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="945" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="946" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="947" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="948" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="949" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="950" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="951" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="952" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="953" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="954" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="955" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="956" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="957" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="958" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="959" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="960" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="961" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="962" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="963" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="964" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="965" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="966" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="967" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="968" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="969" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="970" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="971" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="972" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="973" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="974" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="975" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="976" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="977" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="978" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="979" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="980" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="981" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="982" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="983" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="984" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="985" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="986" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="987" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="988" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="989" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="990" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="991" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="992" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="993" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="994" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="995" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="996" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="997" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="998" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="999" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="1000" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="1001" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="1002" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="1003" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="1004" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="1005" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="1006" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="1007" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="1008" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="1009" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="1010" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="1011" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="1012" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="1013" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="1014" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="1015" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="1016" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="1017" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="121" spans="1:6" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="122" spans="1:6" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="123" spans="1:6" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="124" spans="1:6" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="125" spans="1:6" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="126" spans="1:6" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="127" spans="1:6" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="128" spans="1:6" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="129" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="130" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="131" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="132" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="133" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="134" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="135" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="136" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="137" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="138" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="139" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="140" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="141" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="142" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="143" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="144" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="145" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="146" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="147" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="148" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="149" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="150" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="151" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="152" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="153" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="154" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="155" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="156" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="157" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="158" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="159" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="160" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="161" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="162" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="163" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="164" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="165" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="166" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="167" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="168" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="169" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="170" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="171" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="172" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="173" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="174" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="175" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="176" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="177" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="178" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="179" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="180" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="181" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="182" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="183" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="184" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="185" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="186" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="187" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="188" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="189" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="190" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="191" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="192" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="193" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="194" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="195" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="196" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="197" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="198" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="199" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="200" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="201" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="202" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="203" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="204" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="205" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="206" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="207" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="208" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="209" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="210" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="211" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="212" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="213" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="214" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="215" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="216" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="217" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="218" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="219" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="220" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="221" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="222" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="223" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="224" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="225" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="226" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="227" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="228" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="229" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="230" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="231" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="232" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="233" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="234" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="235" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="236" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="237" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="238" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="239" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="240" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="241" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="242" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="243" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="244" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="245" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="246" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="247" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="248" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="249" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="250" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="251" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="252" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="253" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="254" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="255" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="256" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="257" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="258" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="259" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="260" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="261" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="262" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="263" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="264" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="265" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="266" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="267" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="268" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="269" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="270" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="271" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="272" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="273" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="274" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="275" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="276" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="277" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="278" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="279" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="280" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="281" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="282" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="283" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="284" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="285" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="286" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="287" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="288" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="289" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="290" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="291" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="292" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="293" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="294" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="295" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="296" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="297" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="298" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="299" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="300" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="301" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="302" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="303" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="304" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="305" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="306" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="307" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="308" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="309" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="310" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="311" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="312" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="313" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="314" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="315" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="316" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="317" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="318" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="319" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="320" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="321" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="322" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="323" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="324" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="325" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="326" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="327" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="328" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="329" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="330" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="331" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="332" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="333" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="334" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="335" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="336" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="337" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="338" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="339" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="340" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="341" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="342" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="343" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="344" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="345" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="346" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="347" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="348" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="349" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="350" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="351" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="352" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="353" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="354" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="355" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="356" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="357" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="358" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="359" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="360" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="361" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="362" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="363" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="364" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="365" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="366" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="367" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="368" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="369" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="370" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="371" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="372" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="373" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="374" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="375" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="376" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="377" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="378" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="379" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="380" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="381" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="382" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="383" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="384" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="385" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="386" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="387" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="388" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="389" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="390" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="391" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="392" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="393" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="394" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="395" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="396" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="397" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="398" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="399" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="400" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="401" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="402" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="403" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="404" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="405" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="406" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="407" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="408" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="409" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="410" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="411" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="412" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="413" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="414" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="415" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="416" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="417" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="418" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="419" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="420" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="421" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="422" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="423" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="424" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="425" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="426" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="427" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="428" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="429" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="430" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="431" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="432" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="433" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="434" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="435" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="436" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="437" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="438" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="439" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="440" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="441" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="442" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="443" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="444" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="445" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="446" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="447" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="448" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="449" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="450" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="451" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="452" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="453" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="454" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="455" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="456" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="457" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="458" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="459" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="460" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="461" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="462" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="463" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="464" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="465" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="466" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="467" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="468" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="469" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="470" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="471" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="472" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="473" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="474" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="475" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="476" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="477" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="478" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="479" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="480" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="481" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="482" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="483" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="484" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="485" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="486" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="487" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="488" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="489" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="490" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="491" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="492" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="493" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="494" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="495" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="496" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="497" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="498" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="499" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="500" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="501" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="502" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="503" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="504" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="505" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="506" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="507" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="508" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="509" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="510" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="511" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="512" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="513" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="514" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="515" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="516" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="517" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="518" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="519" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="520" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="521" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="522" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="523" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="524" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="525" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="526" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="527" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="528" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="529" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="530" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="531" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="532" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="533" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="534" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="535" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="536" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="537" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="538" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="539" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="540" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="541" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="542" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="543" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="544" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="545" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="546" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="547" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="548" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="549" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="550" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="551" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="552" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="553" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="554" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="555" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="556" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="557" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="558" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="559" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="560" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="561" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="562" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="563" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="564" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="565" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="566" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="567" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="568" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="569" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="570" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="571" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="572" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="573" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="574" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="575" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="576" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="577" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="578" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="579" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="580" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="581" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="582" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="583" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="584" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="585" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="586" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="587" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="588" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="589" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="590" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="591" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="592" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="593" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="594" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="595" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="596" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="597" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="598" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="599" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="600" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="601" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="602" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="603" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="604" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="605" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="606" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="607" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="608" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="609" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="610" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="611" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="612" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="613" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="614" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="615" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="616" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="617" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="618" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="619" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="620" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="621" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="622" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="623" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="624" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="625" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="626" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="627" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="628" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="629" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="630" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="631" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="632" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="633" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="634" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="635" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="636" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="637" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="638" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="639" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="640" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="641" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="642" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="643" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="644" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="645" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="646" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="647" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="648" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="649" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="650" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="651" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="652" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="653" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="654" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="655" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="656" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="657" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="658" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="659" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="660" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="661" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="662" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="663" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="664" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="665" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="666" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="667" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="668" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="669" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="670" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="671" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="672" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="673" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="674" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="675" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="676" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="677" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="678" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="679" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="680" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="681" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="682" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="683" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="684" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="685" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="686" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="687" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="688" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="689" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="690" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="691" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="692" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="693" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="694" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="695" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="696" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="697" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="698" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="699" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="700" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="701" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="702" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="703" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="704" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="705" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="706" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="707" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="708" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="709" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="710" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="711" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="712" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="713" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="714" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="715" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="716" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="717" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="718" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="719" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="720" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="721" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="722" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="723" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="724" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="725" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="726" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="727" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="728" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="729" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="730" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="731" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="732" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="733" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="734" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="735" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="736" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="737" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="738" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="739" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="740" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="741" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="742" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="743" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="744" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="745" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="746" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="747" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="748" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="749" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="750" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="751" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="752" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="753" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="754" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="755" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="756" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="757" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="758" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="759" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="760" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="761" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="762" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="763" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="764" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="765" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="766" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="767" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="768" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="769" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="770" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="771" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="772" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="773" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="774" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="775" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="776" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="777" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="778" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="779" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="780" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="781" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="782" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="783" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="784" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="785" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="786" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="787" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="788" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="789" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="790" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="791" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="792" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="793" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="794" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="795" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="796" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="797" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="798" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="799" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="800" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="801" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="802" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="803" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="804" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="805" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="806" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="807" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="808" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="809" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="810" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="811" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="812" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="813" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="814" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="815" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="816" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="817" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="818" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="819" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="820" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="821" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="822" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="823" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="824" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="825" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="826" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="827" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="828" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="829" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="830" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="831" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="832" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="833" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="834" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="835" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="836" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="837" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="838" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="839" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="840" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="841" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="842" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="843" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="844" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="845" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="846" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="847" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="848" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="849" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="850" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="851" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="852" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="853" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="854" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="855" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="856" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="857" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="858" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="859" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="860" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="861" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="862" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="863" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="864" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="865" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="866" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="867" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="868" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="869" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="870" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="871" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="872" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="873" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="874" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="875" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="876" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="877" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="878" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="879" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="880" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="881" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="882" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="883" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="884" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="885" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="886" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="887" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="888" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="889" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="890" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="891" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="892" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="893" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="894" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="895" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="896" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="897" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="898" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="899" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="900" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="901" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="902" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="903" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="904" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="905" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="906" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="907" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="908" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="909" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="910" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="911" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="912" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="913" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="914" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="915" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="916" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="917" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="918" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="919" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="920" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="921" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="922" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="923" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="924" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="925" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="926" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="927" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="928" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="929" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="930" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="931" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="932" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="933" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="934" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="935" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="936" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="937" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="938" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="939" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="940" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="941" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="942" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="943" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="944" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="945" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="946" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="947" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="948" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="949" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="950" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="951" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="952" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="953" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="954" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="955" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="956" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="957" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="958" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="959" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="960" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="961" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="962" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="963" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="964" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="965" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="966" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="967" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="968" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="969" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="970" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="971" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="972" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="973" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="974" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="975" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="976" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="977" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="978" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="979" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="980" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="981" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="982" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="983" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="984" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="985" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="986" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="987" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="988" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="989" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="990" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="991" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="992" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="993" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="994" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="995" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="996" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="997" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="998" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="999" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="1000" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="1001" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="1002" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="1003" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="1004" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="1005" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="1006" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="1007" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="1008" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="1009" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="1010" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="1011" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="1012" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="1013" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="1014" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="1015" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="1016" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="1017" ht="13" x14ac:dyDescent="0.15"/>
   </sheetData>
   <autoFilter ref="A1:Y119"/>
   <sortState ref="A2:Y1017">

</xml_diff>

<commit_message>
fixing links in glossary
</commit_message>
<xml_diff>
--- a/usaspending_api/data/USAspendingGlossary.xlsx
+++ b/usaspending_api/data/USAspendingGlossary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nipunmonga/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nipunmonga/Development/DataAct/usaspending-api/usaspending_api/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1513,8 +1513,14 @@
     </r>
   </si>
   <si>
+    <t>https://www.gao.gov/assets/80/76911.pdf</t>
+  </si>
+  <si>
+    <t>https://www.fpds.gov/help/Extent_Competed.htm</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">Learn More: </t>
+      <t>Learn More: [</t>
     </r>
     <r>
       <rPr>
@@ -1523,8 +1529,11 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>https://www.whitehouse.gov/sites/whitehouse.gov/files/omb/assets/a11_current_year/a11_2017.pdf</t>
+      <t>https://www.whitehouse.gov/sites/whitehouse.gov/files/omb/assets/a11_current_year/a11_2017.pdf](https://www.whitehouse.gov/sites/whitehouse.gov/files/omb/assets/a11_current_year/a11_2017.pdf)</t>
     </r>
+  </si>
+  <si>
+    <t>Learn More: [https://www.whitehouse.gov/sites/whitehouse.gov/files/omb/assets/a11_current_year/a11_2017.pdf](https://www.whitehouse.gov/sites/whitehouse.gov/files/omb/assets/a11_current_year/a11_2017.pdf)</t>
   </si>
   <si>
     <r>
@@ -1533,7 +1542,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">Learn More: </t>
+      <t>Learn More: [</t>
     </r>
     <r>
       <rPr>
@@ -1542,17 +1551,15 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>https://www.whitehouse.gov/sites/whitehouse.gov/files/omb/assets/a11_current_year/a11_2017.pdf</t>
+      <t>https://www.gao.gov/assets/80/76911.pdf](https://www.gao.gov/assets/80/76911.pdf)</t>
     </r>
   </si>
   <si>
+    <t>Learn More: [https://www.gao.gov/assets/80/76911.pdf](https://www.gao.gov/assets/80/76911.pdf)</t>
+  </si>
+  <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Learn More: </t>
+      <t>Learn More: [</t>
     </r>
     <r>
       <rPr>
@@ -1561,47 +1568,8 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>https://www.whitehouse.gov/sites/whitehouse.gov/files/omb/assets/a11_current_year/a11_2017.pdf</t>
+      <t>https://www.fpds.gov/help/Extent_Competed.htm](https://www.fpds.gov/help/Extent_Competed.htm)</t>
     </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Learn More: </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>https://www.fpds.gov/help/Extent_Competed.htm</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Learn More: </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>https://www.gao.gov/assets/80/76911.pdf</t>
-    </r>
-  </si>
-  <si>
-    <t>https://www.gao.gov/assets/80/76911.pdf</t>
-  </si>
-  <si>
-    <t>https://www.fpds.gov/help/Extent_Competed.htm</t>
   </si>
 </sst>
 </file>
@@ -1701,9 +1669,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1714,6 +1679,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="4" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2002,8 +1970,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y1017"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2069,11 +2037,11 @@
       <c r="D2" s="3" t="s">
         <v>367</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="10" t="s">
         <v>266</v>
       </c>
-      <c r="F2" s="10" t="s">
-        <v>403</v>
+      <c r="F2" s="9" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="3" spans="1:25" s="6" customFormat="1" ht="39" x14ac:dyDescent="0.15">
@@ -2181,11 +2149,11 @@
       <c r="D9" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="10" t="s">
         <v>266</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
     </row>
     <row r="10" spans="1:25" s="6" customFormat="1" ht="65" x14ac:dyDescent="0.15">
@@ -2333,11 +2301,11 @@
       <c r="D18" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E18" s="11" t="s">
+      <c r="E18" s="10" t="s">
         <v>266</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>403</v>
+        <v>406</v>
       </c>
     </row>
     <row r="19" spans="1:6" s="6" customFormat="1" ht="70.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -2349,7 +2317,7 @@
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
-      <c r="E19" s="8" t="s">
+      <c r="E19" s="7" t="s">
         <v>42</v>
       </c>
       <c r="F19" s="3" t="s">
@@ -2381,7 +2349,7 @@
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
-      <c r="E21" s="8" t="s">
+      <c r="E21" s="7" t="s">
         <v>49</v>
       </c>
       <c r="F21" s="3" t="s">
@@ -2399,7 +2367,7 @@
       <c r="D22" s="3" t="s">
         <v>394</v>
       </c>
-      <c r="E22" s="8"/>
+      <c r="E22" s="7"/>
       <c r="F22" s="3"/>
     </row>
     <row r="23" spans="1:6" s="6" customFormat="1" ht="182" x14ac:dyDescent="0.15">
@@ -2418,7 +2386,7 @@
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
     </row>
-    <row r="24" spans="1:6" s="6" customFormat="1" ht="91" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:6" s="6" customFormat="1" ht="104" x14ac:dyDescent="0.15">
       <c r="A24" s="3" t="s">
         <v>15</v>
       </c>
@@ -2431,11 +2399,11 @@
       <c r="D24" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="E24" s="11" t="s">
+      <c r="E24" s="10" t="s">
         <v>266</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>403</v>
+        <v>406</v>
       </c>
     </row>
     <row r="25" spans="1:6" s="6" customFormat="1" ht="104" x14ac:dyDescent="0.15">
@@ -2447,10 +2415,10 @@
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
-      <c r="E25" s="11" t="s">
-        <v>408</v>
-      </c>
-      <c r="F25" s="8" t="s">
+      <c r="E25" s="10" t="s">
+        <v>403</v>
+      </c>
+      <c r="F25" s="7" t="s">
         <v>407</v>
       </c>
     </row>
@@ -2463,11 +2431,11 @@
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
-      <c r="E26" s="11" t="s">
+      <c r="E26" s="10" t="s">
+        <v>403</v>
+      </c>
+      <c r="F26" s="3" t="s">
         <v>408</v>
-      </c>
-      <c r="F26" s="8" t="s">
-        <v>407</v>
       </c>
     </row>
     <row r="27" spans="1:6" s="6" customFormat="1" ht="91" x14ac:dyDescent="0.15">
@@ -2479,7 +2447,7 @@
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
-      <c r="E27" s="8"/>
+      <c r="E27" s="7"/>
       <c r="F27" s="3"/>
     </row>
     <row r="28" spans="1:6" s="6" customFormat="1" ht="130" x14ac:dyDescent="0.15">
@@ -2495,7 +2463,7 @@
       <c r="D28" s="3" t="s">
         <v>324</v>
       </c>
-      <c r="E28" s="8" t="s">
+      <c r="E28" s="7" t="s">
         <v>61</v>
       </c>
       <c r="F28" s="3" t="s">
@@ -2529,7 +2497,7 @@
       <c r="D30" s="3" t="s">
         <v>395</v>
       </c>
-      <c r="E30" s="8"/>
+      <c r="E30" s="7"/>
       <c r="F30" s="3"/>
     </row>
     <row r="31" spans="1:6" s="6" customFormat="1" ht="247" x14ac:dyDescent="0.15">
@@ -2545,7 +2513,7 @@
       <c r="D31" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E31" s="8" t="s">
+      <c r="E31" s="7" t="s">
         <v>67</v>
       </c>
       <c r="F31" s="3" t="s">
@@ -2577,11 +2545,11 @@
       <c r="D33" s="3" t="s">
         <v>377</v>
       </c>
-      <c r="E33" s="11" t="s">
+      <c r="E33" s="10" t="s">
         <v>266</v>
       </c>
-      <c r="F33" s="7" t="s">
-        <v>404</v>
+      <c r="F33" s="9" t="s">
+        <v>406</v>
       </c>
     </row>
     <row r="34" spans="1:6" s="6" customFormat="1" ht="104" x14ac:dyDescent="0.15">
@@ -2593,7 +2561,7 @@
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
-      <c r="E34" s="8" t="s">
+      <c r="E34" s="7" t="s">
         <v>73</v>
       </c>
       <c r="F34" s="3" t="s">
@@ -2629,7 +2597,7 @@
       <c r="D36" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="E36" s="8" t="s">
+      <c r="E36" s="7" t="s">
         <v>82</v>
       </c>
       <c r="F36" s="3" t="s">
@@ -2645,7 +2613,7 @@
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
-      <c r="E37" s="8" t="s">
+      <c r="E37" s="7" t="s">
         <v>86</v>
       </c>
       <c r="F37" s="3" t="s">
@@ -2677,7 +2645,7 @@
       </c>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
-      <c r="E39" s="8"/>
+      <c r="E39" s="7"/>
       <c r="F39" s="3"/>
     </row>
     <row r="40" spans="1:6" s="6" customFormat="1" ht="104" x14ac:dyDescent="0.15">
@@ -2693,7 +2661,7 @@
       <c r="D40" s="3" t="s">
         <v>396</v>
       </c>
-      <c r="E40" s="8"/>
+      <c r="E40" s="7"/>
       <c r="F40" s="3"/>
     </row>
     <row r="41" spans="1:6" s="6" customFormat="1" ht="91" x14ac:dyDescent="0.15">
@@ -2709,7 +2677,7 @@
       <c r="D41" s="3" t="s">
         <v>397</v>
       </c>
-      <c r="E41" s="8"/>
+      <c r="E41" s="7"/>
       <c r="F41" s="3"/>
     </row>
     <row r="42" spans="1:6" s="6" customFormat="1" ht="130" x14ac:dyDescent="0.15">
@@ -2781,11 +2749,11 @@
       <c r="D45" s="3" t="s">
         <v>378</v>
       </c>
-      <c r="E45" s="11" t="s">
+      <c r="E45" s="10" t="s">
+        <v>404</v>
+      </c>
+      <c r="F45" s="3" t="s">
         <v>409</v>
-      </c>
-      <c r="F45" s="3" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="46" spans="1:6" s="6" customFormat="1" ht="91" x14ac:dyDescent="0.15">
@@ -2829,7 +2797,7 @@
       </c>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
-      <c r="E48" s="8" t="s">
+      <c r="E48" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F48" s="3" t="s">
@@ -2873,7 +2841,7 @@
       </c>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
-      <c r="E51" s="8" t="s">
+      <c r="E51" s="7" t="s">
         <v>111</v>
       </c>
       <c r="F51" s="3" t="s">
@@ -2981,7 +2949,7 @@
       </c>
       <c r="C58" s="3"/>
       <c r="D58" s="3"/>
-      <c r="E58" s="8" t="s">
+      <c r="E58" s="7" t="s">
         <v>120</v>
       </c>
       <c r="F58" s="3" t="s">
@@ -3001,7 +2969,7 @@
       <c r="D59" s="3" t="s">
         <v>400</v>
       </c>
-      <c r="E59" s="8"/>
+      <c r="E59" s="7"/>
       <c r="F59" s="3"/>
     </row>
     <row r="60" spans="1:6" s="6" customFormat="1" ht="143" x14ac:dyDescent="0.15">
@@ -3017,11 +2985,11 @@
       <c r="D60" s="3" t="s">
         <v>375</v>
       </c>
-      <c r="E60" s="11" t="s">
+      <c r="E60" s="10" t="s">
         <v>266</v>
       </c>
-      <c r="F60" s="7" t="s">
-        <v>404</v>
+      <c r="F60" s="9" t="s">
+        <v>406</v>
       </c>
     </row>
     <row r="61" spans="1:6" s="6" customFormat="1" ht="221" x14ac:dyDescent="0.15">
@@ -3065,7 +3033,7 @@
       </c>
       <c r="C63" s="3"/>
       <c r="D63" s="3"/>
-      <c r="E63" s="8" t="s">
+      <c r="E63" s="7" t="s">
         <v>86</v>
       </c>
       <c r="F63" s="3" t="s">
@@ -3081,7 +3049,7 @@
       </c>
       <c r="C64" s="3"/>
       <c r="D64" s="3"/>
-      <c r="E64" s="11" t="s">
+      <c r="E64" s="10" t="s">
         <v>127</v>
       </c>
       <c r="F64" s="3" t="s">
@@ -3185,7 +3153,7 @@
       </c>
       <c r="C71" s="3"/>
       <c r="D71" s="3"/>
-      <c r="E71" s="8" t="s">
+      <c r="E71" s="7" t="s">
         <v>140</v>
       </c>
       <c r="F71" s="3" t="s">
@@ -3201,7 +3169,7 @@
       </c>
       <c r="C72" s="3"/>
       <c r="D72" s="3"/>
-      <c r="E72" s="8"/>
+      <c r="E72" s="7"/>
       <c r="F72" s="3"/>
     </row>
     <row r="73" spans="1:6" s="6" customFormat="1" ht="117" x14ac:dyDescent="0.15">
@@ -3217,7 +3185,7 @@
       <c r="D73" s="3" t="s">
         <v>325</v>
       </c>
-      <c r="E73" s="8" t="s">
+      <c r="E73" s="7" t="s">
         <v>149</v>
       </c>
       <c r="F73" s="3" t="s">
@@ -3253,7 +3221,7 @@
       <c r="D75" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="E75" s="8" t="s">
+      <c r="E75" s="7" t="s">
         <v>266</v>
       </c>
       <c r="F75" s="3" t="s">
@@ -3302,14 +3270,14 @@
       <c r="C78" s="3" t="s">
         <v>370</v>
       </c>
-      <c r="D78" s="9" t="s">
+      <c r="D78" s="8" t="s">
         <v>376</v>
       </c>
-      <c r="E78" s="11" t="s">
+      <c r="E78" s="10" t="s">
         <v>266</v>
       </c>
-      <c r="F78" s="7" t="s">
-        <v>405</v>
+      <c r="F78" s="11" t="s">
+        <v>406</v>
       </c>
     </row>
     <row r="79" spans="1:6" s="6" customFormat="1" ht="260" x14ac:dyDescent="0.15">
@@ -3321,7 +3289,7 @@
       </c>
       <c r="C79" s="3"/>
       <c r="D79" s="3"/>
-      <c r="E79" s="8" t="s">
+      <c r="E79" s="7" t="s">
         <v>161</v>
       </c>
       <c r="F79" s="3" t="s">
@@ -3457,11 +3425,11 @@
       <c r="D87" s="3" t="s">
         <v>369</v>
       </c>
-      <c r="E87" s="11" t="s">
+      <c r="E87" s="10" t="s">
         <v>266</v>
       </c>
-      <c r="F87" s="7" t="s">
-        <v>404</v>
+      <c r="F87" s="9" t="s">
+        <v>406</v>
       </c>
     </row>
     <row r="88" spans="1:6" s="6" customFormat="1" ht="91" x14ac:dyDescent="0.15">
@@ -3569,7 +3537,7 @@
       <c r="D94" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="E94" s="8" t="s">
+      <c r="E94" s="7" t="s">
         <v>181</v>
       </c>
       <c r="F94" s="3" t="s">
@@ -3713,7 +3681,7 @@
       <c r="D103" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="E103" s="8" t="s">
+      <c r="E103" s="7" t="s">
         <v>188</v>
       </c>
       <c r="F103" s="3" t="s">
@@ -3749,7 +3717,7 @@
       <c r="D105" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="E105" s="8" t="s">
+      <c r="E105" s="7" t="s">
         <v>145</v>
       </c>
       <c r="F105" s="3" t="s">
@@ -3769,7 +3737,7 @@
       <c r="D106" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="E106" s="8" t="s">
+      <c r="E106" s="7" t="s">
         <v>201</v>
       </c>
       <c r="F106" s="3" t="s">
@@ -3785,7 +3753,7 @@
       </c>
       <c r="C107" s="3"/>
       <c r="D107" s="3"/>
-      <c r="E107" s="8" t="s">
+      <c r="E107" s="7" t="s">
         <v>205</v>
       </c>
       <c r="F107" s="3" t="s">
@@ -3869,7 +3837,7 @@
       </c>
       <c r="C113" s="3"/>
       <c r="D113" s="3"/>
-      <c r="E113" s="8" t="s">
+      <c r="E113" s="7" t="s">
         <v>86</v>
       </c>
       <c r="F113" s="3" t="s">
@@ -3957,7 +3925,7 @@
       </c>
       <c r="C119" s="3"/>
       <c r="D119" s="3"/>
-      <c r="E119" s="8" t="s">
+      <c r="E119" s="7" t="s">
         <v>229</v>
       </c>
       <c r="F119" s="3" t="s">

</xml_diff>

<commit_message>
Updated glossary with outlined changes
</commit_message>
<xml_diff>
--- a/usaspending_api/data/USAspendingGlossary.xlsx
+++ b/usaspending_api/data/USAspendingGlossary.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10709"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alisaburdeyny/GitHub/usaspending-api/usaspending_api/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kwadwoopoku/usaspending-api/usaspending_api/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{33723B43-2808-D44E-9684-3291065C58BF}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E2DAC1B3-EC01-0741-9546-7B50323AF5FD}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27420" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2180" yWindow="2080" windowWidth="27420" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$Y$119</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$Y$121</definedName>
   </definedNames>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="413">
   <si>
     <t>Term</t>
   </si>
@@ -582,12 +582,6 @@
     <t>The principal place of business, where the majority of the work is performed. For example, in a manufacturing contract, this would be the main plant where items are produced.</t>
   </si>
   <si>
-    <t>Prime Contractor</t>
-  </si>
-  <si>
-    <t>A company, organization, or agency who receives a contract with the federal government. A prime contractor may be a corporation, small business, university, non-profit, or other entity. A prime contractor may hire a sub-contractor to perform work on the contract.</t>
-  </si>
-  <si>
     <t>Procurement Instrument Identifier (PIID)</t>
   </si>
   <si>
@@ -711,19 +705,10 @@
     <t>When an agency needs work done, it can ask for information or bids on the work. These requests are called solicitations. They often come as a RFI (Request for Information) or RFP (Request for Proposal).</t>
   </si>
   <si>
-    <t>Sub-account Code</t>
-  </si>
-  <si>
     <t>Identifies a sub-division of the Treasury Account Symbol (TAS). This is a 3-digit number. It cannot be blank. A sub-account code of "000" means that the TAS is the parent account.</t>
   </si>
   <si>
     <t>This is a component of the TAS. Identifies a Treasury-defined subdivision of the main account. This field cannot be blank. Subaccount 000 indicates the Parent account.</t>
-  </si>
-  <si>
-    <t>Sub-contractor</t>
-  </si>
-  <si>
-    <t>When a company has a contract with the U.S. government, they may hire another company to perform work on the contract. When this happens, the company who received the contract is called the prime contractor. The company hired by the prime is called the sub-contractor.</t>
   </si>
   <si>
     <t>Subsidy Cost</t>
@@ -1207,15 +1192,6 @@
 Current Total Value of Award</t>
   </si>
   <si>
-    <t>See also:
-- [Federal Action Obligation](?glossary=Federal-Action-Obligation) (Federal Action Obligation)
-- [Subsidy Cost](?glossary=subsidy-cost)
-- [Current Total Value of Award](?glossary=Current- Total-Value-of-Award)</t>
-  </si>
-  <si>
-    <t>Awarding Sub Agency</t>
-  </si>
-  <si>
     <t>The Awarding Sub Agency is the sub agency that issues and administers the award. For example, the Internal Revenue Service (IRS) is a sub agency of the Department of the Treasury.</t>
   </si>
   <si>
@@ -1389,9 +1365,6 @@
 These are further broken down into budget sub functions.</t>
   </si>
   <si>
-    <t>Budget Sub function</t>
-  </si>
-  <si>
     <t>The federal budget is divided into functions and sub functions. These categories organize federal spending into topics based on the major purpose the spending serves. There are about 20 major functions (e.g., National Defense, Transportation, Health). Most of these functions are further divided into sub functions.
 For example, the budget function for Health is divided into sub functions for Health care services, Health research and training, and Consumer and occupational health and safety.</t>
   </si>
@@ -1403,9 +1376,6 @@
   </si>
   <si>
     <t>Multiple recipients is a term that replaces recipients’ names, in aggregate awards, to protect recipients’ Personally Identifiable Information (PII) — for example, names, addresses, and Social Security numbers. Agencies are currently required to aggregate these awards on a county level.</t>
-  </si>
-  <si>
-    <t>Funding Sub Agency</t>
   </si>
   <si>
     <t xml:space="preserve">The office within an agency that issues and administers the award. </t>
@@ -1559,6 +1529,63 @@
   </si>
   <si>
     <t>Indicates whether the transaction is subject to the Construction Wage Rate Requirements. The clause is 52.222-6 "Construction Wage Rate Requirements" -that goes with Wage Rate Requirements (Construction) (formerly Davis-Bacon Act).</t>
+  </si>
+  <si>
+    <t>Awarding Sub-Agency</t>
+  </si>
+  <si>
+    <t>Budget Sub-Function</t>
+  </si>
+  <si>
+    <t>Funding Sub-Agency</t>
+  </si>
+  <si>
+    <t>Sub-Account Code</t>
+  </si>
+  <si>
+    <t>Sub-Award</t>
+  </si>
+  <si>
+    <t>An award provided by a pass-through entity to a subrecipient for the subrecipient to carry out part of a federal award received by the pass-through entity.  It does not include payments to a contractor or payments to an individual that is a beneficiary of a federal program.  A subaward may be provided through any form of legal agreement, including an agreement that the pass-through entity considers a contract. (2CFR)</t>
+  </si>
+  <si>
+    <t>Sub-Recipient</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A company, organization, individual, or government entity (i.e., state, local, tribal, or foreign) that receives funding from another recipient of federal funds (a prime recipient), rather than directly from the U.S. government. The sub-recipient may be a sub-contractor or a sub-grantee. For example,  the Dept. of Transporation awards Bridge Company A a bridge construction contract. Bridge Company A needs Bridge Company B to supply the steel, so  Bridge Company A awards Bridge Company B a sub-award.  Bridge Company B is the sub-contractor.  On the grants side, University A receives an R&amp;D grant from the National Science Foundation.  University A needs University B to perform the initial step in the research, so University A awards University B a sub-award. University B is the sub-grantee. </t>
+  </si>
+  <si>
+    <t>A non-Federal entity that receives a sub-award from a pass-through entity to carry out part of a federal program; but does not include an individual that is the beneficiary of such program. (grants.gov)</t>
+  </si>
+  <si>
+    <t>Prime Award</t>
+  </si>
+  <si>
+    <t>A Prime Award is a a federal award that is either:
+(1) Federal financial assistance that a non-Federal entity receives directly from a Federal awarding agency; or
+(2) The cost-reimbursement contract under the Federal Acquisition Regulations that a non-Federal entity receives directly from a Federal awarding agency.
+(Adapted from 2 CFR §200.38)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A prime award is an agreement that the government makes with a non-federal entity for the purpose of carrying out a federal program. The entities receiving the award are known as prime recipients. </t>
+  </si>
+  <si>
+    <t>Prime Recipient</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A company, organization, individual, or government entity (i.e., state, local, tribal, or foreign) that receives funding directly from the U.S. government. They receive this funding through an agreement called a prime award. For example, if the Dept. of Transporation is building a bridge, they can award Bridge Company A the contract to carry out the construction. Bridge Company A would be the prime recipient. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A non-Federal entity that receives a Federal award directly from a Federal awarding agency to carry out an activity under a Federal program. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A sub-award is an agreement that a prime recipient makes with another entity to perform a portion of their award. On our website, these recipients are known as sub-recipients. Sub-awards might also be referred to as a sub-contract or a sub-grant. </t>
+  </si>
+  <si>
+    <t>See also:
+- [Federal Action Obligation](?glossary=federal-action-obligation)
+- [Subsidy Cost](?glossary=subsidy-cost)
+- [Current Total Value of Award](?glossary=Current- Total-Value-of-Award)</t>
   </si>
 </sst>
 </file>
@@ -1638,7 +1665,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1683,6 +1710,15 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1969,11 +2005,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y1018"/>
+  <dimension ref="A1:Y1020"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C71" sqref="C71"/>
+    <sheetView tabSelected="1" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2028,52 +2064,52 @@
     </row>
     <row r="2" spans="1:25" s="6" customFormat="1" ht="130" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>360</v>
+        <v>353</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>356</v>
+        <v>349</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>395</v>
+        <v>386</v>
       </c>
     </row>
     <row r="3" spans="1:25" s="6" customFormat="1" ht="39" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="12"/>
     </row>
     <row r="4" spans="1:25" s="6" customFormat="1" ht="104" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="12"/>
@@ -2083,13 +2119,13 @@
         <v>6</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="12"/>
@@ -2149,13 +2185,13 @@
         <v>18</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>395</v>
+        <v>386</v>
       </c>
     </row>
     <row r="10" spans="1:25" s="6" customFormat="1" ht="65" x14ac:dyDescent="0.15">
@@ -2179,31 +2215,31 @@
         <v>22</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>357</v>
+        <v>350</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="12"/>
     </row>
-    <row r="12" spans="1:25" s="6" customFormat="1" ht="143" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:25" s="6" customFormat="1" ht="130" x14ac:dyDescent="0.15">
       <c r="A12" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>24</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>335</v>
+        <v>412</v>
       </c>
     </row>
     <row r="13" spans="1:25" s="6" customFormat="1" ht="52" x14ac:dyDescent="0.15">
@@ -2239,7 +2275,7 @@
         <v>33</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
     </row>
     <row r="15" spans="1:25" s="6" customFormat="1" ht="65" x14ac:dyDescent="0.15">
@@ -2250,42 +2286,42 @@
         <v>35</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="12"/>
     </row>
     <row r="16" spans="1:25" s="6" customFormat="1" ht="39" x14ac:dyDescent="0.15">
       <c r="A16" s="3" t="s">
-        <v>341</v>
+        <v>334</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>379</v>
+        <v>370</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="12"/>
     </row>
     <row r="17" spans="1:6" s="6" customFormat="1" ht="52" x14ac:dyDescent="0.15">
       <c r="A17" s="3" t="s">
-        <v>336</v>
+        <v>396</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="12"/>
@@ -2304,10 +2340,10 @@
         <v>39</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>396</v>
+        <v>387</v>
       </c>
     </row>
     <row r="19" spans="1:6" s="6" customFormat="1" ht="70.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -2360,14 +2396,14 @@
     </row>
     <row r="22" spans="1:6" s="6" customFormat="1" ht="117" x14ac:dyDescent="0.15">
       <c r="A22" s="3" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3" t="s">
-        <v>383</v>
+        <v>374</v>
       </c>
       <c r="E22" s="7"/>
       <c r="F22" s="12"/>
@@ -2380,7 +2416,7 @@
         <v>52</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>53</v>
@@ -2393,19 +2429,19 @@
         <v>15</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>15</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>396</v>
+        <v>387</v>
       </c>
     </row>
     <row r="25" spans="1:6" s="6" customFormat="1" ht="104" x14ac:dyDescent="0.15">
@@ -2413,39 +2449,39 @@
         <v>54</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>372</v>
+        <v>365</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="9" t="s">
-        <v>392</v>
+        <v>383</v>
       </c>
       <c r="F25" s="13" t="s">
-        <v>397</v>
+        <v>388</v>
       </c>
     </row>
     <row r="26" spans="1:6" s="6" customFormat="1" ht="156" x14ac:dyDescent="0.15">
       <c r="A26" s="3" t="s">
-        <v>373</v>
+        <v>397</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="9" t="s">
-        <v>392</v>
+        <v>383</v>
       </c>
       <c r="F26" s="13" t="s">
-        <v>397</v>
+        <v>388</v>
       </c>
     </row>
     <row r="27" spans="1:6" s="6" customFormat="1" ht="91" x14ac:dyDescent="0.15">
       <c r="A27" s="3" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
@@ -2460,10 +2496,10 @@
         <v>60</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="E28" s="7" t="s">
         <v>61</v>
@@ -2490,16 +2526,16 @@
     </row>
     <row r="30" spans="1:6" s="6" customFormat="1" ht="65" x14ac:dyDescent="0.15">
       <c r="A30" s="3" t="s">
-        <v>403</v>
+        <v>394</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>404</v>
+        <v>395</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>403</v>
+        <v>394</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>404</v>
+        <v>395</v>
       </c>
       <c r="E30" s="7" t="s">
         <v>78</v>
@@ -2510,14 +2546,14 @@
     </row>
     <row r="31" spans="1:6" s="6" customFormat="1" ht="195" x14ac:dyDescent="0.15">
       <c r="A31" s="3" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3" t="s">
-        <v>384</v>
+        <v>375</v>
       </c>
       <c r="E31" s="7"/>
       <c r="F31" s="12"/>
@@ -2556,22 +2592,22 @@
     </row>
     <row r="34" spans="1:6" s="6" customFormat="1" ht="377" x14ac:dyDescent="0.15">
       <c r="A34" s="3" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="F34" s="12" t="s">
-        <v>396</v>
+        <v>387</v>
       </c>
     </row>
     <row r="35" spans="1:6" s="6" customFormat="1" ht="104" x14ac:dyDescent="0.15">
@@ -2595,7 +2631,7 @@
         <v>75</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>76</v>
@@ -2624,26 +2660,26 @@
     </row>
     <row r="38" spans="1:6" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A38" s="3" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="E38" s="3"/>
       <c r="F38" s="12"/>
     </row>
     <row r="39" spans="1:6" s="6" customFormat="1" ht="39" x14ac:dyDescent="0.15">
       <c r="A39" s="3" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
@@ -2652,32 +2688,32 @@
     </row>
     <row r="40" spans="1:6" s="6" customFormat="1" ht="104" x14ac:dyDescent="0.15">
       <c r="A40" s="3" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>385</v>
+        <v>376</v>
       </c>
       <c r="E40" s="7"/>
       <c r="F40" s="12"/>
     </row>
     <row r="41" spans="1:6" s="6" customFormat="1" ht="91" x14ac:dyDescent="0.15">
       <c r="A41" s="3" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>386</v>
+        <v>377</v>
       </c>
       <c r="E41" s="7"/>
       <c r="F41" s="12"/>
@@ -2710,16 +2746,16 @@
         <v>90</v>
       </c>
       <c r="C43" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="D43" s="3" t="s">
         <v>289</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>294</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>91</v>
       </c>
       <c r="F43" s="12" t="s">
-        <v>398</v>
+        <v>389</v>
       </c>
     </row>
     <row r="44" spans="1:6" s="6" customFormat="1" ht="65" x14ac:dyDescent="0.15">
@@ -2749,24 +2785,24 @@
         <v>97</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>367</v>
+        <v>360</v>
       </c>
       <c r="E45" s="9" t="s">
-        <v>393</v>
+        <v>384</v>
       </c>
       <c r="F45" s="12" t="s">
-        <v>394</v>
+        <v>385</v>
       </c>
     </row>
     <row r="46" spans="1:6" s="6" customFormat="1" ht="91" x14ac:dyDescent="0.15">
       <c r="A46" s="3" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>339</v>
+        <v>332</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>126</v>
@@ -2779,7 +2815,7 @@
         <v>98</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>98</v>
@@ -2808,16 +2844,16 @@
     </row>
     <row r="49" spans="1:6" s="6" customFormat="1" ht="39" x14ac:dyDescent="0.15">
       <c r="A49" s="3" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="E49" s="3"/>
       <c r="F49" s="12"/>
@@ -2864,16 +2900,16 @@
     </row>
     <row r="53" spans="1:6" s="6" customFormat="1" ht="65" x14ac:dyDescent="0.15">
       <c r="A53" s="3" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>388</v>
+        <v>379</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>387</v>
+        <v>378</v>
       </c>
       <c r="E53" s="3"/>
       <c r="F53" s="12"/>
@@ -2886,20 +2922,20 @@
         <v>113</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="E54" s="3"/>
       <c r="F54" s="12"/>
     </row>
     <row r="55" spans="1:6" s="6" customFormat="1" ht="104" x14ac:dyDescent="0.15">
       <c r="A55" s="3" t="s">
-        <v>353</v>
+        <v>346</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>354</v>
+        <v>347</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>145</v>
@@ -2912,39 +2948,39 @@
     </row>
     <row r="56" spans="1:6" s="6" customFormat="1" ht="39" x14ac:dyDescent="0.15">
       <c r="A56" s="3" t="s">
-        <v>340</v>
+        <v>333</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>342</v>
+        <v>335</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="E56" s="3"/>
       <c r="F56" s="12"/>
     </row>
     <row r="57" spans="1:6" s="6" customFormat="1" ht="65" x14ac:dyDescent="0.15">
       <c r="A57" s="3" t="s">
-        <v>378</v>
+        <v>398</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>343</v>
+        <v>336</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="E57" s="3"/>
       <c r="F57" s="12"/>
     </row>
     <row r="58" spans="1:6" s="6" customFormat="1" ht="169" x14ac:dyDescent="0.15">
       <c r="A58" s="3" t="s">
-        <v>375</v>
+        <v>367</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>114</v>
@@ -2960,68 +2996,68 @@
     </row>
     <row r="59" spans="1:6" s="6" customFormat="1" ht="182" x14ac:dyDescent="0.15">
       <c r="A59" s="3" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>389</v>
+        <v>380</v>
       </c>
       <c r="E59" s="7"/>
       <c r="F59" s="12"/>
     </row>
     <row r="60" spans="1:6" s="6" customFormat="1" ht="143" x14ac:dyDescent="0.15">
       <c r="A60" s="3" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>364</v>
+        <v>357</v>
       </c>
       <c r="E60" s="9" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="F60" s="11" t="s">
-        <v>396</v>
+        <v>387</v>
       </c>
     </row>
     <row r="61" spans="1:6" s="6" customFormat="1" ht="221" x14ac:dyDescent="0.15">
       <c r="A61" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="B61" s="3" t="s">
         <v>290</v>
       </c>
-      <c r="B61" s="3" t="s">
-        <v>295</v>
-      </c>
       <c r="C61" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="D61" s="3" t="s">
         <v>290</v>
-      </c>
-      <c r="D61" s="3" t="s">
-        <v>295</v>
       </c>
       <c r="E61" s="3"/>
       <c r="F61" s="12"/>
     </row>
     <row r="62" spans="1:6" s="6" customFormat="1" ht="130" x14ac:dyDescent="0.15">
       <c r="A62" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="B62" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="B62" s="3" t="s">
-        <v>296</v>
-      </c>
       <c r="C62" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="D62" s="3" t="s">
         <v>291</v>
-      </c>
-      <c r="D62" s="3" t="s">
-        <v>296</v>
       </c>
       <c r="E62" s="3"/>
       <c r="F62" s="12"/>
@@ -3072,16 +3108,16 @@
     </row>
     <row r="66" spans="1:6" s="6" customFormat="1" ht="65" x14ac:dyDescent="0.15">
       <c r="A66" s="3" t="s">
-        <v>400</v>
+        <v>391</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>401</v>
+        <v>392</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>400</v>
+        <v>391</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>401</v>
+        <v>392</v>
       </c>
       <c r="E66" s="7" t="s">
         <v>137</v>
@@ -3092,26 +3128,26 @@
     </row>
     <row r="67" spans="1:6" s="6" customFormat="1" ht="65" x14ac:dyDescent="0.15">
       <c r="A67" s="3" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>348</v>
+        <v>341</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>348</v>
+        <v>341</v>
       </c>
       <c r="E67" s="3"/>
       <c r="F67" s="12"/>
     </row>
     <row r="68" spans="1:6" s="6" customFormat="1" ht="91" x14ac:dyDescent="0.15">
       <c r="A68" s="3" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>391</v>
+        <v>382</v>
       </c>
       <c r="C68" s="3"/>
       <c r="D68" s="3"/>
@@ -3152,36 +3188,36 @@
     </row>
     <row r="71" spans="1:6" s="6" customFormat="1" ht="91" x14ac:dyDescent="0.15">
       <c r="A71" s="3" t="s">
-        <v>399</v>
+        <v>390</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>402</v>
+        <v>393</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>399</v>
+        <v>390</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>402</v>
+        <v>393</v>
       </c>
       <c r="E71" s="7" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="F71" s="12" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
     </row>
     <row r="72" spans="1:6" s="6" customFormat="1" ht="277.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A72" s="3" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="E72" s="3"/>
       <c r="F72" s="12"/>
@@ -3204,10 +3240,10 @@
     </row>
     <row r="74" spans="1:6" s="6" customFormat="1" ht="78" x14ac:dyDescent="0.15">
       <c r="A74" s="3" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="C74" s="3"/>
       <c r="D74" s="3"/>
@@ -3222,10 +3258,10 @@
         <v>140</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="E75" s="7" t="s">
         <v>141</v>
@@ -3236,16 +3272,16 @@
     </row>
     <row r="76" spans="1:6" s="6" customFormat="1" ht="65" x14ac:dyDescent="0.15">
       <c r="A76" s="3" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="E76" s="3"/>
       <c r="F76" s="12"/>
@@ -3261,13 +3297,13 @@
         <v>143</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="E77" s="7" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="F77" s="12" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
     </row>
     <row r="78" spans="1:6" s="6" customFormat="1" ht="409.6" x14ac:dyDescent="0.15">
@@ -3281,7 +3317,7 @@
         <v>147</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="E78" s="3"/>
       <c r="F78" s="12"/>
@@ -3297,29 +3333,29 @@
         <v>149</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="E79" s="3"/>
       <c r="F79" s="12"/>
     </row>
     <row r="80" spans="1:6" s="6" customFormat="1" ht="143" x14ac:dyDescent="0.15">
       <c r="A80" s="3" t="s">
-        <v>359</v>
+        <v>352</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>359</v>
+        <v>352</v>
       </c>
       <c r="D80" s="8" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="E80" s="9" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="F80" s="14" t="s">
-        <v>396</v>
+        <v>387</v>
       </c>
     </row>
     <row r="81" spans="1:6" s="6" customFormat="1" ht="260" x14ac:dyDescent="0.15">
@@ -3340,16 +3376,16 @@
     </row>
     <row r="82" spans="1:6" s="6" customFormat="1" ht="130" x14ac:dyDescent="0.15">
       <c r="A82" s="3" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="E82" s="3"/>
       <c r="F82" s="12"/>
@@ -3359,133 +3395,133 @@
         <v>155</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="C83" s="3" t="s">
         <v>156</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="E83" s="3"/>
       <c r="F83" s="12"/>
     </row>
     <row r="84" spans="1:6" s="6" customFormat="1" ht="52" x14ac:dyDescent="0.15">
       <c r="A84" s="3" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="E84" s="3"/>
       <c r="F84" s="12"/>
     </row>
     <row r="85" spans="1:6" s="6" customFormat="1" ht="91" x14ac:dyDescent="0.15">
       <c r="A85" s="3" t="s">
-        <v>355</v>
+        <v>348</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="E85" s="3" t="s">
         <v>91</v>
       </c>
       <c r="F85" s="12" t="s">
-        <v>398</v>
+        <v>389</v>
       </c>
     </row>
     <row r="86" spans="1:6" s="6" customFormat="1" ht="91" x14ac:dyDescent="0.15">
       <c r="A86" s="3" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="E86" s="3"/>
       <c r="F86" s="12"/>
     </row>
     <row r="87" spans="1:6" s="6" customFormat="1" ht="117" x14ac:dyDescent="0.15">
       <c r="A87" s="3" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="E87" s="3"/>
       <c r="F87" s="12"/>
     </row>
     <row r="88" spans="1:6" s="6" customFormat="1" ht="39" x14ac:dyDescent="0.15">
       <c r="A88" s="3" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="E88" s="3"/>
       <c r="F88" s="12"/>
     </row>
     <row r="89" spans="1:6" s="6" customFormat="1" ht="338" x14ac:dyDescent="0.15">
       <c r="A89" s="3" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>358</v>
+        <v>351</v>
       </c>
       <c r="E89" s="9" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="F89" s="11" t="s">
-        <v>396</v>
+        <v>387</v>
       </c>
     </row>
     <row r="90" spans="1:6" s="6" customFormat="1" ht="91" x14ac:dyDescent="0.15">
       <c r="A90" s="3" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="C90" s="3" t="s">
         <v>25</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="E90" s="3"/>
       <c r="F90" s="12"/>
@@ -3498,456 +3534,486 @@
         <v>158</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="E91" s="3"/>
       <c r="F91" s="12"/>
     </row>
     <row r="92" spans="1:6" s="6" customFormat="1" ht="65" x14ac:dyDescent="0.15">
       <c r="A92" s="3" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>380</v>
+        <v>371</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="E92" s="3"/>
       <c r="F92" s="12"/>
     </row>
     <row r="93" spans="1:6" s="6" customFormat="1" ht="52" x14ac:dyDescent="0.15">
       <c r="A93" s="3" t="s">
-        <v>381</v>
+        <v>372</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>382</v>
+        <v>373</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="E93" s="3"/>
       <c r="F93" s="12"/>
     </row>
-    <row r="94" spans="1:6" s="6" customFormat="1" ht="78" x14ac:dyDescent="0.15">
-      <c r="A94" s="3" t="s">
-        <v>159</v>
+    <row r="94" spans="1:6" s="6" customFormat="1" ht="104" x14ac:dyDescent="0.15">
+      <c r="A94" s="17" t="s">
+        <v>405</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>160</v>
+        <v>407</v>
       </c>
       <c r="C94" s="3"/>
-      <c r="D94" s="3"/>
+      <c r="D94" s="3" t="s">
+        <v>406</v>
+      </c>
       <c r="E94" s="3"/>
       <c r="F94" s="12"/>
     </row>
-    <row r="95" spans="1:6" s="6" customFormat="1" ht="78" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:6" s="6" customFormat="1" ht="117" x14ac:dyDescent="0.15">
       <c r="A95" s="3" t="s">
-        <v>161</v>
+        <v>408</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="C95" s="3" t="s">
-        <v>161</v>
-      </c>
+        <v>409</v>
+      </c>
+      <c r="C95" s="3"/>
       <c r="D95" s="3" t="s">
-        <v>370</v>
+        <v>410</v>
       </c>
       <c r="E95" s="3"/>
       <c r="F95" s="12"/>
     </row>
-    <row r="96" spans="1:6" s="6" customFormat="1" ht="117" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:6" s="6" customFormat="1" ht="78" x14ac:dyDescent="0.15">
       <c r="A96" s="3" t="s">
-        <v>352</v>
+        <v>159</v>
       </c>
       <c r="B96" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C96" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="D96" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="E96" s="3"/>
+      <c r="F96" s="12"/>
+    </row>
+    <row r="97" spans="1:6" s="6" customFormat="1" ht="117" x14ac:dyDescent="0.15">
+      <c r="A97" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="B97" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="C97" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="D97" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="C96" s="3" t="s">
+      <c r="E97" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="D96" s="3" t="s">
+      <c r="F97" s="12" t="s">
         <v>172</v>
       </c>
-      <c r="E96" s="7" t="s">
-        <v>173</v>
-      </c>
-      <c r="F96" s="12" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6" s="6" customFormat="1" ht="65" x14ac:dyDescent="0.15">
-      <c r="A97" s="3" t="s">
+    </row>
+    <row r="98" spans="1:6" s="6" customFormat="1" ht="65" x14ac:dyDescent="0.15">
+      <c r="A98" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C98" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="B97" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="C97" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="D97" s="3" t="s">
-        <v>258</v>
-      </c>
-      <c r="E97" s="3"/>
-      <c r="F97" s="12"/>
-    </row>
-    <row r="98" spans="1:6" s="6" customFormat="1" ht="130" x14ac:dyDescent="0.15">
-      <c r="A98" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="B98" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="C98" s="3" t="s">
-        <v>168</v>
-      </c>
       <c r="D98" s="3" t="s">
-        <v>169</v>
+        <v>253</v>
       </c>
       <c r="E98" s="3"/>
       <c r="F98" s="12"/>
     </row>
-    <row r="99" spans="1:6" s="6" customFormat="1" ht="52" x14ac:dyDescent="0.15">
+    <row r="99" spans="1:6" s="6" customFormat="1" ht="130" x14ac:dyDescent="0.15">
       <c r="A99" s="3" t="s">
-        <v>236</v>
+        <v>164</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>237</v>
+        <v>165</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>236</v>
+        <v>166</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>390</v>
+        <v>167</v>
       </c>
       <c r="E99" s="3"/>
       <c r="F99" s="12"/>
     </row>
-    <row r="100" spans="1:6" s="6" customFormat="1" ht="104" x14ac:dyDescent="0.15">
+    <row r="100" spans="1:6" s="6" customFormat="1" ht="52" x14ac:dyDescent="0.15">
       <c r="A100" s="3" t="s">
-        <v>330</v>
+        <v>231</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>332</v>
+        <v>232</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>263</v>
+        <v>231</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>264</v>
+        <v>381</v>
       </c>
       <c r="E100" s="3"/>
       <c r="F100" s="12"/>
     </row>
-    <row r="101" spans="1:6" s="6" customFormat="1" ht="39" x14ac:dyDescent="0.15">
+    <row r="101" spans="1:6" s="6" customFormat="1" ht="104" x14ac:dyDescent="0.15">
       <c r="A101" s="3" t="s">
-        <v>175</v>
+        <v>325</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="C101" s="3"/>
-      <c r="D101" s="3"/>
+        <v>327</v>
+      </c>
+      <c r="C101" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="D101" s="3" t="s">
+        <v>259</v>
+      </c>
       <c r="E101" s="3"/>
       <c r="F101" s="12"/>
     </row>
     <row r="102" spans="1:6" s="6" customFormat="1" ht="39" x14ac:dyDescent="0.15">
       <c r="A102" s="3" t="s">
-        <v>345</v>
+        <v>173</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>346</v>
-      </c>
-      <c r="C102" s="3" t="s">
-        <v>298</v>
-      </c>
-      <c r="D102" s="3" t="s">
-        <v>297</v>
-      </c>
+        <v>174</v>
+      </c>
+      <c r="C102" s="3"/>
+      <c r="D102" s="3"/>
       <c r="E102" s="3"/>
       <c r="F102" s="12"/>
     </row>
-    <row r="103" spans="1:6" s="6" customFormat="1" ht="104" x14ac:dyDescent="0.15">
+    <row r="103" spans="1:6" s="6" customFormat="1" ht="39" x14ac:dyDescent="0.15">
       <c r="A103" s="3" t="s">
-        <v>182</v>
+        <v>338</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>183</v>
+        <v>339</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>184</v>
+        <v>293</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>344</v>
+        <v>292</v>
       </c>
       <c r="E103" s="3"/>
       <c r="F103" s="12"/>
     </row>
-    <row r="104" spans="1:6" s="6" customFormat="1" ht="117" x14ac:dyDescent="0.15">
+    <row r="104" spans="1:6" s="6" customFormat="1" ht="104" x14ac:dyDescent="0.15">
       <c r="A104" s="3" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>188</v>
+        <v>337</v>
       </c>
       <c r="E104" s="3"/>
       <c r="F104" s="12"/>
     </row>
-    <row r="105" spans="1:6" s="6" customFormat="1" ht="234" x14ac:dyDescent="0.15">
+    <row r="105" spans="1:6" s="6" customFormat="1" ht="117" x14ac:dyDescent="0.15">
       <c r="A105" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B105" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="C105" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="D105" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="E105" s="3"/>
+      <c r="F105" s="12"/>
+    </row>
+    <row r="106" spans="1:6" s="6" customFormat="1" ht="234" x14ac:dyDescent="0.15">
+      <c r="A106" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="C106" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="D106" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="B105" s="3" t="s">
-        <v>309</v>
-      </c>
-      <c r="C105" s="3" t="s">
+      <c r="E106" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="D105" s="3" t="s">
+      <c r="F106" s="12" t="s">
         <v>179</v>
       </c>
-      <c r="E105" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="F105" s="12" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6" s="6" customFormat="1" ht="26" x14ac:dyDescent="0.15">
-      <c r="A106" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="B106" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="C106" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="D106" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="E106" s="3"/>
-      <c r="F106" s="12"/>
-    </row>
-    <row r="107" spans="1:6" s="6" customFormat="1" ht="78" x14ac:dyDescent="0.15">
+    </row>
+    <row r="107" spans="1:6" s="6" customFormat="1" ht="26" x14ac:dyDescent="0.15">
       <c r="A107" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="B107" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="C107" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="D107" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="E107" s="3"/>
+      <c r="F107" s="12"/>
+    </row>
+    <row r="108" spans="1:6" s="6" customFormat="1" ht="78" x14ac:dyDescent="0.15">
+      <c r="A108" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="B108" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="C108" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="B107" s="3" t="s">
+      <c r="D108" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="C107" s="3" t="s">
+      <c r="E108" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="D107" s="3" t="s">
+      <c r="F108" s="12" t="s">
         <v>192</v>
-      </c>
-      <c r="E107" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="F107" s="12" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="108" spans="1:6" s="6" customFormat="1" ht="65" x14ac:dyDescent="0.15">
-      <c r="A108" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="B108" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="C108" s="3"/>
-      <c r="D108" s="3"/>
-      <c r="E108" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="F108" s="12" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="109" spans="1:6" s="6" customFormat="1" ht="65" x14ac:dyDescent="0.15">
       <c r="A109" s="3" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="C109" s="3"/>
       <c r="D109" s="3"/>
-      <c r="E109" s="3"/>
-      <c r="F109" s="12"/>
-    </row>
-    <row r="110" spans="1:6" s="6" customFormat="1" ht="39" x14ac:dyDescent="0.15">
+      <c r="E109" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="F109" s="12" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" s="6" customFormat="1" ht="65" x14ac:dyDescent="0.15">
       <c r="A110" s="3" t="s">
-        <v>225</v>
+        <v>197</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>310</v>
+        <v>198</v>
       </c>
       <c r="C110" s="3"/>
       <c r="D110" s="3"/>
       <c r="E110" s="3"/>
       <c r="F110" s="12"/>
     </row>
-    <row r="111" spans="1:6" s="6" customFormat="1" ht="52" x14ac:dyDescent="0.15">
+    <row r="111" spans="1:6" s="6" customFormat="1" ht="39" x14ac:dyDescent="0.15">
       <c r="A111" s="3" t="s">
-        <v>201</v>
+        <v>220</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="C111" s="3" t="s">
-        <v>371</v>
-      </c>
-      <c r="D111" s="3" t="s">
-        <v>203</v>
-      </c>
+        <v>305</v>
+      </c>
+      <c r="C111" s="3"/>
+      <c r="D111" s="3"/>
       <c r="E111" s="3"/>
       <c r="F111" s="12"/>
     </row>
-    <row r="112" spans="1:6" s="6" customFormat="1" ht="78" x14ac:dyDescent="0.15">
+    <row r="112" spans="1:6" s="6" customFormat="1" ht="117" x14ac:dyDescent="0.15">
       <c r="A112" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="B112" s="3" t="s">
-        <v>205</v>
+        <v>400</v>
+      </c>
+      <c r="B112" s="18" t="s">
+        <v>411</v>
       </c>
       <c r="C112" s="3"/>
-      <c r="D112" s="3"/>
+      <c r="D112" s="18" t="s">
+        <v>401</v>
+      </c>
       <c r="E112" s="3"/>
       <c r="F112" s="12"/>
     </row>
-    <row r="113" spans="1:6" s="6" customFormat="1" ht="208" x14ac:dyDescent="0.15">
+    <row r="113" spans="1:6" s="6" customFormat="1" ht="52" x14ac:dyDescent="0.15">
       <c r="A113" s="3" t="s">
-        <v>206</v>
+        <v>399</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="C113" s="3" t="s">
-        <v>208</v>
+        <v>364</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="E113" s="3"/>
       <c r="F113" s="12"/>
     </row>
-    <row r="114" spans="1:6" s="6" customFormat="1" ht="78" x14ac:dyDescent="0.15">
+    <row r="114" spans="1:6" s="6" customFormat="1" ht="208" x14ac:dyDescent="0.15">
       <c r="A114" s="3" t="s">
-        <v>210</v>
+        <v>402</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>211</v>
+        <v>403</v>
       </c>
       <c r="C114" s="3"/>
-      <c r="D114" s="3"/>
-      <c r="E114" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="F114" s="12" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="115" spans="1:6" s="6" customFormat="1" ht="39" x14ac:dyDescent="0.15">
+      <c r="D114" s="16" t="s">
+        <v>404</v>
+      </c>
+      <c r="E114" s="3"/>
+      <c r="F114" s="12"/>
+    </row>
+    <row r="115" spans="1:6" s="6" customFormat="1" ht="208" x14ac:dyDescent="0.15">
       <c r="A115" s="3" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="C115" s="3"/>
-      <c r="D115" s="3"/>
+        <v>202</v>
+      </c>
+      <c r="C115" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="D115" s="3" t="s">
+        <v>204</v>
+      </c>
       <c r="E115" s="3"/>
       <c r="F115" s="12"/>
     </row>
-    <row r="116" spans="1:6" s="6" customFormat="1" ht="312" x14ac:dyDescent="0.15">
+    <row r="116" spans="1:6" s="6" customFormat="1" ht="78" x14ac:dyDescent="0.15">
       <c r="A116" s="3" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="C116" s="3" t="s">
-        <v>259</v>
-      </c>
-      <c r="D116" s="3" t="s">
-        <v>260</v>
-      </c>
-      <c r="E116" s="3"/>
-      <c r="F116" s="12"/>
+        <v>206</v>
+      </c>
+      <c r="C116" s="3"/>
+      <c r="D116" s="3"/>
+      <c r="E116" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="F116" s="12" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="117" spans="1:6" s="6" customFormat="1" ht="39" x14ac:dyDescent="0.15">
       <c r="A117" s="3" t="s">
-        <v>292</v>
+        <v>208</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>299</v>
-      </c>
-      <c r="C117" s="3" t="s">
-        <v>292</v>
-      </c>
-      <c r="D117" s="3" t="s">
-        <v>299</v>
-      </c>
+        <v>209</v>
+      </c>
+      <c r="C117" s="3"/>
+      <c r="D117" s="3"/>
       <c r="E117" s="3"/>
       <c r="F117" s="12"/>
     </row>
-    <row r="118" spans="1:6" s="6" customFormat="1" ht="130" x14ac:dyDescent="0.15">
+    <row r="118" spans="1:6" s="6" customFormat="1" ht="312" x14ac:dyDescent="0.15">
       <c r="A118" s="3" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="C118" s="3" t="s">
-        <v>217</v>
+        <v>254</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>311</v>
+        <v>255</v>
       </c>
       <c r="E118" s="3"/>
       <c r="F118" s="12"/>
     </row>
-    <row r="119" spans="1:6" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="119" spans="1:6" s="6" customFormat="1" ht="39" x14ac:dyDescent="0.15">
       <c r="A119" s="3" t="s">
-        <v>238</v>
+        <v>287</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="C119" s="3"/>
-      <c r="D119" s="3"/>
+        <v>294</v>
+      </c>
+      <c r="C119" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="D119" s="3" t="s">
+        <v>294</v>
+      </c>
       <c r="E119" s="3"/>
       <c r="F119" s="12"/>
     </row>
+    <row r="120" spans="1:6" s="6" customFormat="1" ht="130" x14ac:dyDescent="0.15">
+      <c r="A120" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="B120" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="C120" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="D120" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="E120" s="3"/>
+      <c r="F120" s="12"/>
+    </row>
     <row r="121" spans="1:6" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A121" s="3"/>
-      <c r="B121" s="3"/>
+      <c r="A121" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="B121" s="3" t="s">
+        <v>234</v>
+      </c>
       <c r="C121" s="3"/>
       <c r="D121" s="3"/>
       <c r="E121" s="3"/>
       <c r="F121" s="12"/>
     </row>
-    <row r="122" spans="1:6" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="123" spans="1:6" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="123" spans="1:6" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A123" s="3"/>
+      <c r="B123" s="3"/>
+      <c r="C123" s="3"/>
+      <c r="D123" s="3"/>
+      <c r="E123" s="3"/>
+      <c r="F123" s="12"/>
+    </row>
     <row r="124" spans="1:6" ht="13" x14ac:dyDescent="0.15"/>
     <row r="125" spans="1:6" ht="13" x14ac:dyDescent="0.15"/>
     <row r="126" spans="1:6" ht="13" x14ac:dyDescent="0.15"/>
@@ -4843,10 +4909,12 @@
     <row r="1016" ht="13" x14ac:dyDescent="0.15"/>
     <row r="1017" ht="13" x14ac:dyDescent="0.15"/>
     <row r="1018" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="1019" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="1020" ht="13" x14ac:dyDescent="0.15"/>
   </sheetData>
-  <autoFilter ref="A1:Y120" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <sortState ref="A2:Y1018">
-    <sortCondition ref="A2:A1018"/>
+  <autoFilter ref="A1:Y122" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <sortState ref="A2:Y1020">
+    <sortCondition ref="A2:A1020"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="E19" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -4865,11 +4933,11 @@
     <hyperlink ref="E66" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
     <hyperlink ref="E75" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
     <hyperlink ref="E81" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="E96" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="E105" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="E107" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="E108" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="E114" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="E97" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="E106" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="E108" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="E109" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="E116" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
     <hyperlink ref="E71" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
     <hyperlink ref="E34" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
     <hyperlink ref="E2" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>

</xml_diff>

<commit_message>
updated commas into slashes
</commit_message>
<xml_diff>
--- a/usaspending_api/data/USAspendingGlossary.xlsx
+++ b/usaspending_api/data/USAspendingGlossary.xlsx
@@ -5,12 +5,12 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emilybrents/Documents/usaspending-api/usaspending_api/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brianzito/Documents/DATA/usaspending-api/usaspending_api/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E583C9B4-D1B4-B94A-931F-A666561BB030}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{399D179A-79B7-7C44-BCF3-DA2948E9B66A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20" yWindow="460" windowWidth="33600" windowHeight="18940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -409,9 +409,6 @@
   </si>
   <si>
     <t>[Learn more from the FPDS IDC page](https://www.fpds.gov/help/Indefinite_Delivery_Contract.htm)</t>
-  </si>
-  <si>
-    <t>Indefinite Delivery, Indefinite Quantity (IDIQ) Contract</t>
   </si>
   <si>
     <t>An Indefinite Quantity Contract is a type of Indefinite Delivery Contract (IDC). Sometimes the government contracts to buy supplies or services from a vendor over a period of time. For instances that government does not know the exact quantity it will need, an Indefinite Quantity Contract sets a quantity range with a min and max. It does not specify an exact number. For services, this is often called a Task Order Contract. For supplies, this is often called a Delivery Order Contract.</t>
@@ -1607,13 +1604,6 @@
 Vendors compete for the initial contracts. Once selected, they are eligible to compete further for agency-specific tasks.</t>
   </si>
   <si>
-    <t>Indefinite Delivery Contract (IDC) facilitates the delivery of supply and service orders during a set timeframe. This type of contract is awarded to one or more vendors. 
-Types of IDC's Include:
-- Indefinite Delivery, Definite Quantity Contract
-- Indefinite Delivery, Requirements Contract
-- Indefinite Delivery, Indefinite Quantity (IDIQ) Contract</t>
-  </si>
-  <si>
     <t>An Other Transaction (OT) Indefinite Delivery Vehicle is a transaction other than a procurement contract, grant, or cooperative agreement. Since this transaction is defined in the negative, it could take unlimited potential forms. This term is often used to refer to transactions designed to:
 - Support research &amp; development for homeland security.
 - Advance the development, testing, and deployment of critical homeland security technologies.
@@ -1633,6 +1623,16 @@
   <si>
     <t>An indefinite delivery contract (IDC) facilitates the delivery of supply and service orders during a set timeframe. This type of contract is awarded to one or more vendors.
 Definite Quantity Contracts, which are a type of IDC, provide for delivery of a definite quantity of supplies or services for a fixed period, with deliveries to be scheduled at designated locations upon order.</t>
+  </si>
+  <si>
+    <t>Indefinite Delivery Contract (IDC) facilitates the delivery of supply and service orders during a set timeframe. This type of contract is awarded to one or more vendors. 
+Types of IDC's Include:
+- Indefinite Delivery/Definite Quantity Contract
+- Indefinite Delivery/Requirements Contract
+- Indefinite Delivery/Indefinite Quantity (IDIQ) Contract</t>
+  </si>
+  <si>
+    <t>Indefinite Delivery/Indefinite Quantity (IDIQ) Contract</t>
   </si>
 </sst>
 </file>
@@ -1796,7 +1796,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1870,13 +1870,16 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2166,9 +2169,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y1029"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A67" sqref="A67"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A70" sqref="A70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2223,52 +2226,52 @@
     </row>
     <row r="2" spans="1:25" s="11" customFormat="1" ht="140" x14ac:dyDescent="0.15">
       <c r="A2" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="3" spans="1:25" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>245</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>246</v>
-      </c>
       <c r="C3" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>245</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>246</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="12"/>
     </row>
     <row r="4" spans="1:25" s="11" customFormat="1" ht="112" x14ac:dyDescent="0.15">
       <c r="A4" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>314</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>247</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>315</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>247</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>248</v>
       </c>
       <c r="E4" s="8"/>
       <c r="F4" s="12"/>
@@ -2278,13 +2281,13 @@
         <v>6</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E5" s="8"/>
       <c r="F5" s="12"/>
@@ -2344,13 +2347,13 @@
         <v>18</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="10" spans="1:25" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
@@ -2374,7 +2377,7 @@
         <v>22</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
@@ -2386,19 +2389,19 @@
         <v>23</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>24</v>
       </c>
       <c r="D12" s="8" t="s">
+        <v>316</v>
+      </c>
+      <c r="E12" s="8" t="s">
         <v>317</v>
       </c>
-      <c r="E12" s="8" t="s">
-        <v>318</v>
-      </c>
       <c r="F12" s="13" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="13" spans="1:25" s="11" customFormat="1" ht="56" x14ac:dyDescent="0.15">
@@ -2434,7 +2437,7 @@
         <v>33</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="15" spans="1:25" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
@@ -2445,47 +2448,47 @@
         <v>35</v>
       </c>
       <c r="C15" s="8" t="s">
+        <v>302</v>
+      </c>
+      <c r="D15" s="8" t="s">
         <v>303</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>304</v>
       </c>
       <c r="E15" s="8"/>
       <c r="F15" s="12"/>
     </row>
     <row r="16" spans="1:25" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A16" s="8" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C16" s="8" t="s">
+        <v>304</v>
+      </c>
+      <c r="D16" s="8" t="s">
         <v>305</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>306</v>
       </c>
       <c r="E16" s="8"/>
       <c r="F16" s="12"/>
     </row>
     <row r="17" spans="1:6" s="11" customFormat="1" ht="56" x14ac:dyDescent="0.15">
       <c r="A17" s="8" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C17" s="8" t="s">
+        <v>306</v>
+      </c>
+      <c r="D17" s="8" t="s">
         <v>307</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>308</v>
       </c>
       <c r="E17" s="8"/>
       <c r="F17" s="12"/>
     </row>
-    <row r="18" spans="1:6" s="11" customFormat="1" ht="140" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:6" s="11" customFormat="1" ht="126" x14ac:dyDescent="0.15">
       <c r="A18" s="8" t="s">
         <v>36</v>
       </c>
@@ -2499,18 +2502,18 @@
         <v>38</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" s="3" customFormat="1" ht="70.5" customHeight="1" x14ac:dyDescent="0.15">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" s="3" customFormat="1" ht="318" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -2521,7 +2524,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:6" s="11" customFormat="1" ht="70.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:6" s="11" customFormat="1" ht="186" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="8" t="s">
         <v>42</v>
       </c>
@@ -2542,7 +2545,7 @@
         <v>45</v>
       </c>
       <c r="B21" s="24" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -2555,19 +2558,19 @@
     </row>
     <row r="22" spans="1:6" s="11" customFormat="1" ht="126" x14ac:dyDescent="0.15">
       <c r="A22" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="B22" s="8" t="s">
         <v>217</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>218</v>
       </c>
       <c r="C22" s="8"/>
       <c r="D22" s="8" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E22" s="14"/>
       <c r="F22" s="12"/>
     </row>
-    <row r="23" spans="1:6" s="11" customFormat="1" ht="210" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:6" s="11" customFormat="1" ht="196" x14ac:dyDescent="0.15">
       <c r="A23" s="8" t="s">
         <v>48</v>
       </c>
@@ -2575,7 +2578,7 @@
         <v>49</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D23" s="8" t="s">
         <v>50</v>
@@ -2588,19 +2591,19 @@
         <v>15</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C24" s="8" t="s">
         <v>15</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="25" spans="1:6" s="11" customFormat="1" ht="112" x14ac:dyDescent="0.15">
@@ -2608,39 +2611,39 @@
         <v>51</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
       <c r="E25" s="9" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="F25" s="15" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="26" spans="1:6" s="11" customFormat="1" ht="168" x14ac:dyDescent="0.15">
       <c r="A26" s="8" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
       <c r="E26" s="9" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="F26" s="15" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="27" spans="1:6" s="11" customFormat="1" ht="98" x14ac:dyDescent="0.15">
       <c r="A27" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
@@ -2655,10 +2658,10 @@
         <v>57</v>
       </c>
       <c r="C28" s="8" t="s">
+        <v>296</v>
+      </c>
+      <c r="D28" s="8" t="s">
         <v>297</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>298</v>
       </c>
       <c r="E28" s="14" t="s">
         <v>58</v>
@@ -2683,18 +2686,18 @@
       <c r="E29" s="8"/>
       <c r="F29" s="12"/>
     </row>
-    <row r="30" spans="1:6" s="11" customFormat="1" ht="84" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:6" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
       <c r="A30" s="8" t="s">
+        <v>382</v>
+      </c>
+      <c r="B30" s="8" t="s">
         <v>383</v>
       </c>
-      <c r="B30" s="8" t="s">
-        <v>384</v>
-      </c>
       <c r="C30" s="8" t="s">
+        <v>382</v>
+      </c>
+      <c r="D30" s="8" t="s">
         <v>383</v>
-      </c>
-      <c r="D30" s="8" t="s">
-        <v>384</v>
       </c>
       <c r="E30" s="14" t="s">
         <v>75</v>
@@ -2705,14 +2708,14 @@
     </row>
     <row r="31" spans="1:6" s="11" customFormat="1" ht="210" x14ac:dyDescent="0.15">
       <c r="A31" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="B31" s="8" t="s">
         <v>215</v>
-      </c>
-      <c r="B31" s="8" t="s">
-        <v>216</v>
       </c>
       <c r="C31" s="8"/>
       <c r="D31" s="8" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E31" s="14"/>
       <c r="F31" s="12"/>
@@ -2737,7 +2740,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="33" spans="1:6" s="11" customFormat="1" ht="140" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:25" s="11" customFormat="1" ht="140" x14ac:dyDescent="0.15">
       <c r="A33" s="8" t="s">
         <v>66</v>
       </c>
@@ -2749,27 +2752,27 @@
       <c r="E33" s="8"/>
       <c r="F33" s="12"/>
     </row>
-    <row r="34" spans="1:6" s="11" customFormat="1" ht="397" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:25" s="11" customFormat="1" ht="397" x14ac:dyDescent="0.15">
       <c r="A34" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F34" s="12" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="35" spans="1:25" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
       <c r="A35" s="8" t="s">
         <v>68</v>
       </c>
@@ -2785,35 +2788,73 @@
         <v>71</v>
       </c>
     </row>
-    <row r="36" spans="1:6" s="3" customFormat="1" ht="255" x14ac:dyDescent="0.15">
-      <c r="A36" s="1" t="s">
+    <row r="36" spans="1:25" s="3" customFormat="1" ht="56" x14ac:dyDescent="0.15">
+      <c r="A36" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>319</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E36" s="8"/>
+      <c r="F36" s="12"/>
+      <c r="G36" s="11"/>
+      <c r="H36" s="11"/>
+      <c r="I36" s="11"/>
+      <c r="J36" s="11"/>
+      <c r="K36" s="11"/>
+      <c r="L36" s="11"/>
+      <c r="M36" s="11"/>
+      <c r="N36" s="11"/>
+      <c r="O36" s="11"/>
+      <c r="P36" s="11"/>
+      <c r="Q36" s="11"/>
+      <c r="R36" s="11"/>
+      <c r="S36" s="11"/>
+      <c r="T36" s="11"/>
+      <c r="U36" s="11"/>
+      <c r="V36" s="11"/>
+      <c r="W36" s="11"/>
+      <c r="X36" s="11"/>
+      <c r="Y36" s="11"/>
+    </row>
+    <row r="37" spans="1:25" s="11" customFormat="1" ht="255" x14ac:dyDescent="0.15">
+      <c r="A37" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>403</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>404</v>
-      </c>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="2"/>
-    </row>
-    <row r="37" spans="1:6" s="11" customFormat="1" ht="56" x14ac:dyDescent="0.15">
-      <c r="A37" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="B37" s="8" t="s">
-        <v>320</v>
-      </c>
-      <c r="C37" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="D37" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="E37" s="8"/>
-      <c r="F37" s="12"/>
-    </row>
-    <row r="38" spans="1:6" s="11" customFormat="1" ht="98" x14ac:dyDescent="0.15">
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3"/>
+      <c r="I37" s="3"/>
+      <c r="J37" s="3"/>
+      <c r="K37" s="3"/>
+      <c r="L37" s="3"/>
+      <c r="M37" s="3"/>
+      <c r="N37" s="3"/>
+      <c r="O37" s="3"/>
+      <c r="P37" s="3"/>
+      <c r="Q37" s="3"/>
+      <c r="R37" s="3"/>
+      <c r="S37" s="3"/>
+      <c r="T37" s="3"/>
+      <c r="U37" s="3"/>
+      <c r="V37" s="3"/>
+      <c r="W37" s="3"/>
+      <c r="X37" s="3"/>
+      <c r="Y37" s="3"/>
+    </row>
+    <row r="38" spans="1:25" s="11" customFormat="1" ht="84" x14ac:dyDescent="0.15">
       <c r="A38" s="8" t="s">
         <v>77</v>
       </c>
@@ -2829,79 +2870,79 @@
         <v>80</v>
       </c>
     </row>
-    <row r="39" spans="1:6" s="11" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:25" s="11" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A39" s="8" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E39" s="8"/>
       <c r="F39" s="12"/>
     </row>
-    <row r="40" spans="1:6" s="3" customFormat="1" ht="102" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:25" s="3" customFormat="1" ht="102" x14ac:dyDescent="0.15">
       <c r="A40" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>405</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>406</v>
       </c>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
       <c r="F40" s="2"/>
     </row>
-    <row r="41" spans="1:6" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:25" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A41" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="B41" s="8" t="s">
         <v>224</v>
-      </c>
-      <c r="B41" s="8" t="s">
-        <v>225</v>
       </c>
       <c r="C41" s="8"/>
       <c r="D41" s="8"/>
       <c r="E41" s="14"/>
       <c r="F41" s="12"/>
     </row>
-    <row r="42" spans="1:6" s="11" customFormat="1" ht="112" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:25" s="11" customFormat="1" ht="112" x14ac:dyDescent="0.15">
       <c r="A42" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="B42" s="8" t="s">
         <v>226</v>
       </c>
-      <c r="B42" s="8" t="s">
-        <v>227</v>
-      </c>
       <c r="C42" s="8" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E42" s="14"/>
       <c r="F42" s="12"/>
     </row>
-    <row r="43" spans="1:6" s="11" customFormat="1" ht="98" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:25" s="11" customFormat="1" ht="98" x14ac:dyDescent="0.15">
       <c r="A43" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="B43" s="8" t="s">
         <v>228</v>
       </c>
-      <c r="B43" s="8" t="s">
-        <v>229</v>
-      </c>
       <c r="C43" s="8" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E43" s="14"/>
       <c r="F43" s="12"/>
     </row>
-    <row r="44" spans="1:6" s="11" customFormat="1" ht="56" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:25" s="11" customFormat="1" ht="56" x14ac:dyDescent="0.15">
       <c r="A44" s="8" t="s">
         <v>81</v>
       </c>
@@ -2921,7 +2962,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="45" spans="1:6" s="11" customFormat="1" ht="154" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:25" s="11" customFormat="1" ht="140" x14ac:dyDescent="0.15">
       <c r="A45" s="8" t="s">
         <v>86</v>
       </c>
@@ -2929,19 +2970,19 @@
         <v>87</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E45" s="8" t="s">
         <v>88</v>
       </c>
       <c r="F45" s="12" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="46" spans="1:25" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
       <c r="A46" s="8" t="s">
         <v>89</v>
       </c>
@@ -2957,7 +2998,7 @@
       <c r="E46" s="8"/>
       <c r="F46" s="12"/>
     </row>
-    <row r="47" spans="1:6" s="11" customFormat="1" ht="210" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:25" s="11" customFormat="1" ht="210" x14ac:dyDescent="0.15">
       <c r="A47" s="8" t="s">
         <v>92</v>
       </c>
@@ -2968,27 +3009,27 @@
         <v>94</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E47" s="9" t="s">
+        <v>372</v>
+      </c>
+      <c r="F47" s="12" t="s">
         <v>373</v>
       </c>
-      <c r="F47" s="12" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" s="11" customFormat="1" ht="98" x14ac:dyDescent="0.15">
+    </row>
+    <row r="48" spans="1:25" s="11" customFormat="1" ht="98" x14ac:dyDescent="0.15">
       <c r="A48" s="8" t="s">
+        <v>288</v>
+      </c>
+      <c r="B48" s="8" t="s">
         <v>289</v>
       </c>
-      <c r="B48" s="8" t="s">
-        <v>290</v>
-      </c>
       <c r="C48" s="8" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E48" s="8"/>
       <c r="F48" s="12"/>
@@ -2998,7 +3039,7 @@
         <v>95</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C49" s="8" t="s">
         <v>95</v>
@@ -3027,16 +3068,16 @@
     </row>
     <row r="51" spans="1:6" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A51" s="8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E51" s="8"/>
       <c r="F51" s="12"/>
@@ -3058,7 +3099,7 @@
         <v>101</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
@@ -3083,16 +3124,16 @@
     </row>
     <row r="55" spans="1:6" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
       <c r="A55" s="8" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E55" s="8"/>
       <c r="F55" s="12"/>
@@ -3105,68 +3146,68 @@
         <v>109</v>
       </c>
       <c r="C56" s="8" t="s">
+        <v>308</v>
+      </c>
+      <c r="D56" s="8" t="s">
         <v>309</v>
-      </c>
-      <c r="D56" s="8" t="s">
-        <v>310</v>
       </c>
       <c r="E56" s="8"/>
       <c r="F56" s="12"/>
     </row>
     <row r="57" spans="1:6" s="11" customFormat="1" ht="112" x14ac:dyDescent="0.15">
       <c r="A57" s="8" t="s">
+        <v>334</v>
+      </c>
+      <c r="B57" s="8" t="s">
         <v>335</v>
       </c>
-      <c r="B57" s="8" t="s">
-        <v>336</v>
-      </c>
       <c r="C57" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D57" s="8" t="s">
         <v>136</v>
-      </c>
-      <c r="D57" s="8" t="s">
-        <v>137</v>
       </c>
       <c r="E57" s="8"/>
       <c r="F57" s="12"/>
     </row>
     <row r="58" spans="1:6" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A58" s="8" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E58" s="8"/>
       <c r="F58" s="12"/>
     </row>
     <row r="59" spans="1:6" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
       <c r="A59" s="8" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C59" s="8" t="s">
+        <v>311</v>
+      </c>
+      <c r="D59" s="8" t="s">
         <v>312</v>
-      </c>
-      <c r="D59" s="8" t="s">
-        <v>313</v>
       </c>
       <c r="E59" s="8"/>
       <c r="F59" s="12"/>
     </row>
     <row r="60" spans="1:6" s="3" customFormat="1" ht="238" x14ac:dyDescent="0.15">
       <c r="A60" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B60" s="24" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
@@ -3179,46 +3220,46 @@
     </row>
     <row r="61" spans="1:6" s="11" customFormat="1" ht="196" x14ac:dyDescent="0.15">
       <c r="A61" s="8" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E61" s="14"/>
       <c r="F61" s="12"/>
     </row>
     <row r="62" spans="1:6" s="11" customFormat="1" ht="154" x14ac:dyDescent="0.15">
       <c r="A62" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C62" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E62" s="9" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F62" s="10" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="63" spans="1:6" s="3" customFormat="1" ht="119" x14ac:dyDescent="0.15">
       <c r="A63" s="1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
@@ -3227,724 +3268,820 @@
     </row>
     <row r="64" spans="1:6" s="11" customFormat="1" ht="238" x14ac:dyDescent="0.15">
       <c r="A64" s="8" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E64" s="8"/>
       <c r="F64" s="12"/>
     </row>
-    <row r="65" spans="1:6" s="11" customFormat="1" ht="140" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:25" s="11" customFormat="1" ht="140" x14ac:dyDescent="0.15">
       <c r="A65" s="8" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E65" s="8"/>
       <c r="F65" s="12"/>
     </row>
-    <row r="66" spans="1:6" s="3" customFormat="1" ht="187" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:25" s="3" customFormat="1" ht="85" x14ac:dyDescent="0.15">
       <c r="A66" s="1" t="s">
-        <v>414</v>
-      </c>
-      <c r="B66" s="24" t="s">
-        <v>425</v>
+        <v>411</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>412</v>
       </c>
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
-      <c r="E66" s="1" t="s">
+      <c r="E66" s="1"/>
+      <c r="F66" s="2"/>
+    </row>
+    <row r="67" spans="1:25" s="1" customFormat="1" ht="175" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A67" s="27" t="s">
+        <v>413</v>
+      </c>
+      <c r="B67" s="24" t="s">
+        <v>428</v>
+      </c>
+      <c r="C67" s="27"/>
+      <c r="E67" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="F66" s="2" t="s">
+      <c r="F67" s="2" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" s="1" customFormat="1" ht="175" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A67" s="25" t="s">
-        <v>428</v>
-      </c>
-      <c r="B67" s="27" t="s">
-        <v>429</v>
-      </c>
-      <c r="C67" s="26"/>
-      <c r="F67" s="2"/>
-    </row>
-    <row r="68" spans="1:6" s="11" customFormat="1" ht="140" x14ac:dyDescent="0.15">
-      <c r="A68" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="B68" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="C68" s="8"/>
-      <c r="D68" s="8"/>
-      <c r="E68" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="F68" s="12" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" s="3" customFormat="1" ht="170" x14ac:dyDescent="0.15">
+      <c r="G67" s="3"/>
+      <c r="H67" s="3"/>
+      <c r="I67" s="3"/>
+      <c r="J67" s="3"/>
+      <c r="K67" s="3"/>
+      <c r="L67" s="3"/>
+      <c r="M67" s="3"/>
+      <c r="N67" s="3"/>
+      <c r="O67" s="3"/>
+      <c r="P67" s="3"/>
+      <c r="Q67" s="3"/>
+      <c r="R67" s="3"/>
+      <c r="S67" s="3"/>
+      <c r="T67" s="3"/>
+      <c r="U67" s="3"/>
+      <c r="V67" s="3"/>
+      <c r="W67" s="3"/>
+      <c r="X67" s="3"/>
+      <c r="Y67" s="3"/>
+    </row>
+    <row r="68" spans="1:25" s="11" customFormat="1" ht="170" x14ac:dyDescent="0.15">
+      <c r="A68" s="26" t="s">
+        <v>426</v>
+      </c>
+      <c r="B68" s="25" t="s">
+        <v>427</v>
+      </c>
+      <c r="C68" s="28"/>
+      <c r="D68" s="1"/>
+      <c r="E68" s="1"/>
+      <c r="F68" s="2"/>
+      <c r="G68" s="1"/>
+      <c r="H68" s="1"/>
+      <c r="I68" s="1"/>
+      <c r="J68" s="1"/>
+      <c r="K68" s="1"/>
+      <c r="L68" s="1"/>
+      <c r="M68" s="1"/>
+      <c r="N68" s="1"/>
+      <c r="O68" s="1"/>
+      <c r="P68" s="1"/>
+      <c r="Q68" s="1"/>
+      <c r="R68" s="1"/>
+      <c r="S68" s="1"/>
+      <c r="T68" s="1"/>
+      <c r="U68" s="1"/>
+      <c r="V68" s="1"/>
+      <c r="W68" s="1"/>
+      <c r="X68" s="1"/>
+      <c r="Y68" s="1"/>
+    </row>
+    <row r="69" spans="1:25" s="3" customFormat="1" ht="170" x14ac:dyDescent="0.15">
       <c r="A69" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
       <c r="E69" s="1"/>
       <c r="F69" s="2"/>
     </row>
-    <row r="70" spans="1:6" s="3" customFormat="1" ht="85" x14ac:dyDescent="0.15">
-      <c r="A70" s="1" t="s">
-        <v>412</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>413</v>
-      </c>
-      <c r="C70" s="1"/>
-      <c r="D70" s="1"/>
-      <c r="E70" s="1"/>
-      <c r="F70" s="2"/>
-    </row>
-    <row r="71" spans="1:6" s="3" customFormat="1" ht="119" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:25" s="3" customFormat="1" ht="140" x14ac:dyDescent="0.15">
+      <c r="A70" s="8" t="s">
+        <v>429</v>
+      </c>
+      <c r="B70" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="C70" s="8"/>
+      <c r="D70" s="8"/>
+      <c r="E70" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="F70" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="G70" s="11"/>
+      <c r="H70" s="11"/>
+      <c r="I70" s="11"/>
+      <c r="J70" s="11"/>
+      <c r="K70" s="11"/>
+      <c r="L70" s="11"/>
+      <c r="M70" s="11"/>
+      <c r="N70" s="11"/>
+      <c r="O70" s="11"/>
+      <c r="P70" s="11"/>
+      <c r="Q70" s="11"/>
+      <c r="R70" s="11"/>
+      <c r="S70" s="11"/>
+      <c r="T70" s="11"/>
+      <c r="U70" s="11"/>
+      <c r="V70" s="11"/>
+      <c r="W70" s="11"/>
+      <c r="X70" s="11"/>
+      <c r="Y70" s="11"/>
+    </row>
+    <row r="71" spans="1:25" s="3" customFormat="1" ht="119" x14ac:dyDescent="0.15">
       <c r="A71" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="B71" s="1" t="s">
         <v>415</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>416</v>
       </c>
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
       <c r="E71" s="1"/>
       <c r="F71" s="2"/>
     </row>
-    <row r="72" spans="1:6" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:25" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
       <c r="A72" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="B72" s="8" t="s">
         <v>380</v>
       </c>
-      <c r="B72" s="8" t="s">
-        <v>381</v>
-      </c>
       <c r="C72" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="D72" s="8" t="s">
         <v>380</v>
       </c>
-      <c r="D72" s="8" t="s">
-        <v>381</v>
-      </c>
       <c r="E72" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="F72" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="F72" s="12" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
+    </row>
+    <row r="73" spans="1:25" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
       <c r="A73" s="8" t="s">
+        <v>328</v>
+      </c>
+      <c r="B73" s="8" t="s">
         <v>329</v>
       </c>
-      <c r="B73" s="8" t="s">
-        <v>330</v>
-      </c>
       <c r="C73" s="8" t="s">
+        <v>328</v>
+      </c>
+      <c r="D73" s="8" t="s">
         <v>329</v>
-      </c>
-      <c r="D73" s="8" t="s">
-        <v>330</v>
       </c>
       <c r="E73" s="8"/>
       <c r="F73" s="12"/>
     </row>
-    <row r="74" spans="1:6" s="11" customFormat="1" ht="98" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:25" s="11" customFormat="1" ht="98" x14ac:dyDescent="0.15">
       <c r="A74" s="8" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C74" s="8"/>
       <c r="D74" s="8"/>
       <c r="E74" s="8"/>
       <c r="F74" s="12"/>
     </row>
-    <row r="75" spans="1:6" s="11" customFormat="1" ht="182" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:25" s="11" customFormat="1" ht="182" x14ac:dyDescent="0.15">
       <c r="A75" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="B75" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="B75" s="8" t="s">
+      <c r="C75" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="D75" s="8" t="s">
         <v>119</v>
-      </c>
-      <c r="C75" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="D75" s="8" t="s">
-        <v>120</v>
       </c>
       <c r="E75" s="8"/>
       <c r="F75" s="12"/>
     </row>
-    <row r="76" spans="1:6" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:25" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A76" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="B76" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="C76" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="D76" s="8" t="s">
         <v>122</v>
-      </c>
-      <c r="B76" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="C76" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="D76" s="8" t="s">
-        <v>123</v>
       </c>
       <c r="E76" s="8"/>
       <c r="F76" s="12"/>
     </row>
-    <row r="77" spans="1:6" s="11" customFormat="1" ht="98" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:25" s="11" customFormat="1" ht="98" x14ac:dyDescent="0.15">
       <c r="A77" s="8" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C77" s="8" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D77" s="8" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E77" s="14" t="s">
+        <v>202</v>
+      </c>
+      <c r="F77" s="12" t="s">
         <v>203</v>
       </c>
-      <c r="F77" s="12" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" s="11" customFormat="1" ht="277.5" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="78" spans="1:25" s="11" customFormat="1" ht="277.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A78" s="8" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B78" s="8" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C78" s="8" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D78" s="8" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E78" s="8"/>
       <c r="F78" s="12"/>
     </row>
-    <row r="79" spans="1:6" s="3" customFormat="1" ht="277.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:25" s="3" customFormat="1" ht="277.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A79" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="B79" s="1" t="s">
         <v>417</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>418</v>
       </c>
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
       <c r="E79" s="1"/>
       <c r="F79" s="2"/>
     </row>
-    <row r="80" spans="1:6" s="11" customFormat="1" ht="56" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:25" s="11" customFormat="1" ht="56" x14ac:dyDescent="0.15">
       <c r="A80" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="B80" s="8" t="s">
         <v>124</v>
-      </c>
-      <c r="B80" s="8" t="s">
-        <v>125</v>
       </c>
       <c r="C80" s="8"/>
       <c r="D80" s="8"/>
       <c r="E80" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="F80" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="F80" s="12" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" s="11" customFormat="1" ht="84" x14ac:dyDescent="0.15">
+    </row>
+    <row r="81" spans="1:25" s="11" customFormat="1" ht="84" x14ac:dyDescent="0.15">
       <c r="A81" s="8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C81" s="8"/>
       <c r="D81" s="8"/>
       <c r="E81" s="14"/>
       <c r="F81" s="12"/>
     </row>
-    <row r="82" spans="1:6" s="11" customFormat="1" ht="126" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:25" s="11" customFormat="1" ht="126" x14ac:dyDescent="0.15">
       <c r="A82" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="B82" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="B82" s="8" t="s">
+      <c r="C82" s="8" t="s">
+        <v>299</v>
+      </c>
+      <c r="D82" s="8" t="s">
+        <v>298</v>
+      </c>
+      <c r="E82" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="C82" s="8" t="s">
-        <v>300</v>
-      </c>
-      <c r="D82" s="8" t="s">
-        <v>299</v>
-      </c>
-      <c r="E82" s="14" t="s">
+      <c r="F82" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="F82" s="12" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
+    </row>
+    <row r="83" spans="1:25" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
       <c r="A83" s="8" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B83" s="8" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C83" s="8" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D83" s="8" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E83" s="8"/>
       <c r="F83" s="12"/>
     </row>
-    <row r="84" spans="1:6" s="11" customFormat="1" ht="84" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:25" s="11" customFormat="1" ht="84" x14ac:dyDescent="0.15">
       <c r="A84" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="B84" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="B84" s="8" t="s">
-        <v>135</v>
-      </c>
       <c r="C84" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D84" s="8" t="s">
+        <v>235</v>
+      </c>
+      <c r="E84" s="14" t="s">
+        <v>239</v>
+      </c>
+      <c r="F84" s="12" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="85" spans="1:25" s="11" customFormat="1" ht="409.6" x14ac:dyDescent="0.15">
+      <c r="A85" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="B85" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="C85" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="D85" s="8" t="s">
         <v>236</v>
-      </c>
-      <c r="E84" s="14" t="s">
-        <v>240</v>
-      </c>
-      <c r="F84" s="12" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" s="11" customFormat="1" ht="409.6" x14ac:dyDescent="0.15">
-      <c r="A85" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="B85" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="C85" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="D85" s="8" t="s">
-        <v>237</v>
       </c>
       <c r="E85" s="8"/>
       <c r="F85" s="12"/>
     </row>
-    <row r="86" spans="1:6" s="11" customFormat="1" ht="112" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:25" s="11" customFormat="1" ht="140" x14ac:dyDescent="0.15">
       <c r="A86" s="8" t="s">
-        <v>140</v>
+        <v>250</v>
       </c>
       <c r="B86" s="8" t="s">
-        <v>141</v>
+        <v>259</v>
       </c>
       <c r="C86" s="8" t="s">
-        <v>140</v>
+        <v>250</v>
       </c>
       <c r="D86" s="8" t="s">
-        <v>238</v>
+        <v>259</v>
       </c>
       <c r="E86" s="8"/>
       <c r="F86" s="12"/>
     </row>
-    <row r="87" spans="1:6" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:25" s="11" customFormat="1" ht="112" x14ac:dyDescent="0.15">
       <c r="A87" s="8" t="s">
-        <v>419</v>
+        <v>139</v>
       </c>
       <c r="B87" s="8" t="s">
-        <v>420</v>
-      </c>
-      <c r="C87" s="8"/>
-      <c r="D87" s="8"/>
+        <v>140</v>
+      </c>
+      <c r="C87" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="D87" s="8" t="s">
+        <v>237</v>
+      </c>
       <c r="E87" s="8"/>
       <c r="F87" s="12"/>
     </row>
-    <row r="88" spans="1:6" s="11" customFormat="1" ht="154" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:25" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A88" s="8" t="s">
-        <v>341</v>
+        <v>418</v>
       </c>
       <c r="B88" s="8" t="s">
-        <v>357</v>
-      </c>
-      <c r="C88" s="8" t="s">
-        <v>341</v>
-      </c>
-      <c r="D88" s="16" t="s">
-        <v>347</v>
-      </c>
-      <c r="E88" s="9" t="s">
-        <v>240</v>
-      </c>
-      <c r="F88" s="17" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" s="3" customFormat="1" ht="340" x14ac:dyDescent="0.15">
-      <c r="A89" s="1" t="s">
-        <v>421</v>
-      </c>
-      <c r="B89" s="24" t="s">
-        <v>426</v>
-      </c>
-      <c r="C89" s="1"/>
-      <c r="D89" s="1"/>
-      <c r="E89" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="C88" s="8"/>
+      <c r="D88" s="8"/>
+      <c r="E88" s="8"/>
+      <c r="F88" s="12"/>
+    </row>
+    <row r="89" spans="1:25" s="3" customFormat="1" ht="154" x14ac:dyDescent="0.15">
+      <c r="A89" s="8" t="s">
+        <v>340</v>
+      </c>
+      <c r="B89" s="8" t="s">
+        <v>356</v>
+      </c>
+      <c r="C89" s="8" t="s">
+        <v>340</v>
+      </c>
+      <c r="D89" s="16" t="s">
+        <v>346</v>
+      </c>
+      <c r="E89" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="F89" s="17" t="s">
+        <v>375</v>
+      </c>
+      <c r="G89" s="11"/>
+      <c r="H89" s="11"/>
+      <c r="I89" s="11"/>
+      <c r="J89" s="11"/>
+      <c r="K89" s="11"/>
+      <c r="L89" s="11"/>
+      <c r="M89" s="11"/>
+      <c r="N89" s="11"/>
+      <c r="O89" s="11"/>
+      <c r="P89" s="11"/>
+      <c r="Q89" s="11"/>
+      <c r="R89" s="11"/>
+      <c r="S89" s="11"/>
+      <c r="T89" s="11"/>
+      <c r="U89" s="11"/>
+      <c r="V89" s="11"/>
+      <c r="W89" s="11"/>
+      <c r="X89" s="11"/>
+      <c r="Y89" s="11"/>
+    </row>
+    <row r="90" spans="1:25" s="11" customFormat="1" ht="323" x14ac:dyDescent="0.15">
+      <c r="A90" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="B90" s="24" t="s">
+        <v>424</v>
+      </c>
+      <c r="C90" s="1"/>
+      <c r="D90" s="1"/>
+      <c r="E90" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="F90" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="F89" s="2" t="s">
+      <c r="G90" s="3"/>
+      <c r="H90" s="3"/>
+      <c r="I90" s="3"/>
+      <c r="J90" s="3"/>
+      <c r="K90" s="3"/>
+      <c r="L90" s="3"/>
+      <c r="M90" s="3"/>
+      <c r="N90" s="3"/>
+      <c r="O90" s="3"/>
+      <c r="P90" s="3"/>
+      <c r="Q90" s="3"/>
+      <c r="R90" s="3"/>
+      <c r="S90" s="3"/>
+      <c r="T90" s="3"/>
+      <c r="U90" s="3"/>
+      <c r="V90" s="3"/>
+      <c r="W90" s="3"/>
+      <c r="X90" s="3"/>
+      <c r="Y90" s="3"/>
+    </row>
+    <row r="91" spans="1:25" s="11" customFormat="1" ht="154" x14ac:dyDescent="0.15">
+      <c r="A91" s="8" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="90" spans="1:6" s="11" customFormat="1" ht="154" x14ac:dyDescent="0.15">
-      <c r="A90" s="8" t="s">
-        <v>251</v>
-      </c>
-      <c r="B90" s="8" t="s">
-        <v>260</v>
-      </c>
-      <c r="C90" s="8" t="s">
-        <v>251</v>
-      </c>
-      <c r="D90" s="8" t="s">
-        <v>260</v>
-      </c>
-      <c r="E90" s="8"/>
-      <c r="F90" s="12"/>
-    </row>
-    <row r="91" spans="1:6" s="11" customFormat="1" ht="168" x14ac:dyDescent="0.15">
-      <c r="A91" s="8" t="s">
+      <c r="B91" s="8" t="s">
+        <v>350</v>
+      </c>
+      <c r="C91" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="B91" s="8" t="s">
-        <v>351</v>
-      </c>
-      <c r="C91" s="8" t="s">
-        <v>145</v>
-      </c>
       <c r="D91" s="8" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E91" s="8"/>
       <c r="F91" s="12"/>
     </row>
-    <row r="92" spans="1:6" s="11" customFormat="1" ht="56" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:25" s="11" customFormat="1" ht="56" x14ac:dyDescent="0.15">
       <c r="A92" s="8" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B92" s="8" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C92" s="8" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D92" s="8" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E92" s="8"/>
       <c r="F92" s="12"/>
     </row>
-    <row r="93" spans="1:6" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:25" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
       <c r="A93" s="8" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B93" s="8" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C93" s="8" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D93" s="8" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E93" s="8" t="s">
         <v>88</v>
       </c>
       <c r="F93" s="12" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" s="11" customFormat="1" ht="98" x14ac:dyDescent="0.15">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="94" spans="1:25" s="11" customFormat="1" ht="98" x14ac:dyDescent="0.15">
       <c r="A94" s="8" t="s">
+        <v>330</v>
+      </c>
+      <c r="B94" s="8" t="s">
         <v>331</v>
       </c>
-      <c r="B94" s="8" t="s">
-        <v>332</v>
-      </c>
       <c r="C94" s="8" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D94" s="8" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E94" s="8"/>
       <c r="F94" s="12"/>
     </row>
-    <row r="95" spans="1:6" s="11" customFormat="1" ht="126" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:25" s="11" customFormat="1" ht="126" x14ac:dyDescent="0.15">
       <c r="A95" s="8" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B95" s="8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C95" s="8" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D95" s="8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E95" s="8"/>
       <c r="F95" s="12"/>
     </row>
-    <row r="96" spans="1:6" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:25" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A96" s="8" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B96" s="8" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C96" s="8" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D96" s="8" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E96" s="8"/>
       <c r="F96" s="12"/>
     </row>
     <row r="97" spans="1:6" s="11" customFormat="1" ht="358" x14ac:dyDescent="0.15">
       <c r="A97" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B97" s="8" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C97" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D97" s="8" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E97" s="9" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F97" s="10" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="98" spans="1:6" s="11" customFormat="1" ht="98" x14ac:dyDescent="0.15">
       <c r="A98" s="8" t="s">
+        <v>285</v>
+      </c>
+      <c r="B98" s="8" t="s">
         <v>286</v>
-      </c>
-      <c r="B98" s="8" t="s">
-        <v>287</v>
       </c>
       <c r="C98" s="8" t="s">
         <v>25</v>
       </c>
       <c r="D98" s="8" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E98" s="8"/>
       <c r="F98" s="12"/>
     </row>
     <row r="99" spans="1:6" s="11" customFormat="1" ht="56" x14ac:dyDescent="0.15">
       <c r="A99" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="B99" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="B99" s="8" t="s">
-        <v>147</v>
-      </c>
       <c r="C99" s="8" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D99" s="8" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E99" s="8"/>
       <c r="F99" s="12"/>
     </row>
     <row r="100" spans="1:6" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
       <c r="A100" s="8" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B100" s="8" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C100" s="8" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D100" s="8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E100" s="8"/>
       <c r="F100" s="12"/>
     </row>
     <row r="101" spans="1:6" s="11" customFormat="1" ht="56" x14ac:dyDescent="0.15">
       <c r="A101" s="8" t="s">
+        <v>360</v>
+      </c>
+      <c r="B101" s="8" t="s">
         <v>361</v>
       </c>
-      <c r="B101" s="8" t="s">
-        <v>362</v>
-      </c>
       <c r="C101" s="8" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D101" s="8" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E101" s="8"/>
       <c r="F101" s="12"/>
     </row>
-    <row r="102" spans="1:6" s="11" customFormat="1" ht="126" x14ac:dyDescent="0.15">
+    <row r="102" spans="1:6" s="11" customFormat="1" ht="112" x14ac:dyDescent="0.15">
       <c r="A102" s="18" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B102" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C102" s="8"/>
       <c r="D102" s="8" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E102" s="8"/>
       <c r="F102" s="12"/>
     </row>
     <row r="103" spans="1:6" s="11" customFormat="1" ht="126" x14ac:dyDescent="0.15">
       <c r="A103" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="B103" s="8" t="s">
         <v>397</v>
-      </c>
-      <c r="B103" s="8" t="s">
-        <v>398</v>
       </c>
       <c r="C103" s="8"/>
       <c r="D103" s="8" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="E103" s="8"/>
       <c r="F103" s="12"/>
     </row>
     <row r="104" spans="1:6" s="11" customFormat="1" ht="84" x14ac:dyDescent="0.15">
       <c r="A104" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="B104" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="B104" s="8" t="s">
-        <v>149</v>
-      </c>
       <c r="C104" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D104" s="8" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E104" s="8"/>
       <c r="F104" s="12"/>
     </row>
     <row r="105" spans="1:6" s="11" customFormat="1" ht="126" x14ac:dyDescent="0.15">
       <c r="A105" s="8" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B105" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="C105" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="C105" s="8" t="s">
+      <c r="D105" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="D105" s="8" t="s">
+      <c r="E105" s="14" t="s">
         <v>159</v>
       </c>
-      <c r="E105" s="14" t="s">
+      <c r="F105" s="12" t="s">
         <v>160</v>
-      </c>
-      <c r="F105" s="12" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="106" spans="1:6" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
       <c r="A106" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="B106" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="B106" s="8" t="s">
+      <c r="C106" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="C106" s="8" t="s">
-        <v>152</v>
-      </c>
       <c r="D106" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E106" s="8"/>
       <c r="F106" s="12"/>
     </row>
     <row r="107" spans="1:6" s="11" customFormat="1" ht="140" x14ac:dyDescent="0.15">
       <c r="A107" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="B107" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="B107" s="8" t="s">
+      <c r="C107" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="C107" s="8" t="s">
+      <c r="D107" s="8" t="s">
         <v>155</v>
-      </c>
-      <c r="D107" s="8" t="s">
-        <v>156</v>
       </c>
       <c r="E107" s="8"/>
       <c r="F107" s="12"/>
     </row>
     <row r="108" spans="1:6" s="11" customFormat="1" ht="56" x14ac:dyDescent="0.15">
       <c r="A108" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="B108" s="8" t="s">
         <v>220</v>
       </c>
-      <c r="B108" s="8" t="s">
-        <v>221</v>
-      </c>
       <c r="C108" s="8" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D108" s="8" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E108" s="8"/>
       <c r="F108" s="12"/>
     </row>
     <row r="109" spans="1:6" s="3" customFormat="1" ht="85" x14ac:dyDescent="0.15">
       <c r="A109" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="B109" s="1" t="s">
         <v>422</v>
-      </c>
-      <c r="B109" s="1" t="s">
-        <v>423</v>
       </c>
       <c r="C109" s="1"/>
       <c r="D109" s="1"/>
@@ -3953,26 +4090,26 @@
     </row>
     <row r="110" spans="1:6" s="11" customFormat="1" ht="112" x14ac:dyDescent="0.15">
       <c r="A110" s="8" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B110" s="8" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C110" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="D110" s="8" t="s">
         <v>247</v>
-      </c>
-      <c r="D110" s="8" t="s">
-        <v>248</v>
       </c>
       <c r="E110" s="8"/>
       <c r="F110" s="12"/>
     </row>
     <row r="111" spans="1:6" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A111" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="B111" s="8" t="s">
         <v>162</v>
-      </c>
-      <c r="B111" s="8" t="s">
-        <v>163</v>
       </c>
       <c r="C111" s="8"/>
       <c r="D111" s="8"/>
@@ -3981,130 +4118,130 @@
     </row>
     <row r="112" spans="1:6" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A112" s="8" t="s">
+        <v>326</v>
+      </c>
+      <c r="B112" s="8" t="s">
         <v>327</v>
       </c>
-      <c r="B112" s="8" t="s">
-        <v>328</v>
-      </c>
       <c r="C112" s="8" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D112" s="8" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E112" s="8"/>
       <c r="F112" s="12"/>
     </row>
     <row r="113" spans="1:6" s="11" customFormat="1" ht="112" x14ac:dyDescent="0.15">
       <c r="A113" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="B113" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="B113" s="8" t="s">
+      <c r="C113" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="C113" s="8" t="s">
-        <v>171</v>
-      </c>
       <c r="D113" s="8" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E113" s="8"/>
       <c r="F113" s="12"/>
     </row>
     <row r="114" spans="1:6" s="11" customFormat="1" ht="126" x14ac:dyDescent="0.15">
       <c r="A114" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="B114" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="B114" s="8" t="s">
+      <c r="C114" s="8" t="s">
         <v>173</v>
       </c>
-      <c r="C114" s="8" t="s">
+      <c r="D114" s="8" t="s">
         <v>174</v>
-      </c>
-      <c r="D114" s="8" t="s">
-        <v>175</v>
       </c>
       <c r="E114" s="8"/>
       <c r="F114" s="12"/>
     </row>
     <row r="115" spans="1:6" s="11" customFormat="1" ht="252" x14ac:dyDescent="0.15">
       <c r="A115" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="B115" s="8" t="s">
+        <v>292</v>
+      </c>
+      <c r="C115" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="B115" s="8" t="s">
-        <v>293</v>
-      </c>
-      <c r="C115" s="8" t="s">
+      <c r="D115" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="D115" s="8" t="s">
+      <c r="E115" s="14" t="s">
         <v>166</v>
       </c>
-      <c r="E115" s="14" t="s">
+      <c r="F115" s="12" t="s">
         <v>167</v>
-      </c>
-      <c r="F115" s="12" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="116" spans="1:6" s="11" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A116" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="B116" s="8" t="s">
         <v>267</v>
       </c>
-      <c r="B116" s="8" t="s">
-        <v>268</v>
-      </c>
       <c r="C116" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="D116" s="8" t="s">
         <v>267</v>
-      </c>
-      <c r="D116" s="8" t="s">
-        <v>268</v>
       </c>
       <c r="E116" s="8"/>
       <c r="F116" s="12"/>
     </row>
     <row r="117" spans="1:6" s="11" customFormat="1" ht="84" x14ac:dyDescent="0.15">
       <c r="A117" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="B117" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="B117" s="8" t="s">
+      <c r="C117" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="C117" s="8" t="s">
+      <c r="D117" s="8" t="s">
         <v>178</v>
       </c>
-      <c r="D117" s="8" t="s">
+      <c r="E117" s="14" t="s">
         <v>179</v>
       </c>
-      <c r="E117" s="14" t="s">
+      <c r="F117" s="12" t="s">
         <v>180</v>
-      </c>
-      <c r="F117" s="12" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="118" spans="1:6" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A118" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="B118" s="8" t="s">
         <v>182</v>
-      </c>
-      <c r="B118" s="8" t="s">
-        <v>183</v>
       </c>
       <c r="C118" s="8"/>
       <c r="D118" s="8"/>
       <c r="E118" s="14" t="s">
+        <v>183</v>
+      </c>
+      <c r="F118" s="12" t="s">
         <v>184</v>
-      </c>
-      <c r="F118" s="12" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="119" spans="1:6" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
       <c r="A119" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="B119" s="8" t="s">
         <v>186</v>
-      </c>
-      <c r="B119" s="8" t="s">
-        <v>187</v>
       </c>
       <c r="C119" s="8"/>
       <c r="D119" s="8"/>
@@ -4113,82 +4250,82 @@
     </row>
     <row r="120" spans="1:6" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A120" s="8" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B120" s="8" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C120" s="8"/>
       <c r="D120" s="8"/>
       <c r="E120" s="8"/>
       <c r="F120" s="12"/>
     </row>
-    <row r="121" spans="1:6" s="11" customFormat="1" ht="126" x14ac:dyDescent="0.15">
+    <row r="121" spans="1:6" s="11" customFormat="1" ht="56" x14ac:dyDescent="0.15">
       <c r="A121" s="8" t="s">
-        <v>389</v>
-      </c>
-      <c r="B121" s="19" t="s">
-        <v>400</v>
-      </c>
-      <c r="C121" s="8"/>
-      <c r="D121" s="19" t="s">
-        <v>390</v>
+        <v>387</v>
+      </c>
+      <c r="B121" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="C121" s="8" t="s">
+        <v>352</v>
+      </c>
+      <c r="D121" s="8" t="s">
+        <v>188</v>
       </c>
       <c r="E121" s="8"/>
       <c r="F121" s="12"/>
     </row>
-    <row r="122" spans="1:6" s="11" customFormat="1" ht="56" x14ac:dyDescent="0.15">
+    <row r="122" spans="1:6" s="11" customFormat="1" ht="126" x14ac:dyDescent="0.15">
       <c r="A122" s="8" t="s">
         <v>388</v>
       </c>
-      <c r="B122" s="8" t="s">
-        <v>188</v>
-      </c>
-      <c r="C122" s="8" t="s">
-        <v>353</v>
-      </c>
-      <c r="D122" s="8" t="s">
-        <v>189</v>
+      <c r="B122" s="19" t="s">
+        <v>399</v>
+      </c>
+      <c r="C122" s="8"/>
+      <c r="D122" s="19" t="s">
+        <v>389</v>
       </c>
       <c r="E122" s="8"/>
       <c r="F122" s="12"/>
     </row>
-    <row r="123" spans="1:6" s="11" customFormat="1" ht="238" x14ac:dyDescent="0.15">
+    <row r="123" spans="1:6" s="11" customFormat="1" ht="224" x14ac:dyDescent="0.15">
       <c r="A123" s="8" t="s">
+        <v>390</v>
+      </c>
+      <c r="B123" s="8" t="s">
         <v>391</v>
-      </c>
-      <c r="B123" s="8" t="s">
-        <v>392</v>
       </c>
       <c r="C123" s="8"/>
       <c r="D123" s="20" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E123" s="8"/>
       <c r="F123" s="12"/>
     </row>
     <row r="124" spans="1:6" s="11" customFormat="1" ht="224" x14ac:dyDescent="0.15">
       <c r="A124" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="B124" s="8" t="s">
         <v>190</v>
       </c>
-      <c r="B124" s="8" t="s">
+      <c r="C124" s="8" t="s">
         <v>191</v>
       </c>
-      <c r="C124" s="8" t="s">
+      <c r="D124" s="8" t="s">
         <v>192</v>
-      </c>
-      <c r="D124" s="8" t="s">
-        <v>193</v>
       </c>
       <c r="E124" s="8"/>
       <c r="F124" s="12"/>
     </row>
     <row r="125" spans="1:6" s="11" customFormat="1" ht="84" x14ac:dyDescent="0.15">
       <c r="A125" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="B125" s="8" t="s">
         <v>194</v>
-      </c>
-      <c r="B125" s="8" t="s">
-        <v>195</v>
       </c>
       <c r="C125" s="8"/>
       <c r="D125" s="8"/>
@@ -4196,15 +4333,15 @@
         <v>79</v>
       </c>
       <c r="F125" s="12" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="126" spans="1:6" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A126" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="B126" s="8" t="s">
         <v>197</v>
-      </c>
-      <c r="B126" s="8" t="s">
-        <v>198</v>
       </c>
       <c r="C126" s="8"/>
       <c r="D126" s="8"/>
@@ -4213,58 +4350,58 @@
     </row>
     <row r="127" spans="1:6" s="11" customFormat="1" ht="332" x14ac:dyDescent="0.15">
       <c r="A127" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="B127" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="B127" s="8" t="s">
-        <v>200</v>
-      </c>
       <c r="C127" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="D127" s="8" t="s">
         <v>243</v>
-      </c>
-      <c r="D127" s="8" t="s">
-        <v>244</v>
       </c>
       <c r="E127" s="8"/>
       <c r="F127" s="12"/>
     </row>
     <row r="128" spans="1:6" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A128" s="8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B128" s="8" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C128" s="8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D128" s="8" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E128" s="8"/>
       <c r="F128" s="12"/>
     </row>
     <row r="129" spans="1:6" s="11" customFormat="1" ht="140" x14ac:dyDescent="0.15">
       <c r="A129" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="B129" s="8" t="s">
         <v>201</v>
       </c>
-      <c r="B129" s="8" t="s">
-        <v>202</v>
-      </c>
       <c r="C129" s="8" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D129" s="8" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E129" s="8"/>
       <c r="F129" s="12"/>
     </row>
     <row r="130" spans="1:6" s="11" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A130" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="B130" s="8" t="s">
         <v>222</v>
-      </c>
-      <c r="B130" s="8" t="s">
-        <v>223</v>
       </c>
       <c r="C130" s="8"/>
       <c r="D130" s="8"/>
@@ -5177,7 +5314,11 @@
     <row r="1028" ht="13" x14ac:dyDescent="0.15"/>
     <row r="1029" ht="13" x14ac:dyDescent="0.15"/>
   </sheetData>
-  <autoFilter ref="A1:Y131" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:Y131" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Y131">
+      <sortCondition ref="A1:A131"/>
+    </sortState>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Y1029">
     <sortCondition ref="A2:A1029"/>
   </sortState>
@@ -5192,12 +5333,12 @@
     <hyperlink ref="E50" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
     <hyperlink ref="E53" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
     <hyperlink ref="E60" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="E66" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="E68" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="E67" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="E70" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
     <hyperlink ref="E80" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
     <hyperlink ref="E72" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
     <hyperlink ref="E82" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="E89" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="E90" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
     <hyperlink ref="E105" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
     <hyperlink ref="E115" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
     <hyperlink ref="E117" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
@@ -5208,7 +5349,7 @@
     <hyperlink ref="E2" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
     <hyperlink ref="E97" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
     <hyperlink ref="E62" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="E88" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="E89" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
     <hyperlink ref="F2" r:id="rId28" display="https://www.whitehouse.gov/sites/whitehouse.gov/files/omb/assets/a11_current_year/a11_2017.pdf" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
     <hyperlink ref="E9" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
     <hyperlink ref="E18" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
@@ -5217,7 +5358,7 @@
     <hyperlink ref="E24" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
     <hyperlink ref="E47" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
     <hyperlink ref="F62" r:id="rId35" display="https://www.whitehouse.gov/sites/whitehouse.gov/files/omb/assets/a11_current_year/a11_2017.pdf" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="F88" r:id="rId36" display="https://www.whitehouse.gov/sites/whitehouse.gov/files/omb/assets/a11_current_year/a11_2017.pdf" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="F89" r:id="rId36" display="https://www.whitehouse.gov/sites/whitehouse.gov/files/omb/assets/a11_current_year/a11_2017.pdf" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
     <hyperlink ref="F97" r:id="rId37" display="https://www.whitehouse.gov/sites/whitehouse.gov/files/omb/assets/a11_current_year/a11_2017.pdf" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Revert "Update city-search-autocomplete with dev"
</commit_message>
<xml_diff>
--- a/usaspending_api/data/USAspendingGlossary.xlsx
+++ b/usaspending_api/data/USAspendingGlossary.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brianzito/Documents/DATA/usaspending-api/usaspending_api/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emilybrents/Documents/usaspending-api/usaspending_api/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5FFDE5E-1419-F943-ACC3-26BA41657891}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E583C9B4-D1B4-B94A-931F-A666561BB030}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -409,6 +409,9 @@
   </si>
   <si>
     <t>[Learn more from the FPDS IDC page](https://www.fpds.gov/help/Indefinite_Delivery_Contract.htm)</t>
+  </si>
+  <si>
+    <t>Indefinite Delivery, Indefinite Quantity (IDIQ) Contract</t>
   </si>
   <si>
     <t>An Indefinite Quantity Contract is a type of Indefinite Delivery Contract (IDC). Sometimes the government contracts to buy supplies or services from a vendor over a period of time. For instances that government does not know the exact quantity it will need, an Indefinite Quantity Contract sets a quantity range with a min and max. It does not specify an exact number. For services, this is often called a Task Order Contract. For supplies, this is often called a Delivery Order Contract.</t>
@@ -1560,6 +1563,9 @@
     <t>Indefinite Delivery Vehicle (IDV)</t>
   </si>
   <si>
+    <t>Indefinite Delivery / Requirements</t>
+  </si>
+  <si>
     <t>Requirements contracts are for the fulfillment of all purchase requirements of supplies or services for designated government activities during a specified contract period, with deliveries to be scheduled by placing orders with the contractor.</t>
   </si>
   <si>
@@ -1601,6 +1607,13 @@
 Vendors compete for the initial contracts. Once selected, they are eligible to compete further for agency-specific tasks.</t>
   </si>
   <si>
+    <t>Indefinite Delivery Contract (IDC) facilitates the delivery of supply and service orders during a set timeframe. This type of contract is awarded to one or more vendors. 
+Types of IDC's Include:
+- Indefinite Delivery, Definite Quantity Contract
+- Indefinite Delivery, Requirements Contract
+- Indefinite Delivery, Indefinite Quantity (IDIQ) Contract</t>
+  </si>
+  <si>
     <t>An Other Transaction (OT) Indefinite Delivery Vehicle is a transaction other than a procurement contract, grant, or cooperative agreement. Since this transaction is defined in the negative, it could take unlimited potential forms. This term is often used to refer to transactions designed to:
 - Support research &amp; development for homeland security.
 - Advance the development, testing, and deployment of critical homeland security technologies.
@@ -1615,49 +1628,22 @@
 - Agency B establishes a BPA with a graphic design agency for design of brochures and event signage</t>
   </si>
   <si>
+    <t>Indefinite Delivery Contract / Definite Quantity</t>
+  </si>
+  <si>
     <t>An indefinite delivery contract (IDC) facilitates the delivery of supply and service orders during a set timeframe. This type of contract is awarded to one or more vendors.
 Definite Quantity Contracts, which are a type of IDC, provide for delivery of a definite quantity of supplies or services for a fixed period, with deliveries to be scheduled at designated locations upon order.</t>
-  </si>
-  <si>
-    <t>Indefinite Delivery Contract (IDC) facilitates the delivery of supply and service orders during a set timeframe. This type of contract is awarded to one or more vendors. 
-Types of IDC's Include:
-- Indefinite Delivery / Definite Quantity Contract
-- Indefinite Delivery / Requirements Contract
-- Indefinite Delivery / Indefinite Quantity (IDIQ) Contract</t>
-  </si>
-  <si>
-    <t>Indefinite Delivery / Indefinite Quantity (IDIQ) Contract</t>
-  </si>
-  <si>
-    <t>Indefinite Delivery / Requirements Contract</t>
-  </si>
-  <si>
-    <t>Indefinite Delivery / Definite Quantity Contract</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
@@ -1804,63 +1790,63 @@
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="1" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1872,31 +1858,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2189,9 +2166,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y1029"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A69" sqref="A69"/>
+    <sheetView tabSelected="1" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A67" sqref="A67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2246,52 +2223,52 @@
     </row>
     <row r="2" spans="1:25" s="11" customFormat="1" ht="140" x14ac:dyDescent="0.15">
       <c r="A2" s="8" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
     </row>
     <row r="3" spans="1:25" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B3" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>245</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>244</v>
-      </c>
       <c r="D3" s="8" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="12"/>
     </row>
     <row r="4" spans="1:25" s="11" customFormat="1" ht="112" x14ac:dyDescent="0.15">
       <c r="A4" s="8" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="E4" s="8"/>
       <c r="F4" s="12"/>
@@ -2301,13 +2278,13 @@
         <v>6</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="E5" s="8"/>
       <c r="F5" s="12"/>
@@ -2367,13 +2344,13 @@
         <v>18</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
     </row>
     <row r="10" spans="1:25" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
@@ -2397,7 +2374,7 @@
         <v>22</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
@@ -2409,19 +2386,19 @@
         <v>23</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>24</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
     </row>
     <row r="13" spans="1:25" s="11" customFormat="1" ht="56" x14ac:dyDescent="0.15">
@@ -2457,7 +2434,7 @@
         <v>33</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="15" spans="1:25" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
@@ -2468,47 +2445,47 @@
         <v>35</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="E15" s="8"/>
       <c r="F15" s="12"/>
     </row>
     <row r="16" spans="1:25" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A16" s="8" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="E16" s="8"/>
       <c r="F16" s="12"/>
     </row>
     <row r="17" spans="1:6" s="11" customFormat="1" ht="56" x14ac:dyDescent="0.15">
       <c r="A17" s="8" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="E17" s="8"/>
       <c r="F17" s="12"/>
     </row>
-    <row r="18" spans="1:6" s="11" customFormat="1" ht="126" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:6" s="11" customFormat="1" ht="140" x14ac:dyDescent="0.15">
       <c r="A18" s="8" t="s">
         <v>36</v>
       </c>
@@ -2522,18 +2499,18 @@
         <v>38</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" s="3" customFormat="1" ht="318" customHeight="1" x14ac:dyDescent="0.15">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" s="3" customFormat="1" ht="70.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -2544,7 +2521,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:6" s="11" customFormat="1" ht="186" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:6" s="11" customFormat="1" ht="70.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="8" t="s">
         <v>42</v>
       </c>
@@ -2565,7 +2542,7 @@
         <v>45</v>
       </c>
       <c r="B21" s="24" t="s">
-        <v>424</v>
+        <v>427</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -2578,19 +2555,19 @@
     </row>
     <row r="22" spans="1:6" s="11" customFormat="1" ht="126" x14ac:dyDescent="0.15">
       <c r="A22" s="8" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C22" s="8"/>
       <c r="D22" s="8" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="E22" s="14"/>
       <c r="F22" s="12"/>
     </row>
-    <row r="23" spans="1:6" s="11" customFormat="1" ht="196" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:6" s="11" customFormat="1" ht="210" x14ac:dyDescent="0.15">
       <c r="A23" s="8" t="s">
         <v>48</v>
       </c>
@@ -2598,7 +2575,7 @@
         <v>49</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D23" s="8" t="s">
         <v>50</v>
@@ -2611,19 +2588,19 @@
         <v>15</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C24" s="8" t="s">
         <v>15</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="25" spans="1:6" s="11" customFormat="1" ht="112" x14ac:dyDescent="0.15">
@@ -2631,39 +2608,39 @@
         <v>51</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
       <c r="E25" s="9" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="F25" s="15" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
     </row>
     <row r="26" spans="1:6" s="11" customFormat="1" ht="168" x14ac:dyDescent="0.15">
       <c r="A26" s="8" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
       <c r="E26" s="9" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="F26" s="15" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
     </row>
     <row r="27" spans="1:6" s="11" customFormat="1" ht="98" x14ac:dyDescent="0.15">
       <c r="A27" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="B27" s="8" t="s">
         <v>206</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>205</v>
       </c>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
@@ -2678,10 +2655,10 @@
         <v>57</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="E28" s="14" t="s">
         <v>58</v>
@@ -2706,18 +2683,18 @@
       <c r="E29" s="8"/>
       <c r="F29" s="12"/>
     </row>
-    <row r="30" spans="1:6" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:6" s="11" customFormat="1" ht="84" x14ac:dyDescent="0.15">
       <c r="A30" s="8" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="B30" s="8" t="s">
+        <v>384</v>
+      </c>
+      <c r="C30" s="8" t="s">
         <v>383</v>
       </c>
-      <c r="C30" s="8" t="s">
-        <v>382</v>
-      </c>
       <c r="D30" s="8" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="E30" s="14" t="s">
         <v>75</v>
@@ -2728,14 +2705,14 @@
     </row>
     <row r="31" spans="1:6" s="11" customFormat="1" ht="210" x14ac:dyDescent="0.15">
       <c r="A31" s="8" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C31" s="8"/>
       <c r="D31" s="8" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="E31" s="14"/>
       <c r="F31" s="12"/>
@@ -2760,7 +2737,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="33" spans="1:25" s="11" customFormat="1" ht="140" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:6" s="11" customFormat="1" ht="140" x14ac:dyDescent="0.15">
       <c r="A33" s="8" t="s">
         <v>66</v>
       </c>
@@ -2772,27 +2749,27 @@
       <c r="E33" s="8"/>
       <c r="F33" s="12"/>
     </row>
-    <row r="34" spans="1:25" s="11" customFormat="1" ht="397" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:6" s="11" customFormat="1" ht="397" x14ac:dyDescent="0.15">
       <c r="A34" s="8" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F34" s="12" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="35" spans="1:25" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
       <c r="A35" s="8" t="s">
         <v>68</v>
       </c>
@@ -2808,73 +2785,35 @@
         <v>71</v>
       </c>
     </row>
-    <row r="36" spans="1:25" s="3" customFormat="1" ht="56" x14ac:dyDescent="0.15">
-      <c r="A36" s="8" t="s">
+    <row r="36" spans="1:6" s="3" customFormat="1" ht="255" x14ac:dyDescent="0.15">
+      <c r="A36" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="2"/>
+    </row>
+    <row r="37" spans="1:6" s="11" customFormat="1" ht="56" x14ac:dyDescent="0.15">
+      <c r="A37" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B36" s="8" t="s">
-        <v>319</v>
-      </c>
-      <c r="C36" s="8" t="s">
+      <c r="B37" s="8" t="s">
+        <v>320</v>
+      </c>
+      <c r="C37" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="D36" s="8" t="s">
+      <c r="D37" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="E36" s="8"/>
-      <c r="F36" s="12"/>
-      <c r="G36" s="11"/>
-      <c r="H36" s="11"/>
-      <c r="I36" s="11"/>
-      <c r="J36" s="11"/>
-      <c r="K36" s="11"/>
-      <c r="L36" s="11"/>
-      <c r="M36" s="11"/>
-      <c r="N36" s="11"/>
-      <c r="O36" s="11"/>
-      <c r="P36" s="11"/>
-      <c r="Q36" s="11"/>
-      <c r="R36" s="11"/>
-      <c r="S36" s="11"/>
-      <c r="T36" s="11"/>
-      <c r="U36" s="11"/>
-      <c r="V36" s="11"/>
-      <c r="W36" s="11"/>
-      <c r="X36" s="11"/>
-      <c r="Y36" s="11"/>
-    </row>
-    <row r="37" spans="1:25" s="11" customFormat="1" ht="255" x14ac:dyDescent="0.15">
-      <c r="A37" s="1" t="s">
-        <v>402</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>403</v>
-      </c>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="3"/>
-      <c r="H37" s="3"/>
-      <c r="I37" s="3"/>
-      <c r="J37" s="3"/>
-      <c r="K37" s="3"/>
-      <c r="L37" s="3"/>
-      <c r="M37" s="3"/>
-      <c r="N37" s="3"/>
-      <c r="O37" s="3"/>
-      <c r="P37" s="3"/>
-      <c r="Q37" s="3"/>
-      <c r="R37" s="3"/>
-      <c r="S37" s="3"/>
-      <c r="T37" s="3"/>
-      <c r="U37" s="3"/>
-      <c r="V37" s="3"/>
-      <c r="W37" s="3"/>
-      <c r="X37" s="3"/>
-      <c r="Y37" s="3"/>
-    </row>
-    <row r="38" spans="1:25" s="11" customFormat="1" ht="84" x14ac:dyDescent="0.15">
+      <c r="E37" s="8"/>
+      <c r="F37" s="12"/>
+    </row>
+    <row r="38" spans="1:6" s="11" customFormat="1" ht="98" x14ac:dyDescent="0.15">
       <c r="A38" s="8" t="s">
         <v>77</v>
       </c>
@@ -2890,79 +2829,79 @@
         <v>80</v>
       </c>
     </row>
-    <row r="39" spans="1:25" s="11" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:6" s="11" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A39" s="8" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="E39" s="8"/>
       <c r="F39" s="12"/>
     </row>
-    <row r="40" spans="1:25" s="3" customFormat="1" ht="102" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:6" s="3" customFormat="1" ht="102" x14ac:dyDescent="0.15">
       <c r="A40" s="1" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
       <c r="F40" s="2"/>
     </row>
-    <row r="41" spans="1:25" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:6" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A41" s="8" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C41" s="8"/>
       <c r="D41" s="8"/>
       <c r="E41" s="14"/>
       <c r="F41" s="12"/>
     </row>
-    <row r="42" spans="1:25" s="11" customFormat="1" ht="112" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:6" s="11" customFormat="1" ht="112" x14ac:dyDescent="0.15">
       <c r="A42" s="8" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B42" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="C42" s="8" t="s">
         <v>226</v>
       </c>
-      <c r="C42" s="8" t="s">
-        <v>225</v>
-      </c>
       <c r="D42" s="8" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="E42" s="14"/>
       <c r="F42" s="12"/>
     </row>
-    <row r="43" spans="1:25" s="11" customFormat="1" ht="98" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:6" s="11" customFormat="1" ht="98" x14ac:dyDescent="0.15">
       <c r="A43" s="8" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B43" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="C43" s="8" t="s">
         <v>228</v>
       </c>
-      <c r="C43" s="8" t="s">
-        <v>227</v>
-      </c>
       <c r="D43" s="8" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="E43" s="14"/>
       <c r="F43" s="12"/>
     </row>
-    <row r="44" spans="1:25" s="11" customFormat="1" ht="56" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:6" s="11" customFormat="1" ht="56" x14ac:dyDescent="0.15">
       <c r="A44" s="8" t="s">
         <v>81</v>
       </c>
@@ -2982,7 +2921,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="45" spans="1:25" s="11" customFormat="1" ht="140" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:6" s="11" customFormat="1" ht="154" x14ac:dyDescent="0.15">
       <c r="A45" s="8" t="s">
         <v>86</v>
       </c>
@@ -2990,19 +2929,19 @@
         <v>87</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="E45" s="8" t="s">
         <v>88</v>
       </c>
       <c r="F45" s="12" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="46" spans="1:25" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
       <c r="A46" s="8" t="s">
         <v>89</v>
       </c>
@@ -3018,7 +2957,7 @@
       <c r="E46" s="8"/>
       <c r="F46" s="12"/>
     </row>
-    <row r="47" spans="1:25" s="11" customFormat="1" ht="210" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:6" s="11" customFormat="1" ht="210" x14ac:dyDescent="0.15">
       <c r="A47" s="8" t="s">
         <v>92</v>
       </c>
@@ -3029,27 +2968,27 @@
         <v>94</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="E47" s="9" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="F47" s="12" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="48" spans="1:25" s="11" customFormat="1" ht="98" x14ac:dyDescent="0.15">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" s="11" customFormat="1" ht="98" x14ac:dyDescent="0.15">
       <c r="A48" s="8" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E48" s="8"/>
       <c r="F48" s="12"/>
@@ -3059,7 +2998,7 @@
         <v>95</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C49" s="8" t="s">
         <v>95</v>
@@ -3088,16 +3027,16 @@
     </row>
     <row r="51" spans="1:6" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A51" s="8" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="E51" s="8"/>
       <c r="F51" s="12"/>
@@ -3119,7 +3058,7 @@
         <v>101</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
@@ -3144,16 +3083,16 @@
     </row>
     <row r="55" spans="1:6" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
       <c r="A55" s="8" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B55" s="8" t="s">
+        <v>368</v>
+      </c>
+      <c r="C55" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="D55" s="8" t="s">
         <v>367</v>
-      </c>
-      <c r="C55" s="8" t="s">
-        <v>218</v>
-      </c>
-      <c r="D55" s="8" t="s">
-        <v>366</v>
       </c>
       <c r="E55" s="8"/>
       <c r="F55" s="12"/>
@@ -3166,68 +3105,68 @@
         <v>109</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="E56" s="8"/>
       <c r="F56" s="12"/>
     </row>
     <row r="57" spans="1:6" s="11" customFormat="1" ht="112" x14ac:dyDescent="0.15">
       <c r="A57" s="8" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E57" s="8"/>
       <c r="F57" s="12"/>
     </row>
     <row r="58" spans="1:6" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A58" s="8" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="E58" s="8"/>
       <c r="F58" s="12"/>
     </row>
     <row r="59" spans="1:6" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
       <c r="A59" s="8" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="E59" s="8"/>
       <c r="F59" s="12"/>
     </row>
     <row r="60" spans="1:6" s="3" customFormat="1" ht="238" x14ac:dyDescent="0.15">
       <c r="A60" s="1" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B60" s="24" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
@@ -3240,46 +3179,46 @@
     </row>
     <row r="61" spans="1:6" s="11" customFormat="1" ht="196" x14ac:dyDescent="0.15">
       <c r="A61" s="8" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="E61" s="14"/>
       <c r="F61" s="12"/>
     </row>
     <row r="62" spans="1:6" s="11" customFormat="1" ht="154" x14ac:dyDescent="0.15">
       <c r="A62" s="8" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="C62" s="8" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="E62" s="9" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F62" s="10" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="63" spans="1:6" s="3" customFormat="1" ht="119" x14ac:dyDescent="0.15">
       <c r="A63" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="B63" s="1" t="s">
         <v>408</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>407</v>
       </c>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
@@ -3288,820 +3227,724 @@
     </row>
     <row r="64" spans="1:6" s="11" customFormat="1" ht="238" x14ac:dyDescent="0.15">
       <c r="A64" s="8" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="E64" s="8"/>
       <c r="F64" s="12"/>
     </row>
-    <row r="65" spans="1:25" s="11" customFormat="1" ht="140" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:6" s="11" customFormat="1" ht="140" x14ac:dyDescent="0.15">
       <c r="A65" s="8" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="E65" s="8"/>
       <c r="F65" s="12"/>
     </row>
-    <row r="66" spans="1:25" s="3" customFormat="1" ht="85" x14ac:dyDescent="0.15">
-      <c r="A66" s="30" t="s">
-        <v>428</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>411</v>
+    <row r="66" spans="1:6" s="3" customFormat="1" ht="187" x14ac:dyDescent="0.15">
+      <c r="A66" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="B66" s="24" t="s">
+        <v>425</v>
       </c>
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
-      <c r="E66" s="1"/>
-      <c r="F66" s="2"/>
-    </row>
-    <row r="67" spans="1:25" s="1" customFormat="1" ht="175" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A67" s="27" t="s">
-        <v>412</v>
-      </c>
-      <c r="B67" s="29" t="s">
-        <v>426</v>
-      </c>
-      <c r="C67" s="27"/>
-      <c r="E67" s="1" t="s">
+      <c r="E66" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="F67" s="2" t="s">
+      <c r="F66" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="G67" s="3"/>
-      <c r="H67" s="3"/>
-      <c r="I67" s="3"/>
-      <c r="J67" s="3"/>
-      <c r="K67" s="3"/>
-      <c r="L67" s="3"/>
-      <c r="M67" s="3"/>
-      <c r="N67" s="3"/>
-      <c r="O67" s="3"/>
-      <c r="P67" s="3"/>
-      <c r="Q67" s="3"/>
-      <c r="R67" s="3"/>
-      <c r="S67" s="3"/>
-      <c r="T67" s="3"/>
-      <c r="U67" s="3"/>
-      <c r="V67" s="3"/>
-      <c r="W67" s="3"/>
-      <c r="X67" s="3"/>
-      <c r="Y67" s="3"/>
-    </row>
-    <row r="68" spans="1:25" s="11" customFormat="1" ht="170" x14ac:dyDescent="0.15">
-      <c r="A68" s="26" t="s">
+    </row>
+    <row r="67" spans="1:6" s="1" customFormat="1" ht="175" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A67" s="25" t="s">
+        <v>428</v>
+      </c>
+      <c r="B67" s="27" t="s">
         <v>429</v>
       </c>
-      <c r="B68" s="25" t="s">
-        <v>425</v>
-      </c>
-      <c r="C68" s="28"/>
-      <c r="D68" s="1"/>
-      <c r="E68" s="1"/>
-      <c r="F68" s="2"/>
-      <c r="G68" s="1"/>
-      <c r="H68" s="1"/>
-      <c r="I68" s="1"/>
-      <c r="J68" s="1"/>
-      <c r="K68" s="1"/>
-      <c r="L68" s="1"/>
-      <c r="M68" s="1"/>
-      <c r="N68" s="1"/>
-      <c r="O68" s="1"/>
-      <c r="P68" s="1"/>
-      <c r="Q68" s="1"/>
-      <c r="R68" s="1"/>
-      <c r="S68" s="1"/>
-      <c r="T68" s="1"/>
-      <c r="U68" s="1"/>
-      <c r="V68" s="1"/>
-      <c r="W68" s="1"/>
-      <c r="X68" s="1"/>
-      <c r="Y68" s="1"/>
-    </row>
-    <row r="69" spans="1:25" s="3" customFormat="1" ht="170" x14ac:dyDescent="0.15">
+      <c r="C67" s="26"/>
+      <c r="F67" s="2"/>
+    </row>
+    <row r="68" spans="1:6" s="11" customFormat="1" ht="140" x14ac:dyDescent="0.15">
+      <c r="A68" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="B68" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="C68" s="8"/>
+      <c r="D68" s="8"/>
+      <c r="E68" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="F68" s="12" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" s="3" customFormat="1" ht="170" x14ac:dyDescent="0.15">
       <c r="A69" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="B69" s="1" t="s">
         <v>410</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>409</v>
       </c>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
       <c r="E69" s="1"/>
       <c r="F69" s="2"/>
     </row>
-    <row r="70" spans="1:25" s="3" customFormat="1" ht="140" x14ac:dyDescent="0.15">
-      <c r="A70" s="8" t="s">
-        <v>427</v>
-      </c>
-      <c r="B70" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="C70" s="8"/>
-      <c r="D70" s="8"/>
-      <c r="E70" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="F70" s="12" t="s">
-        <v>115</v>
-      </c>
-      <c r="G70" s="11"/>
-      <c r="H70" s="11"/>
-      <c r="I70" s="11"/>
-      <c r="J70" s="11"/>
-      <c r="K70" s="11"/>
-      <c r="L70" s="11"/>
-      <c r="M70" s="11"/>
-      <c r="N70" s="11"/>
-      <c r="O70" s="11"/>
-      <c r="P70" s="11"/>
-      <c r="Q70" s="11"/>
-      <c r="R70" s="11"/>
-      <c r="S70" s="11"/>
-      <c r="T70" s="11"/>
-      <c r="U70" s="11"/>
-      <c r="V70" s="11"/>
-      <c r="W70" s="11"/>
-      <c r="X70" s="11"/>
-      <c r="Y70" s="11"/>
-    </row>
-    <row r="71" spans="1:25" s="3" customFormat="1" ht="119" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:6" s="3" customFormat="1" ht="85" x14ac:dyDescent="0.15">
+      <c r="A70" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="C70" s="1"/>
+      <c r="D70" s="1"/>
+      <c r="E70" s="1"/>
+      <c r="F70" s="2"/>
+    </row>
+    <row r="71" spans="1:6" s="3" customFormat="1" ht="119" x14ac:dyDescent="0.15">
       <c r="A71" s="1" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
       <c r="E71" s="1"/>
       <c r="F71" s="2"/>
     </row>
-    <row r="72" spans="1:25" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:6" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
       <c r="A72" s="8" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="B72" s="8" t="s">
+        <v>381</v>
+      </c>
+      <c r="C72" s="8" t="s">
         <v>380</v>
       </c>
-      <c r="C72" s="8" t="s">
-        <v>379</v>
-      </c>
       <c r="D72" s="8" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="E72" s="14" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F72" s="12" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="73" spans="1:25" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
       <c r="A73" s="8" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B73" s="8" t="s">
+        <v>330</v>
+      </c>
+      <c r="C73" s="8" t="s">
         <v>329</v>
       </c>
-      <c r="C73" s="8" t="s">
-        <v>328</v>
-      </c>
       <c r="D73" s="8" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="E73" s="8"/>
       <c r="F73" s="12"/>
     </row>
-    <row r="74" spans="1:25" s="11" customFormat="1" ht="98" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:6" s="11" customFormat="1" ht="98" x14ac:dyDescent="0.15">
       <c r="A74" s="8" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="C74" s="8"/>
       <c r="D74" s="8"/>
       <c r="E74" s="8"/>
       <c r="F74" s="12"/>
     </row>
-    <row r="75" spans="1:25" s="11" customFormat="1" ht="182" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:6" s="11" customFormat="1" ht="182" x14ac:dyDescent="0.15">
       <c r="A75" s="8" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B75" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="C75" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="C75" s="8" t="s">
-        <v>117</v>
-      </c>
       <c r="D75" s="8" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E75" s="8"/>
       <c r="F75" s="12"/>
     </row>
-    <row r="76" spans="1:25" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:6" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A76" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="B76" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="B76" s="8" t="s">
-        <v>120</v>
-      </c>
       <c r="C76" s="8" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D76" s="8" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E76" s="8"/>
       <c r="F76" s="12"/>
     </row>
-    <row r="77" spans="1:25" s="11" customFormat="1" ht="98" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:6" s="11" customFormat="1" ht="98" x14ac:dyDescent="0.15">
       <c r="A77" s="8" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="C77" s="8" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="D77" s="8" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="E77" s="14" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="F77" s="12" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="78" spans="1:25" s="11" customFormat="1" ht="277.5" customHeight="1" x14ac:dyDescent="0.15">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" s="11" customFormat="1" ht="277.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A78" s="8" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B78" s="8" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C78" s="8" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="D78" s="8" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="E78" s="8"/>
       <c r="F78" s="12"/>
     </row>
-    <row r="79" spans="1:25" s="3" customFormat="1" ht="277.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:6" s="3" customFormat="1" ht="277.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A79" s="1" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
       <c r="E79" s="1"/>
       <c r="F79" s="2"/>
     </row>
-    <row r="80" spans="1:25" s="11" customFormat="1" ht="56" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:6" s="11" customFormat="1" ht="56" x14ac:dyDescent="0.15">
       <c r="A80" s="8" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B80" s="8" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C80" s="8"/>
       <c r="D80" s="8"/>
       <c r="E80" s="14" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F80" s="12" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="81" spans="1:25" s="11" customFormat="1" ht="84" x14ac:dyDescent="0.15">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" s="11" customFormat="1" ht="84" x14ac:dyDescent="0.15">
       <c r="A81" s="8" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="C81" s="8"/>
       <c r="D81" s="8"/>
       <c r="E81" s="14"/>
       <c r="F81" s="12"/>
     </row>
-    <row r="82" spans="1:25" s="11" customFormat="1" ht="126" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:6" s="11" customFormat="1" ht="126" x14ac:dyDescent="0.15">
       <c r="A82" s="8" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B82" s="8" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C82" s="8" t="s">
+        <v>300</v>
+      </c>
+      <c r="D82" s="8" t="s">
         <v>299</v>
       </c>
-      <c r="D82" s="8" t="s">
-        <v>298</v>
-      </c>
       <c r="E82" s="14" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F82" s="12" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="83" spans="1:25" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
       <c r="A83" s="8" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B83" s="8" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C83" s="8" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D83" s="8" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="E83" s="8"/>
       <c r="F83" s="12"/>
     </row>
-    <row r="84" spans="1:25" s="11" customFormat="1" ht="84" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:6" s="11" customFormat="1" ht="84" x14ac:dyDescent="0.15">
       <c r="A84" s="8" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B84" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="C84" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="C84" s="8" t="s">
-        <v>133</v>
-      </c>
       <c r="D84" s="8" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="E84" s="14" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F84" s="12" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="85" spans="1:25" s="11" customFormat="1" ht="409.6" x14ac:dyDescent="0.15">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" s="11" customFormat="1" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A85" s="8" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B85" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="C85" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="C85" s="8" t="s">
-        <v>137</v>
-      </c>
       <c r="D85" s="8" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="E85" s="8"/>
       <c r="F85" s="12"/>
     </row>
-    <row r="86" spans="1:25" s="11" customFormat="1" ht="140" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:6" s="11" customFormat="1" ht="112" x14ac:dyDescent="0.15">
       <c r="A86" s="8" t="s">
-        <v>250</v>
+        <v>140</v>
       </c>
       <c r="B86" s="8" t="s">
-        <v>259</v>
+        <v>141</v>
       </c>
       <c r="C86" s="8" t="s">
-        <v>250</v>
+        <v>140</v>
       </c>
       <c r="D86" s="8" t="s">
-        <v>259</v>
+        <v>238</v>
       </c>
       <c r="E86" s="8"/>
       <c r="F86" s="12"/>
     </row>
-    <row r="87" spans="1:25" s="11" customFormat="1" ht="112" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:6" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A87" s="8" t="s">
-        <v>139</v>
+        <v>419</v>
       </c>
       <c r="B87" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="C87" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="D87" s="8" t="s">
-        <v>237</v>
-      </c>
+        <v>420</v>
+      </c>
+      <c r="C87" s="8"/>
+      <c r="D87" s="8"/>
       <c r="E87" s="8"/>
       <c r="F87" s="12"/>
     </row>
-    <row r="88" spans="1:25" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:6" s="11" customFormat="1" ht="154" x14ac:dyDescent="0.15">
       <c r="A88" s="8" t="s">
-        <v>417</v>
+        <v>341</v>
       </c>
       <c r="B88" s="8" t="s">
-        <v>418</v>
-      </c>
-      <c r="C88" s="8"/>
-      <c r="D88" s="8"/>
-      <c r="E88" s="8"/>
-      <c r="F88" s="12"/>
-    </row>
-    <row r="89" spans="1:25" s="3" customFormat="1" ht="154" x14ac:dyDescent="0.15">
-      <c r="A89" s="8" t="s">
-        <v>340</v>
-      </c>
-      <c r="B89" s="8" t="s">
-        <v>356</v>
-      </c>
-      <c r="C89" s="8" t="s">
-        <v>340</v>
-      </c>
-      <c r="D89" s="16" t="s">
-        <v>346</v>
-      </c>
-      <c r="E89" s="9" t="s">
+        <v>357</v>
+      </c>
+      <c r="C88" s="8" t="s">
+        <v>341</v>
+      </c>
+      <c r="D88" s="16" t="s">
+        <v>347</v>
+      </c>
+      <c r="E88" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="F88" s="17" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" s="3" customFormat="1" ht="340" x14ac:dyDescent="0.15">
+      <c r="A89" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="B89" s="24" t="s">
+        <v>426</v>
+      </c>
+      <c r="C89" s="1"/>
+      <c r="D89" s="1"/>
+      <c r="E89" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="F89" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" s="11" customFormat="1" ht="154" x14ac:dyDescent="0.15">
+      <c r="A90" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="B90" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="C90" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="D90" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="E90" s="8"/>
+      <c r="F90" s="12"/>
+    </row>
+    <row r="91" spans="1:6" s="11" customFormat="1" ht="168" x14ac:dyDescent="0.15">
+      <c r="A91" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="B91" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="C91" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="D91" s="8" t="s">
         <v>239</v>
-      </c>
-      <c r="F89" s="17" t="s">
-        <v>375</v>
-      </c>
-      <c r="G89" s="11"/>
-      <c r="H89" s="11"/>
-      <c r="I89" s="11"/>
-      <c r="J89" s="11"/>
-      <c r="K89" s="11"/>
-      <c r="L89" s="11"/>
-      <c r="M89" s="11"/>
-      <c r="N89" s="11"/>
-      <c r="O89" s="11"/>
-      <c r="P89" s="11"/>
-      <c r="Q89" s="11"/>
-      <c r="R89" s="11"/>
-      <c r="S89" s="11"/>
-      <c r="T89" s="11"/>
-      <c r="U89" s="11"/>
-      <c r="V89" s="11"/>
-      <c r="W89" s="11"/>
-      <c r="X89" s="11"/>
-      <c r="Y89" s="11"/>
-    </row>
-    <row r="90" spans="1:25" s="11" customFormat="1" ht="323" x14ac:dyDescent="0.15">
-      <c r="A90" s="1" t="s">
-        <v>419</v>
-      </c>
-      <c r="B90" s="24" t="s">
-        <v>423</v>
-      </c>
-      <c r="C90" s="1"/>
-      <c r="D90" s="1"/>
-      <c r="E90" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="F90" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="G90" s="3"/>
-      <c r="H90" s="3"/>
-      <c r="I90" s="3"/>
-      <c r="J90" s="3"/>
-      <c r="K90" s="3"/>
-      <c r="L90" s="3"/>
-      <c r="M90" s="3"/>
-      <c r="N90" s="3"/>
-      <c r="O90" s="3"/>
-      <c r="P90" s="3"/>
-      <c r="Q90" s="3"/>
-      <c r="R90" s="3"/>
-      <c r="S90" s="3"/>
-      <c r="T90" s="3"/>
-      <c r="U90" s="3"/>
-      <c r="V90" s="3"/>
-      <c r="W90" s="3"/>
-      <c r="X90" s="3"/>
-      <c r="Y90" s="3"/>
-    </row>
-    <row r="91" spans="1:25" s="11" customFormat="1" ht="154" x14ac:dyDescent="0.15">
-      <c r="A91" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="B91" s="8" t="s">
-        <v>350</v>
-      </c>
-      <c r="C91" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="D91" s="8" t="s">
-        <v>238</v>
       </c>
       <c r="E91" s="8"/>
       <c r="F91" s="12"/>
     </row>
-    <row r="92" spans="1:25" s="11" customFormat="1" ht="56" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:6" s="11" customFormat="1" ht="56" x14ac:dyDescent="0.15">
       <c r="A92" s="8" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B92" s="8" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C92" s="8" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="D92" s="8" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="E92" s="8"/>
       <c r="F92" s="12"/>
     </row>
-    <row r="93" spans="1:25" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:6" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
       <c r="A93" s="8" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B93" s="8" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C93" s="8" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="D93" s="8" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="E93" s="8" t="s">
         <v>88</v>
       </c>
       <c r="F93" s="12" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="94" spans="1:25" s="11" customFormat="1" ht="98" x14ac:dyDescent="0.15">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" s="11" customFormat="1" ht="98" x14ac:dyDescent="0.15">
       <c r="A94" s="8" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="B94" s="8" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="C94" s="8" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="D94" s="8" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="E94" s="8"/>
       <c r="F94" s="12"/>
     </row>
-    <row r="95" spans="1:25" s="11" customFormat="1" ht="126" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:6" s="11" customFormat="1" ht="126" x14ac:dyDescent="0.15">
       <c r="A95" s="8" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B95" s="8" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C95" s="8" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D95" s="8" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="E95" s="8"/>
       <c r="F95" s="12"/>
     </row>
-    <row r="96" spans="1:25" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:6" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A96" s="8" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B96" s="8" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="C96" s="8" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="D96" s="8" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="E96" s="8"/>
       <c r="F96" s="12"/>
     </row>
     <row r="97" spans="1:6" s="11" customFormat="1" ht="358" x14ac:dyDescent="0.15">
       <c r="A97" s="8" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B97" s="8" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="C97" s="8" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D97" s="8" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="E97" s="9" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F97" s="10" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="98" spans="1:6" s="11" customFormat="1" ht="98" x14ac:dyDescent="0.15">
       <c r="A98" s="8" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B98" s="8" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C98" s="8" t="s">
         <v>25</v>
       </c>
       <c r="D98" s="8" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="E98" s="8"/>
       <c r="F98" s="12"/>
     </row>
     <row r="99" spans="1:6" s="11" customFormat="1" ht="56" x14ac:dyDescent="0.15">
       <c r="A99" s="8" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B99" s="8" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C99" s="8" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="D99" s="8" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="E99" s="8"/>
       <c r="F99" s="12"/>
     </row>
     <row r="100" spans="1:6" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
       <c r="A100" s="8" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B100" s="8" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="C100" s="8" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="D100" s="8" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="E100" s="8"/>
       <c r="F100" s="12"/>
     </row>
     <row r="101" spans="1:6" s="11" customFormat="1" ht="56" x14ac:dyDescent="0.15">
       <c r="A101" s="8" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="B101" s="8" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="C101" s="8" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D101" s="8" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="E101" s="8"/>
       <c r="F101" s="12"/>
     </row>
-    <row r="102" spans="1:6" s="11" customFormat="1" ht="112" x14ac:dyDescent="0.15">
+    <row r="102" spans="1:6" s="11" customFormat="1" ht="126" x14ac:dyDescent="0.15">
       <c r="A102" s="18" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="B102" s="8" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="C102" s="8"/>
       <c r="D102" s="8" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="E102" s="8"/>
       <c r="F102" s="12"/>
     </row>
     <row r="103" spans="1:6" s="11" customFormat="1" ht="126" x14ac:dyDescent="0.15">
       <c r="A103" s="8" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B103" s="8" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="C103" s="8"/>
       <c r="D103" s="8" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="E103" s="8"/>
       <c r="F103" s="12"/>
     </row>
     <row r="104" spans="1:6" s="11" customFormat="1" ht="84" x14ac:dyDescent="0.15">
       <c r="A104" s="8" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B104" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="C104" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="C104" s="8" t="s">
-        <v>147</v>
-      </c>
       <c r="D104" s="8" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="E104" s="8"/>
       <c r="F104" s="12"/>
     </row>
-    <row r="105" spans="1:6" s="11" customFormat="1" ht="112" x14ac:dyDescent="0.15">
+    <row r="105" spans="1:6" s="11" customFormat="1" ht="126" x14ac:dyDescent="0.15">
       <c r="A105" s="8" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="B105" s="8" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C105" s="8" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D105" s="8" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E105" s="14" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F105" s="12" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="106" spans="1:6" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
       <c r="A106" s="8" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B106" s="8" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C106" s="8" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D106" s="8" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="E106" s="8"/>
       <c r="F106" s="12"/>
     </row>
     <row r="107" spans="1:6" s="11" customFormat="1" ht="140" x14ac:dyDescent="0.15">
       <c r="A107" s="8" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B107" s="8" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C107" s="8" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D107" s="8" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E107" s="8"/>
       <c r="F107" s="12"/>
     </row>
     <row r="108" spans="1:6" s="11" customFormat="1" ht="56" x14ac:dyDescent="0.15">
       <c r="A108" s="8" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B108" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="C108" s="8" t="s">
         <v>220</v>
       </c>
-      <c r="C108" s="8" t="s">
-        <v>219</v>
-      </c>
       <c r="D108" s="8" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="E108" s="8"/>
       <c r="F108" s="12"/>
     </row>
     <row r="109" spans="1:6" s="3" customFormat="1" ht="85" x14ac:dyDescent="0.15">
       <c r="A109" s="1" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="C109" s="1"/>
       <c r="D109" s="1"/>
@@ -4110,26 +3953,26 @@
     </row>
     <row r="110" spans="1:6" s="11" customFormat="1" ht="112" x14ac:dyDescent="0.15">
       <c r="A110" s="8" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B110" s="8" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C110" s="8" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="D110" s="8" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="E110" s="8"/>
       <c r="F110" s="12"/>
     </row>
     <row r="111" spans="1:6" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A111" s="8" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B111" s="8" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C111" s="8"/>
       <c r="D111" s="8"/>
@@ -4138,130 +3981,130 @@
     </row>
     <row r="112" spans="1:6" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A112" s="8" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B112" s="8" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="C112" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="D112" s="8" t="s">
         <v>281</v>
-      </c>
-      <c r="D112" s="8" t="s">
-        <v>280</v>
       </c>
       <c r="E112" s="8"/>
       <c r="F112" s="12"/>
     </row>
     <row r="113" spans="1:6" s="11" customFormat="1" ht="112" x14ac:dyDescent="0.15">
       <c r="A113" s="8" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B113" s="8" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C113" s="8" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D113" s="8" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="E113" s="8"/>
       <c r="F113" s="12"/>
     </row>
     <row r="114" spans="1:6" s="11" customFormat="1" ht="126" x14ac:dyDescent="0.15">
       <c r="A114" s="8" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B114" s="8" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C114" s="8" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D114" s="8" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="E114" s="8"/>
       <c r="F114" s="12"/>
     </row>
     <row r="115" spans="1:6" s="11" customFormat="1" ht="252" x14ac:dyDescent="0.15">
       <c r="A115" s="8" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B115" s="8" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C115" s="8" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D115" s="8" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E115" s="14" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="F115" s="12" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="116" spans="1:6" s="11" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A116" s="8" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B116" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="C116" s="8" t="s">
         <v>267</v>
       </c>
-      <c r="C116" s="8" t="s">
-        <v>266</v>
-      </c>
       <c r="D116" s="8" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="E116" s="8"/>
       <c r="F116" s="12"/>
     </row>
     <row r="117" spans="1:6" s="11" customFormat="1" ht="84" x14ac:dyDescent="0.15">
       <c r="A117" s="8" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B117" s="8" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C117" s="8" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D117" s="8" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E117" s="14" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="F117" s="12" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="118" spans="1:6" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A118" s="8" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B118" s="8" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C118" s="8"/>
       <c r="D118" s="8"/>
       <c r="E118" s="14" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="F118" s="12" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="119" spans="1:6" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
       <c r="A119" s="8" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B119" s="8" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C119" s="8"/>
       <c r="D119" s="8"/>
@@ -4270,82 +4113,82 @@
     </row>
     <row r="120" spans="1:6" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A120" s="8" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B120" s="8" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C120" s="8"/>
       <c r="D120" s="8"/>
       <c r="E120" s="8"/>
       <c r="F120" s="12"/>
     </row>
-    <row r="121" spans="1:6" s="11" customFormat="1" ht="56" x14ac:dyDescent="0.15">
+    <row r="121" spans="1:6" s="11" customFormat="1" ht="126" x14ac:dyDescent="0.15">
       <c r="A121" s="8" t="s">
-        <v>387</v>
-      </c>
-      <c r="B121" s="8" t="s">
-        <v>187</v>
-      </c>
-      <c r="C121" s="8" t="s">
-        <v>352</v>
-      </c>
-      <c r="D121" s="8" t="s">
-        <v>188</v>
+        <v>389</v>
+      </c>
+      <c r="B121" s="19" t="s">
+        <v>400</v>
+      </c>
+      <c r="C121" s="8"/>
+      <c r="D121" s="19" t="s">
+        <v>390</v>
       </c>
       <c r="E121" s="8"/>
       <c r="F121" s="12"/>
     </row>
-    <row r="122" spans="1:6" s="11" customFormat="1" ht="126" x14ac:dyDescent="0.15">
+    <row r="122" spans="1:6" s="11" customFormat="1" ht="56" x14ac:dyDescent="0.15">
       <c r="A122" s="8" t="s">
         <v>388</v>
       </c>
-      <c r="B122" s="19" t="s">
-        <v>399</v>
-      </c>
-      <c r="C122" s="8"/>
-      <c r="D122" s="19" t="s">
-        <v>389</v>
+      <c r="B122" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="C122" s="8" t="s">
+        <v>353</v>
+      </c>
+      <c r="D122" s="8" t="s">
+        <v>189</v>
       </c>
       <c r="E122" s="8"/>
       <c r="F122" s="12"/>
     </row>
-    <row r="123" spans="1:6" s="11" customFormat="1" ht="224" x14ac:dyDescent="0.15">
+    <row r="123" spans="1:6" s="11" customFormat="1" ht="238" x14ac:dyDescent="0.15">
       <c r="A123" s="8" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B123" s="8" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="C123" s="8"/>
       <c r="D123" s="20" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="E123" s="8"/>
       <c r="F123" s="12"/>
     </row>
     <row r="124" spans="1:6" s="11" customFormat="1" ht="224" x14ac:dyDescent="0.15">
       <c r="A124" s="8" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B124" s="8" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C124" s="8" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D124" s="8" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="E124" s="8"/>
       <c r="F124" s="12"/>
     </row>
     <row r="125" spans="1:6" s="11" customFormat="1" ht="84" x14ac:dyDescent="0.15">
       <c r="A125" s="8" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B125" s="8" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C125" s="8"/>
       <c r="D125" s="8"/>
@@ -4353,15 +4196,15 @@
         <v>79</v>
       </c>
       <c r="F125" s="12" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="126" spans="1:6" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A126" s="8" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B126" s="8" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C126" s="8"/>
       <c r="D126" s="8"/>
@@ -4370,58 +4213,58 @@
     </row>
     <row r="127" spans="1:6" s="11" customFormat="1" ht="332" x14ac:dyDescent="0.15">
       <c r="A127" s="8" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B127" s="8" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C127" s="8" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D127" s="8" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="E127" s="8"/>
       <c r="F127" s="12"/>
     </row>
     <row r="128" spans="1:6" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A128" s="8" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B128" s="8" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C128" s="8" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="D128" s="8" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="E128" s="8"/>
       <c r="F128" s="12"/>
     </row>
     <row r="129" spans="1:6" s="11" customFormat="1" ht="140" x14ac:dyDescent="0.15">
       <c r="A129" s="8" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B129" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="C129" s="8" t="s">
         <v>201</v>
       </c>
-      <c r="C129" s="8" t="s">
-        <v>200</v>
-      </c>
       <c r="D129" s="8" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="E129" s="8"/>
       <c r="F129" s="12"/>
     </row>
     <row r="130" spans="1:6" s="11" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A130" s="8" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B130" s="8" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C130" s="8"/>
       <c r="D130" s="8"/>
@@ -5334,11 +5177,7 @@
     <row r="1028" ht="13" x14ac:dyDescent="0.15"/>
     <row r="1029" ht="13" x14ac:dyDescent="0.15"/>
   </sheetData>
-  <autoFilter ref="A1:Y131" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Y131">
-      <sortCondition ref="A1:A131"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:Y131" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Y1029">
     <sortCondition ref="A2:A1029"/>
   </sortState>
@@ -5353,12 +5192,12 @@
     <hyperlink ref="E50" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
     <hyperlink ref="E53" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
     <hyperlink ref="E60" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="E67" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="E70" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="E66" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="E68" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
     <hyperlink ref="E80" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
     <hyperlink ref="E72" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
     <hyperlink ref="E82" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="E90" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="E89" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
     <hyperlink ref="E105" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
     <hyperlink ref="E115" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
     <hyperlink ref="E117" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
@@ -5369,7 +5208,7 @@
     <hyperlink ref="E2" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
     <hyperlink ref="E97" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
     <hyperlink ref="E62" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="E89" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="E88" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
     <hyperlink ref="F2" r:id="rId28" display="https://www.whitehouse.gov/sites/whitehouse.gov/files/omb/assets/a11_current_year/a11_2017.pdf" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
     <hyperlink ref="E9" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
     <hyperlink ref="E18" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
@@ -5378,7 +5217,7 @@
     <hyperlink ref="E24" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
     <hyperlink ref="E47" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
     <hyperlink ref="F62" r:id="rId35" display="https://www.whitehouse.gov/sites/whitehouse.gov/files/omb/assets/a11_current_year/a11_2017.pdf" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="F89" r:id="rId36" display="https://www.whitehouse.gov/sites/whitehouse.gov/files/omb/assets/a11_current_year/a11_2017.pdf" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="F88" r:id="rId36" display="https://www.whitehouse.gov/sites/whitehouse.gov/files/omb/assets/a11_current_year/a11_2017.pdf" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
     <hyperlink ref="F97" r:id="rId37" display="https://www.whitehouse.gov/sites/whitehouse.gov/files/omb/assets/a11_current_year/a11_2017.pdf" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated Place of Performance official def
</commit_message>
<xml_diff>
--- a/usaspending_api/data/USAspendingGlossary.xlsx
+++ b/usaspending_api/data/USAspendingGlossary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10609"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brianzito/Documents/DATA/usaspending-api/usaspending_api/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tonysappe/dev/fedspendingtransparency/usaspending-api/usaspending_api/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5FFDE5E-1419-F943-ACC3-26BA41657891}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52B52AB9-FEF1-2941-A47A-F607F0B41994}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1028,9 +1028,6 @@
     <t xml:space="preserve">[Object Class definitions](https://www.whitehouse.gov/sites/whitehouse.gov/files/omb/assets/a11_current_year/a11_2017.pdf) </t>
   </si>
   <si>
-    <t>The address where the predominant performance of the award will be accomplished. The address is made up of six components: Address Lines 1 and 2, City, County, State Code, and ZIP+4 or Postal Code.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Recipient/Business types are socio-economic and other organizational/business characteristics that are used to categorize federal contractors and other funding recipients. There are many different recipient/business types, and they span for-profit businesses, non-profits, government entities, individuals, and foreign entities. Some examples are:
 - Historically Black College or University
 - Veteran-Owned Business 
@@ -1633,6 +1630,9 @@
   </si>
   <si>
     <t>Indefinite Delivery / Definite Quantity Contract</t>
+  </si>
+  <si>
+    <t>The address where the predominant performance of the award will be accomplished. The address is made up of four components: City, State Code, and ZIP+4 or Postal Code.</t>
   </si>
 </sst>
 </file>
@@ -1810,7 +1810,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1901,6 +1901,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -2190,8 +2193,8 @@
   <dimension ref="A1:Y1029"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A69" sqref="A69"/>
+      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D99" sqref="D99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2249,19 +2252,19 @@
         <v>213</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>213</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>239</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="3" spans="1:25" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
@@ -2285,7 +2288,7 @@
         <v>246</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>246</v>
@@ -2373,7 +2376,7 @@
         <v>239</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="10" spans="1:25" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
@@ -2397,7 +2400,7 @@
         <v>22</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
@@ -2409,19 +2412,19 @@
         <v>23</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>24</v>
       </c>
       <c r="D12" s="8" t="s">
+        <v>315</v>
+      </c>
+      <c r="E12" s="8" t="s">
         <v>316</v>
       </c>
-      <c r="E12" s="8" t="s">
-        <v>317</v>
-      </c>
       <c r="F12" s="13" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="13" spans="1:25" s="11" customFormat="1" ht="56" x14ac:dyDescent="0.15">
@@ -2468,42 +2471,42 @@
         <v>35</v>
       </c>
       <c r="C15" s="8" t="s">
+        <v>301</v>
+      </c>
+      <c r="D15" s="8" t="s">
         <v>302</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>303</v>
       </c>
       <c r="E15" s="8"/>
       <c r="F15" s="12"/>
     </row>
     <row r="16" spans="1:25" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A16" s="8" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C16" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="D16" s="8" t="s">
         <v>304</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>305</v>
       </c>
       <c r="E16" s="8"/>
       <c r="F16" s="12"/>
     </row>
     <row r="17" spans="1:6" s="11" customFormat="1" ht="56" x14ac:dyDescent="0.15">
       <c r="A17" s="8" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C17" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="D17" s="8" t="s">
         <v>306</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>307</v>
       </c>
       <c r="E17" s="8"/>
       <c r="F17" s="12"/>
@@ -2525,7 +2528,7 @@
         <v>239</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="19" spans="1:6" s="3" customFormat="1" ht="318" customHeight="1" x14ac:dyDescent="0.15">
@@ -2533,7 +2536,7 @@
         <v>39</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -2565,7 +2568,7 @@
         <v>45</v>
       </c>
       <c r="B21" s="24" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -2585,7 +2588,7 @@
       </c>
       <c r="C22" s="8"/>
       <c r="D22" s="8" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E22" s="14"/>
       <c r="F22" s="12"/>
@@ -2623,7 +2626,7 @@
         <v>239</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="25" spans="1:6" s="11" customFormat="1" ht="112" x14ac:dyDescent="0.15">
@@ -2631,31 +2634,31 @@
         <v>51</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
       <c r="E25" s="9" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F25" s="15" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="26" spans="1:6" s="11" customFormat="1" ht="168" x14ac:dyDescent="0.15">
       <c r="A26" s="8" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
       <c r="E26" s="9" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F26" s="15" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="27" spans="1:6" s="11" customFormat="1" ht="98" x14ac:dyDescent="0.15">
@@ -2678,10 +2681,10 @@
         <v>57</v>
       </c>
       <c r="C28" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="D28" s="8" t="s">
         <v>296</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>297</v>
       </c>
       <c r="E28" s="14" t="s">
         <v>58</v>
@@ -2708,16 +2711,16 @@
     </row>
     <row r="30" spans="1:6" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
       <c r="A30" s="8" t="s">
+        <v>381</v>
+      </c>
+      <c r="B30" s="8" t="s">
         <v>382</v>
       </c>
-      <c r="B30" s="8" t="s">
-        <v>383</v>
-      </c>
       <c r="C30" s="8" t="s">
+        <v>381</v>
+      </c>
+      <c r="D30" s="8" t="s">
         <v>382</v>
-      </c>
-      <c r="D30" s="8" t="s">
-        <v>383</v>
       </c>
       <c r="E30" s="14" t="s">
         <v>75</v>
@@ -2735,7 +2738,7 @@
       </c>
       <c r="C31" s="8"/>
       <c r="D31" s="8" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E31" s="14"/>
       <c r="F31" s="12"/>
@@ -2777,19 +2780,19 @@
         <v>211</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C34" s="8" t="s">
         <v>211</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E34" s="9" t="s">
         <v>239</v>
       </c>
       <c r="F34" s="12" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="35" spans="1:25" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
@@ -2813,7 +2816,7 @@
         <v>72</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C36" s="8" t="s">
         <v>73</v>
@@ -2845,10 +2848,10 @@
     </row>
     <row r="37" spans="1:25" s="11" customFormat="1" ht="255" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>402</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>403</v>
       </c>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
@@ -2892,7 +2895,7 @@
     </row>
     <row r="39" spans="1:25" s="11" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A39" s="8" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B39" s="8" t="s">
         <v>257</v>
@@ -2908,10 +2911,10 @@
     </row>
     <row r="40" spans="1:25" s="3" customFormat="1" ht="102" x14ac:dyDescent="0.15">
       <c r="A40" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>404</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>405</v>
       </c>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
@@ -2941,7 +2944,7 @@
         <v>225</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E42" s="14"/>
       <c r="F42" s="12"/>
@@ -2957,7 +2960,7 @@
         <v>227</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E43" s="14"/>
       <c r="F43" s="12"/>
@@ -2999,7 +3002,7 @@
         <v>88</v>
       </c>
       <c r="F45" s="12" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="46" spans="1:25" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
@@ -3029,13 +3032,13 @@
         <v>94</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E47" s="9" t="s">
+        <v>371</v>
+      </c>
+      <c r="F47" s="12" t="s">
         <v>372</v>
-      </c>
-      <c r="F47" s="12" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="48" spans="1:25" s="11" customFormat="1" ht="98" x14ac:dyDescent="0.15">
@@ -3046,7 +3049,7 @@
         <v>289</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D48" s="8" t="s">
         <v>116</v>
@@ -3119,7 +3122,7 @@
         <v>101</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
@@ -3147,13 +3150,13 @@
         <v>218</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C55" s="8" t="s">
         <v>218</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E55" s="8"/>
       <c r="F55" s="12"/>
@@ -3166,20 +3169,20 @@
         <v>109</v>
       </c>
       <c r="C56" s="8" t="s">
+        <v>307</v>
+      </c>
+      <c r="D56" s="8" t="s">
         <v>308</v>
-      </c>
-      <c r="D56" s="8" t="s">
-        <v>309</v>
       </c>
       <c r="E56" s="8"/>
       <c r="F56" s="12"/>
     </row>
     <row r="57" spans="1:6" s="11" customFormat="1" ht="112" x14ac:dyDescent="0.15">
       <c r="A57" s="8" t="s">
+        <v>333</v>
+      </c>
+      <c r="B57" s="8" t="s">
         <v>334</v>
-      </c>
-      <c r="B57" s="8" t="s">
-        <v>335</v>
       </c>
       <c r="C57" s="8" t="s">
         <v>135</v>
@@ -3192,42 +3195,42 @@
     </row>
     <row r="58" spans="1:6" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A58" s="8" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E58" s="8"/>
       <c r="F58" s="12"/>
     </row>
     <row r="59" spans="1:6" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
       <c r="A59" s="8" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C59" s="8" t="s">
+        <v>310</v>
+      </c>
+      <c r="D59" s="8" t="s">
         <v>311</v>
-      </c>
-      <c r="D59" s="8" t="s">
-        <v>312</v>
       </c>
       <c r="E59" s="8"/>
       <c r="F59" s="12"/>
     </row>
     <row r="60" spans="1:6" s="3" customFormat="1" ht="238" x14ac:dyDescent="0.15">
       <c r="A60" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B60" s="24" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
@@ -3249,7 +3252,7 @@
         <v>209</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E61" s="14"/>
       <c r="F61" s="12"/>
@@ -3259,27 +3262,27 @@
         <v>210</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C62" s="8" t="s">
         <v>210</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E62" s="9" t="s">
         <v>239</v>
       </c>
       <c r="F62" s="10" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="63" spans="1:6" s="3" customFormat="1" ht="119" x14ac:dyDescent="0.15">
       <c r="A63" s="1" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
@@ -3320,10 +3323,10 @@
     </row>
     <row r="66" spans="1:25" s="3" customFormat="1" ht="85" x14ac:dyDescent="0.15">
       <c r="A66" s="30" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
@@ -3332,10 +3335,10 @@
     </row>
     <row r="67" spans="1:25" s="1" customFormat="1" ht="175" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A67" s="27" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B67" s="29" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C67" s="27"/>
       <c r="E67" s="1" t="s">
@@ -3366,10 +3369,10 @@
     </row>
     <row r="68" spans="1:25" s="11" customFormat="1" ht="170" x14ac:dyDescent="0.15">
       <c r="A68" s="26" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B68" s="25" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C68" s="28"/>
       <c r="D68" s="1"/>
@@ -3397,10 +3400,10 @@
     </row>
     <row r="69" spans="1:25" s="3" customFormat="1" ht="170" x14ac:dyDescent="0.15">
       <c r="A69" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
@@ -3409,7 +3412,7 @@
     </row>
     <row r="70" spans="1:25" s="3" customFormat="1" ht="140" x14ac:dyDescent="0.15">
       <c r="A70" s="8" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B70" s="8" t="s">
         <v>113</v>
@@ -3444,10 +3447,10 @@
     </row>
     <row r="71" spans="1:25" s="3" customFormat="1" ht="119" x14ac:dyDescent="0.15">
       <c r="A71" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="B71" s="1" t="s">
         <v>413</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>414</v>
       </c>
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
@@ -3456,16 +3459,16 @@
     </row>
     <row r="72" spans="1:25" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
       <c r="A72" s="8" t="s">
+        <v>378</v>
+      </c>
+      <c r="B72" s="8" t="s">
         <v>379</v>
       </c>
-      <c r="B72" s="8" t="s">
-        <v>380</v>
-      </c>
       <c r="C72" s="8" t="s">
+        <v>378</v>
+      </c>
+      <c r="D72" s="8" t="s">
         <v>379</v>
-      </c>
-      <c r="D72" s="8" t="s">
-        <v>380</v>
       </c>
       <c r="E72" s="14" t="s">
         <v>127</v>
@@ -3476,16 +3479,16 @@
     </row>
     <row r="73" spans="1:25" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
       <c r="A73" s="8" t="s">
+        <v>327</v>
+      </c>
+      <c r="B73" s="8" t="s">
         <v>328</v>
       </c>
-      <c r="B73" s="8" t="s">
-        <v>329</v>
-      </c>
       <c r="C73" s="8" t="s">
+        <v>327</v>
+      </c>
+      <c r="D73" s="8" t="s">
         <v>328</v>
-      </c>
-      <c r="D73" s="8" t="s">
-        <v>329</v>
       </c>
       <c r="E73" s="8"/>
       <c r="F73" s="12"/>
@@ -3495,7 +3498,7 @@
         <v>229</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C74" s="8"/>
       <c r="D74" s="8"/>
@@ -3536,16 +3539,16 @@
     </row>
     <row r="77" spans="1:25" s="11" customFormat="1" ht="98" x14ac:dyDescent="0.15">
       <c r="A77" s="8" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C77" s="8" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D77" s="8" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E77" s="14" t="s">
         <v>202</v>
@@ -3556,7 +3559,7 @@
     </row>
     <row r="78" spans="1:25" s="11" customFormat="1" ht="277.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A78" s="8" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B78" s="8" t="s">
         <v>258</v>
@@ -3572,10 +3575,10 @@
     </row>
     <row r="79" spans="1:25" s="3" customFormat="1" ht="277.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A79" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="B79" s="1" t="s">
         <v>415</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>416</v>
       </c>
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
@@ -3603,7 +3606,7 @@
         <v>230</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C81" s="8"/>
       <c r="D81" s="8"/>
@@ -3618,10 +3621,10 @@
         <v>130</v>
       </c>
       <c r="C82" s="8" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D82" s="8" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E82" s="14" t="s">
         <v>131</v>
@@ -3716,10 +3719,10 @@
     </row>
     <row r="88" spans="1:25" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A88" s="8" t="s">
+        <v>416</v>
+      </c>
+      <c r="B88" s="8" t="s">
         <v>417</v>
-      </c>
-      <c r="B88" s="8" t="s">
-        <v>418</v>
       </c>
       <c r="C88" s="8"/>
       <c r="D88" s="8"/>
@@ -3728,22 +3731,22 @@
     </row>
     <row r="89" spans="1:25" s="3" customFormat="1" ht="154" x14ac:dyDescent="0.15">
       <c r="A89" s="8" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B89" s="8" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C89" s="8" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D89" s="16" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E89" s="9" t="s">
         <v>239</v>
       </c>
       <c r="F89" s="17" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="G89" s="11"/>
       <c r="H89" s="11"/>
@@ -3767,10 +3770,10 @@
     </row>
     <row r="90" spans="1:25" s="11" customFormat="1" ht="323" x14ac:dyDescent="0.15">
       <c r="A90" s="1" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B90" s="24" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C90" s="1"/>
       <c r="D90" s="1"/>
@@ -3805,7 +3808,7 @@
         <v>143</v>
       </c>
       <c r="B91" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C91" s="8" t="s">
         <v>144</v>
@@ -3834,7 +3837,7 @@
     </row>
     <row r="93" spans="1:25" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
       <c r="A93" s="8" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B93" s="8" t="s">
         <v>283</v>
@@ -3849,15 +3852,15 @@
         <v>88</v>
       </c>
       <c r="F93" s="12" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="94" spans="1:25" s="11" customFormat="1" ht="98" x14ac:dyDescent="0.15">
       <c r="A94" s="8" t="s">
+        <v>329</v>
+      </c>
+      <c r="B94" s="8" t="s">
         <v>330</v>
-      </c>
-      <c r="B94" s="8" t="s">
-        <v>331</v>
       </c>
       <c r="C94" s="8" t="s">
         <v>252</v>
@@ -3889,7 +3892,7 @@
         <v>254</v>
       </c>
       <c r="B96" s="8" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C96" s="8" t="s">
         <v>254</v>
@@ -3905,19 +3908,19 @@
         <v>212</v>
       </c>
       <c r="B97" s="8" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C97" s="8" t="s">
         <v>212</v>
       </c>
       <c r="D97" s="8" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E97" s="9" t="s">
         <v>239</v>
       </c>
       <c r="F97" s="10" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="98" spans="1:6" s="11" customFormat="1" ht="98" x14ac:dyDescent="0.15">
@@ -3946,8 +3949,8 @@
       <c r="C99" s="8" t="s">
         <v>240</v>
       </c>
-      <c r="D99" s="8" t="s">
-        <v>291</v>
+      <c r="D99" s="31" t="s">
+        <v>429</v>
       </c>
       <c r="E99" s="8"/>
       <c r="F99" s="12"/>
@@ -3957,7 +3960,7 @@
         <v>255</v>
       </c>
       <c r="B100" s="8" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C100" s="8" t="s">
         <v>255</v>
@@ -3970,10 +3973,10 @@
     </row>
     <row r="101" spans="1:6" s="11" customFormat="1" ht="56" x14ac:dyDescent="0.15">
       <c r="A101" s="8" t="s">
+        <v>359</v>
+      </c>
+      <c r="B101" s="8" t="s">
         <v>360</v>
-      </c>
-      <c r="B101" s="8" t="s">
-        <v>361</v>
       </c>
       <c r="C101" s="8" t="s">
         <v>256</v>
@@ -3986,28 +3989,28 @@
     </row>
     <row r="102" spans="1:6" s="11" customFormat="1" ht="112" x14ac:dyDescent="0.15">
       <c r="A102" s="18" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B102" s="8" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C102" s="8"/>
       <c r="D102" s="8" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E102" s="8"/>
       <c r="F102" s="12"/>
     </row>
     <row r="103" spans="1:6" s="11" customFormat="1" ht="126" x14ac:dyDescent="0.15">
       <c r="A103" s="8" t="s">
+        <v>395</v>
+      </c>
+      <c r="B103" s="8" t="s">
         <v>396</v>
-      </c>
-      <c r="B103" s="8" t="s">
-        <v>397</v>
       </c>
       <c r="C103" s="8"/>
       <c r="D103" s="8" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="E103" s="8"/>
       <c r="F103" s="12"/>
@@ -4023,14 +4026,14 @@
         <v>147</v>
       </c>
       <c r="D104" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E104" s="8"/>
       <c r="F104" s="12"/>
     </row>
     <row r="105" spans="1:6" s="11" customFormat="1" ht="112" x14ac:dyDescent="0.15">
       <c r="A105" s="8" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B105" s="8" t="s">
         <v>156</v>
@@ -4091,17 +4094,17 @@
         <v>219</v>
       </c>
       <c r="D108" s="8" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E108" s="8"/>
       <c r="F108" s="12"/>
     </row>
     <row r="109" spans="1:6" s="3" customFormat="1" ht="85" x14ac:dyDescent="0.15">
       <c r="A109" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="B109" s="1" t="s">
         <v>420</v>
-      </c>
-      <c r="B109" s="1" t="s">
-        <v>421</v>
       </c>
       <c r="C109" s="1"/>
       <c r="D109" s="1"/>
@@ -4110,10 +4113,10 @@
     </row>
     <row r="110" spans="1:6" s="11" customFormat="1" ht="112" x14ac:dyDescent="0.15">
       <c r="A110" s="8" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B110" s="8" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C110" s="8" t="s">
         <v>246</v>
@@ -4138,10 +4141,10 @@
     </row>
     <row r="112" spans="1:6" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A112" s="8" t="s">
+        <v>325</v>
+      </c>
+      <c r="B112" s="8" t="s">
         <v>326</v>
-      </c>
-      <c r="B112" s="8" t="s">
-        <v>327</v>
       </c>
       <c r="C112" s="8" t="s">
         <v>281</v>
@@ -4163,7 +4166,7 @@
         <v>170</v>
       </c>
       <c r="D113" s="8" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E113" s="8"/>
       <c r="F113" s="12"/>
@@ -4189,7 +4192,7 @@
         <v>163</v>
       </c>
       <c r="B115" s="8" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C115" s="8" t="s">
         <v>164</v>
@@ -4273,7 +4276,7 @@
         <v>208</v>
       </c>
       <c r="B120" s="8" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C120" s="8"/>
       <c r="D120" s="8"/>
@@ -4282,13 +4285,13 @@
     </row>
     <row r="121" spans="1:6" s="11" customFormat="1" ht="56" x14ac:dyDescent="0.15">
       <c r="A121" s="8" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B121" s="8" t="s">
         <v>187</v>
       </c>
       <c r="C121" s="8" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D121" s="8" t="s">
         <v>188</v>
@@ -4298,28 +4301,28 @@
     </row>
     <row r="122" spans="1:6" s="11" customFormat="1" ht="126" x14ac:dyDescent="0.15">
       <c r="A122" s="8" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B122" s="19" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C122" s="8"/>
       <c r="D122" s="19" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E122" s="8"/>
       <c r="F122" s="12"/>
     </row>
     <row r="123" spans="1:6" s="11" customFormat="1" ht="224" x14ac:dyDescent="0.15">
       <c r="A123" s="8" t="s">
+        <v>389</v>
+      </c>
+      <c r="B123" s="8" t="s">
         <v>390</v>
-      </c>
-      <c r="B123" s="8" t="s">
-        <v>391</v>
       </c>
       <c r="C123" s="8"/>
       <c r="D123" s="20" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="E123" s="8"/>
       <c r="F123" s="12"/>
@@ -4411,7 +4414,7 @@
         <v>200</v>
       </c>
       <c r="D129" s="8" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E129" s="8"/>
       <c r="F129" s="12"/>

</xml_diff>

<commit_message>
Fixed the list format in the TAS glossary definition
</commit_message>
<xml_diff>
--- a/usaspending_api/data/USAspendingGlossary.xlsx
+++ b/usaspending_api/data/USAspendingGlossary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elizabethsalita/Workspace/DATA-Act/usaspending-api/usaspending_api/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4E850CC-1262-814E-A290-CA3DABFDD64D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAEBCCD1-4281-2F46-A721-056D5A3A9845}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20" yWindow="460" windowWidth="33600" windowHeight="18940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1622,17 +1622,17 @@
   <si>
     <t>Treasury and OMB assign a code to each appropriation, receipt, or fund account. This code is similar to a bank account number. It helps identify financial transactions in the federal government. It also aids in reporting accuracy. TAS are sometimes referred as ‘program source’ in legislation. On this website, we group each set of Treasury Accounts that share an Agency Identifier and Main Account Code into a "Federal Account". 
 Seven components make up the TAS:
-•	Allocation Transfer Agency Identifier (ex. 089)
-•	Agency Identifier (ex. 020)
-•	Beginning Period of Availability (ex. 2017)
-•	Ending Period of Availability (ex. 2018)
-•	Availability Type Code (used if there are not specific beginning/ending years) (ex. X)
-•	Main Account Code (ex. 0114)
-•	Sub-Account Code (ex. 000)
+- Allocation Transfer Agency Identifier (ex. 089)
+- Agency Identifier (ex. 020)
+- Beginning Period of Availability (ex. 2017)
+- Ending Period of Availability (ex. 2018)
+- Availability Type Code (used if there are not specific beginning/ending years) (ex. X)
+- Main Account Code (ex. 0114)
+- Sub-Account Code (ex. 000)
 Example TAS:
-•	089-020-2017/2018-0114-000
-•	089-020-2017/2017-0114-000
-•	089-020-X-0114-000</t>
+- 089-020-2017/2018-0114-000
+- 089-020-2017/2017-0114-000
+- 089-020-X-0114-000</t>
   </si>
 </sst>
 </file>
@@ -2193,8 +2193,8 @@
   <dimension ref="A1:Y1029"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C127" sqref="C127"/>
+      <pane ySplit="1" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B128" sqref="B128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4371,7 +4371,7 @@
       <c r="E126" s="8"/>
       <c r="F126" s="12"/>
     </row>
-    <row r="127" spans="1:6" s="11" customFormat="1" ht="332" x14ac:dyDescent="0.15">
+    <row r="127" spans="1:6" s="11" customFormat="1" ht="358" x14ac:dyDescent="0.15">
       <c r="A127" s="8" t="s">
         <v>198</v>
       </c>

</xml_diff>

<commit_message>
Updated list formatting in the TAS glossary entry
</commit_message>
<xml_diff>
--- a/usaspending_api/data/USAspendingGlossary.xlsx
+++ b/usaspending_api/data/USAspendingGlossary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elizabethsalita/Workspace/DATA-Act/usaspending-api/usaspending_api/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4E850CC-1262-814E-A290-CA3DABFDD64D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9B3A609-E8D9-ED4D-B0B4-A89F6045E8D0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1622,17 +1622,17 @@
   <si>
     <t>Treasury and OMB assign a code to each appropriation, receipt, or fund account. This code is similar to a bank account number. It helps identify financial transactions in the federal government. It also aids in reporting accuracy. TAS are sometimes referred as ‘program source’ in legislation. On this website, we group each set of Treasury Accounts that share an Agency Identifier and Main Account Code into a "Federal Account". 
 Seven components make up the TAS:
-•	Allocation Transfer Agency Identifier (ex. 089)
-•	Agency Identifier (ex. 020)
-•	Beginning Period of Availability (ex. 2017)
-•	Ending Period of Availability (ex. 2018)
-•	Availability Type Code (used if there are not specific beginning/ending years) (ex. X)
-•	Main Account Code (ex. 0114)
-•	Sub-Account Code (ex. 000)
+- Allocation Transfer Agency Identifier (ex. 089)
+- Agency Identifier (ex. 020)
+- Beginning Period of Availability (ex. 2017)
+- Ending Period of Availability (ex. 2018)
+- Availability Type Code (used if there are not specific beginning/ending years) (ex. X)
+- Main Account Code (ex. 0114)
+- Sub-Account Code (ex. 000)
 Example TAS:
-•	089-020-2017/2018-0114-000
-•	089-020-2017/2017-0114-000
-•	089-020-X-0114-000</t>
+- 089-020-2017/2018-0114-000
+- 089-020-2017/2017-0114-000
+- 089-020-X-0114-000</t>
   </si>
 </sst>
 </file>
@@ -2193,8 +2193,8 @@
   <dimension ref="A1:Y1029"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C127" sqref="C127"/>
+      <pane ySplit="1" topLeftCell="A127" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B115" sqref="B115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4371,7 +4371,7 @@
       <c r="E126" s="8"/>
       <c r="F126" s="12"/>
     </row>
-    <row r="127" spans="1:6" s="11" customFormat="1" ht="332" x14ac:dyDescent="0.15">
+    <row r="127" spans="1:6" s="11" customFormat="1" ht="358" x14ac:dyDescent="0.15">
       <c r="A127" s="8" t="s">
         <v>198</v>
       </c>

</xml_diff>

<commit_message>
[DEV-3350] Added fed acct details
</commit_message>
<xml_diff>
--- a/usaspending_api/data/USAspendingGlossary.xlsx
+++ b/usaspending_api/data/USAspendingGlossary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emilybrents/Documents/data_act/usaspending-api/usaspending_api/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{162CA111-C088-584C-A59E-57EC0718DC98}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE6D3C93-C5C5-0145-9499-31546EA7FF48}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="429">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="431">
   <si>
     <t>Term</t>
   </si>
@@ -1630,6 +1630,14 @@
   </si>
   <si>
     <t>This is a component of the TAS. Identifies a Treasury-defined subdivision of the main account. This field cannot be blank. Sub Account 000 indicates the Parent account.</t>
+  </si>
+  <si>
+    <t>See also:
+Federal Account</t>
+  </si>
+  <si>
+    <t>See also:
+- [Federal Account](?glossary=federal-account)</t>
   </si>
 </sst>
 </file>
@@ -2198,9 +2206,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y1029"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D121" sqref="D121"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="125" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A127" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E127" sqref="E127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4390,8 +4398,12 @@
       <c r="D127" s="8" t="s">
         <v>240</v>
       </c>
-      <c r="E127" s="8"/>
-      <c r="F127" s="12"/>
+      <c r="E127" s="8" t="s">
+        <v>429</v>
+      </c>
+      <c r="F127" s="12" t="s">
+        <v>430</v>
+      </c>
     </row>
     <row r="128" spans="1:6" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A128" s="8" t="s">
@@ -4409,7 +4421,7 @@
       <c r="E128" s="8"/>
       <c r="F128" s="12"/>
     </row>
-    <row r="129" spans="1:6" s="11" customFormat="1" ht="140" x14ac:dyDescent="0.15">
+    <row r="129" spans="1:6" s="11" customFormat="1" ht="126" x14ac:dyDescent="0.15">
       <c r="A129" s="8" t="s">
         <v>197</v>
       </c>

</xml_diff>

<commit_message>
[DEV-4524] updating glossary entry for PSC
</commit_message>
<xml_diff>
--- a/usaspending_api/data/USAspendingGlossary.xlsx
+++ b/usaspending_api/data/USAspendingGlossary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10308"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonathanhill/DATAACT/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maxkendall/DataAct/us/usaspending-api/usaspending_api/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74E09C0D-5F99-1D43-95E6-EACF8E7B8F31}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7DC5DE2-5A5D-8C48-BA0E-653D04730656}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="32700" windowHeight="18720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -541,9 +541,6 @@
   <si>
     <t>Two codes that together identify the program and weapons system or equipment purchased by a DOD agency. The first character is a number 1-4 that identifies the DOD component. The last 3 characters identify that  component's program, system, or equipment.
 [Read more about this code](https://www.fpds.gov/help/SystemEquipment.htm) on the General Services Administration website.</t>
-  </si>
-  <si>
-    <t>A Product and Service Code (PSC) is a 4-digit code that identifies the type of product or service purchased. While NAICS codes identify industry, PSCs tell you the type of product or service. PSCs start with 3 categories: Services, Products, and R&amp;D. They then break down into 100+ classes. PSCs contain both numbers and letters. They are more granular than NAICS codes: there are twice as many.</t>
   </si>
   <si>
     <t>Product or Service Code</t>
@@ -1797,6 +1794,13 @@
       </rPr>
       <t>](?glossary=record-type)</t>
     </r>
+  </si>
+  <si>
+    <t>A Product or Service Code (PSC) is a 4-character code that identifies the type of product, service, or research &amp; development (R&amp;D) purchased. While NAICS codes identify the industry most relevant to a contract, PSCs tell you what the contract is specifically purchasing. For example, a contract’s NAICS code might point to the “Industrial Building Construction” industry, while that same contract’s PSC points to “Construct Hospitals and Infirmaries.” There are nearly three times as many PSCs (over 2,900) as there are NAICS codes (just over 1000), which in many cases allows a more granular PSC designation than NAICS code designation for a given contract.
+All PSC are 4 characters long, but there is an embedded hierarchy in the codes. 
+R&amp;D: begin with ‘A’ (indicating R&amp;D), followed by a second letter, followed by a number, followed by a number (four levels of hierarchy). Example: AA11.
+Services: begin with ‘B’ to ‘Z’ (indicating the subcategory of Service), followed by a number, followed by two letters (four levels of hierarchy if you include the “Service” designation). Example: C1AA
+Products: begin with two numbers (indicating the subcategory of Product), followed by two more numbers (three levels of hierarchy if you include the “Product” designation). Example: 1005</t>
   </si>
 </sst>
 </file>
@@ -2381,8 +2385,8 @@
   <dimension ref="A1:Y1030"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A115" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D116" sqref="D116"/>
+      <pane ySplit="1" topLeftCell="A105" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B105" sqref="B105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2437,52 +2441,52 @@
     </row>
     <row r="2" spans="1:25" s="11" customFormat="1" ht="140" x14ac:dyDescent="0.15">
       <c r="A2" s="8" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="3" spans="1:25" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>241</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>242</v>
-      </c>
       <c r="C3" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>241</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>242</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="12"/>
     </row>
     <row r="4" spans="1:25" s="11" customFormat="1" ht="112" x14ac:dyDescent="0.15">
       <c r="A4" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>308</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>243</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>309</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>243</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>244</v>
       </c>
       <c r="E4" s="8"/>
       <c r="F4" s="12"/>
@@ -2492,13 +2496,13 @@
         <v>6</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E5" s="8"/>
       <c r="F5" s="12"/>
@@ -2558,13 +2562,13 @@
         <v>18</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="10" spans="1:25" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
@@ -2588,7 +2592,7 @@
         <v>22</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
@@ -2600,19 +2604,19 @@
         <v>23</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>24</v>
       </c>
       <c r="D12" s="8" t="s">
+        <v>310</v>
+      </c>
+      <c r="E12" s="8" t="s">
         <v>311</v>
       </c>
-      <c r="E12" s="8" t="s">
-        <v>312</v>
-      </c>
       <c r="F12" s="13" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="13" spans="1:25" s="11" customFormat="1" ht="56" x14ac:dyDescent="0.15">
@@ -2648,7 +2652,7 @@
         <v>33</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="15" spans="1:25" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
@@ -2659,42 +2663,42 @@
         <v>35</v>
       </c>
       <c r="C15" s="8" t="s">
+        <v>296</v>
+      </c>
+      <c r="D15" s="8" t="s">
         <v>297</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>298</v>
       </c>
       <c r="E15" s="8"/>
       <c r="F15" s="12"/>
     </row>
     <row r="16" spans="1:25" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A16" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C16" s="8" t="s">
+        <v>298</v>
+      </c>
+      <c r="D16" s="8" t="s">
         <v>299</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>300</v>
       </c>
       <c r="E16" s="8"/>
       <c r="F16" s="12"/>
     </row>
     <row r="17" spans="1:6" s="11" customFormat="1" ht="56" x14ac:dyDescent="0.15">
       <c r="A17" s="8" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C17" s="8" t="s">
+        <v>300</v>
+      </c>
+      <c r="D17" s="8" t="s">
         <v>301</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>302</v>
       </c>
       <c r="E17" s="8"/>
       <c r="F17" s="12"/>
@@ -2713,10 +2717,10 @@
         <v>38</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="19" spans="1:6" s="3" customFormat="1" ht="318" customHeight="1" x14ac:dyDescent="0.15">
@@ -2724,7 +2728,7 @@
         <v>39</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -2756,7 +2760,7 @@
         <v>45</v>
       </c>
       <c r="B21" s="24" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -2769,14 +2773,14 @@
     </row>
     <row r="22" spans="1:6" s="11" customFormat="1" ht="126" x14ac:dyDescent="0.15">
       <c r="A22" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="B22" s="8" t="s">
         <v>213</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>214</v>
       </c>
       <c r="C22" s="8"/>
       <c r="D22" s="8" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E22" s="14"/>
       <c r="F22" s="12"/>
@@ -2789,7 +2793,7 @@
         <v>49</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D23" s="8" t="s">
         <v>50</v>
@@ -2802,19 +2806,19 @@
         <v>15</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C24" s="8" t="s">
         <v>15</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="25" spans="1:6" s="11" customFormat="1" ht="112" x14ac:dyDescent="0.15">
@@ -2822,39 +2826,39 @@
         <v>51</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
       <c r="E25" s="9" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="F25" s="15" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="26" spans="1:6" s="11" customFormat="1" ht="168" x14ac:dyDescent="0.15">
       <c r="A26" s="8" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
       <c r="E26" s="9" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="F26" s="15" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="27" spans="1:6" s="11" customFormat="1" ht="98" x14ac:dyDescent="0.15">
       <c r="A27" s="8" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
@@ -2869,10 +2873,10 @@
         <v>57</v>
       </c>
       <c r="C28" s="8" t="s">
+        <v>290</v>
+      </c>
+      <c r="D28" s="8" t="s">
         <v>291</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>292</v>
       </c>
       <c r="E28" s="14" t="s">
         <v>58</v>
@@ -2899,16 +2903,16 @@
     </row>
     <row r="30" spans="1:6" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
       <c r="A30" s="8" t="s">
+        <v>374</v>
+      </c>
+      <c r="B30" s="8" t="s">
         <v>375</v>
       </c>
-      <c r="B30" s="8" t="s">
-        <v>376</v>
-      </c>
       <c r="C30" s="8" t="s">
+        <v>374</v>
+      </c>
+      <c r="D30" s="8" t="s">
         <v>375</v>
-      </c>
-      <c r="D30" s="8" t="s">
-        <v>376</v>
       </c>
       <c r="E30" s="14" t="s">
         <v>75</v>
@@ -2919,14 +2923,14 @@
     </row>
     <row r="31" spans="1:6" s="11" customFormat="1" ht="210" x14ac:dyDescent="0.15">
       <c r="A31" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="B31" s="8" t="s">
         <v>211</v>
-      </c>
-      <c r="B31" s="8" t="s">
-        <v>212</v>
       </c>
       <c r="C31" s="8"/>
       <c r="D31" s="8" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E31" s="14"/>
       <c r="F31" s="12"/>
@@ -2965,22 +2969,22 @@
     </row>
     <row r="34" spans="1:25" s="11" customFormat="1" ht="397" x14ac:dyDescent="0.15">
       <c r="A34" s="8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F34" s="12" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="35" spans="1:25" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
@@ -3004,7 +3008,7 @@
         <v>72</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C36" s="8" t="s">
         <v>73</v>
@@ -3036,10 +3040,10 @@
     </row>
     <row r="37" spans="1:25" s="11" customFormat="1" ht="255" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>394</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>395</v>
       </c>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
@@ -3083,26 +3087,26 @@
     </row>
     <row r="39" spans="1:25" s="11" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A39" s="8" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E39" s="8"/>
       <c r="F39" s="12"/>
     </row>
     <row r="40" spans="1:25" s="3" customFormat="1" ht="102" x14ac:dyDescent="0.15">
       <c r="A40" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>396</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>397</v>
       </c>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
@@ -3111,10 +3115,10 @@
     </row>
     <row r="41" spans="1:25" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A41" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="B41" s="8" t="s">
         <v>220</v>
-      </c>
-      <c r="B41" s="8" t="s">
-        <v>221</v>
       </c>
       <c r="C41" s="8"/>
       <c r="D41" s="8"/>
@@ -3123,32 +3127,32 @@
     </row>
     <row r="42" spans="1:25" s="11" customFormat="1" ht="112" x14ac:dyDescent="0.15">
       <c r="A42" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="B42" s="8" t="s">
         <v>222</v>
       </c>
-      <c r="B42" s="8" t="s">
-        <v>223</v>
-      </c>
       <c r="C42" s="8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E42" s="14"/>
       <c r="F42" s="12"/>
     </row>
     <row r="43" spans="1:25" s="11" customFormat="1" ht="98" x14ac:dyDescent="0.15">
       <c r="A43" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="B43" s="8" t="s">
         <v>224</v>
       </c>
-      <c r="B43" s="8" t="s">
-        <v>225</v>
-      </c>
       <c r="C43" s="8" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E43" s="14"/>
       <c r="F43" s="12"/>
@@ -3181,16 +3185,16 @@
         <v>87</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E45" s="8" t="s">
         <v>88</v>
       </c>
       <c r="F45" s="12" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="46" spans="1:25" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
@@ -3220,24 +3224,24 @@
         <v>94</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E47" s="9" t="s">
+        <v>364</v>
+      </c>
+      <c r="F47" s="12" t="s">
         <v>365</v>
-      </c>
-      <c r="F47" s="12" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="48" spans="1:25" s="11" customFormat="1" ht="98" x14ac:dyDescent="0.15">
       <c r="A48" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="B48" s="8" t="s">
         <v>284</v>
       </c>
-      <c r="B48" s="8" t="s">
-        <v>285</v>
-      </c>
       <c r="C48" s="8" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D48" s="8" t="s">
         <v>116</v>
@@ -3250,7 +3254,7 @@
         <v>95</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C49" s="8" t="s">
         <v>95</v>
@@ -3279,16 +3283,16 @@
     </row>
     <row r="51" spans="1:6" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A51" s="8" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E51" s="8"/>
       <c r="F51" s="12"/>
@@ -3310,7 +3314,7 @@
         <v>101</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
@@ -3335,16 +3339,16 @@
     </row>
     <row r="55" spans="1:6" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
       <c r="A55" s="8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E55" s="8"/>
       <c r="F55" s="12"/>
@@ -3357,20 +3361,20 @@
         <v>109</v>
       </c>
       <c r="C56" s="8" t="s">
+        <v>302</v>
+      </c>
+      <c r="D56" s="8" t="s">
         <v>303</v>
-      </c>
-      <c r="D56" s="8" t="s">
-        <v>304</v>
       </c>
       <c r="E56" s="8"/>
       <c r="F56" s="12"/>
     </row>
     <row r="57" spans="1:6" s="11" customFormat="1" ht="112" x14ac:dyDescent="0.15">
       <c r="A57" s="8" t="s">
+        <v>328</v>
+      </c>
+      <c r="B57" s="8" t="s">
         <v>329</v>
-      </c>
-      <c r="B57" s="8" t="s">
-        <v>330</v>
       </c>
       <c r="C57" s="8" t="s">
         <v>135</v>
@@ -3383,42 +3387,42 @@
     </row>
     <row r="58" spans="1:6" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A58" s="8" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E58" s="8"/>
       <c r="F58" s="12"/>
     </row>
     <row r="59" spans="1:6" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
       <c r="A59" s="8" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C59" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="D59" s="8" t="s">
         <v>306</v>
-      </c>
-      <c r="D59" s="8" t="s">
-        <v>307</v>
       </c>
       <c r="E59" s="8"/>
       <c r="F59" s="12"/>
     </row>
     <row r="60" spans="1:6" s="3" customFormat="1" ht="238" x14ac:dyDescent="0.15">
       <c r="A60" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B60" s="24" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
@@ -3431,46 +3435,46 @@
     </row>
     <row r="61" spans="1:6" s="11" customFormat="1" ht="196" x14ac:dyDescent="0.15">
       <c r="A61" s="8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E61" s="14"/>
       <c r="F61" s="12"/>
     </row>
     <row r="62" spans="1:6" s="11" customFormat="1" ht="154" x14ac:dyDescent="0.15">
       <c r="A62" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C62" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E62" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F62" s="10" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="63" spans="1:6" s="3" customFormat="1" ht="119" x14ac:dyDescent="0.15">
       <c r="A63" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
@@ -3479,42 +3483,42 @@
     </row>
     <row r="64" spans="1:6" s="11" customFormat="1" ht="238" x14ac:dyDescent="0.15">
       <c r="A64" s="8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E64" s="8"/>
       <c r="F64" s="12"/>
     </row>
     <row r="65" spans="1:25" s="11" customFormat="1" ht="140" x14ac:dyDescent="0.15">
       <c r="A65" s="8" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E65" s="8"/>
       <c r="F65" s="12"/>
     </row>
     <row r="66" spans="1:25" s="3" customFormat="1" ht="85" x14ac:dyDescent="0.15">
       <c r="A66" s="30" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
@@ -3523,10 +3527,10 @@
     </row>
     <row r="67" spans="1:25" s="1" customFormat="1" ht="175" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A67" s="27" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B67" s="29" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C67" s="27"/>
       <c r="E67" s="1" t="s">
@@ -3557,10 +3561,10 @@
     </row>
     <row r="68" spans="1:25" s="11" customFormat="1" ht="170" x14ac:dyDescent="0.15">
       <c r="A68" s="26" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B68" s="25" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C68" s="28"/>
       <c r="D68" s="1"/>
@@ -3588,10 +3592,10 @@
     </row>
     <row r="69" spans="1:25" s="3" customFormat="1" ht="170" x14ac:dyDescent="0.15">
       <c r="A69" s="1" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
@@ -3600,7 +3604,7 @@
     </row>
     <row r="70" spans="1:25" s="3" customFormat="1" ht="140" x14ac:dyDescent="0.15">
       <c r="A70" s="8" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B70" s="8" t="s">
         <v>113</v>
@@ -3635,10 +3639,10 @@
     </row>
     <row r="71" spans="1:25" s="3" customFormat="1" ht="119" x14ac:dyDescent="0.15">
       <c r="A71" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="B71" s="1" t="s">
         <v>405</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>406</v>
       </c>
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
@@ -3647,16 +3651,16 @@
     </row>
     <row r="72" spans="1:25" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
       <c r="A72" s="8" t="s">
+        <v>371</v>
+      </c>
+      <c r="B72" s="8" t="s">
         <v>372</v>
       </c>
-      <c r="B72" s="8" t="s">
-        <v>373</v>
-      </c>
       <c r="C72" s="8" t="s">
+        <v>371</v>
+      </c>
+      <c r="D72" s="8" t="s">
         <v>372</v>
-      </c>
-      <c r="D72" s="8" t="s">
-        <v>373</v>
       </c>
       <c r="E72" s="14" t="s">
         <v>127</v>
@@ -3667,26 +3671,26 @@
     </row>
     <row r="73" spans="1:25" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
       <c r="A73" s="8" t="s">
+        <v>322</v>
+      </c>
+      <c r="B73" s="8" t="s">
         <v>323</v>
       </c>
-      <c r="B73" s="8" t="s">
-        <v>324</v>
-      </c>
       <c r="C73" s="8" t="s">
+        <v>322</v>
+      </c>
+      <c r="D73" s="8" t="s">
         <v>323</v>
-      </c>
-      <c r="D73" s="8" t="s">
-        <v>324</v>
       </c>
       <c r="E73" s="8"/>
       <c r="F73" s="12"/>
     </row>
     <row r="74" spans="1:25" s="11" customFormat="1" ht="98" x14ac:dyDescent="0.15">
       <c r="A74" s="8" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C74" s="8"/>
       <c r="D74" s="8"/>
@@ -3727,46 +3731,46 @@
     </row>
     <row r="77" spans="1:25" s="11" customFormat="1" ht="98" x14ac:dyDescent="0.15">
       <c r="A77" s="8" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C77" s="8" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D77" s="8" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E77" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="F77" s="12" t="s">
         <v>199</v>
-      </c>
-      <c r="F77" s="12" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="78" spans="1:25" s="11" customFormat="1" ht="277.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A78" s="8" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B78" s="8" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C78" s="8" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D78" s="8" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E78" s="8"/>
       <c r="F78" s="12"/>
     </row>
     <row r="79" spans="1:25" s="3" customFormat="1" ht="277.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A79" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="B79" s="1" t="s">
         <v>407</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>408</v>
       </c>
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
@@ -3791,16 +3795,16 @@
     </row>
     <row r="81" spans="1:25" s="11" customFormat="1" ht="224" x14ac:dyDescent="0.15">
       <c r="A81" s="8" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B81" s="35" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C81" s="8"/>
       <c r="D81" s="8"/>
       <c r="E81" s="14"/>
       <c r="F81" s="12" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="82" spans="1:25" s="11" customFormat="1" ht="126" x14ac:dyDescent="0.15">
@@ -3811,10 +3815,10 @@
         <v>130</v>
       </c>
       <c r="C82" s="8" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D82" s="8" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E82" s="14" t="s">
         <v>131</v>
@@ -3825,16 +3829,16 @@
     </row>
     <row r="83" spans="1:25" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
       <c r="A83" s="8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B83" s="8" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C83" s="8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D83" s="8" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E83" s="8"/>
       <c r="F83" s="12"/>
@@ -3850,13 +3854,13 @@
         <v>133</v>
       </c>
       <c r="D84" s="8" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E84" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F84" s="12" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="85" spans="1:25" s="11" customFormat="1" ht="409.6" x14ac:dyDescent="0.15">
@@ -3870,23 +3874,23 @@
         <v>137</v>
       </c>
       <c r="D85" s="8" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E85" s="8"/>
       <c r="F85" s="12"/>
     </row>
     <row r="86" spans="1:25" s="11" customFormat="1" ht="140" x14ac:dyDescent="0.15">
       <c r="A86" s="8" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B86" s="8" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C86" s="8" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D86" s="8" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E86" s="8"/>
       <c r="F86" s="12"/>
@@ -3902,17 +3906,17 @@
         <v>139</v>
       </c>
       <c r="D87" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E87" s="8"/>
       <c r="F87" s="12"/>
     </row>
     <row r="88" spans="1:25" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A88" s="8" t="s">
+        <v>408</v>
+      </c>
+      <c r="B88" s="8" t="s">
         <v>409</v>
-      </c>
-      <c r="B88" s="8" t="s">
-        <v>410</v>
       </c>
       <c r="C88" s="8"/>
       <c r="D88" s="8"/>
@@ -3921,22 +3925,22 @@
     </row>
     <row r="89" spans="1:25" s="3" customFormat="1" ht="154" x14ac:dyDescent="0.15">
       <c r="A89" s="8" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B89" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C89" s="8" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D89" s="16" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E89" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F89" s="17" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="G89" s="11"/>
       <c r="H89" s="11"/>
@@ -3960,10 +3964,10 @@
     </row>
     <row r="90" spans="1:25" s="11" customFormat="1" ht="323" x14ac:dyDescent="0.15">
       <c r="A90" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B90" s="24" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C90" s="1"/>
       <c r="D90" s="1"/>
@@ -3998,133 +4002,133 @@
         <v>143</v>
       </c>
       <c r="B91" s="8" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C91" s="8" t="s">
         <v>144</v>
       </c>
       <c r="D91" s="8" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E91" s="8"/>
       <c r="F91" s="12"/>
     </row>
     <row r="92" spans="1:25" s="11" customFormat="1" ht="56" x14ac:dyDescent="0.15">
       <c r="A92" s="8" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B92" s="8" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C92" s="8" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D92" s="8" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E92" s="8"/>
       <c r="F92" s="12"/>
     </row>
     <row r="93" spans="1:25" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
       <c r="A93" s="8" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B93" s="8" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C93" s="8" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D93" s="8" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E93" s="8" t="s">
         <v>88</v>
       </c>
       <c r="F93" s="12" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="94" spans="1:25" s="11" customFormat="1" ht="98" x14ac:dyDescent="0.15">
       <c r="A94" s="8" t="s">
+        <v>324</v>
+      </c>
+      <c r="B94" s="8" t="s">
         <v>325</v>
       </c>
-      <c r="B94" s="8" t="s">
-        <v>326</v>
-      </c>
       <c r="C94" s="8" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D94" s="8" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E94" s="8"/>
       <c r="F94" s="12"/>
     </row>
     <row r="95" spans="1:25" s="11" customFormat="1" ht="126" x14ac:dyDescent="0.15">
       <c r="A95" s="8" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B95" s="8" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C95" s="8" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D95" s="8" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E95" s="8"/>
       <c r="F95" s="12"/>
     </row>
     <row r="96" spans="1:25" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A96" s="8" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B96" s="8" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C96" s="8" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D96" s="8" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E96" s="8"/>
       <c r="F96" s="12"/>
     </row>
     <row r="97" spans="1:6" s="11" customFormat="1" ht="358" x14ac:dyDescent="0.15">
       <c r="A97" s="8" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B97" s="8" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C97" s="8" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D97" s="8" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E97" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F97" s="10" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="98" spans="1:6" s="11" customFormat="1" ht="98" x14ac:dyDescent="0.15">
       <c r="A98" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="B98" s="8" t="s">
         <v>281</v>
-      </c>
-      <c r="B98" s="8" t="s">
-        <v>282</v>
       </c>
       <c r="C98" s="8" t="s">
         <v>25</v>
       </c>
       <c r="D98" s="8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E98" s="8"/>
       <c r="F98" s="12"/>
@@ -4137,70 +4141,70 @@
         <v>146</v>
       </c>
       <c r="C99" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D99" s="31" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="E99" s="8"/>
       <c r="F99" s="12"/>
     </row>
     <row r="100" spans="1:6" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
       <c r="A100" s="8" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B100" s="8" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C100" s="8" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D100" s="8" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E100" s="8"/>
       <c r="F100" s="12"/>
     </row>
     <row r="101" spans="1:6" s="11" customFormat="1" ht="56" x14ac:dyDescent="0.15">
       <c r="A101" s="8" t="s">
+        <v>352</v>
+      </c>
+      <c r="B101" s="8" t="s">
         <v>353</v>
       </c>
-      <c r="B101" s="8" t="s">
-        <v>354</v>
-      </c>
       <c r="C101" s="8" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D101" s="8" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E101" s="8"/>
       <c r="F101" s="12"/>
     </row>
     <row r="102" spans="1:6" s="11" customFormat="1" ht="112" x14ac:dyDescent="0.15">
       <c r="A102" s="18" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B102" s="8" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C102" s="8"/>
       <c r="D102" s="8" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E102" s="8"/>
       <c r="F102" s="12"/>
     </row>
     <row r="103" spans="1:6" s="11" customFormat="1" ht="126" x14ac:dyDescent="0.15">
       <c r="A103" s="8" t="s">
+        <v>387</v>
+      </c>
+      <c r="B103" s="8" t="s">
         <v>388</v>
-      </c>
-      <c r="B103" s="8" t="s">
-        <v>389</v>
       </c>
       <c r="C103" s="8"/>
       <c r="D103" s="8" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E103" s="8"/>
       <c r="F103" s="12"/>
@@ -4216,29 +4220,29 @@
         <v>147</v>
       </c>
       <c r="D104" s="8" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E104" s="8"/>
       <c r="F104" s="12"/>
     </row>
-    <row r="105" spans="1:6" s="11" customFormat="1" ht="112" x14ac:dyDescent="0.15">
+    <row r="105" spans="1:6" s="11" customFormat="1" ht="384" x14ac:dyDescent="0.15">
       <c r="A105" s="8" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B105" s="8" t="s">
+        <v>435</v>
+      </c>
+      <c r="C105" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="C105" s="8" t="s">
+      <c r="D105" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="D105" s="8" t="s">
+      <c r="E105" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="E105" s="14" t="s">
+      <c r="F105" s="12" t="s">
         <v>159</v>
-      </c>
-      <c r="F105" s="12" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="106" spans="1:6" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
@@ -4252,7 +4256,7 @@
         <v>151</v>
       </c>
       <c r="D106" s="8" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E106" s="8"/>
       <c r="F106" s="12"/>
@@ -4275,26 +4279,26 @@
     </row>
     <row r="108" spans="1:6" s="11" customFormat="1" ht="56" x14ac:dyDescent="0.15">
       <c r="A108" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="B108" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="B108" s="8" t="s">
-        <v>217</v>
-      </c>
       <c r="C108" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D108" s="8" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E108" s="8"/>
       <c r="F108" s="12"/>
     </row>
     <row r="109" spans="1:6" s="3" customFormat="1" ht="85" x14ac:dyDescent="0.15">
       <c r="A109" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="B109" s="1" t="s">
         <v>412</v>
-      </c>
-      <c r="B109" s="1" t="s">
-        <v>413</v>
       </c>
       <c r="C109" s="1"/>
       <c r="D109" s="1"/>
@@ -4303,26 +4307,26 @@
     </row>
     <row r="110" spans="1:6" s="11" customFormat="1" ht="112" x14ac:dyDescent="0.15">
       <c r="A110" s="8" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B110" s="8" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C110" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="D110" s="8" t="s">
         <v>243</v>
-      </c>
-      <c r="D110" s="8" t="s">
-        <v>244</v>
       </c>
       <c r="E110" s="8"/>
       <c r="F110" s="12"/>
     </row>
     <row r="111" spans="1:6" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A111" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="B111" s="8" t="s">
         <v>161</v>
-      </c>
-      <c r="B111" s="8" t="s">
-        <v>162</v>
       </c>
       <c r="C111" s="8"/>
       <c r="D111" s="8"/>
@@ -4331,146 +4335,146 @@
     </row>
     <row r="112" spans="1:6" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A112" s="8" t="s">
+        <v>320</v>
+      </c>
+      <c r="B112" s="8" t="s">
         <v>321</v>
       </c>
-      <c r="B112" s="8" t="s">
-        <v>322</v>
-      </c>
       <c r="C112" s="8" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D112" s="8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E112" s="8"/>
       <c r="F112" s="12"/>
     </row>
     <row r="113" spans="1:6" s="11" customFormat="1" ht="112" x14ac:dyDescent="0.15">
       <c r="A113" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="B113" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="B113" s="8" t="s">
+      <c r="C113" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="C113" s="8" t="s">
-        <v>170</v>
-      </c>
       <c r="D113" s="8" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E113" s="8"/>
       <c r="F113" s="12"/>
     </row>
     <row r="114" spans="1:6" s="11" customFormat="1" ht="126" x14ac:dyDescent="0.15">
       <c r="A114" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="B114" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="B114" s="8" t="s">
+      <c r="C114" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="C114" s="8" t="s">
+      <c r="D114" s="8" t="s">
         <v>173</v>
-      </c>
-      <c r="D114" s="8" t="s">
-        <v>174</v>
       </c>
       <c r="E114" s="8"/>
       <c r="F114" s="12"/>
     </row>
     <row r="115" spans="1:6" s="11" customFormat="1" ht="252" x14ac:dyDescent="0.15">
       <c r="A115" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="B115" s="8" t="s">
+        <v>286</v>
+      </c>
+      <c r="C115" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="B115" s="8" t="s">
-        <v>287</v>
-      </c>
-      <c r="C115" s="8" t="s">
+      <c r="D115" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="D115" s="8" t="s">
+      <c r="E115" s="14" t="s">
         <v>165</v>
       </c>
-      <c r="E115" s="14" t="s">
+      <c r="F115" s="12" t="s">
         <v>166</v>
-      </c>
-      <c r="F115" s="12" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="116" spans="1:6" s="11" customFormat="1" ht="80" x14ac:dyDescent="0.15">
       <c r="A116" s="8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B116" s="35" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C116" s="8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D116" s="35" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E116" s="8"/>
       <c r="F116" s="12" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="117" spans="1:6" s="11" customFormat="1" ht="144" x14ac:dyDescent="0.15">
       <c r="A117" s="8" t="s">
+        <v>429</v>
+      </c>
+      <c r="B117" s="35" t="s">
         <v>430</v>
-      </c>
-      <c r="B117" s="35" t="s">
-        <v>431</v>
       </c>
       <c r="C117" s="8"/>
       <c r="D117" s="33"/>
       <c r="E117" s="8"/>
       <c r="F117" s="34" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="118" spans="1:6" s="11" customFormat="1" ht="84" x14ac:dyDescent="0.15">
       <c r="A118" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="B118" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="B118" s="8" t="s">
+      <c r="C118" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="C118" s="8" t="s">
+      <c r="D118" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="D118" s="8" t="s">
+      <c r="E118" s="14" t="s">
         <v>178</v>
       </c>
-      <c r="E118" s="14" t="s">
+      <c r="F118" s="12" t="s">
         <v>179</v>
-      </c>
-      <c r="F118" s="12" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="119" spans="1:6" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A119" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="B119" s="8" t="s">
         <v>181</v>
-      </c>
-      <c r="B119" s="8" t="s">
-        <v>182</v>
       </c>
       <c r="C119" s="8"/>
       <c r="D119" s="8"/>
       <c r="E119" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="F119" s="12" t="s">
         <v>183</v>
-      </c>
-      <c r="F119" s="12" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="120" spans="1:6" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
       <c r="A120" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="B120" s="8" t="s">
         <v>185</v>
-      </c>
-      <c r="B120" s="8" t="s">
-        <v>186</v>
       </c>
       <c r="C120" s="8"/>
       <c r="D120" s="8"/>
@@ -4479,10 +4483,10 @@
     </row>
     <row r="121" spans="1:6" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A121" s="8" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B121" s="8" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C121" s="8"/>
       <c r="D121" s="8"/>
@@ -4491,70 +4495,70 @@
     </row>
     <row r="122" spans="1:6" s="11" customFormat="1" ht="84" x14ac:dyDescent="0.15">
       <c r="A122" s="8" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B122" s="32" t="s">
+        <v>422</v>
+      </c>
+      <c r="C122" s="8" t="s">
         <v>423</v>
       </c>
-      <c r="C122" s="8" t="s">
-        <v>424</v>
-      </c>
       <c r="D122" s="8" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="E122" s="8"/>
       <c r="F122" s="12"/>
     </row>
     <row r="123" spans="1:6" s="11" customFormat="1" ht="126" x14ac:dyDescent="0.15">
       <c r="A123" s="8" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B123" s="19" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C123" s="8"/>
       <c r="D123" s="19" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E123" s="8"/>
       <c r="F123" s="12"/>
     </row>
     <row r="124" spans="1:6" s="11" customFormat="1" ht="224" x14ac:dyDescent="0.15">
       <c r="A124" s="8" t="s">
+        <v>381</v>
+      </c>
+      <c r="B124" s="8" t="s">
         <v>382</v>
-      </c>
-      <c r="B124" s="8" t="s">
-        <v>383</v>
       </c>
       <c r="C124" s="8"/>
       <c r="D124" s="20" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E124" s="8"/>
       <c r="F124" s="12"/>
     </row>
     <row r="125" spans="1:6" s="11" customFormat="1" ht="224" x14ac:dyDescent="0.15">
       <c r="A125" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="B125" s="8" t="s">
         <v>187</v>
       </c>
-      <c r="B125" s="8" t="s">
+      <c r="C125" s="8" t="s">
         <v>188</v>
       </c>
-      <c r="C125" s="8" t="s">
+      <c r="D125" s="8" t="s">
         <v>189</v>
-      </c>
-      <c r="D125" s="8" t="s">
-        <v>190</v>
       </c>
       <c r="E125" s="8"/>
       <c r="F125" s="12"/>
     </row>
     <row r="126" spans="1:6" s="11" customFormat="1" ht="84" x14ac:dyDescent="0.15">
       <c r="A126" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="B126" s="8" t="s">
         <v>191</v>
-      </c>
-      <c r="B126" s="8" t="s">
-        <v>192</v>
       </c>
       <c r="C126" s="8"/>
       <c r="D126" s="8"/>
@@ -4562,15 +4566,15 @@
         <v>79</v>
       </c>
       <c r="F126" s="12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="127" spans="1:6" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A127" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="B127" s="8" t="s">
         <v>194</v>
-      </c>
-      <c r="B127" s="8" t="s">
-        <v>195</v>
       </c>
       <c r="C127" s="8"/>
       <c r="D127" s="8"/>
@@ -4579,62 +4583,62 @@
     </row>
     <row r="128" spans="1:6" s="11" customFormat="1" ht="358" x14ac:dyDescent="0.15">
       <c r="A128" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B128" s="8" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C128" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="D128" s="8" t="s">
         <v>239</v>
       </c>
-      <c r="D128" s="8" t="s">
-        <v>240</v>
-      </c>
       <c r="E128" s="8" t="s">
+        <v>426</v>
+      </c>
+      <c r="F128" s="12" t="s">
         <v>427</v>
-      </c>
-      <c r="F128" s="12" t="s">
-        <v>428</v>
       </c>
     </row>
     <row r="129" spans="1:6" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A129" s="8" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B129" s="8" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C129" s="8" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D129" s="8" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E129" s="8"/>
       <c r="F129" s="12"/>
     </row>
     <row r="130" spans="1:6" s="11" customFormat="1" ht="140" x14ac:dyDescent="0.15">
       <c r="A130" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="B130" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="B130" s="8" t="s">
-        <v>198</v>
-      </c>
       <c r="C130" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D130" s="8" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E130" s="8"/>
       <c r="F130" s="12"/>
     </row>
     <row r="131" spans="1:6" s="11" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A131" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="B131" s="8" t="s">
         <v>218</v>
-      </c>
-      <c r="B131" s="8" t="s">
-        <v>219</v>
       </c>
       <c r="C131" s="8"/>
       <c r="D131" s="8"/>

</xml_diff>

<commit_message>
[DEV-4524] Adding necessary format to workbook
</commit_message>
<xml_diff>
--- a/usaspending_api/data/USAspendingGlossary.xlsx
+++ b/usaspending_api/data/USAspendingGlossary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10413"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maxkendall/DataAct/us/usaspending-api/usaspending_api/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7DC5DE2-5A5D-8C48-BA0E-653D04730656}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DE6FA3D-39BE-CA4F-A5E7-2163F36A9868}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="32700" windowHeight="18720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1798,20 +1798,27 @@
   <si>
     <t>A Product or Service Code (PSC) is a 4-character code that identifies the type of product, service, or research &amp; development (R&amp;D) purchased. While NAICS codes identify the industry most relevant to a contract, PSCs tell you what the contract is specifically purchasing. For example, a contract’s NAICS code might point to the “Industrial Building Construction” industry, while that same contract’s PSC points to “Construct Hospitals and Infirmaries.” There are nearly three times as many PSCs (over 2,900) as there are NAICS codes (just over 1000), which in many cases allows a more granular PSC designation than NAICS code designation for a given contract.
 All PSC are 4 characters long, but there is an embedded hierarchy in the codes. 
-R&amp;D: begin with ‘A’ (indicating R&amp;D), followed by a second letter, followed by a number, followed by a number (four levels of hierarchy). Example: AA11.
-Services: begin with ‘B’ to ‘Z’ (indicating the subcategory of Service), followed by a number, followed by two letters (four levels of hierarchy if you include the “Service” designation). Example: C1AA
-Products: begin with two numbers (indicating the subcategory of Product), followed by two more numbers (three levels of hierarchy if you include the “Product” designation). Example: 1005</t>
+- **R&amp;D**: begin with ‘A’ (indicating R&amp;D), followed by a second letter, followed by a number, followed by a number (four levels of hierarchy). Example: AA11.
+- **Services**: begin with ‘B’ to ‘Z’ (indicating the subcategory of Service), followed by a number, followed by two letters (four levels of hierarchy if you include the “Service” designation). Example: C1AA
+- **Products**: begin with two numbers (indicating the subcategory of Product), followed by two more numbers (three levels of hierarchy if you include the “Product” designation). Example: 1005</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
@@ -1984,63 +1991,63 @@
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="1" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="1" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2052,50 +2059,53 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -2385,7 +2395,7 @@
   <dimension ref="A1:Y1030"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A105" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A103" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B105" sqref="B105"/>
     </sheetView>
   </sheetViews>
@@ -3421,7 +3431,7 @@
       <c r="A60" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="B60" s="24" t="s">
+      <c r="B60" s="36" t="s">
         <v>413</v>
       </c>
       <c r="C60" s="1"/>
@@ -3966,7 +3976,7 @@
       <c r="A90" s="1" t="s">
         <v>410</v>
       </c>
-      <c r="B90" s="24" t="s">
+      <c r="B90" s="36" t="s">
         <v>414</v>
       </c>
       <c r="C90" s="1"/>
@@ -4225,7 +4235,7 @@
       <c r="E104" s="8"/>
       <c r="F104" s="12"/>
     </row>
-    <row r="105" spans="1:6" s="11" customFormat="1" ht="384" x14ac:dyDescent="0.15">
+    <row r="105" spans="1:6" s="11" customFormat="1" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A105" s="8" t="s">
         <v>327</v>
       </c>

</xml_diff>

<commit_message>
[DEV-5119] Update glossary titles and URL
</commit_message>
<xml_diff>
--- a/usaspending_api/data/USAspendingGlossary.xlsx
+++ b/usaspending_api/data/USAspendingGlossary.xlsx
@@ -5,12 +5,12 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maxkendall/DataAct/us/usaspending-api/usaspending_api/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kirkbarden/Development/usaspending-api/usaspending_api/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DE6FA3D-39BE-CA4F-A5E7-2163F36A9868}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{925020FF-F4C7-6141-ACB4-61079926C48E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="32700" windowHeight="18720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -216,12 +216,6 @@
     <t>The Catalog of Federal Domestic Assistance (CFDA) provides a full listing of federal programs that are available to organizations, government agencies (state, local, tribal), U.S. territories, and individuals who are authorized to do business with the government. A CFDA program can be a project, service, or activity. Each CFDA program has a unique, 5-digit number in the form of XX.XXX. The first two digits represent the funding agency. The last three digits represent the program.</t>
   </si>
   <si>
-    <t>https://www.cfda.gov/</t>
-  </si>
-  <si>
-    <t>[Visit the CFDA Website](https://www.cfda.gov/)</t>
-  </si>
-  <si>
     <t>Contract Pricing Type</t>
   </si>
   <si>
@@ -377,9 +371,6 @@
   </si>
   <si>
     <t>[Learn more from the GSA Acquisition Manual](https://www.acquisition.gov/gsam/current/html/Part538.html)</t>
-  </si>
-  <si>
-    <t>Federal Assistance</t>
   </si>
   <si>
     <t>A federal program, service, or activity that directly aids organizations, individuals, or state/local/tribal governments. Sectors include education, health, public safety and public welfare - to name a few. Financial assistance is distributed in many forms, including grants, loans, direct payments, or insurance.</t>
@@ -1140,9 +1131,6 @@
     <t xml:space="preserve">The date that the award begins. </t>
   </si>
   <si>
-    <t>Product/Service Code (PSC)</t>
-  </si>
-  <si>
     <t>Funding Obligated</t>
   </si>
   <si>
@@ -1801,6 +1789,18 @@
 - **R&amp;D**: begin with ‘A’ (indicating R&amp;D), followed by a second letter, followed by a number, followed by a number (four levels of hierarchy). Example: AA11.
 - **Services**: begin with ‘B’ to ‘Z’ (indicating the subcategory of Service), followed by a number, followed by two letters (four levels of hierarchy if you include the “Service” designation). Example: C1AA
 - **Products**: begin with two numbers (indicating the subcategory of Product), followed by two more numbers (three levels of hierarchy if you include the “Product” designation). Example: 1005</t>
+  </si>
+  <si>
+    <t>Financial Assistance</t>
+  </si>
+  <si>
+    <t>https://beta.sam.gov/help/assistance-listing</t>
+  </si>
+  <si>
+    <t>Product or Service Code (PSC)</t>
+  </si>
+  <si>
+    <t>[Visit the CFDA Website](https://beta.sam.gov/help/assistance-listing)</t>
   </si>
 </sst>
 </file>
@@ -2394,9 +2394,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y1030"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A103" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B105" sqref="B105"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="125" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2451,52 +2451,52 @@
     </row>
     <row r="2" spans="1:25" s="11" customFormat="1" ht="140" x14ac:dyDescent="0.15">
       <c r="A2" s="8" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
     </row>
     <row r="3" spans="1:25" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="12"/>
     </row>
     <row r="4" spans="1:25" s="11" customFormat="1" ht="112" x14ac:dyDescent="0.15">
       <c r="A4" s="8" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="E4" s="8"/>
       <c r="F4" s="12"/>
@@ -2506,13 +2506,13 @@
         <v>6</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="E5" s="8"/>
       <c r="F5" s="12"/>
@@ -2572,13 +2572,13 @@
         <v>18</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
     </row>
     <row r="10" spans="1:25" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
@@ -2602,7 +2602,7 @@
         <v>22</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
@@ -2614,19 +2614,19 @@
         <v>23</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>24</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
     </row>
     <row r="13" spans="1:25" s="11" customFormat="1" ht="56" x14ac:dyDescent="0.15">
@@ -2662,7 +2662,7 @@
         <v>33</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="15" spans="1:25" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
@@ -2673,42 +2673,42 @@
         <v>35</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="E15" s="8"/>
       <c r="F15" s="12"/>
     </row>
     <row r="16" spans="1:25" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A16" s="8" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="E16" s="8"/>
       <c r="F16" s="12"/>
     </row>
     <row r="17" spans="1:6" s="11" customFormat="1" ht="56" x14ac:dyDescent="0.15">
       <c r="A17" s="8" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="E17" s="8"/>
       <c r="F17" s="12"/>
@@ -2727,10 +2727,10 @@
         <v>38</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
     </row>
     <row r="19" spans="1:6" s="3" customFormat="1" ht="318" customHeight="1" x14ac:dyDescent="0.15">
@@ -2738,7 +2738,7 @@
         <v>39</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -2770,7 +2770,7 @@
         <v>45</v>
       </c>
       <c r="B21" s="24" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -2783,14 +2783,14 @@
     </row>
     <row r="22" spans="1:6" s="11" customFormat="1" ht="126" x14ac:dyDescent="0.15">
       <c r="A22" s="8" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C22" s="8"/>
       <c r="D22" s="8" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="E22" s="14"/>
       <c r="F22" s="12"/>
@@ -2803,7 +2803,7 @@
         <v>49</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="D23" s="8" t="s">
         <v>50</v>
@@ -2816,19 +2816,19 @@
         <v>15</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C24" s="8" t="s">
         <v>15</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
     </row>
     <row r="25" spans="1:6" s="11" customFormat="1" ht="112" x14ac:dyDescent="0.15">
@@ -2836,39 +2836,39 @@
         <v>51</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
       <c r="E25" s="9" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="F25" s="15" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
     </row>
     <row r="26" spans="1:6" s="11" customFormat="1" ht="168" x14ac:dyDescent="0.15">
       <c r="A26" s="8" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
       <c r="E26" s="9" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="F26" s="15" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
     </row>
     <row r="27" spans="1:6" s="11" customFormat="1" ht="98" x14ac:dyDescent="0.15">
       <c r="A27" s="8" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
@@ -2883,16 +2883,16 @@
         <v>57</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>291</v>
-      </c>
-      <c r="E28" s="14" t="s">
-        <v>58</v>
+        <v>288</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>433</v>
       </c>
       <c r="F28" s="12" t="s">
-        <v>59</v>
+        <v>435</v>
       </c>
     </row>
     <row r="29" spans="1:6" s="11" customFormat="1" ht="56" x14ac:dyDescent="0.15">
@@ -2913,64 +2913,64 @@
     </row>
     <row r="30" spans="1:6" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
       <c r="A30" s="8" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="E30" s="14" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F30" s="12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="31" spans="1:6" s="11" customFormat="1" ht="210" x14ac:dyDescent="0.15">
       <c r="A31" s="8" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C31" s="8"/>
       <c r="D31" s="8" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="E31" s="14"/>
       <c r="F31" s="12"/>
     </row>
     <row r="32" spans="1:6" s="11" customFormat="1" ht="266" x14ac:dyDescent="0.15">
       <c r="A32" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C32" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="D32" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="E32" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="D32" s="8" t="s">
+      <c r="F32" s="12" t="s">
         <v>63</v>
-      </c>
-      <c r="E32" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="F32" s="12" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="33" spans="1:25" s="11" customFormat="1" ht="140" x14ac:dyDescent="0.15">
       <c r="A33" s="8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
@@ -2979,52 +2979,52 @@
     </row>
     <row r="34" spans="1:25" s="11" customFormat="1" ht="397" x14ac:dyDescent="0.15">
       <c r="A34" s="8" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="F34" s="12" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
     </row>
     <row r="35" spans="1:25" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
       <c r="A35" s="8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C35" s="8"/>
       <c r="D35" s="8"/>
       <c r="E35" s="14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F35" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="36" spans="1:25" s="3" customFormat="1" ht="56" x14ac:dyDescent="0.15">
       <c r="A36" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>310</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="D36" s="8" t="s">
         <v>72</v>
-      </c>
-      <c r="B36" s="8" t="s">
-        <v>313</v>
-      </c>
-      <c r="C36" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="D36" s="8" t="s">
-        <v>74</v>
       </c>
       <c r="E36" s="8"/>
       <c r="F36" s="12"/>
@@ -3050,10 +3050,10 @@
     </row>
     <row r="37" spans="1:25" s="11" customFormat="1" ht="255" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
@@ -3081,42 +3081,42 @@
     </row>
     <row r="38" spans="1:25" s="11" customFormat="1" ht="84" x14ac:dyDescent="0.15">
       <c r="A38" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C38" s="8"/>
       <c r="D38" s="8"/>
       <c r="E38" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F38" s="12" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="39" spans="1:25" s="11" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A39" s="8" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="E39" s="8"/>
       <c r="F39" s="12"/>
     </row>
     <row r="40" spans="1:25" s="3" customFormat="1" ht="102" x14ac:dyDescent="0.15">
       <c r="A40" s="1" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
@@ -3125,10 +3125,10 @@
     </row>
     <row r="41" spans="1:25" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A41" s="8" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C41" s="8"/>
       <c r="D41" s="8"/>
@@ -3137,182 +3137,182 @@
     </row>
     <row r="42" spans="1:25" s="11" customFormat="1" ht="112" x14ac:dyDescent="0.15">
       <c r="A42" s="8" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="E42" s="14"/>
       <c r="F42" s="12"/>
     </row>
     <row r="43" spans="1:25" s="11" customFormat="1" ht="98" x14ac:dyDescent="0.15">
       <c r="A43" s="8" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="E43" s="14"/>
       <c r="F43" s="12"/>
     </row>
     <row r="44" spans="1:25" s="11" customFormat="1" ht="56" x14ac:dyDescent="0.15">
       <c r="A44" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D44" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="B44" s="8" t="s">
+      <c r="E44" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="C44" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="D44" s="8" t="s">
+      <c r="F44" s="12" t="s">
         <v>83</v>
-      </c>
-      <c r="E44" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="F44" s="12" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="45" spans="1:25" s="11" customFormat="1" ht="140" x14ac:dyDescent="0.15">
       <c r="A45" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="E45" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="B45" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="C45" s="8" t="s">
-        <v>267</v>
-      </c>
-      <c r="D45" s="8" t="s">
-        <v>272</v>
-      </c>
-      <c r="E45" s="8" t="s">
-        <v>88</v>
-      </c>
       <c r="F45" s="12" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
     </row>
     <row r="46" spans="1:25" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
       <c r="A46" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="D46" s="8" t="s">
         <v>89</v>
-      </c>
-      <c r="B46" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="C46" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="D46" s="8" t="s">
-        <v>91</v>
       </c>
       <c r="E46" s="8"/>
       <c r="F46" s="12"/>
     </row>
     <row r="47" spans="1:25" s="11" customFormat="1" ht="210" x14ac:dyDescent="0.15">
       <c r="A47" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="C47" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="B47" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="C47" s="8" t="s">
-        <v>94</v>
-      </c>
       <c r="D47" s="8" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="E47" s="9" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="F47" s="12" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
     </row>
     <row r="48" spans="1:25" s="11" customFormat="1" ht="98" x14ac:dyDescent="0.15">
       <c r="A48" s="8" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E48" s="8"/>
       <c r="F48" s="12"/>
     </row>
     <row r="49" spans="1:6" s="11" customFormat="1" ht="112" x14ac:dyDescent="0.15">
       <c r="A49" s="8" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E49" s="8"/>
       <c r="F49" s="12"/>
     </row>
     <row r="50" spans="1:6" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A50" s="8" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C50" s="8"/>
       <c r="D50" s="8"/>
       <c r="E50" s="14" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F50" s="12" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="51" spans="1:6" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A51" s="8" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="E51" s="8"/>
       <c r="F51" s="12"/>
     </row>
     <row r="52" spans="1:6" s="11" customFormat="1" ht="98" x14ac:dyDescent="0.15">
       <c r="A52" s="8" t="s">
-        <v>104</v>
+        <v>432</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C52" s="8"/>
       <c r="D52" s="8"/>
@@ -3321,26 +3321,26 @@
     </row>
     <row r="53" spans="1:6" s="3" customFormat="1" ht="85" x14ac:dyDescent="0.15">
       <c r="A53" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
       <c r="E53" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="54" spans="1:6" s="11" customFormat="1" ht="168" x14ac:dyDescent="0.15">
       <c r="A54" s="8" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C54" s="8"/>
       <c r="D54" s="8"/>
@@ -3349,142 +3349,142 @@
     </row>
     <row r="55" spans="1:6" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
       <c r="A55" s="8" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="E55" s="8"/>
       <c r="F55" s="12"/>
     </row>
     <row r="56" spans="1:6" s="11" customFormat="1" ht="84" x14ac:dyDescent="0.15">
       <c r="A56" s="8" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="E56" s="8"/>
       <c r="F56" s="12"/>
     </row>
     <row r="57" spans="1:6" s="11" customFormat="1" ht="112" x14ac:dyDescent="0.15">
       <c r="A57" s="8" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E57" s="8"/>
       <c r="F57" s="12"/>
     </row>
     <row r="58" spans="1:6" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A58" s="8" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="E58" s="8"/>
       <c r="F58" s="12"/>
     </row>
     <row r="59" spans="1:6" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
       <c r="A59" s="8" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="E59" s="8"/>
       <c r="F59" s="12"/>
     </row>
     <row r="60" spans="1:6" s="3" customFormat="1" ht="238" x14ac:dyDescent="0.15">
       <c r="A60" s="1" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="B60" s="36" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
       <c r="E60" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="61" spans="1:6" s="11" customFormat="1" ht="196" x14ac:dyDescent="0.15">
       <c r="A61" s="8" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="E61" s="14"/>
       <c r="F61" s="12"/>
     </row>
     <row r="62" spans="1:6" s="11" customFormat="1" ht="154" x14ac:dyDescent="0.15">
       <c r="A62" s="8" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="C62" s="8" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="E62" s="9" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="F62" s="10" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
     </row>
     <row r="63" spans="1:6" s="3" customFormat="1" ht="119" x14ac:dyDescent="0.15">
       <c r="A63" s="1" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
@@ -3493,42 +3493,42 @@
     </row>
     <row r="64" spans="1:6" s="11" customFormat="1" ht="238" x14ac:dyDescent="0.15">
       <c r="A64" s="8" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="E64" s="8"/>
       <c r="F64" s="12"/>
     </row>
     <row r="65" spans="1:25" s="11" customFormat="1" ht="140" x14ac:dyDescent="0.15">
       <c r="A65" s="8" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="E65" s="8"/>
       <c r="F65" s="12"/>
     </row>
     <row r="66" spans="1:25" s="3" customFormat="1" ht="85" x14ac:dyDescent="0.15">
       <c r="A66" s="30" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
@@ -3537,17 +3537,17 @@
     </row>
     <row r="67" spans="1:25" s="1" customFormat="1" ht="175" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A67" s="27" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="B67" s="29" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="C67" s="27"/>
       <c r="E67" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="G67" s="3"/>
       <c r="H67" s="3"/>
@@ -3571,10 +3571,10 @@
     </row>
     <row r="68" spans="1:25" s="11" customFormat="1" ht="170" x14ac:dyDescent="0.15">
       <c r="A68" s="26" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="B68" s="25" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="C68" s="28"/>
       <c r="D68" s="1"/>
@@ -3602,10 +3602,10 @@
     </row>
     <row r="69" spans="1:25" s="3" customFormat="1" ht="170" x14ac:dyDescent="0.15">
       <c r="A69" s="1" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
@@ -3614,18 +3614,18 @@
     </row>
     <row r="70" spans="1:25" s="3" customFormat="1" ht="140" x14ac:dyDescent="0.15">
       <c r="A70" s="8" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="B70" s="8" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C70" s="8"/>
       <c r="D70" s="8"/>
       <c r="E70" s="9" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="F70" s="12" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="G70" s="11"/>
       <c r="H70" s="11"/>
@@ -3649,10 +3649,10 @@
     </row>
     <row r="71" spans="1:25" s="3" customFormat="1" ht="119" x14ac:dyDescent="0.15">
       <c r="A71" s="1" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
@@ -3661,46 +3661,46 @@
     </row>
     <row r="72" spans="1:25" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
       <c r="A72" s="8" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="B72" s="8" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="C72" s="8" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="D72" s="8" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="E72" s="14" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="F72" s="12" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="73" spans="1:25" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
       <c r="A73" s="8" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="C73" s="8" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="D73" s="8" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="E73" s="8"/>
       <c r="F73" s="12"/>
     </row>
     <row r="74" spans="1:25" s="11" customFormat="1" ht="98" x14ac:dyDescent="0.15">
       <c r="A74" s="8" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="C74" s="8"/>
       <c r="D74" s="8"/>
@@ -3709,78 +3709,78 @@
     </row>
     <row r="75" spans="1:25" s="11" customFormat="1" ht="182" x14ac:dyDescent="0.15">
       <c r="A75" s="8" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B75" s="8" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C75" s="8" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D75" s="8" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E75" s="8"/>
       <c r="F75" s="12"/>
     </row>
     <row r="76" spans="1:25" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A76" s="8" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B76" s="8" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C76" s="8" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D76" s="8" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E76" s="8"/>
       <c r="F76" s="12"/>
     </row>
     <row r="77" spans="1:25" s="11" customFormat="1" ht="98" x14ac:dyDescent="0.15">
       <c r="A77" s="8" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="C77" s="8" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="D77" s="8" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="E77" s="14" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="F77" s="12" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="78" spans="1:25" s="11" customFormat="1" ht="277.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A78" s="8" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B78" s="8" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="C78" s="8" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="D78" s="8" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="E78" s="8"/>
       <c r="F78" s="12"/>
     </row>
     <row r="79" spans="1:25" s="3" customFormat="1" ht="277.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A79" s="1" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
@@ -3789,144 +3789,144 @@
     </row>
     <row r="80" spans="1:25" s="11" customFormat="1" ht="56" x14ac:dyDescent="0.15">
       <c r="A80" s="8" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B80" s="8" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C80" s="8"/>
       <c r="D80" s="8"/>
       <c r="E80" s="14" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="F80" s="12" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="81" spans="1:25" s="11" customFormat="1" ht="224" x14ac:dyDescent="0.15">
       <c r="A81" s="8" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B81" s="35" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="C81" s="8"/>
       <c r="D81" s="8"/>
       <c r="E81" s="14"/>
       <c r="F81" s="12" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
     </row>
     <row r="82" spans="1:25" s="11" customFormat="1" ht="126" x14ac:dyDescent="0.15">
       <c r="A82" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="B82" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C82" s="8" t="s">
+        <v>290</v>
+      </c>
+      <c r="D82" s="8" t="s">
+        <v>289</v>
+      </c>
+      <c r="E82" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="F82" s="12" t="s">
         <v>129</v>
-      </c>
-      <c r="B82" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="C82" s="8" t="s">
-        <v>293</v>
-      </c>
-      <c r="D82" s="8" t="s">
-        <v>292</v>
-      </c>
-      <c r="E82" s="14" t="s">
-        <v>131</v>
-      </c>
-      <c r="F82" s="12" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="83" spans="1:25" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
       <c r="A83" s="8" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B83" s="8" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="C83" s="8" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D83" s="8" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="E83" s="8"/>
       <c r="F83" s="12"/>
     </row>
     <row r="84" spans="1:25" s="11" customFormat="1" ht="84" x14ac:dyDescent="0.15">
       <c r="A84" s="8" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B84" s="8" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C84" s="8" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D84" s="8" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="E84" s="14" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="F84" s="12" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="85" spans="1:25" s="11" customFormat="1" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A85" s="8" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B85" s="8" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C85" s="8" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D85" s="8" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="E85" s="8"/>
       <c r="F85" s="12"/>
     </row>
     <row r="86" spans="1:25" s="11" customFormat="1" ht="140" x14ac:dyDescent="0.15">
       <c r="A86" s="8" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="B86" s="8" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C86" s="8" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="D86" s="8" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="E86" s="8"/>
       <c r="F86" s="12"/>
     </row>
     <row r="87" spans="1:25" s="11" customFormat="1" ht="112" x14ac:dyDescent="0.15">
       <c r="A87" s="8" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B87" s="8" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C87" s="8" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D87" s="8" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="E87" s="8"/>
       <c r="F87" s="12"/>
     </row>
     <row r="88" spans="1:25" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A88" s="8" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="B88" s="8" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="C88" s="8"/>
       <c r="D88" s="8"/>
@@ -3935,22 +3935,22 @@
     </row>
     <row r="89" spans="1:25" s="3" customFormat="1" ht="154" x14ac:dyDescent="0.15">
       <c r="A89" s="8" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="B89" s="8" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="C89" s="8" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="D89" s="16" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="E89" s="9" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="F89" s="17" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="G89" s="11"/>
       <c r="H89" s="11"/>
@@ -3974,18 +3974,18 @@
     </row>
     <row r="90" spans="1:25" s="11" customFormat="1" ht="323" x14ac:dyDescent="0.15">
       <c r="A90" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="B90" s="36" t="s">
         <v>410</v>
-      </c>
-      <c r="B90" s="36" t="s">
-        <v>414</v>
       </c>
       <c r="C90" s="1"/>
       <c r="D90" s="1"/>
       <c r="E90" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="G90" s="3"/>
       <c r="H90" s="3"/>
@@ -4009,306 +4009,306 @@
     </row>
     <row r="91" spans="1:25" s="11" customFormat="1" ht="154" x14ac:dyDescent="0.15">
       <c r="A91" s="8" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B91" s="8" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="C91" s="8" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D91" s="8" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="E91" s="8"/>
       <c r="F91" s="12"/>
     </row>
     <row r="92" spans="1:25" s="11" customFormat="1" ht="56" x14ac:dyDescent="0.15">
       <c r="A92" s="8" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="B92" s="8" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C92" s="8" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="D92" s="8" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="E92" s="8"/>
       <c r="F92" s="12"/>
     </row>
     <row r="93" spans="1:25" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
       <c r="A93" s="8" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="B93" s="8" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="C93" s="8" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="D93" s="8" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="E93" s="8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F93" s="12" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
     </row>
     <row r="94" spans="1:25" s="11" customFormat="1" ht="98" x14ac:dyDescent="0.15">
       <c r="A94" s="8" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="B94" s="8" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="C94" s="8" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="D94" s="8" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="E94" s="8"/>
       <c r="F94" s="12"/>
     </row>
     <row r="95" spans="1:25" s="11" customFormat="1" ht="126" x14ac:dyDescent="0.15">
       <c r="A95" s="8" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B95" s="8" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C95" s="8" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="D95" s="8" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="E95" s="8"/>
       <c r="F95" s="12"/>
     </row>
     <row r="96" spans="1:25" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A96" s="8" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B96" s="8" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="C96" s="8" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="D96" s="8" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="E96" s="8"/>
       <c r="F96" s="12"/>
     </row>
     <row r="97" spans="1:6" s="11" customFormat="1" ht="358" x14ac:dyDescent="0.15">
       <c r="A97" s="8" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B97" s="8" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="C97" s="8" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D97" s="8" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E97" s="9" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="F97" s="10" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
     </row>
     <row r="98" spans="1:6" s="11" customFormat="1" ht="98" x14ac:dyDescent="0.15">
       <c r="A98" s="8" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="B98" s="8" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C98" s="8" t="s">
         <v>25</v>
       </c>
       <c r="D98" s="8" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="E98" s="8"/>
       <c r="F98" s="12"/>
     </row>
     <row r="99" spans="1:6" s="11" customFormat="1" ht="56" x14ac:dyDescent="0.15">
       <c r="A99" s="8" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B99" s="8" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C99" s="8" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="D99" s="31" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="E99" s="8"/>
       <c r="F99" s="12"/>
     </row>
     <row r="100" spans="1:6" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
       <c r="A100" s="8" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B100" s="8" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="C100" s="8" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="D100" s="8" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="E100" s="8"/>
       <c r="F100" s="12"/>
     </row>
     <row r="101" spans="1:6" s="11" customFormat="1" ht="56" x14ac:dyDescent="0.15">
       <c r="A101" s="8" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="B101" s="8" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="C101" s="8" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="D101" s="8" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="E101" s="8"/>
       <c r="F101" s="12"/>
     </row>
     <row r="102" spans="1:6" s="11" customFormat="1" ht="112" x14ac:dyDescent="0.15">
       <c r="A102" s="18" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="B102" s="8" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="C102" s="8"/>
       <c r="D102" s="8" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="E102" s="8"/>
       <c r="F102" s="12"/>
     </row>
     <row r="103" spans="1:6" s="11" customFormat="1" ht="126" x14ac:dyDescent="0.15">
       <c r="A103" s="8" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="B103" s="8" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="C103" s="8"/>
       <c r="D103" s="8" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="E103" s="8"/>
       <c r="F103" s="12"/>
     </row>
     <row r="104" spans="1:6" s="11" customFormat="1" ht="84" x14ac:dyDescent="0.15">
       <c r="A104" s="8" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B104" s="8" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C104" s="8" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D104" s="8" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="E104" s="8"/>
       <c r="F104" s="12"/>
     </row>
     <row r="105" spans="1:6" s="11" customFormat="1" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A105" s="8" t="s">
-        <v>327</v>
+        <v>434</v>
       </c>
       <c r="B105" s="8" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="C105" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="D105" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E105" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="F105" s="12" t="s">
         <v>156</v>
-      </c>
-      <c r="D105" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="E105" s="14" t="s">
-        <v>158</v>
-      </c>
-      <c r="F105" s="12" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="106" spans="1:6" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
       <c r="A106" s="8" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B106" s="8" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C106" s="8" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D106" s="8" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="E106" s="8"/>
       <c r="F106" s="12"/>
     </row>
     <row r="107" spans="1:6" s="11" customFormat="1" ht="140" x14ac:dyDescent="0.15">
       <c r="A107" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="B107" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="C107" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="D107" s="8" t="s">
         <v>152</v>
-      </c>
-      <c r="B107" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="C107" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="D107" s="8" t="s">
-        <v>155</v>
       </c>
       <c r="E107" s="8"/>
       <c r="F107" s="12"/>
     </row>
     <row r="108" spans="1:6" s="11" customFormat="1" ht="56" x14ac:dyDescent="0.15">
       <c r="A108" s="8" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B108" s="8" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C108" s="8" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D108" s="8" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="E108" s="8"/>
       <c r="F108" s="12"/>
     </row>
     <row r="109" spans="1:6" s="3" customFormat="1" ht="85" x14ac:dyDescent="0.15">
       <c r="A109" s="1" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="C109" s="1"/>
       <c r="D109" s="1"/>
@@ -4317,26 +4317,26 @@
     </row>
     <row r="110" spans="1:6" s="11" customFormat="1" ht="112" x14ac:dyDescent="0.15">
       <c r="A110" s="8" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="B110" s="8" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="C110" s="8" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="D110" s="8" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="E110" s="8"/>
       <c r="F110" s="12"/>
     </row>
     <row r="111" spans="1:6" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A111" s="8" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B111" s="8" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C111" s="8"/>
       <c r="D111" s="8"/>
@@ -4345,146 +4345,146 @@
     </row>
     <row r="112" spans="1:6" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A112" s="8" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B112" s="8" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="C112" s="8" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D112" s="8" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="E112" s="8"/>
       <c r="F112" s="12"/>
     </row>
     <row r="113" spans="1:6" s="11" customFormat="1" ht="112" x14ac:dyDescent="0.15">
       <c r="A113" s="8" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B113" s="8" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C113" s="8" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D113" s="8" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="E113" s="8"/>
       <c r="F113" s="12"/>
     </row>
     <row r="114" spans="1:6" s="11" customFormat="1" ht="126" x14ac:dyDescent="0.15">
       <c r="A114" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="B114" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="C114" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="D114" s="8" t="s">
         <v>170</v>
-      </c>
-      <c r="B114" s="8" t="s">
-        <v>171</v>
-      </c>
-      <c r="C114" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="D114" s="8" t="s">
-        <v>173</v>
       </c>
       <c r="E114" s="8"/>
       <c r="F114" s="12"/>
     </row>
     <row r="115" spans="1:6" s="11" customFormat="1" ht="252" x14ac:dyDescent="0.15">
       <c r="A115" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="B115" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="C115" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="D115" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="E115" s="14" t="s">
         <v>162</v>
       </c>
-      <c r="B115" s="8" t="s">
-        <v>286</v>
-      </c>
-      <c r="C115" s="8" t="s">
+      <c r="F115" s="12" t="s">
         <v>163</v>
-      </c>
-      <c r="D115" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="E115" s="14" t="s">
-        <v>165</v>
-      </c>
-      <c r="F115" s="12" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="116" spans="1:6" s="11" customFormat="1" ht="80" x14ac:dyDescent="0.15">
       <c r="A116" s="8" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="B116" s="35" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="C116" s="8" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="D116" s="35" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="E116" s="8"/>
       <c r="F116" s="12" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
     </row>
     <row r="117" spans="1:6" s="11" customFormat="1" ht="144" x14ac:dyDescent="0.15">
       <c r="A117" s="8" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="B117" s="35" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="C117" s="8"/>
       <c r="D117" s="33"/>
       <c r="E117" s="8"/>
       <c r="F117" s="34" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
     </row>
     <row r="118" spans="1:6" s="11" customFormat="1" ht="84" x14ac:dyDescent="0.15">
       <c r="A118" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="B118" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="C118" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="D118" s="8" t="s">
         <v>174</v>
       </c>
-      <c r="B118" s="8" t="s">
+      <c r="E118" s="14" t="s">
         <v>175</v>
       </c>
-      <c r="C118" s="8" t="s">
+      <c r="F118" s="12" t="s">
         <v>176</v>
-      </c>
-      <c r="D118" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="E118" s="14" t="s">
-        <v>178</v>
-      </c>
-      <c r="F118" s="12" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="119" spans="1:6" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A119" s="8" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B119" s="8" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C119" s="8"/>
       <c r="D119" s="8"/>
       <c r="E119" s="14" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="F119" s="12" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="120" spans="1:6" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
       <c r="A120" s="8" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B120" s="8" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C120" s="8"/>
       <c r="D120" s="8"/>
@@ -4493,10 +4493,10 @@
     </row>
     <row r="121" spans="1:6" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A121" s="8" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B121" s="8" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="C121" s="8"/>
       <c r="D121" s="8"/>
@@ -4505,86 +4505,86 @@
     </row>
     <row r="122" spans="1:6" s="11" customFormat="1" ht="84" x14ac:dyDescent="0.15">
       <c r="A122" s="8" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="B122" s="32" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="C122" s="8" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="D122" s="8" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="E122" s="8"/>
       <c r="F122" s="12"/>
     </row>
     <row r="123" spans="1:6" s="11" customFormat="1" ht="126" x14ac:dyDescent="0.15">
       <c r="A123" s="8" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="B123" s="19" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="C123" s="8"/>
       <c r="D123" s="19" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="E123" s="8"/>
       <c r="F123" s="12"/>
     </row>
     <row r="124" spans="1:6" s="11" customFormat="1" ht="224" x14ac:dyDescent="0.15">
       <c r="A124" s="8" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="B124" s="8" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="C124" s="8"/>
       <c r="D124" s="20" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="E124" s="8"/>
       <c r="F124" s="12"/>
     </row>
     <row r="125" spans="1:6" s="11" customFormat="1" ht="224" x14ac:dyDescent="0.15">
       <c r="A125" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="B125" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="C125" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="D125" s="8" t="s">
         <v>186</v>
-      </c>
-      <c r="B125" s="8" t="s">
-        <v>187</v>
-      </c>
-      <c r="C125" s="8" t="s">
-        <v>188</v>
-      </c>
-      <c r="D125" s="8" t="s">
-        <v>189</v>
       </c>
       <c r="E125" s="8"/>
       <c r="F125" s="12"/>
     </row>
     <row r="126" spans="1:6" s="11" customFormat="1" ht="84" x14ac:dyDescent="0.15">
       <c r="A126" s="8" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B126" s="8" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C126" s="8"/>
       <c r="D126" s="8"/>
       <c r="E126" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F126" s="12" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="127" spans="1:6" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A127" s="8" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B127" s="8" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C127" s="8"/>
       <c r="D127" s="8"/>
@@ -4593,62 +4593,62 @@
     </row>
     <row r="128" spans="1:6" s="11" customFormat="1" ht="358" x14ac:dyDescent="0.15">
       <c r="A128" s="8" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B128" s="8" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="C128" s="8" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="D128" s="8" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="E128" s="8" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="F128" s="12" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
     </row>
     <row r="129" spans="1:6" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A129" s="8" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="B129" s="8" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C129" s="8" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D129" s="8" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="E129" s="8"/>
       <c r="F129" s="12"/>
     </row>
     <row r="130" spans="1:6" s="11" customFormat="1" ht="140" x14ac:dyDescent="0.15">
       <c r="A130" s="8" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B130" s="8" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C130" s="8" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="D130" s="8" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="E130" s="8"/>
       <c r="F130" s="12"/>
     </row>
     <row r="131" spans="1:6" s="11" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A131" s="8" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B131" s="8" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C131" s="8"/>
       <c r="D131" s="8"/>

</xml_diff>

<commit_message>
dev-5789 added definitions for DEFC and NIA
</commit_message>
<xml_diff>
--- a/usaspending_api/data/USAspendingGlossary.xlsx
+++ b/usaspending_api/data/USAspendingGlossary.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10713"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kirkbarden/Development/usaspending-api/usaspending_api/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brianzito/Documents/DATA/usaspending-api/usaspending_api/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{925020FF-F4C7-6141-ACB4-61079926C48E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5963317C-0A80-3A45-8318-2D72F8B7167B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20" yWindow="460" windowWidth="33600" windowHeight="19080" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$Y$131</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$Y$133</definedName>
   </definedNames>
   <calcPr calcId="0"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="436">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="442">
   <si>
     <t>Term</t>
   </si>
@@ -1802,12 +1802,45 @@
   <si>
     <t>[Visit the CFDA Website](https://beta.sam.gov/help/assistance-listing)</t>
   </si>
+  <si>
+    <t>Disaster Emergency Fund Code (DEFC)</t>
+  </si>
+  <si>
+    <t>Disaster Emergency Fund Code (DEFC) is used to track the spending of funding for disasters and emergencies such as COVID-19. Each code links to one or more legislative bills that authorized the funding.</t>
+  </si>
+  <si>
+    <t>The Office of Management and Budget (OMB), working with the Department of Treasury’s Fiscal Service, has identified a Government-wide Treasury Account Symbol Adjusted Trial Balance System (GTAS) attribute called ‘Disaster Emergency Fund Code (DEFC)’ to track appropriations classified as disaster or emergency. This code applies to the budgetary resources, obligations incurred, unobligated and obligated balances, and outlays that result from these appropriations.
+As established in Memorandum M-18-08,  the domain value set for DEFC is a single letter from ‘A’ to ‘Z’. The default domain value for all funding without disaster or emergency designation is ‘Q’. OMB assigns a new DEFC domain value from the set to each enacted appropriation with disaster or emergency funding. The corresponding domain title for each DEFC domain value identifies the associated public law number(s) and whether the funding is disaster or emergency.
+Memorandum M-20-21 amended the above to allow agencies to use DEFC to meet reporting requirements for COVID-19 supplemental funding, which required tracking of funds not designated as emergency.
+Agencies use the following DEFC domain values and titles for COVID-19 supplemental funding:
+•	DEFC ‘L’ – Public Law 116-123, designated as emergency
+•	DEFC ‘M’ – Public Law 116-127, designated as emergency
+•	DEFC ‘N’ – Public Law 116-136, designated as emergency
+•	DEFC ‘O’ – Public Law 116-136 and Public Law 116-139, not designated as emergency
+•	DEFC ‘P’ – Public Law 116-139, designated as emergency
+•	DEFC ‘Q’ – Excluded from tracking, continue to use for non-emergency/non-disaster designated appropriations
+Note that the National Interest Action (NIA) code is also used to track COVID-19 spending. However, it only applies to procurement actions (i.e., contracts) and is not necessarily tied to COVID-19 supplemental appropriations. Thus, awards with the COVID-19 NIA value may not have a COVID-19 DEFC value, and vice versa.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">National Interest Action (NIA) </t>
+  </si>
+  <si>
+    <t>The National Interest Action values are used to categorize procurement actions related to emergency contingency responses or other nationally significant events. The length of the value is no more than 4 characters. A new NIA value was created to address the COVID-19 pandemic and this value is valid for actions signed between 3/13/2020 and 9/30/2020.
+Below are examples of NIA values:
+•	H19M – Hurricane Michael 2019
+•	H19D – Hurricane Dorian 2019
+•	P20C – COVID-19 2020
+Note that the Disaster Emergency Fund Code (DEFC) is also used to track COVID-19 spending. However, it is not limited to contracts and is necessarily tied to COVID-19 supplemental appropriations. Thus, awards with the COVID-19 NIA value may not have a COVID-19 DEFC value, and vice versa.</t>
+  </si>
+  <si>
+    <t>The National Interest Action (NIA) code categorizes federal contracts that are related to emergency responses or other nationally significant events.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1910,6 +1943,18 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF1D1C1D"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1997,7 +2042,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -2107,6 +2152,8 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="20% - Accent6" xfId="5" builtinId="50"/>
@@ -2392,11 +2439,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y1030"/>
+  <dimension ref="A1:Y1032"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="125" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B83" sqref="B83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3151,1520 +3198,1550 @@
       <c r="E42" s="14"/>
       <c r="F42" s="12"/>
     </row>
-    <row r="43" spans="1:25" s="11" customFormat="1" ht="98" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:25" s="11" customFormat="1" ht="117" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="8" t="s">
-        <v>220</v>
+        <v>436</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>221</v>
+        <v>437</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>220</v>
+        <v>436</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>353</v>
+        <v>438</v>
       </c>
       <c r="E43" s="14"/>
       <c r="F43" s="12"/>
     </row>
-    <row r="44" spans="1:25" s="11" customFormat="1" ht="56" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:25" s="11" customFormat="1" ht="98" x14ac:dyDescent="0.15">
       <c r="A44" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="D44" s="8" t="s">
+        <v>353</v>
+      </c>
+      <c r="E44" s="14"/>
+      <c r="F44" s="12"/>
+    </row>
+    <row r="45" spans="1:25" s="11" customFormat="1" ht="56" x14ac:dyDescent="0.15">
+      <c r="A45" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="B44" s="8" t="s">
+      <c r="B45" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="C44" s="8" t="s">
+      <c r="C45" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="D44" s="8" t="s">
+      <c r="D45" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="E44" s="8" t="s">
+      <c r="E45" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="F44" s="12" t="s">
+      <c r="F45" s="12" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="45" spans="1:25" s="11" customFormat="1" ht="140" x14ac:dyDescent="0.15">
-      <c r="A45" s="8" t="s">
+    <row r="46" spans="1:25" s="11" customFormat="1" ht="140" x14ac:dyDescent="0.15">
+      <c r="A46" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="B45" s="8" t="s">
+      <c r="B46" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="C45" s="8" t="s">
+      <c r="C46" s="8" t="s">
         <v>264</v>
       </c>
-      <c r="D45" s="8" t="s">
+      <c r="D46" s="8" t="s">
         <v>269</v>
       </c>
-      <c r="E45" s="8" t="s">
+      <c r="E46" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="F45" s="12" t="s">
+      <c r="F46" s="12" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="46" spans="1:25" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
-      <c r="A46" s="8" t="s">
+    <row r="47" spans="1:25" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
+      <c r="A47" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="B46" s="8" t="s">
+      <c r="B47" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C46" s="8" t="s">
+      <c r="C47" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="D46" s="8" t="s">
+      <c r="D47" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="E46" s="8"/>
-      <c r="F46" s="12"/>
-    </row>
-    <row r="47" spans="1:25" s="11" customFormat="1" ht="210" x14ac:dyDescent="0.15">
-      <c r="A47" s="8" t="s">
+      <c r="E47" s="8"/>
+      <c r="F47" s="12"/>
+    </row>
+    <row r="48" spans="1:25" s="11" customFormat="1" ht="210" x14ac:dyDescent="0.15">
+      <c r="A48" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="B47" s="8" t="s">
+      <c r="B48" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="C47" s="8" t="s">
+      <c r="C48" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="D47" s="8" t="s">
+      <c r="D48" s="8" t="s">
         <v>338</v>
       </c>
-      <c r="E47" s="9" t="s">
+      <c r="E48" s="9" t="s">
         <v>360</v>
       </c>
-      <c r="F47" s="12" t="s">
+      <c r="F48" s="12" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="48" spans="1:25" s="11" customFormat="1" ht="98" x14ac:dyDescent="0.15">
-      <c r="A48" s="8" t="s">
+    <row r="49" spans="1:6" s="11" customFormat="1" ht="98" x14ac:dyDescent="0.15">
+      <c r="A49" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="B48" s="8" t="s">
+      <c r="B49" s="8" t="s">
         <v>281</v>
       </c>
-      <c r="C48" s="8" t="s">
+      <c r="C49" s="8" t="s">
         <v>311</v>
       </c>
-      <c r="D48" s="8" t="s">
+      <c r="D49" s="8" t="s">
         <v>113</v>
-      </c>
-      <c r="E48" s="8"/>
-      <c r="F48" s="12"/>
-    </row>
-    <row r="49" spans="1:6" s="11" customFormat="1" ht="112" x14ac:dyDescent="0.15">
-      <c r="A49" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="B49" s="8" t="s">
-        <v>200</v>
-      </c>
-      <c r="C49" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="D49" s="8" t="s">
-        <v>94</v>
       </c>
       <c r="E49" s="8"/>
       <c r="F49" s="12"/>
     </row>
-    <row r="50" spans="1:6" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:6" s="11" customFormat="1" ht="112" x14ac:dyDescent="0.15">
       <c r="A50" s="8" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="C50" s="8"/>
-      <c r="D50" s="8"/>
-      <c r="E50" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="F50" s="12" t="s">
-        <v>98</v>
-      </c>
+        <v>200</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="D50" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E50" s="8"/>
+      <c r="F50" s="12"/>
     </row>
     <row r="51" spans="1:6" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A51" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C51" s="8"/>
+      <c r="D51" s="8"/>
+      <c r="E51" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="F51" s="12" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
+      <c r="A52" s="8" t="s">
         <v>260</v>
       </c>
-      <c r="B51" s="8" t="s">
+      <c r="B52" s="8" t="s">
         <v>262</v>
       </c>
-      <c r="C51" s="8" t="s">
+      <c r="C52" s="8" t="s">
         <v>260</v>
       </c>
-      <c r="D51" s="8" t="s">
+      <c r="D52" s="8" t="s">
         <v>262</v>
       </c>
-      <c r="E51" s="8"/>
-      <c r="F51" s="12"/>
-    </row>
-    <row r="52" spans="1:6" s="11" customFormat="1" ht="98" x14ac:dyDescent="0.15">
-      <c r="A52" s="8" t="s">
-        <v>432</v>
-      </c>
-      <c r="B52" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="C52" s="8"/>
-      <c r="D52" s="8"/>
       <c r="E52" s="8"/>
       <c r="F52" s="12"/>
     </row>
-    <row r="53" spans="1:6" s="3" customFormat="1" ht="85" x14ac:dyDescent="0.15">
-      <c r="A53" s="1" t="s">
+    <row r="53" spans="1:6" s="11" customFormat="1" ht="98" x14ac:dyDescent="0.15">
+      <c r="A53" s="8" t="s">
+        <v>432</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="C53" s="8"/>
+      <c r="D53" s="8"/>
+      <c r="E53" s="8"/>
+      <c r="F53" s="12"/>
+    </row>
+    <row r="54" spans="1:6" s="3" customFormat="1" ht="85" x14ac:dyDescent="0.15">
+      <c r="A54" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="B54" s="1" t="s">
         <v>393</v>
       </c>
-      <c r="C53" s="1"/>
-      <c r="D53" s="1"/>
-      <c r="E53" s="1" t="s">
+      <c r="C54" s="1"/>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="F53" s="2" t="s">
+      <c r="F54" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="54" spans="1:6" s="11" customFormat="1" ht="168" x14ac:dyDescent="0.15">
-      <c r="A54" s="8" t="s">
+    <row r="55" spans="1:6" s="11" customFormat="1" ht="168" x14ac:dyDescent="0.15">
+      <c r="A55" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="B54" s="8" t="s">
+      <c r="B55" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="C54" s="8"/>
-      <c r="D54" s="8"/>
-      <c r="E54" s="8"/>
-      <c r="F54" s="12"/>
-    </row>
-    <row r="55" spans="1:6" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
-      <c r="A55" s="8" t="s">
-        <v>211</v>
-      </c>
-      <c r="B55" s="8" t="s">
-        <v>355</v>
-      </c>
-      <c r="C55" s="8" t="s">
-        <v>211</v>
-      </c>
-      <c r="D55" s="8" t="s">
-        <v>354</v>
-      </c>
+      <c r="C55" s="8"/>
+      <c r="D55" s="8"/>
       <c r="E55" s="8"/>
       <c r="F55" s="12"/>
     </row>
-    <row r="56" spans="1:6" s="11" customFormat="1" ht="84" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:6" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
       <c r="A56" s="8" t="s">
-        <v>105</v>
+        <v>211</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>106</v>
+        <v>355</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>299</v>
+        <v>211</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>300</v>
+        <v>354</v>
       </c>
       <c r="E56" s="8"/>
       <c r="F56" s="12"/>
     </row>
-    <row r="57" spans="1:6" s="11" customFormat="1" ht="112" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:6" s="11" customFormat="1" ht="84" x14ac:dyDescent="0.15">
       <c r="A57" s="8" t="s">
-        <v>324</v>
+        <v>105</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>325</v>
+        <v>106</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>132</v>
+        <v>299</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>133</v>
+        <v>300</v>
       </c>
       <c r="E57" s="8"/>
       <c r="F57" s="12"/>
     </row>
-    <row r="58" spans="1:6" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:6" s="11" customFormat="1" ht="112" x14ac:dyDescent="0.15">
       <c r="A58" s="8" t="s">
-        <v>312</v>
+        <v>324</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>314</v>
+        <v>325</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>301</v>
+        <v>132</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>339</v>
+        <v>133</v>
       </c>
       <c r="E58" s="8"/>
       <c r="F58" s="12"/>
     </row>
-    <row r="59" spans="1:6" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:6" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A59" s="8" t="s">
-        <v>374</v>
+        <v>312</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>303</v>
+        <v>339</v>
       </c>
       <c r="E59" s="8"/>
       <c r="F59" s="12"/>
     </row>
-    <row r="60" spans="1:6" s="3" customFormat="1" ht="238" x14ac:dyDescent="0.15">
-      <c r="A60" s="1" t="s">
+    <row r="60" spans="1:6" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
+      <c r="A60" s="8" t="s">
+        <v>374</v>
+      </c>
+      <c r="B60" s="8" t="s">
+        <v>315</v>
+      </c>
+      <c r="C60" s="8" t="s">
+        <v>302</v>
+      </c>
+      <c r="D60" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="E60" s="8"/>
+      <c r="F60" s="12"/>
+    </row>
+    <row r="61" spans="1:6" s="3" customFormat="1" ht="238" x14ac:dyDescent="0.15">
+      <c r="A61" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="B60" s="36" t="s">
+      <c r="B61" s="36" t="s">
         <v>409</v>
       </c>
-      <c r="C60" s="1"/>
-      <c r="D60" s="1"/>
-      <c r="E60" s="1" t="s">
+      <c r="C61" s="1"/>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="F60" s="2" t="s">
+      <c r="F61" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="61" spans="1:6" s="11" customFormat="1" ht="196" x14ac:dyDescent="0.15">
-      <c r="A61" s="8" t="s">
+    <row r="62" spans="1:6" s="11" customFormat="1" ht="196" x14ac:dyDescent="0.15">
+      <c r="A62" s="8" t="s">
         <v>202</v>
       </c>
-      <c r="B61" s="8" t="s">
+      <c r="B62" s="8" t="s">
         <v>224</v>
       </c>
-      <c r="C61" s="8" t="s">
+      <c r="C62" s="8" t="s">
         <v>202</v>
       </c>
-      <c r="D61" s="8" t="s">
+      <c r="D62" s="8" t="s">
         <v>356</v>
       </c>
-      <c r="E61" s="14"/>
-      <c r="F61" s="12"/>
-    </row>
-    <row r="62" spans="1:6" s="11" customFormat="1" ht="154" x14ac:dyDescent="0.15">
-      <c r="A62" s="8" t="s">
+      <c r="E62" s="14"/>
+      <c r="F62" s="12"/>
+    </row>
+    <row r="63" spans="1:6" s="11" customFormat="1" ht="154" x14ac:dyDescent="0.15">
+      <c r="A63" s="8" t="s">
         <v>203</v>
       </c>
-      <c r="B62" s="8" t="s">
+      <c r="B63" s="8" t="s">
         <v>332</v>
       </c>
-      <c r="C62" s="8" t="s">
+      <c r="C63" s="8" t="s">
         <v>203</v>
       </c>
-      <c r="D62" s="8" t="s">
+      <c r="D63" s="8" t="s">
         <v>335</v>
       </c>
-      <c r="E62" s="9" t="s">
+      <c r="E63" s="9" t="s">
         <v>232</v>
       </c>
-      <c r="F62" s="10" t="s">
+      <c r="F63" s="10" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="63" spans="1:6" s="3" customFormat="1" ht="119" x14ac:dyDescent="0.15">
-      <c r="A63" s="1" t="s">
+    <row r="64" spans="1:6" s="3" customFormat="1" ht="119" x14ac:dyDescent="0.15">
+      <c r="A64" s="1" t="s">
         <v>395</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="B64" s="1" t="s">
         <v>394</v>
       </c>
-      <c r="C63" s="1"/>
-      <c r="D63" s="1"/>
-      <c r="E63" s="1"/>
-      <c r="F63" s="2"/>
-    </row>
-    <row r="64" spans="1:6" s="11" customFormat="1" ht="238" x14ac:dyDescent="0.15">
-      <c r="A64" s="8" t="s">
+      <c r="C64" s="1"/>
+      <c r="D64" s="1"/>
+      <c r="E64" s="1"/>
+      <c r="F64" s="2"/>
+    </row>
+    <row r="65" spans="1:25" s="11" customFormat="1" ht="238" x14ac:dyDescent="0.15">
+      <c r="A65" s="8" t="s">
         <v>265</v>
       </c>
-      <c r="B64" s="8" t="s">
+      <c r="B65" s="8" t="s">
         <v>270</v>
       </c>
-      <c r="C64" s="8" t="s">
+      <c r="C65" s="8" t="s">
         <v>265</v>
       </c>
-      <c r="D64" s="8" t="s">
+      <c r="D65" s="8" t="s">
         <v>270</v>
-      </c>
-      <c r="E64" s="8"/>
-      <c r="F64" s="12"/>
-    </row>
-    <row r="65" spans="1:25" s="11" customFormat="1" ht="140" x14ac:dyDescent="0.15">
-      <c r="A65" s="8" t="s">
-        <v>266</v>
-      </c>
-      <c r="B65" s="8" t="s">
-        <v>271</v>
-      </c>
-      <c r="C65" s="8" t="s">
-        <v>266</v>
-      </c>
-      <c r="D65" s="8" t="s">
-        <v>271</v>
       </c>
       <c r="E65" s="8"/>
       <c r="F65" s="12"/>
     </row>
-    <row r="66" spans="1:25" s="3" customFormat="1" ht="85" x14ac:dyDescent="0.15">
-      <c r="A66" s="30" t="s">
+    <row r="66" spans="1:25" s="11" customFormat="1" ht="140" x14ac:dyDescent="0.15">
+      <c r="A66" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="B66" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="C66" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="D66" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="E66" s="8"/>
+      <c r="F66" s="12"/>
+    </row>
+    <row r="67" spans="1:25" s="3" customFormat="1" ht="85" x14ac:dyDescent="0.15">
+      <c r="A67" s="30" t="s">
         <v>415</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="B67" s="1" t="s">
         <v>398</v>
       </c>
-      <c r="C66" s="1"/>
-      <c r="D66" s="1"/>
-      <c r="E66" s="1"/>
-      <c r="F66" s="2"/>
-    </row>
-    <row r="67" spans="1:25" s="1" customFormat="1" ht="175" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A67" s="27" t="s">
+      <c r="C67" s="1"/>
+      <c r="D67" s="1"/>
+      <c r="E67" s="1"/>
+      <c r="F67" s="2"/>
+    </row>
+    <row r="68" spans="1:25" s="1" customFormat="1" ht="175" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A68" s="27" t="s">
         <v>399</v>
       </c>
-      <c r="B67" s="29" t="s">
+      <c r="B68" s="29" t="s">
         <v>413</v>
       </c>
-      <c r="C67" s="27"/>
-      <c r="E67" s="1" t="s">
+      <c r="C68" s="27"/>
+      <c r="E68" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="F67" s="2" t="s">
+      <c r="F68" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="G67" s="3"/>
-      <c r="H67" s="3"/>
-      <c r="I67" s="3"/>
-      <c r="J67" s="3"/>
-      <c r="K67" s="3"/>
-      <c r="L67" s="3"/>
-      <c r="M67" s="3"/>
-      <c r="N67" s="3"/>
-      <c r="O67" s="3"/>
-      <c r="P67" s="3"/>
-      <c r="Q67" s="3"/>
-      <c r="R67" s="3"/>
-      <c r="S67" s="3"/>
-      <c r="T67" s="3"/>
-      <c r="U67" s="3"/>
-      <c r="V67" s="3"/>
-      <c r="W67" s="3"/>
-      <c r="X67" s="3"/>
-      <c r="Y67" s="3"/>
-    </row>
-    <row r="68" spans="1:25" s="11" customFormat="1" ht="170" x14ac:dyDescent="0.15">
-      <c r="A68" s="26" t="s">
+      <c r="G68" s="3"/>
+      <c r="H68" s="3"/>
+      <c r="I68" s="3"/>
+      <c r="J68" s="3"/>
+      <c r="K68" s="3"/>
+      <c r="L68" s="3"/>
+      <c r="M68" s="3"/>
+      <c r="N68" s="3"/>
+      <c r="O68" s="3"/>
+      <c r="P68" s="3"/>
+      <c r="Q68" s="3"/>
+      <c r="R68" s="3"/>
+      <c r="S68" s="3"/>
+      <c r="T68" s="3"/>
+      <c r="U68" s="3"/>
+      <c r="V68" s="3"/>
+      <c r="W68" s="3"/>
+      <c r="X68" s="3"/>
+      <c r="Y68" s="3"/>
+    </row>
+    <row r="69" spans="1:25" s="11" customFormat="1" ht="170" x14ac:dyDescent="0.15">
+      <c r="A69" s="26" t="s">
         <v>416</v>
       </c>
-      <c r="B68" s="25" t="s">
+      <c r="B69" s="25" t="s">
         <v>412</v>
       </c>
-      <c r="C68" s="28"/>
-      <c r="D68" s="1"/>
-      <c r="E68" s="1"/>
-      <c r="F68" s="2"/>
-      <c r="G68" s="1"/>
-      <c r="H68" s="1"/>
-      <c r="I68" s="1"/>
-      <c r="J68" s="1"/>
-      <c r="K68" s="1"/>
-      <c r="L68" s="1"/>
-      <c r="M68" s="1"/>
-      <c r="N68" s="1"/>
-      <c r="O68" s="1"/>
-      <c r="P68" s="1"/>
-      <c r="Q68" s="1"/>
-      <c r="R68" s="1"/>
-      <c r="S68" s="1"/>
-      <c r="T68" s="1"/>
-      <c r="U68" s="1"/>
-      <c r="V68" s="1"/>
-      <c r="W68" s="1"/>
-      <c r="X68" s="1"/>
-      <c r="Y68" s="1"/>
-    </row>
-    <row r="69" spans="1:25" s="3" customFormat="1" ht="170" x14ac:dyDescent="0.15">
-      <c r="A69" s="1" t="s">
-        <v>397</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>396</v>
-      </c>
-      <c r="C69" s="1"/>
+      <c r="C69" s="28"/>
       <c r="D69" s="1"/>
       <c r="E69" s="1"/>
       <c r="F69" s="2"/>
-    </row>
-    <row r="70" spans="1:25" s="3" customFormat="1" ht="140" x14ac:dyDescent="0.15">
-      <c r="A70" s="8" t="s">
+      <c r="G69" s="1"/>
+      <c r="H69" s="1"/>
+      <c r="I69" s="1"/>
+      <c r="J69" s="1"/>
+      <c r="K69" s="1"/>
+      <c r="L69" s="1"/>
+      <c r="M69" s="1"/>
+      <c r="N69" s="1"/>
+      <c r="O69" s="1"/>
+      <c r="P69" s="1"/>
+      <c r="Q69" s="1"/>
+      <c r="R69" s="1"/>
+      <c r="S69" s="1"/>
+      <c r="T69" s="1"/>
+      <c r="U69" s="1"/>
+      <c r="V69" s="1"/>
+      <c r="W69" s="1"/>
+      <c r="X69" s="1"/>
+      <c r="Y69" s="1"/>
+    </row>
+    <row r="70" spans="1:25" s="3" customFormat="1" ht="170" x14ac:dyDescent="0.15">
+      <c r="A70" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="C70" s="1"/>
+      <c r="D70" s="1"/>
+      <c r="E70" s="1"/>
+      <c r="F70" s="2"/>
+    </row>
+    <row r="71" spans="1:25" s="3" customFormat="1" ht="140" x14ac:dyDescent="0.15">
+      <c r="A71" s="8" t="s">
         <v>414</v>
       </c>
-      <c r="B70" s="8" t="s">
+      <c r="B71" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="C70" s="8"/>
-      <c r="D70" s="8"/>
-      <c r="E70" s="9" t="s">
+      <c r="C71" s="8"/>
+      <c r="D71" s="8"/>
+      <c r="E71" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="F70" s="12" t="s">
+      <c r="F71" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="G70" s="11"/>
-      <c r="H70" s="11"/>
-      <c r="I70" s="11"/>
-      <c r="J70" s="11"/>
-      <c r="K70" s="11"/>
-      <c r="L70" s="11"/>
-      <c r="M70" s="11"/>
-      <c r="N70" s="11"/>
-      <c r="O70" s="11"/>
-      <c r="P70" s="11"/>
-      <c r="Q70" s="11"/>
-      <c r="R70" s="11"/>
-      <c r="S70" s="11"/>
-      <c r="T70" s="11"/>
-      <c r="U70" s="11"/>
-      <c r="V70" s="11"/>
-      <c r="W70" s="11"/>
-      <c r="X70" s="11"/>
-      <c r="Y70" s="11"/>
-    </row>
-    <row r="71" spans="1:25" s="3" customFormat="1" ht="119" x14ac:dyDescent="0.15">
-      <c r="A71" s="1" t="s">
+      <c r="G71" s="11"/>
+      <c r="H71" s="11"/>
+      <c r="I71" s="11"/>
+      <c r="J71" s="11"/>
+      <c r="K71" s="11"/>
+      <c r="L71" s="11"/>
+      <c r="M71" s="11"/>
+      <c r="N71" s="11"/>
+      <c r="O71" s="11"/>
+      <c r="P71" s="11"/>
+      <c r="Q71" s="11"/>
+      <c r="R71" s="11"/>
+      <c r="S71" s="11"/>
+      <c r="T71" s="11"/>
+      <c r="U71" s="11"/>
+      <c r="V71" s="11"/>
+      <c r="W71" s="11"/>
+      <c r="X71" s="11"/>
+      <c r="Y71" s="11"/>
+    </row>
+    <row r="72" spans="1:25" s="3" customFormat="1" ht="119" x14ac:dyDescent="0.15">
+      <c r="A72" s="1" t="s">
         <v>400</v>
       </c>
-      <c r="B71" s="1" t="s">
+      <c r="B72" s="1" t="s">
         <v>401</v>
       </c>
-      <c r="C71" s="1"/>
-      <c r="D71" s="1"/>
-      <c r="E71" s="1"/>
-      <c r="F71" s="2"/>
-    </row>
-    <row r="72" spans="1:25" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
-      <c r="A72" s="8" t="s">
-        <v>367</v>
-      </c>
-      <c r="B72" s="8" t="s">
-        <v>368</v>
-      </c>
-      <c r="C72" s="8" t="s">
-        <v>367</v>
-      </c>
-      <c r="D72" s="8" t="s">
-        <v>368</v>
-      </c>
-      <c r="E72" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="F72" s="12" t="s">
-        <v>125</v>
-      </c>
+      <c r="C72" s="1"/>
+      <c r="D72" s="1"/>
+      <c r="E72" s="1"/>
+      <c r="F72" s="2"/>
     </row>
     <row r="73" spans="1:25" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
       <c r="A73" s="8" t="s">
+        <v>367</v>
+      </c>
+      <c r="B73" s="8" t="s">
+        <v>368</v>
+      </c>
+      <c r="C73" s="8" t="s">
+        <v>367</v>
+      </c>
+      <c r="D73" s="8" t="s">
+        <v>368</v>
+      </c>
+      <c r="E73" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="F73" s="12" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="74" spans="1:25" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
+      <c r="A74" s="8" t="s">
         <v>319</v>
       </c>
-      <c r="B73" s="8" t="s">
+      <c r="B74" s="8" t="s">
         <v>320</v>
       </c>
-      <c r="C73" s="8" t="s">
+      <c r="C74" s="8" t="s">
         <v>319</v>
       </c>
-      <c r="D73" s="8" t="s">
+      <c r="D74" s="8" t="s">
         <v>320</v>
       </c>
-      <c r="E73" s="8"/>
-      <c r="F73" s="12"/>
-    </row>
-    <row r="74" spans="1:25" s="11" customFormat="1" ht="98" x14ac:dyDescent="0.15">
-      <c r="A74" s="8" t="s">
-        <v>222</v>
-      </c>
-      <c r="B74" s="8" t="s">
-        <v>358</v>
-      </c>
-      <c r="C74" s="8"/>
-      <c r="D74" s="8"/>
       <c r="E74" s="8"/>
       <c r="F74" s="12"/>
     </row>
-    <row r="75" spans="1:25" s="11" customFormat="1" ht="182" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:25" s="11" customFormat="1" ht="98" x14ac:dyDescent="0.15">
       <c r="A75" s="8" t="s">
-        <v>114</v>
+        <v>222</v>
       </c>
       <c r="B75" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="C75" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="D75" s="8" t="s">
-        <v>116</v>
-      </c>
+        <v>358</v>
+      </c>
+      <c r="C75" s="8"/>
+      <c r="D75" s="8"/>
       <c r="E75" s="8"/>
       <c r="F75" s="12"/>
     </row>
-    <row r="76" spans="1:25" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:25" s="11" customFormat="1" ht="182" x14ac:dyDescent="0.15">
       <c r="A76" s="8" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B76" s="8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C76" s="8" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D76" s="8" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E76" s="8"/>
       <c r="F76" s="12"/>
     </row>
-    <row r="77" spans="1:25" s="11" customFormat="1" ht="98" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:25" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A77" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B77" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="C77" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="D77" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="E77" s="8"/>
+      <c r="F77" s="12"/>
+    </row>
+    <row r="78" spans="1:25" s="11" customFormat="1" ht="98" x14ac:dyDescent="0.15">
+      <c r="A78" s="8" t="s">
         <v>366</v>
       </c>
-      <c r="B77" s="8" t="s">
+      <c r="B78" s="8" t="s">
         <v>369</v>
       </c>
-      <c r="C77" s="8" t="s">
+      <c r="C78" s="8" t="s">
         <v>366</v>
       </c>
-      <c r="D77" s="8" t="s">
+      <c r="D78" s="8" t="s">
         <v>369</v>
       </c>
-      <c r="E77" s="14" t="s">
+      <c r="E78" s="14" t="s">
         <v>195</v>
       </c>
-      <c r="F77" s="12" t="s">
+      <c r="F78" s="12" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="78" spans="1:25" s="11" customFormat="1" ht="277.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A78" s="8" t="s">
+    <row r="79" spans="1:25" s="11" customFormat="1" ht="277.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A79" s="8" t="s">
         <v>292</v>
       </c>
-      <c r="B78" s="8" t="s">
+      <c r="B79" s="8" t="s">
         <v>251</v>
       </c>
-      <c r="C78" s="8" t="s">
+      <c r="C79" s="8" t="s">
         <v>242</v>
       </c>
-      <c r="D78" s="8" t="s">
+      <c r="D79" s="8" t="s">
         <v>251</v>
       </c>
-      <c r="E78" s="8"/>
-      <c r="F78" s="12"/>
-    </row>
-    <row r="79" spans="1:25" s="3" customFormat="1" ht="277.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A79" s="1" t="s">
+      <c r="E79" s="8"/>
+      <c r="F79" s="12"/>
+    </row>
+    <row r="80" spans="1:25" s="3" customFormat="1" ht="277.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A80" s="1" t="s">
         <v>402</v>
       </c>
-      <c r="B79" s="1" t="s">
+      <c r="B80" s="1" t="s">
         <v>403</v>
       </c>
-      <c r="C79" s="1"/>
-      <c r="D79" s="1"/>
-      <c r="E79" s="1"/>
-      <c r="F79" s="2"/>
-    </row>
-    <row r="80" spans="1:25" s="11" customFormat="1" ht="56" x14ac:dyDescent="0.15">
-      <c r="A80" s="8" t="s">
+      <c r="C80" s="1"/>
+      <c r="D80" s="1"/>
+      <c r="E80" s="1"/>
+      <c r="F80" s="2"/>
+    </row>
+    <row r="81" spans="1:25" s="11" customFormat="1" ht="56" x14ac:dyDescent="0.15">
+      <c r="A81" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="B80" s="8" t="s">
+      <c r="B81" s="8" t="s">
         <v>121</v>
-      </c>
-      <c r="C80" s="8"/>
-      <c r="D80" s="8"/>
-      <c r="E80" s="14" t="s">
-        <v>122</v>
-      </c>
-      <c r="F80" s="12" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="81" spans="1:25" s="11" customFormat="1" ht="224" x14ac:dyDescent="0.15">
-      <c r="A81" s="8" t="s">
-        <v>223</v>
-      </c>
-      <c r="B81" s="35" t="s">
-        <v>427</v>
       </c>
       <c r="C81" s="8"/>
       <c r="D81" s="8"/>
-      <c r="E81" s="14"/>
+      <c r="E81" s="14" t="s">
+        <v>122</v>
+      </c>
       <c r="F81" s="12" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="82" spans="1:25" s="11" customFormat="1" ht="224" x14ac:dyDescent="0.15">
+      <c r="A82" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="B82" s="35" t="s">
+        <v>427</v>
+      </c>
+      <c r="C82" s="8"/>
+      <c r="D82" s="8"/>
+      <c r="E82" s="14"/>
+      <c r="F82" s="12" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="82" spans="1:25" s="11" customFormat="1" ht="126" x14ac:dyDescent="0.15">
-      <c r="A82" s="8" t="s">
+    <row r="83" spans="1:25" s="11" customFormat="1" ht="126" x14ac:dyDescent="0.15">
+      <c r="A83" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="B82" s="8" t="s">
+      <c r="B83" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="C82" s="8" t="s">
+      <c r="C83" s="8" t="s">
         <v>290</v>
       </c>
-      <c r="D82" s="8" t="s">
+      <c r="D83" s="8" t="s">
         <v>289</v>
       </c>
-      <c r="E82" s="14" t="s">
+      <c r="E83" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="F82" s="12" t="s">
+      <c r="F83" s="12" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="83" spans="1:25" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
-      <c r="A83" s="8" t="s">
+    <row r="84" spans="1:25" s="11" customFormat="1" ht="238" x14ac:dyDescent="0.2">
+      <c r="A84" s="8" t="s">
+        <v>439</v>
+      </c>
+      <c r="B84" s="38" t="s">
+        <v>441</v>
+      </c>
+      <c r="C84" s="37" t="s">
+        <v>439</v>
+      </c>
+      <c r="D84" s="8" t="s">
+        <v>440</v>
+      </c>
+      <c r="E84" s="14"/>
+      <c r="F84" s="12"/>
+    </row>
+    <row r="85" spans="1:25" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
+      <c r="A85" s="8" t="s">
         <v>261</v>
       </c>
-      <c r="B83" s="8" t="s">
+      <c r="B85" s="8" t="s">
         <v>263</v>
       </c>
-      <c r="C83" s="8" t="s">
+      <c r="C85" s="8" t="s">
         <v>261</v>
       </c>
-      <c r="D83" s="8" t="s">
+      <c r="D85" s="8" t="s">
         <v>263</v>
-      </c>
-      <c r="E83" s="8"/>
-      <c r="F83" s="12"/>
-    </row>
-    <row r="84" spans="1:25" s="11" customFormat="1" ht="84" x14ac:dyDescent="0.15">
-      <c r="A84" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="B84" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="C84" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="D84" s="8" t="s">
-        <v>228</v>
-      </c>
-      <c r="E84" s="14" t="s">
-        <v>232</v>
-      </c>
-      <c r="F84" s="12" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="85" spans="1:25" s="11" customFormat="1" ht="409.6" x14ac:dyDescent="0.15">
-      <c r="A85" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="B85" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="C85" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="D85" s="8" t="s">
-        <v>229</v>
       </c>
       <c r="E85" s="8"/>
       <c r="F85" s="12"/>
     </row>
-    <row r="86" spans="1:25" s="11" customFormat="1" ht="140" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:25" s="11" customFormat="1" ht="84" x14ac:dyDescent="0.15">
       <c r="A86" s="8" t="s">
-        <v>243</v>
+        <v>130</v>
       </c>
       <c r="B86" s="8" t="s">
-        <v>252</v>
+        <v>131</v>
       </c>
       <c r="C86" s="8" t="s">
-        <v>243</v>
+        <v>130</v>
       </c>
       <c r="D86" s="8" t="s">
-        <v>252</v>
-      </c>
-      <c r="E86" s="8"/>
-      <c r="F86" s="12"/>
-    </row>
-    <row r="87" spans="1:25" s="11" customFormat="1" ht="112" x14ac:dyDescent="0.15">
+        <v>228</v>
+      </c>
+      <c r="E86" s="14" t="s">
+        <v>232</v>
+      </c>
+      <c r="F86" s="12" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="87" spans="1:25" s="11" customFormat="1" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A87" s="8" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B87" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C87" s="8" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D87" s="8" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E87" s="8"/>
       <c r="F87" s="12"/>
     </row>
-    <row r="88" spans="1:25" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:25" s="11" customFormat="1" ht="140" x14ac:dyDescent="0.15">
       <c r="A88" s="8" t="s">
-        <v>404</v>
+        <v>243</v>
       </c>
       <c r="B88" s="8" t="s">
-        <v>405</v>
-      </c>
-      <c r="C88" s="8"/>
-      <c r="D88" s="8"/>
+        <v>252</v>
+      </c>
+      <c r="C88" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="D88" s="8" t="s">
+        <v>252</v>
+      </c>
       <c r="E88" s="8"/>
       <c r="F88" s="12"/>
     </row>
-    <row r="89" spans="1:25" s="3" customFormat="1" ht="154" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:25" s="11" customFormat="1" ht="112" x14ac:dyDescent="0.15">
       <c r="A89" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="B89" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="C89" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="D89" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="E89" s="8"/>
+      <c r="F89" s="12"/>
+    </row>
+    <row r="90" spans="1:25" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
+      <c r="A90" s="8" t="s">
+        <v>404</v>
+      </c>
+      <c r="B90" s="8" t="s">
+        <v>405</v>
+      </c>
+      <c r="C90" s="8"/>
+      <c r="D90" s="8"/>
+      <c r="E90" s="8"/>
+      <c r="F90" s="12"/>
+    </row>
+    <row r="91" spans="1:25" s="3" customFormat="1" ht="154" x14ac:dyDescent="0.15">
+      <c r="A91" s="8" t="s">
         <v>330</v>
       </c>
-      <c r="B89" s="8" t="s">
+      <c r="B91" s="8" t="s">
         <v>345</v>
       </c>
-      <c r="C89" s="8" t="s">
+      <c r="C91" s="8" t="s">
         <v>330</v>
       </c>
-      <c r="D89" s="16" t="s">
+      <c r="D91" s="16" t="s">
         <v>336</v>
       </c>
-      <c r="E89" s="9" t="s">
+      <c r="E91" s="9" t="s">
         <v>232</v>
       </c>
-      <c r="F89" s="17" t="s">
+      <c r="F91" s="17" t="s">
         <v>363</v>
       </c>
-      <c r="G89" s="11"/>
-      <c r="H89" s="11"/>
-      <c r="I89" s="11"/>
-      <c r="J89" s="11"/>
-      <c r="K89" s="11"/>
-      <c r="L89" s="11"/>
-      <c r="M89" s="11"/>
-      <c r="N89" s="11"/>
-      <c r="O89" s="11"/>
-      <c r="P89" s="11"/>
-      <c r="Q89" s="11"/>
-      <c r="R89" s="11"/>
-      <c r="S89" s="11"/>
-      <c r="T89" s="11"/>
-      <c r="U89" s="11"/>
-      <c r="V89" s="11"/>
-      <c r="W89" s="11"/>
-      <c r="X89" s="11"/>
-      <c r="Y89" s="11"/>
-    </row>
-    <row r="90" spans="1:25" s="11" customFormat="1" ht="323" x14ac:dyDescent="0.15">
-      <c r="A90" s="1" t="s">
+      <c r="G91" s="11"/>
+      <c r="H91" s="11"/>
+      <c r="I91" s="11"/>
+      <c r="J91" s="11"/>
+      <c r="K91" s="11"/>
+      <c r="L91" s="11"/>
+      <c r="M91" s="11"/>
+      <c r="N91" s="11"/>
+      <c r="O91" s="11"/>
+      <c r="P91" s="11"/>
+      <c r="Q91" s="11"/>
+      <c r="R91" s="11"/>
+      <c r="S91" s="11"/>
+      <c r="T91" s="11"/>
+      <c r="U91" s="11"/>
+      <c r="V91" s="11"/>
+      <c r="W91" s="11"/>
+      <c r="X91" s="11"/>
+      <c r="Y91" s="11"/>
+    </row>
+    <row r="92" spans="1:25" s="11" customFormat="1" ht="323" x14ac:dyDescent="0.15">
+      <c r="A92" s="1" t="s">
         <v>406</v>
       </c>
-      <c r="B90" s="36" t="s">
+      <c r="B92" s="36" t="s">
         <v>410</v>
       </c>
-      <c r="C90" s="1"/>
-      <c r="D90" s="1"/>
-      <c r="E90" s="1" t="s">
+      <c r="C92" s="1"/>
+      <c r="D92" s="1"/>
+      <c r="E92" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="F90" s="2" t="s">
+      <c r="F92" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="G90" s="3"/>
-      <c r="H90" s="3"/>
-      <c r="I90" s="3"/>
-      <c r="J90" s="3"/>
-      <c r="K90" s="3"/>
-      <c r="L90" s="3"/>
-      <c r="M90" s="3"/>
-      <c r="N90" s="3"/>
-      <c r="O90" s="3"/>
-      <c r="P90" s="3"/>
-      <c r="Q90" s="3"/>
-      <c r="R90" s="3"/>
-      <c r="S90" s="3"/>
-      <c r="T90" s="3"/>
-      <c r="U90" s="3"/>
-      <c r="V90" s="3"/>
-      <c r="W90" s="3"/>
-      <c r="X90" s="3"/>
-      <c r="Y90" s="3"/>
-    </row>
-    <row r="91" spans="1:25" s="11" customFormat="1" ht="154" x14ac:dyDescent="0.15">
-      <c r="A91" s="8" t="s">
+      <c r="G92" s="3"/>
+      <c r="H92" s="3"/>
+      <c r="I92" s="3"/>
+      <c r="J92" s="3"/>
+      <c r="K92" s="3"/>
+      <c r="L92" s="3"/>
+      <c r="M92" s="3"/>
+      <c r="N92" s="3"/>
+      <c r="O92" s="3"/>
+      <c r="P92" s="3"/>
+      <c r="Q92" s="3"/>
+      <c r="R92" s="3"/>
+      <c r="S92" s="3"/>
+      <c r="T92" s="3"/>
+      <c r="U92" s="3"/>
+      <c r="V92" s="3"/>
+      <c r="W92" s="3"/>
+      <c r="X92" s="3"/>
+      <c r="Y92" s="3"/>
+    </row>
+    <row r="93" spans="1:25" s="11" customFormat="1" ht="154" x14ac:dyDescent="0.15">
+      <c r="A93" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="B91" s="8" t="s">
+      <c r="B93" s="8" t="s">
         <v>340</v>
       </c>
-      <c r="C91" s="8" t="s">
+      <c r="C93" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="D91" s="8" t="s">
+      <c r="D93" s="8" t="s">
         <v>231</v>
       </c>
-      <c r="E91" s="8"/>
-      <c r="F91" s="12"/>
-    </row>
-    <row r="92" spans="1:25" s="11" customFormat="1" ht="56" x14ac:dyDescent="0.15">
-      <c r="A92" s="8" t="s">
+      <c r="E93" s="8"/>
+      <c r="F93" s="12"/>
+    </row>
+    <row r="94" spans="1:25" s="11" customFormat="1" ht="56" x14ac:dyDescent="0.15">
+      <c r="A94" s="8" t="s">
         <v>244</v>
       </c>
-      <c r="B92" s="8" t="s">
+      <c r="B94" s="8" t="s">
         <v>253</v>
       </c>
-      <c r="C92" s="8" t="s">
+      <c r="C94" s="8" t="s">
         <v>244</v>
       </c>
-      <c r="D92" s="8" t="s">
+      <c r="D94" s="8" t="s">
         <v>253</v>
-      </c>
-      <c r="E92" s="8"/>
-      <c r="F92" s="12"/>
-    </row>
-    <row r="93" spans="1:25" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
-      <c r="A93" s="8" t="s">
-        <v>326</v>
-      </c>
-      <c r="B93" s="8" t="s">
-        <v>275</v>
-      </c>
-      <c r="C93" s="8" t="s">
-        <v>268</v>
-      </c>
-      <c r="D93" s="8" t="s">
-        <v>275</v>
-      </c>
-      <c r="E93" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="F93" s="12" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="94" spans="1:25" s="11" customFormat="1" ht="98" x14ac:dyDescent="0.15">
-      <c r="A94" s="8" t="s">
-        <v>321</v>
-      </c>
-      <c r="B94" s="8" t="s">
-        <v>322</v>
-      </c>
-      <c r="C94" s="8" t="s">
-        <v>245</v>
-      </c>
-      <c r="D94" s="8" t="s">
-        <v>254</v>
       </c>
       <c r="E94" s="8"/>
       <c r="F94" s="12"/>
     </row>
-    <row r="95" spans="1:25" s="11" customFormat="1" ht="126" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:25" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
       <c r="A95" s="8" t="s">
-        <v>246</v>
+        <v>326</v>
       </c>
       <c r="B95" s="8" t="s">
-        <v>255</v>
+        <v>275</v>
       </c>
       <c r="C95" s="8" t="s">
-        <v>246</v>
+        <v>268</v>
       </c>
       <c r="D95" s="8" t="s">
-        <v>255</v>
-      </c>
-      <c r="E95" s="8"/>
-      <c r="F95" s="12"/>
-    </row>
-    <row r="96" spans="1:25" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
+        <v>275</v>
+      </c>
+      <c r="E95" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="F95" s="12" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="96" spans="1:25" s="11" customFormat="1" ht="98" x14ac:dyDescent="0.15">
       <c r="A96" s="8" t="s">
-        <v>247</v>
+        <v>321</v>
       </c>
       <c r="B96" s="8" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C96" s="8" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D96" s="8" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E96" s="8"/>
       <c r="F96" s="12"/>
     </row>
-    <row r="97" spans="1:6" s="11" customFormat="1" ht="358" x14ac:dyDescent="0.15">
+    <row r="97" spans="1:6" s="11" customFormat="1" ht="126" x14ac:dyDescent="0.15">
       <c r="A97" s="8" t="s">
-        <v>205</v>
+        <v>246</v>
       </c>
       <c r="B97" s="8" t="s">
-        <v>333</v>
+        <v>255</v>
       </c>
       <c r="C97" s="8" t="s">
-        <v>205</v>
+        <v>246</v>
       </c>
       <c r="D97" s="8" t="s">
-        <v>329</v>
-      </c>
-      <c r="E97" s="9" t="s">
-        <v>232</v>
-      </c>
-      <c r="F97" s="10" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6" s="11" customFormat="1" ht="98" x14ac:dyDescent="0.15">
+        <v>255</v>
+      </c>
+      <c r="E97" s="8"/>
+      <c r="F97" s="12"/>
+    </row>
+    <row r="98" spans="1:6" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A98" s="8" t="s">
-        <v>277</v>
+        <v>247</v>
       </c>
       <c r="B98" s="8" t="s">
-        <v>278</v>
+        <v>323</v>
       </c>
       <c r="C98" s="8" t="s">
-        <v>25</v>
+        <v>247</v>
       </c>
       <c r="D98" s="8" t="s">
-        <v>227</v>
+        <v>256</v>
       </c>
       <c r="E98" s="8"/>
       <c r="F98" s="12"/>
     </row>
-    <row r="99" spans="1:6" s="11" customFormat="1" ht="56" x14ac:dyDescent="0.15">
+    <row r="99" spans="1:6" s="11" customFormat="1" ht="358" x14ac:dyDescent="0.15">
       <c r="A99" s="8" t="s">
-        <v>142</v>
+        <v>205</v>
       </c>
       <c r="B99" s="8" t="s">
-        <v>143</v>
+        <v>333</v>
       </c>
       <c r="C99" s="8" t="s">
-        <v>233</v>
-      </c>
-      <c r="D99" s="31" t="s">
-        <v>417</v>
-      </c>
-      <c r="E99" s="8"/>
-      <c r="F99" s="12"/>
-    </row>
-    <row r="100" spans="1:6" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
+        <v>205</v>
+      </c>
+      <c r="D99" s="8" t="s">
+        <v>329</v>
+      </c>
+      <c r="E99" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="F99" s="10" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" s="11" customFormat="1" ht="98" x14ac:dyDescent="0.15">
       <c r="A100" s="8" t="s">
-        <v>248</v>
+        <v>277</v>
       </c>
       <c r="B100" s="8" t="s">
-        <v>347</v>
+        <v>278</v>
       </c>
       <c r="C100" s="8" t="s">
-        <v>248</v>
+        <v>25</v>
       </c>
       <c r="D100" s="8" t="s">
-        <v>257</v>
+        <v>227</v>
       </c>
       <c r="E100" s="8"/>
       <c r="F100" s="12"/>
     </row>
     <row r="101" spans="1:6" s="11" customFormat="1" ht="56" x14ac:dyDescent="0.15">
       <c r="A101" s="8" t="s">
-        <v>348</v>
+        <v>142</v>
       </c>
       <c r="B101" s="8" t="s">
-        <v>349</v>
+        <v>143</v>
       </c>
       <c r="C101" s="8" t="s">
-        <v>249</v>
-      </c>
-      <c r="D101" s="8" t="s">
-        <v>258</v>
+        <v>233</v>
+      </c>
+      <c r="D101" s="31" t="s">
+        <v>417</v>
       </c>
       <c r="E101" s="8"/>
       <c r="F101" s="12"/>
     </row>
-    <row r="102" spans="1:6" s="11" customFormat="1" ht="112" x14ac:dyDescent="0.15">
-      <c r="A102" s="18" t="s">
-        <v>380</v>
+    <row r="102" spans="1:6" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
+      <c r="A102" s="8" t="s">
+        <v>248</v>
       </c>
       <c r="B102" s="8" t="s">
-        <v>382</v>
-      </c>
-      <c r="C102" s="8"/>
+        <v>347</v>
+      </c>
+      <c r="C102" s="8" t="s">
+        <v>248</v>
+      </c>
       <c r="D102" s="8" t="s">
-        <v>381</v>
+        <v>257</v>
       </c>
       <c r="E102" s="8"/>
       <c r="F102" s="12"/>
     </row>
-    <row r="103" spans="1:6" s="11" customFormat="1" ht="126" x14ac:dyDescent="0.15">
+    <row r="103" spans="1:6" s="11" customFormat="1" ht="56" x14ac:dyDescent="0.15">
       <c r="A103" s="8" t="s">
-        <v>383</v>
+        <v>348</v>
       </c>
       <c r="B103" s="8" t="s">
-        <v>384</v>
-      </c>
-      <c r="C103" s="8"/>
+        <v>349</v>
+      </c>
+      <c r="C103" s="8" t="s">
+        <v>249</v>
+      </c>
       <c r="D103" s="8" t="s">
-        <v>385</v>
+        <v>258</v>
       </c>
       <c r="E103" s="8"/>
       <c r="F103" s="12"/>
     </row>
-    <row r="104" spans="1:6" s="11" customFormat="1" ht="84" x14ac:dyDescent="0.15">
-      <c r="A104" s="8" t="s">
-        <v>144</v>
+    <row r="104" spans="1:6" s="11" customFormat="1" ht="112" x14ac:dyDescent="0.15">
+      <c r="A104" s="18" t="s">
+        <v>380</v>
       </c>
       <c r="B104" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="C104" s="8" t="s">
-        <v>144</v>
-      </c>
+        <v>382</v>
+      </c>
+      <c r="C104" s="8"/>
       <c r="D104" s="8" t="s">
-        <v>341</v>
+        <v>381</v>
       </c>
       <c r="E104" s="8"/>
       <c r="F104" s="12"/>
     </row>
-    <row r="105" spans="1:6" s="11" customFormat="1" ht="409.6" x14ac:dyDescent="0.15">
+    <row r="105" spans="1:6" s="11" customFormat="1" ht="126" x14ac:dyDescent="0.15">
       <c r="A105" s="8" t="s">
-        <v>434</v>
+        <v>383</v>
       </c>
       <c r="B105" s="8" t="s">
-        <v>431</v>
-      </c>
-      <c r="C105" s="8" t="s">
-        <v>153</v>
-      </c>
+        <v>384</v>
+      </c>
+      <c r="C105" s="8"/>
       <c r="D105" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="E105" s="14" t="s">
-        <v>155</v>
-      </c>
-      <c r="F105" s="12" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
+        <v>385</v>
+      </c>
+      <c r="E105" s="8"/>
+      <c r="F105" s="12"/>
+    </row>
+    <row r="106" spans="1:6" s="11" customFormat="1" ht="84" x14ac:dyDescent="0.15">
       <c r="A106" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B106" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C106" s="8" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D106" s="8" t="s">
-        <v>234</v>
+        <v>341</v>
       </c>
       <c r="E106" s="8"/>
       <c r="F106" s="12"/>
     </row>
-    <row r="107" spans="1:6" s="11" customFormat="1" ht="140" x14ac:dyDescent="0.15">
+    <row r="107" spans="1:6" s="11" customFormat="1" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A107" s="8" t="s">
-        <v>149</v>
+        <v>434</v>
       </c>
       <c r="B107" s="8" t="s">
-        <v>150</v>
+        <v>431</v>
       </c>
       <c r="C107" s="8" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="D107" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="E107" s="8"/>
-      <c r="F107" s="12"/>
-    </row>
-    <row r="108" spans="1:6" s="11" customFormat="1" ht="56" x14ac:dyDescent="0.15">
+        <v>154</v>
+      </c>
+      <c r="E107" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="F107" s="12" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
       <c r="A108" s="8" t="s">
-        <v>212</v>
+        <v>146</v>
       </c>
       <c r="B108" s="8" t="s">
-        <v>213</v>
+        <v>147</v>
       </c>
       <c r="C108" s="8" t="s">
-        <v>212</v>
+        <v>148</v>
       </c>
       <c r="D108" s="8" t="s">
-        <v>357</v>
+        <v>234</v>
       </c>
       <c r="E108" s="8"/>
       <c r="F108" s="12"/>
     </row>
-    <row r="109" spans="1:6" s="3" customFormat="1" ht="85" x14ac:dyDescent="0.15">
-      <c r="A109" s="1" t="s">
-        <v>407</v>
-      </c>
-      <c r="B109" s="1" t="s">
-        <v>408</v>
-      </c>
-      <c r="C109" s="1"/>
-      <c r="D109" s="1"/>
-      <c r="E109" s="1"/>
-      <c r="F109" s="2"/>
-    </row>
-    <row r="110" spans="1:6" s="11" customFormat="1" ht="112" x14ac:dyDescent="0.15">
+    <row r="109" spans="1:6" s="11" customFormat="1" ht="140" x14ac:dyDescent="0.15">
+      <c r="A109" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="B109" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="C109" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="D109" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="E109" s="8"/>
+      <c r="F109" s="12"/>
+    </row>
+    <row r="110" spans="1:6" s="11" customFormat="1" ht="56" x14ac:dyDescent="0.15">
       <c r="A110" s="8" t="s">
-        <v>304</v>
+        <v>212</v>
       </c>
       <c r="B110" s="8" t="s">
-        <v>306</v>
+        <v>213</v>
       </c>
       <c r="C110" s="8" t="s">
-        <v>239</v>
+        <v>212</v>
       </c>
       <c r="D110" s="8" t="s">
-        <v>240</v>
+        <v>357</v>
       </c>
       <c r="E110" s="8"/>
       <c r="F110" s="12"/>
     </row>
-    <row r="111" spans="1:6" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
-      <c r="A111" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="B111" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="C111" s="8"/>
-      <c r="D111" s="8"/>
-      <c r="E111" s="8"/>
-      <c r="F111" s="12"/>
-    </row>
-    <row r="112" spans="1:6" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
+    <row r="111" spans="1:6" s="3" customFormat="1" ht="85" x14ac:dyDescent="0.15">
+      <c r="A111" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="C111" s="1"/>
+      <c r="D111" s="1"/>
+      <c r="E111" s="1"/>
+      <c r="F111" s="2"/>
+    </row>
+    <row r="112" spans="1:6" s="11" customFormat="1" ht="112" x14ac:dyDescent="0.15">
       <c r="A112" s="8" t="s">
-        <v>317</v>
+        <v>304</v>
       </c>
       <c r="B112" s="8" t="s">
-        <v>318</v>
+        <v>306</v>
       </c>
       <c r="C112" s="8" t="s">
-        <v>273</v>
+        <v>239</v>
       </c>
       <c r="D112" s="8" t="s">
-        <v>272</v>
+        <v>240</v>
       </c>
       <c r="E112" s="8"/>
       <c r="F112" s="12"/>
     </row>
-    <row r="113" spans="1:6" s="11" customFormat="1" ht="112" x14ac:dyDescent="0.15">
+    <row r="113" spans="1:6" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A113" s="8" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="B113" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="C113" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="D113" s="8" t="s">
-        <v>316</v>
-      </c>
+        <v>158</v>
+      </c>
+      <c r="C113" s="8"/>
+      <c r="D113" s="8"/>
       <c r="E113" s="8"/>
       <c r="F113" s="12"/>
     </row>
-    <row r="114" spans="1:6" s="11" customFormat="1" ht="126" x14ac:dyDescent="0.15">
+    <row r="114" spans="1:6" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A114" s="8" t="s">
-        <v>167</v>
+        <v>317</v>
       </c>
       <c r="B114" s="8" t="s">
-        <v>168</v>
+        <v>318</v>
       </c>
       <c r="C114" s="8" t="s">
-        <v>169</v>
+        <v>273</v>
       </c>
       <c r="D114" s="8" t="s">
-        <v>170</v>
+        <v>272</v>
       </c>
       <c r="E114" s="8"/>
       <c r="F114" s="12"/>
     </row>
-    <row r="115" spans="1:6" s="11" customFormat="1" ht="252" x14ac:dyDescent="0.15">
+    <row r="115" spans="1:6" s="11" customFormat="1" ht="112" x14ac:dyDescent="0.15">
       <c r="A115" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="B115" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="C115" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="D115" s="8" t="s">
+        <v>316</v>
+      </c>
+      <c r="E115" s="8"/>
+      <c r="F115" s="12"/>
+    </row>
+    <row r="116" spans="1:6" s="11" customFormat="1" ht="126" x14ac:dyDescent="0.15">
+      <c r="A116" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="B116" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="C116" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="D116" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="E116" s="8"/>
+      <c r="F116" s="12"/>
+    </row>
+    <row r="117" spans="1:6" s="11" customFormat="1" ht="252" x14ac:dyDescent="0.15">
+      <c r="A117" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="B115" s="8" t="s">
+      <c r="B117" s="8" t="s">
         <v>283</v>
       </c>
-      <c r="C115" s="8" t="s">
+      <c r="C117" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="D115" s="8" t="s">
+      <c r="D117" s="8" t="s">
         <v>161</v>
       </c>
-      <c r="E115" s="14" t="s">
+      <c r="E117" s="14" t="s">
         <v>162</v>
       </c>
-      <c r="F115" s="12" t="s">
+      <c r="F117" s="12" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="116" spans="1:6" s="11" customFormat="1" ht="80" x14ac:dyDescent="0.15">
-      <c r="A116" s="8" t="s">
+    <row r="118" spans="1:6" s="11" customFormat="1" ht="80" x14ac:dyDescent="0.15">
+      <c r="A118" s="8" t="s">
         <v>259</v>
       </c>
-      <c r="B116" s="35" t="s">
+      <c r="B118" s="35" t="s">
         <v>424</v>
       </c>
-      <c r="C116" s="8" t="s">
+      <c r="C118" s="8" t="s">
         <v>259</v>
       </c>
-      <c r="D116" s="35" t="s">
+      <c r="D118" s="35" t="s">
         <v>424</v>
       </c>
-      <c r="E116" s="8"/>
-      <c r="F116" s="12" t="s">
+      <c r="E118" s="8"/>
+      <c r="F118" s="12" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="117" spans="1:6" s="11" customFormat="1" ht="144" x14ac:dyDescent="0.15">
-      <c r="A117" s="8" t="s">
+    <row r="119" spans="1:6" s="11" customFormat="1" ht="144" x14ac:dyDescent="0.15">
+      <c r="A119" s="8" t="s">
         <v>425</v>
       </c>
-      <c r="B117" s="35" t="s">
+      <c r="B119" s="35" t="s">
         <v>426</v>
       </c>
-      <c r="C117" s="8"/>
-      <c r="D117" s="33"/>
-      <c r="E117" s="8"/>
-      <c r="F117" s="34" t="s">
+      <c r="C119" s="8"/>
+      <c r="D119" s="33"/>
+      <c r="E119" s="8"/>
+      <c r="F119" s="34" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="118" spans="1:6" s="11" customFormat="1" ht="84" x14ac:dyDescent="0.15">
-      <c r="A118" s="8" t="s">
+    <row r="120" spans="1:6" s="11" customFormat="1" ht="84" x14ac:dyDescent="0.15">
+      <c r="A120" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="B118" s="8" t="s">
+      <c r="B120" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="C118" s="8" t="s">
+      <c r="C120" s="8" t="s">
         <v>173</v>
       </c>
-      <c r="D118" s="8" t="s">
+      <c r="D120" s="8" t="s">
         <v>174</v>
       </c>
-      <c r="E118" s="14" t="s">
+      <c r="E120" s="14" t="s">
         <v>175</v>
       </c>
-      <c r="F118" s="12" t="s">
+      <c r="F120" s="12" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="119" spans="1:6" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
-      <c r="A119" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="B119" s="8" t="s">
-        <v>178</v>
-      </c>
-      <c r="C119" s="8"/>
-      <c r="D119" s="8"/>
-      <c r="E119" s="14" t="s">
-        <v>179</v>
-      </c>
-      <c r="F119" s="12" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="120" spans="1:6" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
-      <c r="A120" s="8" t="s">
-        <v>181</v>
-      </c>
-      <c r="B120" s="8" t="s">
-        <v>182</v>
-      </c>
-      <c r="C120" s="8"/>
-      <c r="D120" s="8"/>
-      <c r="E120" s="8"/>
-      <c r="F120" s="12"/>
     </row>
     <row r="121" spans="1:6" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A121" s="8" t="s">
-        <v>201</v>
+        <v>177</v>
       </c>
       <c r="B121" s="8" t="s">
-        <v>284</v>
+        <v>178</v>
       </c>
       <c r="C121" s="8"/>
       <c r="D121" s="8"/>
-      <c r="E121" s="8"/>
-      <c r="F121" s="12"/>
-    </row>
-    <row r="122" spans="1:6" s="11" customFormat="1" ht="84" x14ac:dyDescent="0.15">
+      <c r="E121" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="F121" s="12" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
       <c r="A122" s="8" t="s">
-        <v>419</v>
-      </c>
-      <c r="B122" s="32" t="s">
-        <v>418</v>
-      </c>
-      <c r="C122" s="8" t="s">
-        <v>419</v>
-      </c>
-      <c r="D122" s="8" t="s">
-        <v>421</v>
-      </c>
+        <v>181</v>
+      </c>
+      <c r="B122" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="C122" s="8"/>
+      <c r="D122" s="8"/>
       <c r="E122" s="8"/>
       <c r="F122" s="12"/>
     </row>
-    <row r="123" spans="1:6" s="11" customFormat="1" ht="126" x14ac:dyDescent="0.15">
+    <row r="123" spans="1:6" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A123" s="8" t="s">
-        <v>375</v>
-      </c>
-      <c r="B123" s="19" t="s">
-        <v>386</v>
+        <v>201</v>
+      </c>
+      <c r="B123" s="8" t="s">
+        <v>284</v>
       </c>
       <c r="C123" s="8"/>
-      <c r="D123" s="19" t="s">
-        <v>376</v>
-      </c>
+      <c r="D123" s="8"/>
       <c r="E123" s="8"/>
       <c r="F123" s="12"/>
     </row>
-    <row r="124" spans="1:6" s="11" customFormat="1" ht="224" x14ac:dyDescent="0.15">
+    <row r="124" spans="1:6" s="11" customFormat="1" ht="84" x14ac:dyDescent="0.15">
       <c r="A124" s="8" t="s">
-        <v>377</v>
-      </c>
-      <c r="B124" s="8" t="s">
-        <v>378</v>
-      </c>
-      <c r="C124" s="8"/>
-      <c r="D124" s="20" t="s">
-        <v>379</v>
+        <v>419</v>
+      </c>
+      <c r="B124" s="32" t="s">
+        <v>418</v>
+      </c>
+      <c r="C124" s="8" t="s">
+        <v>419</v>
+      </c>
+      <c r="D124" s="8" t="s">
+        <v>421</v>
       </c>
       <c r="E124" s="8"/>
       <c r="F124" s="12"/>
     </row>
-    <row r="125" spans="1:6" s="11" customFormat="1" ht="224" x14ac:dyDescent="0.15">
+    <row r="125" spans="1:6" s="11" customFormat="1" ht="126" x14ac:dyDescent="0.15">
       <c r="A125" s="8" t="s">
-        <v>183</v>
-      </c>
-      <c r="B125" s="8" t="s">
-        <v>184</v>
-      </c>
-      <c r="C125" s="8" t="s">
-        <v>185</v>
-      </c>
-      <c r="D125" s="8" t="s">
-        <v>186</v>
+        <v>375</v>
+      </c>
+      <c r="B125" s="19" t="s">
+        <v>386</v>
+      </c>
+      <c r="C125" s="8"/>
+      <c r="D125" s="19" t="s">
+        <v>376</v>
       </c>
       <c r="E125" s="8"/>
       <c r="F125" s="12"/>
     </row>
-    <row r="126" spans="1:6" s="11" customFormat="1" ht="84" x14ac:dyDescent="0.15">
+    <row r="126" spans="1:6" s="11" customFormat="1" ht="224" x14ac:dyDescent="0.15">
       <c r="A126" s="8" t="s">
-        <v>187</v>
+        <v>377</v>
       </c>
       <c r="B126" s="8" t="s">
-        <v>188</v>
+        <v>378</v>
       </c>
       <c r="C126" s="8"/>
-      <c r="D126" s="8"/>
-      <c r="E126" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="F126" s="12" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="127" spans="1:6" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
+      <c r="D126" s="20" t="s">
+        <v>379</v>
+      </c>
+      <c r="E126" s="8"/>
+      <c r="F126" s="12"/>
+    </row>
+    <row r="127" spans="1:6" s="11" customFormat="1" ht="224" x14ac:dyDescent="0.15">
       <c r="A127" s="8" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="B127" s="8" t="s">
-        <v>191</v>
-      </c>
-      <c r="C127" s="8"/>
-      <c r="D127" s="8"/>
+        <v>184</v>
+      </c>
+      <c r="C127" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="D127" s="8" t="s">
+        <v>186</v>
+      </c>
       <c r="E127" s="8"/>
       <c r="F127" s="12"/>
     </row>
-    <row r="128" spans="1:6" s="11" customFormat="1" ht="358" x14ac:dyDescent="0.15">
+    <row r="128" spans="1:6" s="11" customFormat="1" ht="84" x14ac:dyDescent="0.15">
       <c r="A128" s="8" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="B128" s="8" t="s">
-        <v>420</v>
-      </c>
-      <c r="C128" s="8" t="s">
-        <v>235</v>
-      </c>
-      <c r="D128" s="8" t="s">
-        <v>236</v>
-      </c>
-      <c r="E128" s="8" t="s">
-        <v>422</v>
+        <v>188</v>
+      </c>
+      <c r="C128" s="8"/>
+      <c r="D128" s="8"/>
+      <c r="E128" s="14" t="s">
+        <v>77</v>
       </c>
       <c r="F128" s="12" t="s">
-        <v>423</v>
+        <v>189</v>
       </c>
     </row>
     <row r="129" spans="1:6" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A129" s="8" t="s">
-        <v>267</v>
+        <v>190</v>
       </c>
       <c r="B129" s="8" t="s">
-        <v>274</v>
-      </c>
-      <c r="C129" s="8" t="s">
-        <v>267</v>
-      </c>
-      <c r="D129" s="8" t="s">
-        <v>274</v>
-      </c>
+        <v>191</v>
+      </c>
+      <c r="C129" s="8"/>
+      <c r="D129" s="8"/>
       <c r="E129" s="8"/>
       <c r="F129" s="12"/>
     </row>
-    <row r="130" spans="1:6" s="11" customFormat="1" ht="140" x14ac:dyDescent="0.15">
+    <row r="130" spans="1:6" s="11" customFormat="1" ht="358" x14ac:dyDescent="0.15">
       <c r="A130" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B130" s="8" t="s">
-        <v>194</v>
+        <v>420</v>
       </c>
       <c r="C130" s="8" t="s">
-        <v>193</v>
+        <v>235</v>
       </c>
       <c r="D130" s="8" t="s">
-        <v>285</v>
-      </c>
-      <c r="E130" s="8"/>
-      <c r="F130" s="12"/>
-    </row>
-    <row r="131" spans="1:6" s="11" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+        <v>236</v>
+      </c>
+      <c r="E130" s="8" t="s">
+        <v>422</v>
+      </c>
+      <c r="F130" s="12" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A131" s="8" t="s">
-        <v>214</v>
+        <v>267</v>
       </c>
       <c r="B131" s="8" t="s">
-        <v>215</v>
-      </c>
-      <c r="C131" s="8"/>
-      <c r="D131" s="8"/>
+        <v>274</v>
+      </c>
+      <c r="C131" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="D131" s="8" t="s">
+        <v>274</v>
+      </c>
       <c r="E131" s="8"/>
       <c r="F131" s="12"/>
     </row>
-    <row r="133" spans="1:6" s="11" customFormat="1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A133" s="8"/>
-      <c r="B133" s="8"/>
+    <row r="132" spans="1:6" s="11" customFormat="1" ht="140" x14ac:dyDescent="0.15">
+      <c r="A132" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="B132" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="C132" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="D132" s="8" t="s">
+        <v>285</v>
+      </c>
+      <c r="E132" s="8"/>
+      <c r="F132" s="12"/>
+    </row>
+    <row r="133" spans="1:6" s="11" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A133" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="B133" s="8" t="s">
+        <v>215</v>
+      </c>
       <c r="C133" s="8"/>
       <c r="D133" s="8"/>
       <c r="E133" s="8"/>
       <c r="F133" s="12"/>
     </row>
-    <row r="134" spans="1:6" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="135" spans="1:6" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="135" spans="1:6" s="11" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A135" s="8"/>
+      <c r="B135" s="8"/>
+      <c r="C135" s="8"/>
+      <c r="D135" s="8"/>
+      <c r="E135" s="8"/>
+      <c r="F135" s="12"/>
+    </row>
     <row r="136" spans="1:6" ht="13" x14ac:dyDescent="0.15"/>
     <row r="137" spans="1:6" ht="13" x14ac:dyDescent="0.15"/>
     <row r="138" spans="1:6" ht="13" x14ac:dyDescent="0.15"/>
@@ -5560,14 +5637,16 @@
     <row r="1028" ht="13" x14ac:dyDescent="0.15"/>
     <row r="1029" ht="13" x14ac:dyDescent="0.15"/>
     <row r="1030" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="1031" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="1032" ht="13" x14ac:dyDescent="0.15"/>
   </sheetData>
-  <autoFilter ref="A1:Y132" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Y132">
-      <sortCondition ref="A1:A132"/>
+  <autoFilter ref="A1:Y134" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Y134">
+      <sortCondition ref="A1:A134"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Y1030">
-    <sortCondition ref="A2:A1030"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Y1032">
+    <sortCondition ref="A2:A1032"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="E19" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -5577,36 +5656,36 @@
     <hyperlink ref="E35" r:id="rId5" location="se2.1.200_124" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
     <hyperlink ref="E30" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
     <hyperlink ref="E38" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="E50" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="E53" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="E60" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="E67" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="E70" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="E80" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="E72" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="E82" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="E90" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="E105" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="E115" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="E118" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="E119" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="E126" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="E77" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="E51" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="E54" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="E61" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="E68" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="E71" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="E81" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="E73" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="E83" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="E92" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="E107" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="E117" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="E120" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="E121" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="E128" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="E78" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
     <hyperlink ref="E34" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
     <hyperlink ref="E2" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="E97" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="E62" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="E89" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="E99" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="E63" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="E91" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
     <hyperlink ref="F2" r:id="rId28" display="https://www.whitehouse.gov/sites/whitehouse.gov/files/omb/assets/a11_current_year/a11_2017.pdf" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
     <hyperlink ref="E9" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
     <hyperlink ref="E18" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
     <hyperlink ref="E26" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
     <hyperlink ref="E25" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
     <hyperlink ref="E24" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="E47" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="F62" r:id="rId35" display="https://www.whitehouse.gov/sites/whitehouse.gov/files/omb/assets/a11_current_year/a11_2017.pdf" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="F89" r:id="rId36" display="https://www.whitehouse.gov/sites/whitehouse.gov/files/omb/assets/a11_current_year/a11_2017.pdf" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="F97" r:id="rId37" display="https://www.whitehouse.gov/sites/whitehouse.gov/files/omb/assets/a11_current_year/a11_2017.pdf" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="E48" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="F63" r:id="rId35" display="https://www.whitehouse.gov/sites/whitehouse.gov/files/omb/assets/a11_current_year/a11_2017.pdf" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="F91" r:id="rId36" display="https://www.whitehouse.gov/sites/whitehouse.gov/files/omb/assets/a11_current_year/a11_2017.pdf" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="F99" r:id="rId37" display="https://www.whitehouse.gov/sites/whitehouse.gov/files/omb/assets/a11_current_year/a11_2017.pdf" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId38"/>

</xml_diff>

<commit_message>
[DEV-7045] Adds DEFC V to glossary
</commit_message>
<xml_diff>
--- a/usaspending_api/data/USAspendingGlossary.xlsx
+++ b/usaspending_api/data/USAspendingGlossary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10212"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emilybrents/Documents/data_act/usaspending-api/usaspending_api/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/williamcollins/projects/data_act/usaspending-api/usaspending_api/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5180E5B-D727-A548-9C17-5F70DA69C8AC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3213AAD-5BEE-034C-A5ED-8F388618D009}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18900" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="45460" yWindow="-8020" windowWidth="33600" windowHeight="18900" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1837,7 +1837,8 @@
 - **DEFC ‘N’**  Public Law 116-136, designated as emergency
 - **DEFC ‘O’**  Public Law 116-136, Public Law 116-139, and Public Law 116-260, not designated as emergency
 - **DEFC ‘P’**  Public Law 116-139, designated as emergency
-- **DEFC 'U'**  Public Law 116-260, designated as emergency
+- **DEFC ‘U‘'**  Public Law 116-260, designated as emergency
+- **DEFC 'V'**  Public Law 117-2, American Rescue Plan Act of 2021, not designated as emergency
 Note that the National Interest Action (NIA) code is also used to track COVID-19 spending. However, it only applies to procurement actions (i.e., contracts) and is not necessarily tied to COVID-19 supplemental appropriations. Thus, awards with the COVID-19 NIA value may not have a COVID-19 DEFC value, and vice versa.</t>
   </si>
 </sst>

</xml_diff>

<commit_message>
[DEV-7045] Fixes quotes on DEFC U
</commit_message>
<xml_diff>
--- a/usaspending_api/data/USAspendingGlossary.xlsx
+++ b/usaspending_api/data/USAspendingGlossary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/williamcollins/projects/data_act/usaspending-api/usaspending_api/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3213AAD-5BEE-034C-A5ED-8F388618D009}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CC52F07-2621-2F41-970C-48043D17329E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45460" yWindow="-8020" windowWidth="33600" windowHeight="18900" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40960" yWindow="-14400" windowWidth="51200" windowHeight="28340" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1837,7 +1837,7 @@
 - **DEFC ‘N’**  Public Law 116-136, designated as emergency
 - **DEFC ‘O’**  Public Law 116-136, Public Law 116-139, and Public Law 116-260, not designated as emergency
 - **DEFC ‘P’**  Public Law 116-139, designated as emergency
-- **DEFC ‘U‘'**  Public Law 116-260, designated as emergency
+- **DEFC ‘U’**  Public Law 116-260, designated as emergency
 - **DEFC 'V'**  Public Law 117-2, American Rescue Plan Act of 2021, not designated as emergency
 Note that the National Interest Action (NIA) code is also used to track COVID-19 spending. However, it only applies to procurement actions (i.e., contracts) and is not necessarily tied to COVID-19 supplemental appropriations. Thus, awards with the COVID-19 NIA value may not have a COVID-19 DEFC value, and vice versa.</t>
   </si>
@@ -2451,8 +2451,8 @@
   <dimension ref="A1:Y1032"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D44" sqref="D44"/>
+      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
[DEV-7045] Fixes quotes on DEFC V
</commit_message>
<xml_diff>
--- a/usaspending_api/data/USAspendingGlossary.xlsx
+++ b/usaspending_api/data/USAspendingGlossary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/williamcollins/projects/data_act/usaspending-api/usaspending_api/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CC52F07-2621-2F41-970C-48043D17329E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA423F9A-B44B-1C4D-9073-456D2E72C9A8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40960" yWindow="-14400" windowWidth="51200" windowHeight="28340" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1838,7 +1838,7 @@
 - **DEFC ‘O’**  Public Law 116-136, Public Law 116-139, and Public Law 116-260, not designated as emergency
 - **DEFC ‘P’**  Public Law 116-139, designated as emergency
 - **DEFC ‘U’**  Public Law 116-260, designated as emergency
-- **DEFC 'V'**  Public Law 117-2, American Rescue Plan Act of 2021, not designated as emergency
+- **DEFC ‘V’**  Public Law 117-2, American Rescue Plan Act of 2021, not designated as emergency
 Note that the National Interest Action (NIA) code is also used to track COVID-19 spending. However, it only applies to procurement actions (i.e., contracts) and is not necessarily tied to COVID-19 supplemental appropriations. Thus, awards with the COVID-19 NIA value may not have a COVID-19 DEFC value, and vice versa.</t>
   </si>
 </sst>
@@ -2451,8 +2451,8 @@
   <dimension ref="A1:Y1032"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E48" sqref="E48"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>